<commit_message>
feat(functions): Add ISERROR and ISERR functions.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -376,7 +376,7 @@
   <dimension ref="B1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16:L17"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -693,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>[1]Sheet1!$A$1+1</f>
         <v>3</v>
@@ -709,7 +709,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>[1]Sheet1!$A$1+[1]Sheet1!$A$2</f>
         <v>4</v>
@@ -723,20 +723,24 @@
       <c r="J18" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <f ca="1">IFERROR(INDIRECT("ab")+1, 33)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E19">
         <f>D16*3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H20">
         <f t="array" ref="H20:H24">IF(G9:G12&lt;&gt;H10:H13,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F21">
         <f>C19+1</f>
         <v>1</v>
@@ -744,20 +748,32 @@
       <c r="H21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L21" t="b">
+        <f>ISERROR(J18)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L23" t="b">
+        <f>ISERR(J16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H24" t="e">
         <v>#N/A</v>
+      </c>
+      <c r="L24" t="b">
+        <f>ISERR(K12)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a wrapper for numpy ufuncs, mapped some Excel functions to ufuncs and provided tests
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sandboxes\excel2py\formulas\test\test_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16305" tabRatio="500"/>
   </bookViews>
@@ -21,7 +26,7 @@
     <definedName name="f">Sheet1!$G$2:$H$5</definedName>
     <definedName name="g">Sheet2!$B$2:$B$5</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,9 +36,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ca</t>
+  </si>
+  <si>
+    <t>LN</t>
+  </si>
+  <si>
+    <t>LOG</t>
+  </si>
+  <si>
+    <t>EXP</t>
+  </si>
+  <si>
+    <t>SIN</t>
+  </si>
+  <si>
+    <t>ACOS</t>
+  </si>
+  <si>
+    <t>ACOSH</t>
+  </si>
+  <si>
+    <t>COS</t>
+  </si>
+  <si>
+    <t>COSH</t>
+  </si>
+  <si>
+    <t>ASIN</t>
+  </si>
+  <si>
+    <t>ASINH</t>
+  </si>
+  <si>
+    <t>ATAN</t>
+  </si>
+  <si>
+    <t>ATAN2</t>
+  </si>
+  <si>
+    <t>ATANH</t>
+  </si>
+  <si>
+    <t>SINH</t>
+  </si>
+  <si>
+    <t>TAN</t>
+  </si>
+  <si>
+    <t>TANH</t>
   </si>
 </sst>
 </file>
@@ -81,6 +134,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -365,7 +421,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -373,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N24"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -693,7 +749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>[1]Sheet1!$A$1+1</f>
         <v>3</v>
@@ -709,7 +765,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>[1]Sheet1!$A$1+[1]Sheet1!$A$2</f>
         <v>4</v>
@@ -728,19 +784,19 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E19">
         <f>D16*3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H20">
         <f t="array" ref="H20:H24">IF(G9:G12&lt;&gt;H10:H13,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F21">
         <f>C19+1</f>
         <v>1</v>
@@ -753,12 +809,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H23">
         <v>1</v>
       </c>
@@ -767,7 +823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H24" t="e">
         <v>#N/A</v>
       </c>
@@ -776,8 +832,710 @@
         <v>1</v>
       </c>
     </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>2.5</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
+      <c r="F26">
+        <v>-1</v>
+      </c>
+      <c r="H26">
+        <f>LN(B26)</f>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f>LN(C26)</f>
+        <v>0.91629073187415511</v>
+      </c>
+      <c r="J26">
+        <f>LN(D26)</f>
+        <v>1.0986122886681098</v>
+      </c>
+      <c r="K26">
+        <f>LN(E26)</f>
+        <v>2.3025850929940459</v>
+      </c>
+      <c r="L26" t="e">
+        <f>LN(F26)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N26">
+        <f t="array" ref="N26">SUM(LN(B26:E26))</f>
+        <v>4.317488113536311</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>2.5</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <v>-1</v>
+      </c>
+      <c r="H27">
+        <f>LOG(B27)</f>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ref="I27:L29" si="0">LOG(C27)</f>
+        <v>0.3979400086720376</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>0.47712125471966244</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L27" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N27">
+        <f t="array" ref="N27">SUM(LOG(B27:E27))</f>
+        <v>1.8750612633917001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>2.5</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>10</v>
+      </c>
+      <c r="H28">
+        <f>EXP(B28)</f>
+        <v>2.7182818284590451</v>
+      </c>
+      <c r="I28">
+        <f t="shared" ref="I28:K28" si="1">EXP(C28)</f>
+        <v>12.182493960703473</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>20.085536923187668</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>22026.465794806718</v>
+      </c>
+      <c r="L28" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N28">
+        <f t="array" ref="N28">SUM(EXP(B28:E28))</f>
+        <v>22061.452107519068</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0.2</v>
+      </c>
+      <c r="D29">
+        <v>0.5</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <f>ACOS(B29)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I29">
+        <f t="shared" ref="I29:L29" si="2">ACOS(C29)</f>
+        <v>1.3694384060045657</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L29" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N29">
+        <f t="array" ref="N29">SUM(ACOS(B29:E29))</f>
+        <v>3.9874322839960596</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>0.5</v>
+      </c>
+      <c r="H30">
+        <f>ACOSH(B30)</f>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f t="shared" ref="I30:L30" si="3">ACOSH(C30)</f>
+        <v>1.3169578969248166</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="3"/>
+        <v>1.7627471740390861</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="3"/>
+        <v>2.0634370688955608</v>
+      </c>
+      <c r="L30" t="e">
+        <f>ACOSH(F30)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N30">
+        <f t="array" ref="N30">SUM(ACOSH(B30:E30))</f>
+        <v>5.1431421398594637</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0.2</v>
+      </c>
+      <c r="D31">
+        <v>0.5</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <f>ASIN(B31)</f>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" ref="I31:L31" si="4">ASIN(C31)</f>
+        <v>0.20135792079033082</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="4"/>
+        <v>0.52359877559829893</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="4"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="L31" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N31">
+        <f t="array" ref="N31">SUM(ASIN(B31:E31))</f>
+        <v>2.2957530231835266</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>-5</v>
+      </c>
+      <c r="C32">
+        <v>-1</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>20</v>
+      </c>
+      <c r="F32">
+        <v>100</v>
+      </c>
+      <c r="H32">
+        <f>ASINH(B32)</f>
+        <v>-2.3124383412727525</v>
+      </c>
+      <c r="I32">
+        <f t="shared" ref="I32:L32" si="5">ASINH(C32)</f>
+        <v>-0.88137358701954294</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="5"/>
+        <v>3.6895038689889059</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="5"/>
+        <v>5.2983423656105888</v>
+      </c>
+      <c r="N32">
+        <f t="array" ref="N32">SUM(ASINH(B32:E32))</f>
+        <v>0.49569194069661027</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0.2</v>
+      </c>
+      <c r="D33">
+        <v>0.5</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>-10</v>
+      </c>
+      <c r="H33">
+        <f>ATAN(B33)</f>
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <f t="shared" ref="I33:L33" si="6">ATAN(C33)</f>
+        <v>0.19739555984988078</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="6"/>
+        <v>0.46364760900080609</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="6"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="6"/>
+        <v>-1.4711276743037347</v>
+      </c>
+      <c r="N33">
+        <f t="array" ref="N33">SUM(ATAN(B33:E33))</f>
+        <v>1.4464413322481351</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0.2</v>
+      </c>
+      <c r="D34">
+        <v>0.5</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <f>ATAN2(B34,C34)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I34">
+        <f t="shared" ref="I34:L34" si="7">ATAN2(C34,D34)</f>
+        <v>1.1902899496825317</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="7"/>
+        <v>1.1071487177940904</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="7"/>
+        <v>1.1071487177940904</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <f t="array" ref="N34">SUM(ATAN2(B34:E34,C34:F34))</f>
+        <v>4.975383712065609</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0.1</v>
+      </c>
+      <c r="D35">
+        <v>0.5</v>
+      </c>
+      <c r="E35">
+        <v>0.95</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <f>ATANH(B35)</f>
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f>ATANH(C35)</f>
+        <v>0.10033534773107562</v>
+      </c>
+      <c r="J35">
+        <f>ATANH(D35)</f>
+        <v>0.54930614433405489</v>
+      </c>
+      <c r="K35">
+        <f>ATANH(E35)</f>
+        <v>1.8317808230648227</v>
+      </c>
+      <c r="L35" t="e">
+        <f>ATANH(F35)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N35">
+        <f t="array" ref="N35">SUM(ATANH(B35:E35))</f>
+        <v>2.4814223151299535</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0.5</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>-1</v>
+      </c>
+      <c r="F36">
+        <v>10</v>
+      </c>
+      <c r="H36">
+        <f>COS(B36)</f>
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <f t="shared" ref="I36:L36" si="8">COS(C36)</f>
+        <v>0.87758256189037276</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="8"/>
+        <v>0.54030230586813977</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="8"/>
+        <v>0.54030230586813977</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="8"/>
+        <v>-0.83907152907645244</v>
+      </c>
+      <c r="N36">
+        <f t="array" ref="N36">SUM(COS(B36:E36))</f>
+        <v>2.9581871736266523</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0.5</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>-1</v>
+      </c>
+      <c r="F37">
+        <v>10</v>
+      </c>
+      <c r="H37">
+        <f>COSH(B37)</f>
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <f t="shared" ref="I37:L37" si="9">COSH(C37)</f>
+        <v>1.1276259652063807</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="9"/>
+        <v>1.5430806348152437</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="9"/>
+        <v>1.5430806348152437</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="9"/>
+        <v>11013.232920103324</v>
+      </c>
+      <c r="N37">
+        <f t="array" ref="N37">SUM(COSH(B37:E37))</f>
+        <v>5.2137872348368681</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0.5</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>-1</v>
+      </c>
+      <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="H38">
+        <f>SIN(B38)</f>
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f t="shared" ref="I38:L38" si="10">SIN(C38)</f>
+        <v>0.47942553860420301</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="10"/>
+        <v>0.8414709848078965</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="10"/>
+        <v>-0.8414709848078965</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="10"/>
+        <v>-0.54402111088936977</v>
+      </c>
+      <c r="N38">
+        <f t="array" ref="N38">SUM(SIN(B38:E38))</f>
+        <v>0.47942553860420301</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0.5</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>-1</v>
+      </c>
+      <c r="F39">
+        <v>10</v>
+      </c>
+      <c r="H39">
+        <f>SINH(B39)</f>
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <f t="shared" ref="I39:L39" si="11">SINH(C39)</f>
+        <v>0.52109530549374738</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="11"/>
+        <v>1.1752011936438014</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="11"/>
+        <v>-1.1752011936438014</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="11"/>
+        <v>11013.232874703393</v>
+      </c>
+      <c r="N39">
+        <f t="array" ref="N39">SUM(SINH(B39:E39))</f>
+        <v>0.5210953054937475</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0.5</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>-1</v>
+      </c>
+      <c r="F40">
+        <v>10</v>
+      </c>
+      <c r="H40">
+        <f>TAN(B40)</f>
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <f t="shared" ref="I40:L40" si="12">TAN(C40)</f>
+        <v>0.54630248984379048</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="12"/>
+        <v>1.5574077246549023</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="12"/>
+        <v>-1.5574077246549023</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="12"/>
+        <v>0.64836082745908663</v>
+      </c>
+      <c r="N40">
+        <f t="array" ref="N40">SUM(TAN(B40:E40))</f>
+        <v>0.54630248984379071</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0.5</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>-1</v>
+      </c>
+      <c r="F41">
+        <v>10</v>
+      </c>
+      <c r="H41">
+        <f>TANH(B41)</f>
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <f t="shared" ref="I41:L41" si="13">TANH(C41)</f>
+        <v>0.46211715726000979</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="13"/>
+        <v>0.76159415595576485</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="13"/>
+        <v>-0.76159415595576485</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="13"/>
+        <v>0.99999999587769262</v>
+      </c>
+      <c r="N41">
+        <f t="array" ref="N41">SUM(TANH(B41:E41))</f>
+        <v>0.46211715726000979</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added MIN and MAX to the test.xlsx
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>ca</t>
   </si>
@@ -87,6 +87,18 @@
   </si>
   <si>
     <t>TANH</t>
+  </si>
+  <si>
+    <t>ABS</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>MIN</t>
   </si>
 </sst>
 </file>
@@ -122,9 +134,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -749,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>[1]Sheet1!$A$1+1</f>
         <v>3</v>
@@ -765,7 +780,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>[1]Sheet1!$A$1+[1]Sheet1!$A$2</f>
         <v>4</v>
@@ -784,19 +799,19 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E19">
         <f>D16*3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H20">
         <f t="array" ref="H20:H24">IF(G9:G12&lt;&gt;H10:H13,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F21">
         <f>C19+1</f>
         <v>1</v>
@@ -809,12 +824,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H23">
         <v>1</v>
       </c>
@@ -823,7 +838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H24" t="e">
         <v>#N/A</v>
       </c>
@@ -832,7 +847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -848,35 +863,42 @@
       <c r="E26">
         <v>10</v>
       </c>
-      <c r="F26">
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26">
         <v>-1</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <f>LN(B26)</f>
         <v>0</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <f>LN(C26)</f>
         <v>0.91629073187415511</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <f>LN(D26)</f>
         <v>1.0986122886681098</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <f>LN(E26)</f>
         <v>2.3025850929940459</v>
       </c>
-      <c r="L26" t="e">
+      <c r="M26" t="e">
         <f>LN(F26)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N26" t="e">
+        <f>LN(G26)</f>
         <v>#NUM!</v>
       </c>
-      <c r="N26">
-        <f t="array" ref="N26">SUM(LN(B26:E26))</f>
+      <c r="O26">
+        <f t="array" ref="O26">SUM(LN(B26:E26))</f>
         <v>4.317488113536311</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -892,35 +914,42 @@
       <c r="E27">
         <v>10</v>
       </c>
-      <c r="F27">
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27">
         <v>-1</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <f>LOG(B27)</f>
         <v>0</v>
       </c>
-      <c r="I27">
-        <f t="shared" ref="I27:L29" si="0">LOG(C27)</f>
+      <c r="J27">
+        <f>LOG(C27)</f>
         <v>0.3979400086720376</v>
       </c>
-      <c r="J27">
-        <f t="shared" si="0"/>
+      <c r="K27">
+        <f>LOG(D27)</f>
         <v>0.47712125471966244</v>
       </c>
-      <c r="K27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L27" t="e">
-        <f t="shared" si="0"/>
+      <c r="L27">
+        <f>LOG(E27)</f>
+        <v>1</v>
+      </c>
+      <c r="M27" t="e">
+        <f>LOG(F27)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N27" t="e">
+        <f>LOG(G27)</f>
         <v>#NUM!</v>
       </c>
-      <c r="N27">
-        <f t="array" ref="N27">SUM(LOG(B27:E27))</f>
+      <c r="O27">
+        <f t="array" ref="O27">SUM(LOG(B27:E27))</f>
         <v>1.8750612633917001</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -936,32 +965,42 @@
       <c r="E28">
         <v>10</v>
       </c>
-      <c r="H28">
+      <c r="F28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="I28">
         <f>EXP(B28)</f>
         <v>2.7182818284590451</v>
       </c>
-      <c r="I28">
-        <f t="shared" ref="I28:K28" si="1">EXP(C28)</f>
+      <c r="J28">
+        <f>EXP(C28)</f>
         <v>12.182493960703473</v>
       </c>
-      <c r="J28">
-        <f t="shared" si="1"/>
+      <c r="K28">
+        <f>EXP(D28)</f>
         <v>20.085536923187668</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="1"/>
+      <c r="L28">
+        <f>EXP(E28)</f>
         <v>22026.465794806718</v>
       </c>
-      <c r="L28" t="e">
-        <f t="shared" si="0"/>
+      <c r="M28" t="e">
+        <f>EXP(F28)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N28" t="e">
+        <f>LOG(G28)</f>
         <v>#NUM!</v>
       </c>
-      <c r="N28">
-        <f t="array" ref="N28">SUM(EXP(B28:E28))</f>
+      <c r="O28">
+        <f t="array" ref="O28">SUM(EXP(B28:E28))</f>
         <v>22061.452107519068</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -977,35 +1016,42 @@
       <c r="E29">
         <v>1</v>
       </c>
-      <c r="F29">
+      <c r="F29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29">
         <v>2</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <f>ACOS(B29)</f>
         <v>1.5707963267948966</v>
       </c>
-      <c r="I29">
-        <f t="shared" ref="I29:L29" si="2">ACOS(C29)</f>
+      <c r="J29">
+        <f>ACOS(C29)</f>
         <v>1.3694384060045657</v>
       </c>
-      <c r="J29">
-        <f t="shared" si="2"/>
+      <c r="K29">
+        <f>ACOS(D29)</f>
         <v>1.0471975511965976</v>
       </c>
-      <c r="K29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L29" t="e">
-        <f t="shared" si="2"/>
+      <c r="L29">
+        <f>ACOS(E29)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" t="e">
+        <f>ACOS(F29)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N29" t="e">
+        <f>ACOS(G29)</f>
         <v>#NUM!</v>
       </c>
-      <c r="N29">
-        <f t="array" ref="N29">SUM(ACOS(B29:E29))</f>
+      <c r="O29">
+        <f t="array" ref="O29">SUM(ACOS(B29:E29))</f>
         <v>3.9874322839960596</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1021,35 +1067,42 @@
       <c r="E30">
         <v>4</v>
       </c>
-      <c r="F30">
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30">
         <v>0.5</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <f>ACOSH(B30)</f>
         <v>0</v>
       </c>
-      <c r="I30">
-        <f t="shared" ref="I30:L30" si="3">ACOSH(C30)</f>
+      <c r="J30">
+        <f>ACOSH(C30)</f>
         <v>1.3169578969248166</v>
       </c>
-      <c r="J30">
-        <f t="shared" si="3"/>
+      <c r="K30">
+        <f>ACOSH(D30)</f>
         <v>1.7627471740390861</v>
       </c>
-      <c r="K30">
-        <f t="shared" si="3"/>
+      <c r="L30">
+        <f>ACOSH(E30)</f>
         <v>2.0634370688955608</v>
       </c>
-      <c r="L30" t="e">
+      <c r="M30" t="e">
         <f>ACOSH(F30)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N30" t="e">
+        <f>ACOSH(G30)</f>
         <v>#NUM!</v>
       </c>
-      <c r="N30">
-        <f t="array" ref="N30">SUM(ACOSH(B30:E30))</f>
+      <c r="O30">
+        <f t="array" ref="O30">SUM(ACOSH(B30:E30))</f>
         <v>5.1431421398594637</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1065,35 +1118,42 @@
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="F31">
+      <c r="F31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31">
         <v>2</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <f>ASIN(B31)</f>
         <v>0</v>
       </c>
-      <c r="I31">
-        <f t="shared" ref="I31:L31" si="4">ASIN(C31)</f>
+      <c r="J31">
+        <f>ASIN(C31)</f>
         <v>0.20135792079033082</v>
       </c>
-      <c r="J31">
-        <f t="shared" si="4"/>
+      <c r="K31">
+        <f>ASIN(D31)</f>
         <v>0.52359877559829893</v>
       </c>
-      <c r="K31">
-        <f t="shared" si="4"/>
+      <c r="L31">
+        <f>ASIN(E31)</f>
         <v>1.5707963267948966</v>
       </c>
-      <c r="L31" t="e">
-        <f t="shared" si="4"/>
+      <c r="M31" t="e">
+        <f>ASIN(F31)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N31" t="e">
+        <f>ASIN(G31)</f>
         <v>#NUM!</v>
       </c>
-      <c r="N31">
-        <f t="array" ref="N31">SUM(ASIN(B31:E31))</f>
+      <c r="O31">
+        <f t="array" ref="O31">SUM(ASIN(B31:E31))</f>
         <v>2.2957530231835266</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1109,35 +1169,35 @@
       <c r="E32">
         <v>20</v>
       </c>
-      <c r="F32">
-        <v>100</v>
-      </c>
-      <c r="H32">
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32">
         <f>ASINH(B32)</f>
         <v>-2.3124383412727525</v>
       </c>
-      <c r="I32">
-        <f t="shared" ref="I32:L32" si="5">ASINH(C32)</f>
+      <c r="J32">
+        <f>ASINH(C32)</f>
         <v>-0.88137358701954294</v>
       </c>
-      <c r="J32">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="K32">
-        <f t="shared" si="5"/>
+        <f>ASINH(D32)</f>
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f>ASINH(E32)</f>
         <v>3.6895038689889059</v>
       </c>
-      <c r="L32">
-        <f t="shared" si="5"/>
-        <v>5.2983423656105888</v>
-      </c>
-      <c r="N32">
-        <f t="array" ref="N32">SUM(ASINH(B32:E32))</f>
+      <c r="M32" t="e">
+        <f>ASINH(F32)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O32">
+        <f t="array" ref="O32">SUM(ASINH(B32:E32))</f>
         <v>0.49569194069661027</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1153,35 +1213,35 @@
       <c r="E33">
         <v>1</v>
       </c>
-      <c r="F33">
-        <v>-10</v>
-      </c>
-      <c r="H33">
+      <c r="F33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33">
         <f>ATAN(B33)</f>
         <v>0</v>
       </c>
-      <c r="I33">
-        <f t="shared" ref="I33:L33" si="6">ATAN(C33)</f>
+      <c r="J33">
+        <f>ATAN(C33)</f>
         <v>0.19739555984988078</v>
       </c>
-      <c r="J33">
-        <f t="shared" si="6"/>
+      <c r="K33">
+        <f>ATAN(D33)</f>
         <v>0.46364760900080609</v>
       </c>
-      <c r="K33">
-        <f t="shared" si="6"/>
+      <c r="L33">
+        <f>ATAN(E33)</f>
         <v>0.78539816339744828</v>
       </c>
-      <c r="L33">
-        <f t="shared" si="6"/>
-        <v>-1.4711276743037347</v>
-      </c>
-      <c r="N33">
-        <f t="array" ref="N33">SUM(ATAN(B33:E33))</f>
+      <c r="M33" t="e">
+        <f>ATAN(F33)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O33">
+        <f t="array" ref="O33">SUM(ATAN(B33:E33))</f>
         <v>1.4464413322481351</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1189,43 +1249,43 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D34">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>2</v>
-      </c>
-      <c r="H34">
+        <v>-4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34">
         <f>ATAN2(B34,C34)</f>
         <v>1.5707963267948966</v>
       </c>
-      <c r="I34">
-        <f t="shared" ref="I34:L34" si="7">ATAN2(C34,D34)</f>
-        <v>1.1902899496825317</v>
-      </c>
       <c r="J34">
-        <f t="shared" si="7"/>
+        <f>ATAN2(C34,D34)</f>
         <v>1.1071487177940904</v>
       </c>
       <c r="K34">
-        <f t="shared" si="7"/>
-        <v>1.1071487177940904</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N34">
-        <f t="array" ref="N34">SUM(ATAN2(B34:E34,C34:F34))</f>
-        <v>4.975383712065609</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+        <f>ATAN2(D34,E34)</f>
+        <v>-1.1071487177940904</v>
+      </c>
+      <c r="L34" t="e">
+        <f>ATAN2(E34,F34)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M34" t="e">
+        <f>ATAN2(F34,G34)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O34">
+        <f t="array" ref="O34">SUM(ATAN2(B34:D34,C34:E34))</f>
+        <v>1.5707963267948966</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1236,40 +1296,40 @@
         <v>0.1</v>
       </c>
       <c r="D35">
-        <v>0.5</v>
+        <v>0.99</v>
       </c>
       <c r="E35">
-        <v>0.95</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35">
         <f>ATANH(B35)</f>
         <v>0</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <f>ATANH(C35)</f>
         <v>0.10033534773107562</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <f>ATANH(D35)</f>
-        <v>0.54930614433405489</v>
-      </c>
-      <c r="K35">
+        <v>2.6466524123622457</v>
+      </c>
+      <c r="L35" t="e">
         <f>ATANH(E35)</f>
-        <v>1.8317808230648227</v>
-      </c>
-      <c r="L35" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M35" t="e">
         <f>ATANH(F35)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N35">
-        <f t="array" ref="N35">SUM(ATANH(B35:E35))</f>
-        <v>2.4814223151299535</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O35">
+        <f t="array" ref="O35">SUM(ATANH(B35:D35))</f>
+        <v>2.7469877600933215</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1285,35 +1345,35 @@
       <c r="E36">
         <v>-1</v>
       </c>
-      <c r="F36">
-        <v>10</v>
-      </c>
-      <c r="H36">
+      <c r="F36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36">
         <f>COS(B36)</f>
         <v>1</v>
       </c>
-      <c r="I36">
-        <f t="shared" ref="I36:L36" si="8">COS(C36)</f>
+      <c r="J36">
+        <f>COS(C36)</f>
         <v>0.87758256189037276</v>
       </c>
-      <c r="J36">
-        <f t="shared" si="8"/>
+      <c r="K36">
+        <f>COS(D36)</f>
         <v>0.54030230586813977</v>
       </c>
-      <c r="K36">
-        <f t="shared" si="8"/>
+      <c r="L36">
+        <f>COS(E36)</f>
         <v>0.54030230586813977</v>
       </c>
-      <c r="L36">
-        <f t="shared" si="8"/>
-        <v>-0.83907152907645244</v>
-      </c>
-      <c r="N36">
-        <f t="array" ref="N36">SUM(COS(B36:E36))</f>
+      <c r="M36" t="e">
+        <f>COS(F36)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O36">
+        <f t="array" ref="O36">SUM(COS(B36:E36))</f>
         <v>2.9581871736266523</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1329,35 +1389,35 @@
       <c r="E37">
         <v>-1</v>
       </c>
-      <c r="F37">
-        <v>10</v>
-      </c>
-      <c r="H37">
+      <c r="F37" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37">
         <f>COSH(B37)</f>
         <v>1</v>
       </c>
-      <c r="I37">
-        <f t="shared" ref="I37:L37" si="9">COSH(C37)</f>
+      <c r="J37">
+        <f>COSH(C37)</f>
         <v>1.1276259652063807</v>
       </c>
-      <c r="J37">
-        <f t="shared" si="9"/>
+      <c r="K37">
+        <f>COSH(D37)</f>
         <v>1.5430806348152437</v>
       </c>
-      <c r="K37">
-        <f t="shared" si="9"/>
+      <c r="L37">
+        <f>COSH(E37)</f>
         <v>1.5430806348152437</v>
       </c>
-      <c r="L37">
-        <f t="shared" si="9"/>
-        <v>11013.232920103324</v>
-      </c>
-      <c r="N37">
-        <f t="array" ref="N37">SUM(COSH(B37:E37))</f>
+      <c r="M37" t="e">
+        <f>COSH(F37)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O37">
+        <f t="array" ref="O37">SUM(COSH(B37:E37))</f>
         <v>5.2137872348368681</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1373,35 +1433,35 @@
       <c r="E38">
         <v>-1</v>
       </c>
-      <c r="F38">
-        <v>10</v>
-      </c>
-      <c r="H38">
+      <c r="F38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38">
         <f>SIN(B38)</f>
         <v>0</v>
       </c>
-      <c r="I38">
-        <f t="shared" ref="I38:L38" si="10">SIN(C38)</f>
+      <c r="J38">
+        <f>SIN(C38)</f>
         <v>0.47942553860420301</v>
       </c>
-      <c r="J38">
-        <f t="shared" si="10"/>
+      <c r="K38">
+        <f>SIN(D38)</f>
         <v>0.8414709848078965</v>
       </c>
-      <c r="K38">
-        <f t="shared" si="10"/>
+      <c r="L38">
+        <f>SIN(E38)</f>
         <v>-0.8414709848078965</v>
       </c>
-      <c r="L38">
-        <f t="shared" si="10"/>
-        <v>-0.54402111088936977</v>
-      </c>
-      <c r="N38">
-        <f t="array" ref="N38">SUM(SIN(B38:E38))</f>
+      <c r="M38" t="e">
+        <f>SIN(F38)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O38">
+        <f t="array" ref="O38">SUM(SIN(B38:E38))</f>
         <v>0.47942553860420301</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1417,35 +1477,35 @@
       <c r="E39">
         <v>-1</v>
       </c>
-      <c r="F39">
-        <v>10</v>
-      </c>
-      <c r="H39">
+      <c r="F39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39">
         <f>SINH(B39)</f>
         <v>0</v>
       </c>
-      <c r="I39">
-        <f t="shared" ref="I39:L39" si="11">SINH(C39)</f>
+      <c r="J39">
+        <f>SINH(C39)</f>
         <v>0.52109530549374738</v>
       </c>
-      <c r="J39">
-        <f t="shared" si="11"/>
+      <c r="K39">
+        <f>SINH(D39)</f>
         <v>1.1752011936438014</v>
       </c>
-      <c r="K39">
-        <f t="shared" si="11"/>
+      <c r="L39">
+        <f>SINH(E39)</f>
         <v>-1.1752011936438014</v>
       </c>
-      <c r="L39">
-        <f t="shared" si="11"/>
-        <v>11013.232874703393</v>
-      </c>
-      <c r="N39">
-        <f t="array" ref="N39">SUM(SINH(B39:E39))</f>
+      <c r="M39" t="e">
+        <f>SINH(F39)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O39">
+        <f t="array" ref="O39">SUM(SINH(B39:E39))</f>
         <v>0.5210953054937475</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -1461,35 +1521,35 @@
       <c r="E40">
         <v>-1</v>
       </c>
-      <c r="F40">
-        <v>10</v>
-      </c>
-      <c r="H40">
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40">
         <f>TAN(B40)</f>
         <v>0</v>
       </c>
-      <c r="I40">
-        <f t="shared" ref="I40:L40" si="12">TAN(C40)</f>
+      <c r="J40">
+        <f>TAN(C40)</f>
         <v>0.54630248984379048</v>
       </c>
-      <c r="J40">
-        <f t="shared" si="12"/>
+      <c r="K40">
+        <f>TAN(D40)</f>
         <v>1.5574077246549023</v>
       </c>
-      <c r="K40">
-        <f t="shared" si="12"/>
+      <c r="L40">
+        <f>TAN(E40)</f>
         <v>-1.5574077246549023</v>
       </c>
-      <c r="L40">
-        <f t="shared" si="12"/>
-        <v>0.64836082745908663</v>
-      </c>
-      <c r="N40">
-        <f t="array" ref="N40">SUM(TAN(B40:E40))</f>
+      <c r="M40" t="e">
+        <f>TAN(F40)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O40">
+        <f t="array" ref="O40">SUM(TAN(B40:E40))</f>
         <v>0.54630248984379071</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1500,38 +1560,133 @@
         <v>0.5</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E41">
-        <v>-1</v>
-      </c>
-      <c r="F41">
         <v>10</v>
       </c>
-      <c r="H41">
+      <c r="F41" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41">
         <f>TANH(B41)</f>
         <v>0</v>
       </c>
-      <c r="I41">
-        <f t="shared" ref="I41:L41" si="13">TANH(C41)</f>
+      <c r="J41">
+        <f>TANH(C41)</f>
         <v>0.46211715726000979</v>
       </c>
-      <c r="J41">
-        <f t="shared" si="13"/>
-        <v>0.76159415595576485</v>
-      </c>
       <c r="K41">
-        <f t="shared" si="13"/>
+        <f>TANH(D41)</f>
         <v>-0.76159415595576485</v>
       </c>
       <c r="L41">
-        <f t="shared" si="13"/>
+        <f>TANH(E41)</f>
         <v>0.99999999587769262</v>
       </c>
-      <c r="N41">
-        <f t="array" ref="N41">SUM(TANH(B41:E41))</f>
-        <v>0.46211715726000979</v>
-      </c>
+      <c r="M41" t="e">
+        <f>TANH(F41)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O41">
+        <f t="array" ref="O41">SUM(TANH(B41:E41))</f>
+        <v>0.70052299718193756</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42">
+        <v>-10</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>10</v>
+      </c>
+      <c r="E42">
+        <v>-1.5</v>
+      </c>
+      <c r="F42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42">
+        <f>ABS(B42)</f>
+        <v>10</v>
+      </c>
+      <c r="J42">
+        <f>ABS(C42)</f>
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <f>ABS(D42)</f>
+        <v>10</v>
+      </c>
+      <c r="L42">
+        <f>ABS(E42)</f>
+        <v>1.5</v>
+      </c>
+      <c r="M42" t="e">
+        <f>ABS(F42)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O42">
+        <f t="array" ref="O42">SUM(ABS(B42:E42))</f>
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43">
+        <v>-10</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>10</v>
+      </c>
+      <c r="E43">
+        <v>100</v>
+      </c>
+      <c r="F43" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43">
+        <f>MAX(B43:F43)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>-10</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>10</v>
+      </c>
+      <c r="E44">
+        <v>100</v>
+      </c>
+      <c r="F44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44">
+        <f>MIN(B44:F44)</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F47" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
made the ufunc wrapper work with multi input functions, e.g., power, mod, and atan2
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>ca</t>
   </si>
@@ -99,6 +99,21 @@
   </si>
   <si>
     <t>MIN</t>
+  </si>
+  <si>
+    <t>RADIANS</t>
+  </si>
+  <si>
+    <t>DEGREES</t>
+  </si>
+  <si>
+    <t>POWER</t>
+  </si>
+  <si>
+    <t>MOD</t>
+  </si>
+  <si>
+    <t>SQRT</t>
   </si>
 </sst>
 </file>
@@ -444,13 +459,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="7" width="11.375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F1">
@@ -1249,40 +1267,40 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E34">
-        <v>-4</v>
+        <v>-10</v>
       </c>
       <c r="F34" t="s">
         <v>18</v>
       </c>
       <c r="I34">
         <f>ATAN2(B34,C34)</f>
-        <v>1.5707963267948966</v>
+        <v>-1.5707963267948966</v>
       </c>
       <c r="J34">
-        <f>ATAN2(C34,D34)</f>
-        <v>1.1071487177940904</v>
+        <f t="shared" ref="J34:M34" si="0">ATAN2(C34,D34)</f>
+        <v>1.9513027039072615</v>
       </c>
       <c r="K34">
-        <f>ATAN2(D34,E34)</f>
-        <v>-1.1071487177940904</v>
+        <f t="shared" si="0"/>
+        <v>-1.3258176636680326</v>
       </c>
       <c r="L34" t="e">
-        <f>ATAN2(E34,F34)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="M34" t="e">
-        <f>ATAN2(F34,G34)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="O34">
         <f t="array" ref="O34">SUM(ATAN2(B34:D34,C34:E34))</f>
-        <v>1.5707963267948966</v>
+        <v>-0.94531128655566765</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -1685,8 +1703,256 @@
         <v>-10</v>
       </c>
     </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="C45">
+        <f>-PI()/4</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="D45">
+        <v>120</v>
+      </c>
+      <c r="F45" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45">
+        <f>DEGREES(B45)</f>
+        <v>180</v>
+      </c>
+      <c r="J45">
+        <f>DEGREES(C45)</f>
+        <v>-45</v>
+      </c>
+      <c r="K45">
+        <f>DEGREES(D45)</f>
+        <v>6875.4935415698783</v>
+      </c>
+      <c r="L45">
+        <f>DEGREES(E45)</f>
+        <v>0</v>
+      </c>
+      <c r="M45" t="e">
+        <f>DEGREES(F45)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O45">
+        <f t="array" ref="O45">SUM(DEGREES(B45:E45))</f>
+        <v>7010.4935415698783</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46">
+        <v>120</v>
+      </c>
+      <c r="C46">
+        <v>-45</v>
+      </c>
+      <c r="D46">
+        <v>-720</v>
+      </c>
+      <c r="F46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46">
+        <f>RADIANS(B46)</f>
+        <v>2.0943951023931953</v>
+      </c>
+      <c r="J46">
+        <f t="shared" ref="J46:M46" si="1">RADIANS(C46)</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="1"/>
+        <v>-12.566370614359172</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M46" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O46">
+        <f t="array" ref="O46">SUM(RADIANS(B46:E46))</f>
+        <v>-11.257373675363425</v>
+      </c>
+    </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F47" s="2"/>
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>3.5</v>
+      </c>
+      <c r="D47">
+        <v>-0.5</v>
+      </c>
+      <c r="E47">
+        <v>9</v>
+      </c>
+      <c r="F47" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47">
+        <f>POWER(B47,C47)</f>
+        <v>11.313708498984759</v>
+      </c>
+      <c r="J47">
+        <f>POWER(C47,D47)</f>
+        <v>0.53452248382484879</v>
+      </c>
+      <c r="K47">
+        <f>POWER(D47,E47)</f>
+        <v>-1.953125E-3</v>
+      </c>
+      <c r="L47" t="e">
+        <f>POWER(E47,F47)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M47" t="e">
+        <f>POWER(F47,G47)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O47">
+        <f t="array" ref="O47">SUM(POWER(B47:D47,C47:E47))</f>
+        <v>11.846277857809609</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48">
+        <v>31.5</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>6.7</v>
+      </c>
+      <c r="E48">
+        <v>5</v>
+      </c>
+      <c r="F48" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48">
+        <f>MOD(B48,C48)</f>
+        <v>1.5</v>
+      </c>
+      <c r="J48">
+        <f>MOD(C48,D48)</f>
+        <v>3.3</v>
+      </c>
+      <c r="K48">
+        <f>MOD(D48,E48)</f>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="L48" t="e">
+        <f>MOD(E48,F48)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M48" t="e">
+        <f>MOD(F48,G48)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O48">
+        <f t="array" ref="O48">SUM(MOD(B48:D48,C48:E48))</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>3.5</v>
+      </c>
+      <c r="D49">
+        <v>9</v>
+      </c>
+      <c r="E49">
+        <v>-0.5</v>
+      </c>
+      <c r="F49" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49">
+        <f>SQRT(B49)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="J49">
+        <f t="shared" ref="J49:M49" si="2">SQRT(C49)</f>
+        <v>1.8708286933869707</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="L49" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M49" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O49">
+        <f t="array" ref="O49">SUM(SQRT(B49:D49))</f>
+        <v>6.2850422557600663</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F52" s="2"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F54" s="2"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F56" s="2"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F57" s="2"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F58" s="2"/>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H60" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix(functions), #4: Correct `power`, `arctan2`, and `mod` error results.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sandboxes\excel2py\formulas\test\test_files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16305" tabRatio="500"/>
   </bookViews>
@@ -26,7 +21,7 @@
     <definedName name="f">Sheet1!$G$2:$H$5</definedName>
     <definedName name="g">Sheet2!$B$2:$B$5</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -451,7 +446,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -459,15 +454,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD66"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="7" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
@@ -782,7 +779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>[1]Sheet1!$A$1+1</f>
         <v>3</v>
@@ -798,7 +795,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>[1]Sheet1!$A$1+[1]Sheet1!$A$2</f>
         <v>4</v>
@@ -817,19 +814,19 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E19">
         <f>D16*3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H20">
         <f t="array" ref="H20:H24">IF(G9:G12&lt;&gt;H10:H13,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F21">
         <f>C19+1</f>
         <v>1</v>
@@ -842,12 +839,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H23">
         <v>1</v>
       </c>
@@ -856,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H24" t="e">
         <v>#N/A</v>
       </c>
@@ -865,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -892,31 +889,41 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <f>LN(C26)</f>
+        <f t="shared" ref="I26:N26" si="0">LN(C26)</f>
         <v>0.91629073187415511</v>
       </c>
       <c r="K26">
-        <f>LN(D26)</f>
+        <f t="shared" si="0"/>
         <v>1.0986122886681098</v>
       </c>
       <c r="L26">
-        <f>LN(E26)</f>
+        <f t="shared" si="0"/>
         <v>2.3025850929940459</v>
       </c>
       <c r="M26" t="e">
-        <f>LN(F26)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="N26" t="e">
-        <f>LN(G26)</f>
+        <f t="shared" si="0"/>
         <v>#NUM!</v>
       </c>
       <c r="O26">
         <f t="array" ref="O26">SUM(LN(B26:E26))</f>
         <v>4.317488113536311</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P26">
+        <f t="array" ref="P26:R26">LN(B26:E26)</f>
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0.91629073187415511</v>
+      </c>
+      <c r="R26">
+        <v>1.0986122886681098</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -943,31 +950,44 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <f>LOG(C27)</f>
+        <f t="shared" ref="I27:P27" si="1">LOG(C27)</f>
         <v>0.3979400086720376</v>
       </c>
       <c r="K27">
-        <f>LOG(D27)</f>
+        <f t="shared" si="1"/>
         <v>0.47712125471966244</v>
       </c>
       <c r="L27">
-        <f>LOG(E27)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M27" t="e">
-        <f>LOG(F27)</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="N27" t="e">
-        <f>LOG(G27)</f>
+        <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
       <c r="O27">
         <f t="array" ref="O27">SUM(LOG(B27:E27))</f>
         <v>1.8750612633917001</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P27">
+        <f t="array" ref="P27:S27">LOG(B27:E27)</f>
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0.3979400086720376</v>
+      </c>
+      <c r="R27">
+        <v>0.47712125471966244</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1017,8 +1037,21 @@
         <f t="array" ref="O28">SUM(EXP(B28:E28))</f>
         <v>22061.452107519068</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P28">
+        <f t="array" ref="P28:S28">EXP(B28:E28)</f>
+        <v>2.7182818284590451</v>
+      </c>
+      <c r="Q28">
+        <v>12.182493960703473</v>
+      </c>
+      <c r="R28">
+        <v>20.085536923187668</v>
+      </c>
+      <c r="S28">
+        <v>22026.465794806718</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1041,35 +1074,48 @@
         <v>2</v>
       </c>
       <c r="I29">
-        <f>ACOS(B29)</f>
+        <f t="shared" ref="I29:P29" si="2">ACOS(B29)</f>
         <v>1.5707963267948966</v>
       </c>
       <c r="J29">
-        <f>ACOS(C29)</f>
+        <f t="shared" si="2"/>
         <v>1.3694384060045657</v>
       </c>
       <c r="K29">
-        <f>ACOS(D29)</f>
+        <f t="shared" si="2"/>
         <v>1.0471975511965976</v>
       </c>
       <c r="L29">
-        <f>ACOS(E29)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M29" t="e">
-        <f>ACOS(F29)</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N29" t="e">
-        <f>ACOS(G29)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="O29">
         <f t="array" ref="O29">SUM(ACOS(B29:E29))</f>
         <v>3.9874322839960596</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P29">
+        <f t="array" ref="P29:S29">ACOS(B29:E29)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="Q29">
+        <v>1.3694384060045657</v>
+      </c>
+      <c r="R29">
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1092,35 +1138,48 @@
         <v>0.5</v>
       </c>
       <c r="I30">
-        <f>ACOSH(B30)</f>
+        <f t="shared" ref="I30:P30" si="3">ACOSH(B30)</f>
         <v>0</v>
       </c>
       <c r="J30">
-        <f>ACOSH(C30)</f>
+        <f t="shared" si="3"/>
         <v>1.3169578969248166</v>
       </c>
       <c r="K30">
-        <f>ACOSH(D30)</f>
+        <f t="shared" si="3"/>
         <v>1.7627471740390861</v>
       </c>
       <c r="L30">
-        <f>ACOSH(E30)</f>
+        <f t="shared" si="3"/>
         <v>2.0634370688955608</v>
       </c>
       <c r="M30" t="e">
-        <f>ACOSH(F30)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="N30" t="e">
-        <f>ACOSH(G30)</f>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="O30">
         <f t="array" ref="O30">SUM(ACOSH(B30:E30))</f>
         <v>5.1431421398594637</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P30">
+        <f t="array" ref="P30:S30">ACOSH(B30:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>1.3169578969248166</v>
+      </c>
+      <c r="R30">
+        <v>1.7627471740390861</v>
+      </c>
+      <c r="S30">
+        <v>2.0634370688955608</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1143,35 +1202,48 @@
         <v>2</v>
       </c>
       <c r="I31">
-        <f>ASIN(B31)</f>
+        <f t="shared" ref="I31:P31" si="4">ASIN(B31)</f>
         <v>0</v>
       </c>
       <c r="J31">
-        <f>ASIN(C31)</f>
+        <f t="shared" si="4"/>
         <v>0.20135792079033082</v>
       </c>
       <c r="K31">
-        <f>ASIN(D31)</f>
+        <f t="shared" si="4"/>
         <v>0.52359877559829893</v>
       </c>
       <c r="L31">
-        <f>ASIN(E31)</f>
+        <f t="shared" si="4"/>
         <v>1.5707963267948966</v>
       </c>
       <c r="M31" t="e">
-        <f>ASIN(F31)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N31" t="e">
-        <f>ASIN(G31)</f>
+        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
       <c r="O31">
         <f t="array" ref="O31">SUM(ASIN(B31:E31))</f>
         <v>2.2957530231835266</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P31">
+        <f t="array" ref="P31:S31">ASIN(B31:E31)</f>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0.20135792079033082</v>
+      </c>
+      <c r="R31">
+        <v>0.52359877559829893</v>
+      </c>
+      <c r="S31">
+        <v>1.5707963267948966</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1214,8 +1286,21 @@
         <f t="array" ref="O32">SUM(ASINH(B32:E32))</f>
         <v>0.49569194069661027</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P32">
+        <f t="array" ref="P32:S32">ASINH(B32:E32)</f>
+        <v>-2.3124383412727525</v>
+      </c>
+      <c r="Q32">
+        <v>-0.88137358701954294</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>3.6895038689889059</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1223,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <v>0.2</v>
+        <v>-1</v>
       </c>
       <c r="D33">
         <v>0.5</v>
@@ -1240,7 +1325,7 @@
       </c>
       <c r="J33">
         <f>ATAN(C33)</f>
-        <v>0.19739555984988078</v>
+        <v>-0.78539816339744828</v>
       </c>
       <c r="K33">
         <f>ATAN(D33)</f>
@@ -1256,10 +1341,23 @@
       </c>
       <c r="O33">
         <f t="array" ref="O33">SUM(ATAN(B33:E33))</f>
-        <v>1.4464413322481351</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.46364760900080609</v>
+      </c>
+      <c r="P33">
+        <f t="array" ref="P33:S33">ATAN(B33:E33)</f>
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="R33">
+        <v>0.46364760900080609</v>
+      </c>
+      <c r="S33">
+        <v>0.78539816339744828</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1267,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D34">
         <v>2.5</v>
@@ -1278,32 +1376,39 @@
       <c r="F34" t="s">
         <v>18</v>
       </c>
-      <c r="I34">
+      <c r="I34" t="e">
         <f>ATAN2(B34,C34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J34">
+        <f t="shared" ref="J34:M34" si="5">ATAN2(C34,D34)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="5"/>
+        <v>-1.3258176636680326</v>
+      </c>
+      <c r="L34" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M34" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O34" t="e">
+        <f t="array" ref="O34">SUM(ATAN2(B34:D34,C34:E34))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P34">
+        <f t="array" ref="P34:Q34">ATAN2(B34:C34,D34:E34)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="Q34">
         <v>-1.5707963267948966</v>
       </c>
-      <c r="J34">
-        <f t="shared" ref="J34:M34" si="0">ATAN2(C34,D34)</f>
-        <v>1.9513027039072615</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="0"/>
-        <v>-1.3258176636680326</v>
-      </c>
-      <c r="L34" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M34" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O34">
-        <f t="array" ref="O34">SUM(ATAN2(B34:D34,C34:E34))</f>
-        <v>-0.94531128655566765</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1346,8 +1451,21 @@
         <f t="array" ref="O35">SUM(ATANH(B35:D35))</f>
         <v>2.7469877600933215</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P35">
+        <f t="array" ref="P35:S35">ATANH(B35:E35)</f>
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0.10033534773107562</v>
+      </c>
+      <c r="R35">
+        <v>2.6466524123622457</v>
+      </c>
+      <c r="S35" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1390,8 +1508,21 @@
         <f t="array" ref="O36">SUM(COS(B36:E36))</f>
         <v>2.9581871736266523</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P36">
+        <f t="array" ref="P36:S36">COS(B36:E36)</f>
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <v>0.87758256189037276</v>
+      </c>
+      <c r="R36">
+        <v>0.54030230586813977</v>
+      </c>
+      <c r="S36">
+        <v>0.54030230586813977</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1434,8 +1565,21 @@
         <f t="array" ref="O37">SUM(COSH(B37:E37))</f>
         <v>5.2137872348368681</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P37">
+        <f t="array" ref="P37:S37">COSH(B37:E37)</f>
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <v>1.1276259652063807</v>
+      </c>
+      <c r="R37">
+        <v>1.5430806348152437</v>
+      </c>
+      <c r="S37">
+        <v>1.5430806348152437</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1478,8 +1622,21 @@
         <f t="array" ref="O38">SUM(SIN(B38:E38))</f>
         <v>0.47942553860420301</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P38">
+        <f t="array" ref="P38:S38">SIN(B38:E38)</f>
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0.47942553860420301</v>
+      </c>
+      <c r="R38">
+        <v>0.8414709848078965</v>
+      </c>
+      <c r="S38">
+        <v>-0.8414709848078965</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1522,8 +1679,21 @@
         <f t="array" ref="O39">SUM(SINH(B39:E39))</f>
         <v>0.5210953054937475</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P39">
+        <f t="array" ref="P39:S39">SINH(B39:E39)</f>
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0.52109530549374738</v>
+      </c>
+      <c r="R39">
+        <v>1.1752011936438014</v>
+      </c>
+      <c r="S39">
+        <v>-1.1752011936438014</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -1566,8 +1736,21 @@
         <f t="array" ref="O40">SUM(TAN(B40:E40))</f>
         <v>0.54630248984379071</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P40">
+        <f t="array" ref="P40:S40">TAN(B40:E40)</f>
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0.54630248984379048</v>
+      </c>
+      <c r="R40">
+        <v>1.5574077246549023</v>
+      </c>
+      <c r="S40">
+        <v>-1.5574077246549023</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1610,8 +1793,24 @@
         <f t="array" ref="O41">SUM(TANH(B41:E41))</f>
         <v>0.70052299718193756</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P41">
+        <f t="array" ref="P41:T41">TANH(B41:F41)</f>
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>0.46211715726000979</v>
+      </c>
+      <c r="R41">
+        <v>-0.76159415595576485</v>
+      </c>
+      <c r="S41">
+        <v>0.99999999587769262</v>
+      </c>
+      <c r="T41" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -1654,8 +1853,21 @@
         <f t="array" ref="O42">SUM(ABS(B42:E42))</f>
         <v>21.5</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P42">
+        <f t="array" ref="P42:S42">ABS(B42:E42)</f>
+        <v>10</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <v>10</v>
+      </c>
+      <c r="S42">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -1678,8 +1890,12 @@
         <f>MAX(B43:F43)</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P43">
+        <f>MAX(B26:F49)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -1702,8 +1918,12 @@
         <f>MIN(B44:F44)</f>
         <v>-10</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P44">
+        <f>MIN(B26:F49)</f>
+        <v>-720</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -1745,8 +1965,21 @@
         <f t="array" ref="O45">SUM(DEGREES(B45:E45))</f>
         <v>7010.4935415698783</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P45">
+        <f t="array" ref="P45:S45">DEGREES(B45:E45)</f>
+        <v>180</v>
+      </c>
+      <c r="Q45">
+        <v>-45</v>
+      </c>
+      <c r="R45">
+        <v>6875.4935415698783</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -1767,71 +2000,100 @@
         <v>2.0943951023931953</v>
       </c>
       <c r="J46">
-        <f t="shared" ref="J46:M46" si="1">RADIANS(C46)</f>
+        <f t="shared" ref="J46:M46" si="6">RADIANS(C46)</f>
         <v>-0.78539816339744828</v>
       </c>
       <c r="K46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>-12.566370614359172</v>
       </c>
       <c r="L46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="O46">
         <f t="array" ref="O46">SUM(RADIANS(B46:E46))</f>
         <v>-11.257373675363425</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P46">
+        <f t="array" ref="P46:S46">RADIANS(B46:E46)</f>
+        <v>2.0943951023931953</v>
+      </c>
+      <c r="Q46">
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="R46">
+        <v>-12.566370614359172</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>23</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47">
-        <v>3.5</v>
+        <v>-1</v>
       </c>
       <c r="D47">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>9</v>
-      </c>
-      <c r="F47" t="s">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>-1</v>
+      </c>
+      <c r="G47" t="s">
         <v>18</v>
       </c>
       <c r="I47">
         <f>POWER(B47,C47)</f>
-        <v>11.313708498984759</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J47">
         <f>POWER(C47,D47)</f>
-        <v>0.53452248382484879</v>
-      </c>
-      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="K47" t="e">
         <f>POWER(D47,E47)</f>
-        <v>-1.953125E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="L47" t="e">
         <f>POWER(E47,F47)</f>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="M47" t="e">
         <f>POWER(F47,G47)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O47">
+      <c r="O47" t="e">
         <f t="array" ref="O47">SUM(POWER(B47:D47,C47:E47))</f>
-        <v>11.846277857809609</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+        <v>#NUM!</v>
+      </c>
+      <c r="P47">
+        <f t="array" ref="P47:S47">POWER(B47:C47,D47:E47)</f>
+        <v>1</v>
+      </c>
+      <c r="Q47">
+        <v>1</v>
+      </c>
+      <c r="R47" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S47" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -1839,7 +2101,7 @@
         <v>31.5</v>
       </c>
       <c r="C48">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D48">
         <v>6.7</v>
@@ -1850,13 +2112,13 @@
       <c r="F48" t="s">
         <v>18</v>
       </c>
-      <c r="I48">
+      <c r="I48" t="e">
         <f>MOD(B48,C48)</f>
-        <v>1.5</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="J48">
         <f>MOD(C48,D48)</f>
-        <v>3.3</v>
+        <v>0</v>
       </c>
       <c r="K48">
         <f>MOD(D48,E48)</f>
@@ -1870,12 +2132,25 @@
         <f>MOD(F48,G48)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O48">
+      <c r="O48" t="e">
         <f t="array" ref="O48">SUM(MOD(B48:D48,C48:E48))</f>
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P48">
+        <f t="array" ref="P48:S48">MOD(B48:C48,D48:E48)</f>
+        <v>4.6999999999999993</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S48" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -1899,59 +2174,72 @@
         <v>1.4142135623730951</v>
       </c>
       <c r="J49">
-        <f t="shared" ref="J49:M49" si="2">SQRT(C49)</f>
+        <f t="shared" ref="J49:M49" si="7">SQRT(C49)</f>
         <v>1.8708286933869707</v>
       </c>
       <c r="K49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="L49" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#NUM!</v>
       </c>
       <c r="M49" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="O49">
         <f t="array" ref="O49">SUM(SQRT(B49:D49))</f>
         <v>6.2850422557600663</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P49">
+        <f t="array" ref="P49:S49">SQRT(B49:E49)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="Q49">
+        <v>1.8708286933869707</v>
+      </c>
+      <c r="R49">
+        <v>3</v>
+      </c>
+      <c r="S49" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H60" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(functions), #4: Add `sumproduct` function.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>ca</t>
   </si>
@@ -109,19 +109,28 @@
   </si>
   <si>
     <t>SQRT</t>
+  </si>
+  <si>
+    <t>SUMPRODUCT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,12 +153,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +456,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -454,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T60"/>
+  <dimension ref="A1:U60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -889,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <f t="shared" ref="I26:N26" si="0">LN(C26)</f>
+        <f t="shared" ref="J26:N26" si="0">LN(C26)</f>
         <v>0.91629073187415511</v>
       </c>
       <c r="K26">
@@ -950,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <f t="shared" ref="I27:P27" si="1">LOG(C27)</f>
+        <f t="shared" ref="J27:N27" si="1">LOG(C27)</f>
         <v>0.3979400086720376</v>
       </c>
       <c r="K27">
@@ -1074,7 +1084,7 @@
         <v>2</v>
       </c>
       <c r="I29">
-        <f t="shared" ref="I29:P29" si="2">ACOS(B29)</f>
+        <f t="shared" ref="I29:N29" si="2">ACOS(B29)</f>
         <v>1.5707963267948966</v>
       </c>
       <c r="J29">
@@ -1138,7 +1148,7 @@
         <v>0.5</v>
       </c>
       <c r="I30">
-        <f t="shared" ref="I30:P30" si="3">ACOSH(B30)</f>
+        <f t="shared" ref="I30:N30" si="3">ACOSH(B30)</f>
         <v>0</v>
       </c>
       <c r="J30">
@@ -1202,7 +1212,7 @@
         <v>2</v>
       </c>
       <c r="I31">
-        <f t="shared" ref="I31:P31" si="4">ASIN(B31)</f>
+        <f t="shared" ref="I31:N31" si="4">ASIN(B31)</f>
         <v>0</v>
       </c>
       <c r="J31">
@@ -1300,7 +1310,7 @@
         <v>3.6895038689889059</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1357,7 +1367,7 @@
         <v>0.78539816339744828</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1407,8 +1417,15 @@
       <c r="Q34">
         <v>-1.5707963267948966</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T34">
+        <f t="array" ref="T34:U34">ATAN2(B34:C34,D34)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="U34">
+        <v>1.5707963267948966</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1465,7 +1482,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1522,7 +1539,7 @@
         <v>0.54030230586813977</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1579,7 +1596,7 @@
         <v>1.5430806348152437</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1636,7 +1653,7 @@
         <v>-0.8414709848078965</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1693,7 +1710,7 @@
         <v>-1.1752011936438014</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -1750,7 +1767,7 @@
         <v>-1.5574077246549023</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1810,7 +1827,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -1867,7 +1884,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -1895,7 +1912,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -1923,7 +1940,7 @@
         <v>-720</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -1979,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -2033,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -2093,7 +2110,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -2149,6 +2166,10 @@
       <c r="S48" t="e">
         <v>#N/A</v>
       </c>
+      <c r="T48" s="3">
+        <f t="array" ref="T48">SUM(MOD(B48:E48,2))</f>
+        <v>3.2</v>
+      </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -2205,6 +2226,42 @@
       </c>
       <c r="S49" t="e">
         <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50">
+        <f>SUMPRODUCT(B50:C50,C50:D50,D50:E50)</f>
+        <v>6</v>
+      </c>
+      <c r="J50">
+        <f>SUMPRODUCT(C50:D50,D50:E50,E50:F50)</f>
+        <v>6</v>
+      </c>
+      <c r="K50">
+        <f>SUMPRODUCT(D50:E50,E50:F50,F50:G50)</f>
+        <v>0</v>
+      </c>
+      <c r="L50" t="e">
+        <f>SUMPRODUCT(E50:F50,F50:G50,G50)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix(functions): Correct `iserror` `iserr` functions.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -477,12 +477,12 @@
     <col min="23" max="24" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -502,7 +502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -522,7 +522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -556,7 +556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -588,7 +588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="J6" t="e">
         <f>J4:K5</f>
         <v>#VALUE!</v>
@@ -605,7 +605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>SUM(B2:E5)</f>
         <v>40</v>
@@ -637,7 +637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="J8">
         <f t="array" ref="J8:K10">G2:H2</f>
         <v>5</v>
@@ -645,8 +645,20 @@
       <c r="K8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <f>IFERROR(SUM(B2:E4),2)</f>
+        <v>26</v>
+      </c>
+      <c r="Q8" t="b">
+        <f>ISERR(#VALUE!)</f>
+        <v>1</v>
+      </c>
+      <c r="R8" t="b">
+        <f>ISERROR(SUM(D2:G4))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>SUM(a,b,d,e,f,g)</f>
         <v>104</v>
@@ -680,8 +692,20 @@
       <c r="K9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <f>IFERROR(SUM(J4:M6),2)</f>
+        <v>2</v>
+      </c>
+      <c r="Q9" t="b">
+        <f>ISERR(#N/A)</f>
+        <v>0</v>
+      </c>
+      <c r="R9" t="b">
+        <f>ISERROR(SUM(J6:M8))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D10">
         <f>SUM(B2:E5)</f>
         <v>40</v>
@@ -702,8 +726,12 @@
       <c r="K10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="R10" t="b">
+        <f>ISERROR(SUM(H16:K18))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F11">
         <f>SUM(G10:G11,G12)</f>
         <v>25</v>
@@ -714,8 +742,12 @@
       <c r="H11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="R11" t="e">
+        <f>SUM(H16:K18)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="G12">
         <v>9</v>
       </c>
@@ -726,8 +758,12 @@
         <f>J8:K10 L6:M7</f>
         <v>#NULL!</v>
       </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="R12" t="e">
+        <f>MIN(H16:J18)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>0</v>
       </c>
@@ -735,8 +771,12 @@
         <f>"ciao"&amp;B13&amp;" cc" &amp;C13</f>
         <v>ciao ccca</v>
       </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="R13" t="e">
+        <f>SUMPRODUCT(H16:J18)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E14" t="str">
         <f>"ciao"&amp;B13&amp;" cc" &amp;C13</f>
         <v>ciao ccca</v>
@@ -753,7 +793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1</v>
       </c>
@@ -771,7 +811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H16">
         <f t="array" ref="H16:J18">G11:H12</f>
         <v>9</v>

</xml_diff>

<commit_message>
feat(functions), #11: Add `HEX2OCT`, `HEX2BIN`, `HEX2DEC`, `OCT2HEX`, `OCT2BIN`, `OCT2DEC`, `BIN2HEX`, `BIN2OCT`, `BIN2DEC`, `DEC2HEX`, `DEC2OCT`, and `DEC2BIN` functions.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5C0092-D81D-1643-A5F4-836DCAE164F3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE79BC65-31AC-C94A-B994-F853FB7FB6C7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -23,9 +23,10 @@
     <sheet name="CORE" sheetId="1" r:id="rId8"/>
     <sheet name="REF" sheetId="2" r:id="rId9"/>
     <sheet name="OPERATORS" sheetId="13" r:id="rId10"/>
+    <sheet name="ENGINEERING" sheetId="15" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="a">CORE!$B$2:$C$3</definedName>
@@ -35,7 +36,7 @@
     <definedName name="f">CORE!$G$2:$H$5</definedName>
     <definedName name="g">REF!$B$2:$B$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="427">
   <si>
     <t>ca</t>
   </si>
@@ -1155,6 +1156,177 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>BESSELI</t>
+  </si>
+  <si>
+    <t>BESSELJ</t>
+  </si>
+  <si>
+    <t>BESSELK</t>
+  </si>
+  <si>
+    <t>BESSELY</t>
+  </si>
+  <si>
+    <t>BIN2DEC</t>
+  </si>
+  <si>
+    <t>BIN2HEX</t>
+  </si>
+  <si>
+    <t>BIN2OCT</t>
+  </si>
+  <si>
+    <t>BITAND</t>
+  </si>
+  <si>
+    <t>BITLSHIFT</t>
+  </si>
+  <si>
+    <t>BITOR</t>
+  </si>
+  <si>
+    <t>BITRSHIFT</t>
+  </si>
+  <si>
+    <t>BITXOR</t>
+  </si>
+  <si>
+    <t>COMPLEX</t>
+  </si>
+  <si>
+    <t>CONVERT</t>
+  </si>
+  <si>
+    <t>DEC2BIN</t>
+  </si>
+  <si>
+    <t>DEC2HEX</t>
+  </si>
+  <si>
+    <t>DEC2OCT</t>
+  </si>
+  <si>
+    <t>DELTA</t>
+  </si>
+  <si>
+    <t>ERF</t>
+  </si>
+  <si>
+    <t>ERF.PRECISE</t>
+  </si>
+  <si>
+    <t>ERFC</t>
+  </si>
+  <si>
+    <t>ERFC.PRECISE</t>
+  </si>
+  <si>
+    <t>GESTEP</t>
+  </si>
+  <si>
+    <t>HEX2BIN</t>
+  </si>
+  <si>
+    <t>HEX2DEC</t>
+  </si>
+  <si>
+    <t>HEX2OCT</t>
+  </si>
+  <si>
+    <t>IMABS</t>
+  </si>
+  <si>
+    <t>IMAGINARY</t>
+  </si>
+  <si>
+    <t>IMARGUMENT</t>
+  </si>
+  <si>
+    <t>IMCONJUGATE</t>
+  </si>
+  <si>
+    <t>IMCOS</t>
+  </si>
+  <si>
+    <t>IMCOSH</t>
+  </si>
+  <si>
+    <t>IMCOT</t>
+  </si>
+  <si>
+    <t>IMCSC</t>
+  </si>
+  <si>
+    <t>IMCSCH</t>
+  </si>
+  <si>
+    <t>IMDIV</t>
+  </si>
+  <si>
+    <t>IMEXP</t>
+  </si>
+  <si>
+    <t>IMLN</t>
+  </si>
+  <si>
+    <t>IMLOG10</t>
+  </si>
+  <si>
+    <t>IMLOG2</t>
+  </si>
+  <si>
+    <t>IMPOWER</t>
+  </si>
+  <si>
+    <t>IMPRODUCT</t>
+  </si>
+  <si>
+    <t>IMREAL</t>
+  </si>
+  <si>
+    <t>IMSEC</t>
+  </si>
+  <si>
+    <t>IMSECH</t>
+  </si>
+  <si>
+    <t>IMSIN</t>
+  </si>
+  <si>
+    <t>IMSINH</t>
+  </si>
+  <si>
+    <t>IMSQRT</t>
+  </si>
+  <si>
+    <t>IMSUB</t>
+  </si>
+  <si>
+    <t>IMSUM</t>
+  </si>
+  <si>
+    <t>IMTAN</t>
+  </si>
+  <si>
+    <t>OCT2BIN</t>
+  </si>
+  <si>
+    <t>OCT2DEC</t>
+  </si>
+  <si>
+    <t>OCT2HEX</t>
+  </si>
+  <si>
+    <t>fffffffffe</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>f000000000</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1336,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1204,6 +1376,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.3"/>
+      <color rgb="FFE6DB74"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1253,7 +1431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1302,11 +1480,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1613,7 +1796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52929E63-D802-7443-B5FD-6A6404B94706}">
   <dimension ref="A1:AV81"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1650,70 +1833,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -1723,22 +1906,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -1748,36 +1931,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="27" t="s">
+      <c r="Y2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="27" t="s">
+      <c r="AG2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="27"/>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="27"/>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="27"/>
-      <c r="AR2" s="27"/>
-      <c r="AS2" s="27"/>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="31"/>
+      <c r="AS2" s="31"/>
+      <c r="AT2" s="31"/>
+      <c r="AU2" s="31"/>
+      <c r="AV2" s="31"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
@@ -11808,107 +11991,107 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06743156-B15F-3C4D-BF5C-DF8A4FD21BB1}">
   <dimension ref="A1:AV81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.5" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.1640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.83203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.1640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.83203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4" style="30" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5" style="30" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.83203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.83203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="5.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.1640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="5.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="29" max="31" width="4.83203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.83203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="33" max="48" width="5.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="49" max="16384" width="10.83203125" style="30"/>
+    <col min="1" max="1" width="6.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.83203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.83203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4" style="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5" style="29" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.83203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.83203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="5.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="5.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="4.83203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.83203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="33" max="48" width="5.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="49" max="16384" width="10.83203125" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
     </row>
     <row r="2" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="26" t="s">
         <v>38</v>
       </c>
@@ -11918,22 +12101,22 @@
       <c r="I2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="26" t="s">
         <v>38</v>
       </c>
@@ -11943,39 +12126,39 @@
       <c r="X2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="27" t="s">
+      <c r="Y2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
       <c r="AF2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="27" t="s">
+      <c r="AG2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="27"/>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="27"/>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="27"/>
-      <c r="AR2" s="27"/>
-      <c r="AS2" s="27"/>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="31"/>
+      <c r="AS2" s="31"/>
+      <c r="AT2" s="31"/>
+      <c r="AU2" s="31"/>
+      <c r="AV2" s="31"/>
     </row>
     <row r="3" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>355</v>
       </c>
       <c r="B3" s="14">
@@ -12138,7 +12321,7 @@
       </c>
     </row>
     <row r="4" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>356</v>
       </c>
       <c r="B4" s="14">
@@ -12300,7 +12483,7 @@
       </c>
     </row>
     <row r="5" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="29" t="s">
         <v>357</v>
       </c>
       <c r="B5" s="14">
@@ -12461,7 +12644,7 @@
       </c>
     </row>
     <row r="6" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="29" t="s">
         <v>358</v>
       </c>
       <c r="B6" s="14">
@@ -12622,7 +12805,7 @@
       </c>
     </row>
     <row r="7" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>359</v>
       </c>
       <c r="B7" s="14">
@@ -12784,7 +12967,7 @@
       </c>
     </row>
     <row r="8" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>360</v>
       </c>
       <c r="B8" s="14">
@@ -12946,7 +13129,7 @@
       </c>
     </row>
     <row r="9" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>361</v>
       </c>
       <c r="B9" s="14">
@@ -13083,7 +13266,7 @@
       <c r="AV9" s="4"/>
     </row>
     <row r="10" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="28" t="s">
         <v>362</v>
       </c>
       <c r="B10" s="14">
@@ -13220,7 +13403,7 @@
       <c r="AV10" s="4"/>
     </row>
     <row r="11" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="28" t="s">
         <v>363</v>
       </c>
       <c r="B11" s="14">
@@ -13357,7 +13540,7 @@
       <c r="AV11" s="4"/>
     </row>
     <row r="12" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="28" t="s">
         <v>364</v>
       </c>
       <c r="B12" s="14">
@@ -13494,7 +13677,7 @@
       <c r="AV12" s="4"/>
     </row>
     <row r="13" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>365</v>
       </c>
       <c r="B13" s="14">
@@ -13631,7 +13814,7 @@
       <c r="AV13" s="4"/>
     </row>
     <row r="14" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="28" t="s">
         <v>366</v>
       </c>
       <c r="B14" s="14">
@@ -13768,7 +13951,7 @@
       <c r="AV14" s="4"/>
     </row>
     <row r="15" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="28" t="s">
         <v>367</v>
       </c>
       <c r="B15" s="14">
@@ -13905,7 +14088,7 @@
       <c r="AV15" s="4"/>
     </row>
     <row r="16" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="28" t="s">
         <v>368</v>
       </c>
       <c r="B16" s="14">
@@ -14042,7 +14225,7 @@
       <c r="AV16" s="4"/>
     </row>
     <row r="17" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="28" t="s">
         <v>369</v>
       </c>
       <c r="B17" s="14">
@@ -14179,7 +14362,7 @@
       <c r="AV17" s="4"/>
     </row>
     <row r="18" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="29"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -14229,7 +14412,7 @@
       <c r="AV18" s="4"/>
     </row>
     <row r="19" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="29"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -14279,7 +14462,7 @@
       <c r="AV19" s="4"/>
     </row>
     <row r="20" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="29"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -14404,6 +14587,1878 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E55D778-8138-E945-B7BE-C1CFFC3F5C7B}">
+  <dimension ref="A1:BJ56"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="41" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="46" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="49" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A1" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y2" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
+      <c r="AF2" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG2" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="31"/>
+      <c r="AS2" s="31"/>
+      <c r="AT2" s="31"/>
+      <c r="AU2" s="31"/>
+      <c r="AV2" s="31"/>
+    </row>
+    <row r="3" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A3" s="16" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="4" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A4" s="16" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A5" s="30" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A6" s="30" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="7" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A7" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="B7" s="14">
+        <v>0</v>
+      </c>
+      <c r="C7" s="14">
+        <v>111111111</v>
+      </c>
+      <c r="D7" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1000000000</v>
+      </c>
+      <c r="F7" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="I7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K7" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L7" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N7" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O7" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P7" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q7" s="6">
+        <f>BIN2DEC(B7)</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="6">
+        <f t="shared" ref="R7:AE7" si="0">BIN2DEC(C7)</f>
+        <v>511</v>
+      </c>
+      <c r="S7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T7" s="6">
+        <f t="shared" si="0"/>
+        <v>-512</v>
+      </c>
+      <c r="U7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V7" s="6">
+        <f>BIN2DEC(G7)</f>
+        <v>0</v>
+      </c>
+      <c r="W7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="X7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="14"/>
+      <c r="AH7" s="14"/>
+      <c r="AI7" s="14"/>
+      <c r="AJ7" s="14"/>
+      <c r="AK7" s="14"/>
+      <c r="AL7" s="6"/>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="6"/>
+      <c r="AO7" s="6"/>
+      <c r="AP7" s="6"/>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="9"/>
+      <c r="AT7" s="9"/>
+      <c r="AU7" s="9"/>
+      <c r="AV7" s="6"/>
+      <c r="AW7" s="6"/>
+      <c r="AX7" s="6"/>
+      <c r="AY7" s="6"/>
+      <c r="AZ7" s="6"/>
+      <c r="BA7" s="6"/>
+      <c r="BB7" s="6"/>
+      <c r="BC7" s="6"/>
+      <c r="BD7" s="6"/>
+      <c r="BE7" s="6"/>
+      <c r="BF7" s="6"/>
+      <c r="BG7" s="6"/>
+      <c r="BH7" s="6"/>
+      <c r="BI7" s="6"/>
+      <c r="BJ7" s="6"/>
+    </row>
+    <row r="8" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A8" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0</v>
+      </c>
+      <c r="C8" s="14">
+        <v>111111111</v>
+      </c>
+      <c r="D8" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E8" s="14">
+        <v>1000000000</v>
+      </c>
+      <c r="F8" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="I8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K8" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L8" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N8" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O8" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P8" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q8" s="6" t="str">
+        <f>BIN2HEX(B8)</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="6" t="str">
+        <f t="shared" ref="R8:AE8" si="1">BIN2HEX(C8)</f>
+        <v>1FF</v>
+      </c>
+      <c r="S8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T8" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>FFFFFFFE00</v>
+      </c>
+      <c r="U8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V8" s="6" t="e">
+        <f>BIN2HEX(G8,0)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="W8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="X8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="6"/>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="6"/>
+      <c r="AO8" s="6"/>
+      <c r="AP8" s="6"/>
+      <c r="AQ8" s="6"/>
+      <c r="AR8" s="6"/>
+      <c r="AS8" s="6"/>
+      <c r="AT8" s="6"/>
+      <c r="AU8" s="6"/>
+    </row>
+    <row r="9" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A9" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="B9" s="14">
+        <v>0</v>
+      </c>
+      <c r="C9" s="14">
+        <v>111111111</v>
+      </c>
+      <c r="D9" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E9" s="14">
+        <v>1000000000</v>
+      </c>
+      <c r="F9" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="I9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K9" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L9" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N9" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O9" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P9" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q9" s="6" t="str">
+        <f>BIN2OCT(B9)</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="6" t="str">
+        <f t="shared" ref="R9:AE9" si="2">BIN2OCT(C9)</f>
+        <v>777</v>
+      </c>
+      <c r="S9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T9" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>7777777000</v>
+      </c>
+      <c r="U9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V9" s="6" t="e">
+        <f>BIN2OCT(G9,0)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="W9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="X9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A10" s="16" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="11" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A11" s="16" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="12" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A12" s="16" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="13" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A13" s="16" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="14" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A14" s="16" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="15" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A15" s="16" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="16" spans="1:62" x14ac:dyDescent="0.15">
+      <c r="A16" s="16" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="17" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A17" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="B17" s="14">
+        <f>C17+1</f>
+        <v>512.70000000000005</v>
+      </c>
+      <c r="C17" s="14">
+        <v>511.7</v>
+      </c>
+      <c r="D17" s="14">
+        <v>100</v>
+      </c>
+      <c r="E17" s="14">
+        <f>-C17-1</f>
+        <v>-512.70000000000005</v>
+      </c>
+      <c r="F17" s="14">
+        <f>E17-1</f>
+        <v>-513.70000000000005</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="I17" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K17" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L17" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N17" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O17" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P17" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q17" s="6" t="e">
+        <f>DEC2BIN(B17)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="R17" s="6" t="str">
+        <f t="shared" ref="R17:AE17" si="3">DEC2BIN(C17)</f>
+        <v>111111111</v>
+      </c>
+      <c r="S17" s="6" t="e">
+        <f>DEC2BIN(D17,1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="T17" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>1000000000</v>
+      </c>
+      <c r="U17" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V17" s="6" t="str">
+        <f>DEC2BIN(G17,3)</f>
+        <v>000</v>
+      </c>
+      <c r="W17" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X17" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y17" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z17" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA17" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB17" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC17" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD17" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE17" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A18" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="B18" s="14">
+        <f t="shared" ref="B18:B19" si="4">C18+1</f>
+        <v>549755813888.69995</v>
+      </c>
+      <c r="C18" s="14">
+        <v>549755813887.70001</v>
+      </c>
+      <c r="D18" s="14">
+        <v>100</v>
+      </c>
+      <c r="E18" s="14">
+        <f t="shared" ref="E18:E19" si="5">-C18-1</f>
+        <v>-549755813888.69995</v>
+      </c>
+      <c r="F18" s="14">
+        <f t="shared" ref="F18:F19" si="6">E18-1</f>
+        <v>-549755813889.69995</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="I18" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K18" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L18" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N18" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O18" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P18" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q18" s="6" t="e">
+        <f>DEC2HEX(B18)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="R18" s="6" t="str">
+        <f t="shared" ref="R18:AE18" si="7">DEC2HEX(C18)</f>
+        <v>7FFFFFFFFF</v>
+      </c>
+      <c r="S18" s="6" t="e">
+        <f>DEC2HEX(D18,1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="T18" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>8000000000</v>
+      </c>
+      <c r="U18" s="6" t="e">
+        <f>DEC2HEX(F18)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="V18" s="6" t="str">
+        <f>DEC2HEX(G18,1)</f>
+        <v>0</v>
+      </c>
+      <c r="W18" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X18" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y18" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z18" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA18" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB18" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC18" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD18" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE18" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF18" s="11"/>
+      <c r="AG18" s="6"/>
+      <c r="AH18" s="6"/>
+      <c r="AI18" s="6"/>
+      <c r="AJ18" s="6"/>
+      <c r="AK18" s="6"/>
+      <c r="AL18" s="6"/>
+      <c r="AM18" s="6"/>
+      <c r="AN18" s="6"/>
+      <c r="AO18" s="6"/>
+      <c r="AP18" s="6"/>
+      <c r="AQ18" s="6"/>
+      <c r="AR18" s="6"/>
+      <c r="AS18" s="6"/>
+      <c r="AT18" s="6"/>
+      <c r="AU18" s="6"/>
+    </row>
+    <row r="19" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A19" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="B19" s="14">
+        <f t="shared" si="4"/>
+        <v>536870912.70000005</v>
+      </c>
+      <c r="C19" s="14">
+        <v>536870911.69999999</v>
+      </c>
+      <c r="D19" s="14">
+        <v>100</v>
+      </c>
+      <c r="E19" s="14">
+        <f t="shared" si="5"/>
+        <v>-536870912.70000005</v>
+      </c>
+      <c r="F19" s="14">
+        <f t="shared" si="6"/>
+        <v>-536870913.70000005</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="I19" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K19" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L19" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N19" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O19" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P19" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q19" s="6" t="e">
+        <f>DEC2OCT(B19)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="R19" s="6" t="str">
+        <f t="shared" ref="R19:AE19" si="8">DEC2OCT(C19)</f>
+        <v>3777777777</v>
+      </c>
+      <c r="S19" s="6" t="e">
+        <f>DEC2OCT(D19,1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="T19" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>4000000000</v>
+      </c>
+      <c r="U19" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V19" s="6" t="e">
+        <f>DEC2OCT(G19,0)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="W19" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X19" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y19" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z19" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA19" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB19" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC19" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD19" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE19" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A20" s="16" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="21" spans="1:47" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="L21" s="33"/>
+    </row>
+    <row r="22" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A22" s="16" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="23" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A23" s="4" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="24" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A24" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="25" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A25" s="4" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="26" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A26" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="B26" s="14">
+        <v>0</v>
+      </c>
+      <c r="C26" s="14">
+        <v>9999999999</v>
+      </c>
+      <c r="D26" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E26" s="14">
+        <v>11111111111</v>
+      </c>
+      <c r="F26" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="I26" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K26" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L26" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M26" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N26" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O26" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P26" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q26" s="6" t="str">
+        <f>HEX2BIN(B26)</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="6" t="e">
+        <f>HEX2BIN(C26)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="S26" s="6" t="e">
+        <f>HEX2BIN(D26)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="T26" s="6" t="e">
+        <f t="shared" ref="S26:AE26" si="9">HEX2BIN(E26)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="U26" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V26" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="W26" s="6" t="str">
+        <f>HEX2BIN(H26)</f>
+        <v>1111111110</v>
+      </c>
+      <c r="X26" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y26" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z26" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA26" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB26" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC26" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD26" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE26" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF26" s="10"/>
+      <c r="AG26" s="6" t="e">
+        <f t="array" ref="AG26:AN26">HEX2BIN(B26:I26)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AH26" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI26" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AJ26" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AK26" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL26" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM26" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN26" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A27" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B27" s="14">
+        <v>0</v>
+      </c>
+      <c r="C27" s="14">
+        <v>9999999999</v>
+      </c>
+      <c r="D27" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E27" s="14">
+        <v>11111111111</v>
+      </c>
+      <c r="F27" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="I27" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K27" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L27" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M27" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N27" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O27" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P27" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q27" s="6">
+        <f>HEX2DEC(B27)</f>
+        <v>0</v>
+      </c>
+      <c r="R27" s="6">
+        <f>HEX2DEC(C27)</f>
+        <v>-439804651111</v>
+      </c>
+      <c r="S27" s="6" t="e">
+        <f>HEX2DEC(D27)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="T27" s="6" t="e">
+        <f t="shared" ref="R27:AE27" si="10">HEX2DEC(E27)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="U27" s="6" t="e">
+        <f>HEX2DEC(F27)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="V27" s="6">
+        <f>HEX2DEC(G27)</f>
+        <v>0</v>
+      </c>
+      <c r="W27" s="6">
+        <f>HEX2DEC(H27)</f>
+        <v>-68719476736</v>
+      </c>
+      <c r="X27" s="6" t="e">
+        <f>HEX2DEC(I27)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y27" s="6" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z27" s="6" t="e">
+        <f t="shared" si="10"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA27" s="6" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB27" s="6" t="e">
+        <f t="shared" si="10"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC27" s="6" t="e">
+        <f t="shared" si="10"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD27" s="6" t="e">
+        <f t="shared" si="10"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE27" s="6" t="e">
+        <f t="shared" si="10"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="6" t="e">
+        <f t="array" ref="AG27:AN27">HEX2DEC(B27:I27)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AH27" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI27" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AJ27" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AK27" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL27" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM27" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN27" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO27" s="6"/>
+      <c r="AP27" s="6"/>
+      <c r="AQ27" s="6"/>
+      <c r="AR27" s="6"/>
+      <c r="AS27" s="6"/>
+      <c r="AT27" s="6"/>
+      <c r="AU27" s="6"/>
+    </row>
+    <row r="28" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A28" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="B28" s="14">
+        <v>0</v>
+      </c>
+      <c r="C28" s="14">
+        <v>9999999999</v>
+      </c>
+      <c r="D28" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E28" s="14">
+        <v>11111111111</v>
+      </c>
+      <c r="F28" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="I28" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K28" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L28" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M28" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N28" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O28" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P28" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q28" s="6" t="str">
+        <f>HEX2OCT(B28)</f>
+        <v>0</v>
+      </c>
+      <c r="R28" s="6" t="e">
+        <f t="shared" ref="R28:AE28" si="11">HEX2OCT(C28)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="S28" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T28" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U28" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V28" s="6" t="str">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W28" s="6" t="str">
+        <f>HEX2OCT(H28)</f>
+        <v>7777777776</v>
+      </c>
+      <c r="X28" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y28" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z28" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA28" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB28" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC28" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD28" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE28" s="6" t="e">
+        <f t="shared" si="11"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF28" s="10"/>
+      <c r="AG28" s="6" t="e">
+        <f t="array" ref="AG28:AN28">HEX2OCT(B28:I28)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AH28" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI28" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AJ28" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AK28" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL28" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM28" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN28" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="30" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A30" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A31" s="4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="32" spans="1:47" x14ac:dyDescent="0.15">
+      <c r="A32" s="4" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="4" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" s="4" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="4" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40" s="4" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A41" s="4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A42" s="4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A43" s="4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A44" s="4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A45" s="4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A46" s="4" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A47" s="4" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A48" s="4" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="A50" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="A51" s="4" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="A52" s="4" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="A53" s="4" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="A54" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="B54" s="14">
+        <v>0</v>
+      </c>
+      <c r="C54" s="14">
+        <v>7777777777</v>
+      </c>
+      <c r="D54" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E54" s="14">
+        <v>11111111111</v>
+      </c>
+      <c r="F54" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="I54" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J54" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K54" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L54" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M54" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N54" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O54" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P54" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q54" s="6" t="str">
+        <f>OCT2BIN(B54)</f>
+        <v>0</v>
+      </c>
+      <c r="R54" s="6" t="str">
+        <f t="shared" ref="R54:AE54" si="12">OCT2BIN(C54)</f>
+        <v>1111111111</v>
+      </c>
+      <c r="S54" s="6" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T54" s="6" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U54" s="6" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V54" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W54" s="6" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="X54" s="6" t="e">
+        <f t="shared" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y54" s="6" t="e">
+        <f t="shared" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z54" s="6" t="e">
+        <f t="shared" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA54" s="6" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB54" s="6" t="e">
+        <f t="shared" si="12"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC54" s="6" t="e">
+        <f t="shared" si="12"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD54" s="6" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE54" s="6" t="e">
+        <f t="shared" si="12"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="A55" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="B55" s="14">
+        <v>0</v>
+      </c>
+      <c r="C55" s="14">
+        <v>7777777777</v>
+      </c>
+      <c r="D55" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E55" s="14">
+        <v>11111111111</v>
+      </c>
+      <c r="F55" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="I55" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J55" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K55" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L55" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M55" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N55" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O55" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P55" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q55" s="6">
+        <f>OCT2DEC(B55)</f>
+        <v>0</v>
+      </c>
+      <c r="R55" s="6">
+        <f t="shared" ref="R55:AE55" si="13">OCT2DEC(C55)</f>
+        <v>-1</v>
+      </c>
+      <c r="S55" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T55" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U55" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V55" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="W55" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="X55" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y55" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z55" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA55" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB55" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC55" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD55" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE55" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.15">
+      <c r="A56" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="B56" s="14">
+        <v>0</v>
+      </c>
+      <c r="C56" s="14">
+        <v>7777777777</v>
+      </c>
+      <c r="D56" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E56" s="14">
+        <v>11111111111</v>
+      </c>
+      <c r="F56" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="I56" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J56" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K56" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L56" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M56" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N56" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O56" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P56" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q56" s="6" t="str">
+        <f>OCT2HEX(B56)</f>
+        <v>0</v>
+      </c>
+      <c r="R56" s="6" t="str">
+        <f t="shared" ref="R56:AE56" si="14">OCT2HEX(C56)</f>
+        <v>FFFFFFFFFF</v>
+      </c>
+      <c r="S56" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T56" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U56" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V56" s="6" t="str">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="W56" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="X56" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y56" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z56" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA56" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB56" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC56" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD56" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE56" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1752443E-D395-6347-A5AF-550B6945E519}">
   <dimension ref="A1:BJ57"/>
@@ -14457,70 +16512,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -14530,22 +16585,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -14555,36 +16610,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="27" t="s">
+      <c r="Y2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="27" t="s">
+      <c r="AG2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="27"/>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="27"/>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="27"/>
-      <c r="AR2" s="27"/>
-      <c r="AS2" s="27"/>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="31"/>
+      <c r="AS2" s="31"/>
+      <c r="AT2" s="31"/>
+      <c r="AU2" s="31"/>
+      <c r="AV2" s="31"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -15213,70 +17268,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -15286,22 +17341,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -15311,36 +17366,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="27" t="s">
+      <c r="Y2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="27" t="s">
+      <c r="AG2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="27"/>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="27"/>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="27"/>
-      <c r="AR2" s="27"/>
-      <c r="AS2" s="27"/>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="31"/>
+      <c r="AS2" s="31"/>
+      <c r="AT2" s="31"/>
+      <c r="AU2" s="31"/>
+      <c r="AV2" s="31"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -17193,70 +19248,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -17266,22 +19321,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -17291,36 +19346,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="27" t="s">
+      <c r="Y2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="27" t="s">
+      <c r="AG2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="27"/>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="27"/>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="27"/>
-      <c r="AR2" s="27"/>
-      <c r="AS2" s="27"/>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="31"/>
+      <c r="AS2" s="31"/>
+      <c r="AT2" s="31"/>
+      <c r="AU2" s="31"/>
+      <c r="AV2" s="31"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -18406,70 +20461,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -18479,22 +20534,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -18504,36 +20559,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="27" t="s">
+      <c r="Y2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="27" t="s">
+      <c r="AG2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="27"/>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="27"/>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="27"/>
-      <c r="AR2" s="27"/>
-      <c r="AS2" s="27"/>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="31"/>
+      <c r="AS2" s="31"/>
+      <c r="AT2" s="31"/>
+      <c r="AU2" s="31"/>
+      <c r="AV2" s="31"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -19016,70 +21071,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="19" t="s">
         <v>38</v>
       </c>
@@ -19089,22 +21144,22 @@
       <c r="I2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="19" t="s">
         <v>38</v>
       </c>
@@ -19114,36 +21169,36 @@
       <c r="X2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="27" t="s">
+      <c r="Y2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
       <c r="AF2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="27" t="s">
+      <c r="AG2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="27"/>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="27"/>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="27"/>
-      <c r="AR2" s="27"/>
-      <c r="AS2" s="27"/>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="31"/>
+      <c r="AS2" s="31"/>
+      <c r="AT2" s="31"/>
+      <c r="AU2" s="31"/>
+      <c r="AV2" s="31"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -19303,7 +21358,7 @@
       </c>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="32" t="s">
         <v>338</v>
       </c>
       <c r="B10" s="22">
@@ -19461,7 +21516,7 @@
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A11" s="28"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -19568,7 +21623,7 @@
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A12" s="28"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -19691,7 +21746,7 @@
       <c r="Q15" s="6"/>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="32" t="s">
         <v>342</v>
       </c>
       <c r="B16" s="22">
@@ -19853,7 +21908,7 @@
       </c>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A17" s="28"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -19984,7 +22039,7 @@
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A18" s="28"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
@@ -20115,7 +22170,7 @@
       </c>
     </row>
     <row r="19" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A19" s="28"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
@@ -20246,7 +22301,7 @@
       </c>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A20" s="28"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
@@ -20377,7 +22432,7 @@
       </c>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A21" s="28"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -20508,7 +22563,7 @@
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A22" s="28"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
@@ -20639,7 +22694,7 @@
       </c>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A23" s="28"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
@@ -20770,7 +22825,7 @@
       </c>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A24" s="28"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -20900,7 +22955,7 @@
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="32" t="s">
         <v>352</v>
       </c>
       <c r="B25" s="22">
@@ -21025,7 +23080,7 @@
       <c r="AU25" s="6"/>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A26" s="28"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="22">
         <v>-2</v>
       </c>
@@ -21134,7 +23189,7 @@
       <c r="AG26" s="6"/>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A27" s="28"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="22">
         <v>-2</v>
       </c>
@@ -21243,7 +23298,7 @@
       <c r="AG27" s="6"/>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A28" s="28"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="22">
         <v>-2</v>
       </c>
@@ -21352,7 +23407,7 @@
       <c r="AG28" s="6"/>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A29" s="28"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="22">
         <v>-2</v>
       </c>
@@ -21461,7 +23516,7 @@
       <c r="AG29" s="6"/>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A30" s="28"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="22">
         <v>-2</v>
       </c>
@@ -21570,7 +23625,7 @@
       <c r="AG30" s="6"/>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A31" s="28"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="22">
         <v>-2</v>
       </c>
@@ -21679,7 +23734,7 @@
       <c r="AG31" s="6"/>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A32" s="28"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="22">
         <v>-2</v>
       </c>
@@ -21788,7 +23843,7 @@
       <c r="AG32" s="6"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A33" s="28"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="22">
         <v>-2</v>
       </c>
@@ -21897,7 +23952,7 @@
       <c r="AG33" s="6"/>
     </row>
     <row r="34" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="32" t="s">
         <v>351</v>
       </c>
       <c r="B34" s="22">
@@ -22022,7 +24077,7 @@
       <c r="AU34" s="6"/>
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A35" s="28"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="22">
         <v>-2</v>
       </c>
@@ -22131,7 +24186,7 @@
       <c r="AG35" s="6"/>
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A36" s="28"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="22">
         <v>-2</v>
       </c>
@@ -22240,7 +24295,7 @@
       <c r="AG36" s="6"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A37" s="28"/>
+      <c r="A37" s="32"/>
       <c r="B37" s="22">
         <v>-2</v>
       </c>
@@ -22349,7 +24404,7 @@
       <c r="AG37" s="6"/>
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A38" s="28"/>
+      <c r="A38" s="32"/>
       <c r="B38" s="22">
         <v>-2</v>
       </c>
@@ -22458,7 +24513,7 @@
       <c r="AG38" s="6"/>
     </row>
     <row r="39" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A39" s="28"/>
+      <c r="A39" s="32"/>
       <c r="B39" s="22">
         <v>-2</v>
       </c>
@@ -22567,7 +24622,7 @@
       <c r="AG39" s="6"/>
     </row>
     <row r="40" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A40" s="28"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="22">
         <v>-2</v>
       </c>
@@ -22676,7 +24731,7 @@
       <c r="AG40" s="6"/>
     </row>
     <row r="41" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A41" s="28"/>
+      <c r="A41" s="32"/>
       <c r="B41" s="22">
         <v>-2</v>
       </c>
@@ -22785,7 +24840,7 @@
       <c r="AG41" s="6"/>
     </row>
     <row r="42" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A42" s="28"/>
+      <c r="A42" s="32"/>
       <c r="B42" s="22">
         <v>-2</v>
       </c>
@@ -22894,7 +24949,7 @@
       <c r="AG42" s="6"/>
     </row>
     <row r="43" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="32" t="s">
         <v>353</v>
       </c>
       <c r="B43" s="22">
@@ -23019,7 +25074,7 @@
       <c r="AU43" s="6"/>
     </row>
     <row r="44" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A44" s="28"/>
+      <c r="A44" s="32"/>
       <c r="B44" s="22">
         <v>-2</v>
       </c>
@@ -23128,7 +25183,7 @@
       <c r="AG44" s="6"/>
     </row>
     <row r="45" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A45" s="28"/>
+      <c r="A45" s="32"/>
       <c r="B45" s="22">
         <v>-2</v>
       </c>
@@ -23237,7 +25292,7 @@
       <c r="AG45" s="6"/>
     </row>
     <row r="46" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A46" s="28"/>
+      <c r="A46" s="32"/>
       <c r="B46" s="22">
         <v>-2</v>
       </c>
@@ -23346,7 +25401,7 @@
       <c r="AG46" s="6"/>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A47" s="28"/>
+      <c r="A47" s="32"/>
       <c r="B47" s="22">
         <v>-2</v>
       </c>
@@ -23455,7 +25510,7 @@
       <c r="AG47" s="6"/>
     </row>
     <row r="48" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A48" s="28"/>
+      <c r="A48" s="32"/>
       <c r="B48" s="22">
         <v>-2</v>
       </c>
@@ -23564,7 +25619,7 @@
       <c r="AG48" s="6"/>
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A49" s="28"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="22">
         <v>-2</v>
       </c>
@@ -23673,7 +25728,7 @@
       <c r="AG49" s="6"/>
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A50" s="28"/>
+      <c r="A50" s="32"/>
       <c r="B50" s="22">
         <v>-2</v>
       </c>
@@ -23782,7 +25837,7 @@
       <c r="AG50" s="6"/>
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A51" s="28"/>
+      <c r="A51" s="32"/>
       <c r="B51" s="22">
         <v>-2</v>
       </c>
@@ -24061,7 +26116,7 @@
       <c r="AE56" s="6"/>
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A57" s="28" t="s">
+      <c r="A57" s="32" t="s">
         <v>348</v>
       </c>
       <c r="B57" s="22">
@@ -24170,7 +26225,7 @@
       </c>
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A58" s="28"/>
+      <c r="A58" s="32"/>
       <c r="B58" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -24277,7 +26332,7 @@
       </c>
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="A59" s="28"/>
+      <c r="A59" s="32"/>
       <c r="B59" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -24673,12 +26728,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A25:A33"/>
-    <mergeCell ref="A34:A42"/>
-    <mergeCell ref="A43:A51"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A16:A24"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:P1"/>
     <mergeCell ref="Q1:AV1"/>
@@ -24687,6 +26736,12 @@
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="Y2:AE2"/>
     <mergeCell ref="AG2:AV2"/>
+    <mergeCell ref="A25:A33"/>
+    <mergeCell ref="A34:A42"/>
+    <mergeCell ref="A43:A51"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A16:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -24698,7 +26753,7 @@
   <dimension ref="A1:BJ22"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="AM5" sqref="AM5"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -24749,70 +26804,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -24822,22 +26877,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -24847,36 +26902,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="27" t="s">
+      <c r="Y2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="27" t="s">
+      <c r="AG2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="27"/>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="27"/>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="27"/>
-      <c r="AR2" s="27"/>
-      <c r="AS2" s="27"/>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="31"/>
+      <c r="AS2" s="31"/>
+      <c r="AT2" s="31"/>
+      <c r="AU2" s="31"/>
+      <c r="AV2" s="31"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">

</xml_diff>

<commit_message>
feat(functions), #26: Add `SWITCH`.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DC866F-E404-6247-93D7-C41DC5991C1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1FEE7C-6462-064E-95BE-6C9C5541E743}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="770" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="427">
   <si>
     <t>ca</t>
   </si>
@@ -1802,7 +1802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -27781,7 +27781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BJ22"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -27805,7 +27805,8 @@
     <col min="17" max="17" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2.5" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="2.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.5" style="4" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -27815,20 +27816,22 @@
     <col min="29" max="30" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="2.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="2.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="2.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="2.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="2.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="2.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="3" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="3.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="2.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="49" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
@@ -28431,8 +28434,165 @@
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="17" t="s">
         <v>234</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0</v>
+      </c>
+      <c r="C11" s="14">
+        <v>2</v>
+      </c>
+      <c r="D11" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E11" s="14">
+        <v>10</v>
+      </c>
+      <c r="F11" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K11" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L11" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N11" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O11" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P11" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q11" s="4">
+        <f t="shared" ref="Q11:S11" si="9">_xlfn.SWITCH(B11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>3</v>
+      </c>
+      <c r="R11" s="4">
+        <f t="shared" ref="R11" si="10">_xlfn.SWITCH(C11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="4">
+        <f t="shared" ref="S11" si="11">_xlfn.SWITCH(D11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>5</v>
+      </c>
+      <c r="T11" s="4">
+        <f t="shared" ref="T11" si="12">_xlfn.SWITCH(E11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>7</v>
+      </c>
+      <c r="U11" s="4">
+        <f t="shared" ref="U11" si="13">_xlfn.SWITCH(F11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>6</v>
+      </c>
+      <c r="V11" s="4">
+        <f t="shared" ref="V11" si="14">_xlfn.SWITCH(G11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>3</v>
+      </c>
+      <c r="W11" s="4">
+        <f t="shared" ref="W11" si="15">_xlfn.SWITCH(H11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>99</v>
+      </c>
+      <c r="X11" s="4">
+        <f t="shared" ref="X11" si="16">_xlfn.SWITCH(I11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>2</v>
+      </c>
+      <c r="Y11" s="4" t="e">
+        <f t="shared" ref="Y11" si="17">_xlfn.SWITCH(J11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z11" s="4" t="e">
+        <f t="shared" ref="Z11" si="18">_xlfn.SWITCH(K11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA11" s="4" t="e">
+        <f t="shared" ref="AA11" si="19">_xlfn.SWITCH(L11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB11" s="4" t="e">
+        <f t="shared" ref="AB11" si="20">_xlfn.SWITCH(M11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC11" s="4" t="e">
+        <f t="shared" ref="AC11" si="21">_xlfn.SWITCH(N11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD11" s="4" t="e">
+        <f t="shared" ref="AD11" si="22">_xlfn.SWITCH(O11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE11" s="4" t="e">
+        <f t="shared" ref="AE11:AF11" si="23">_xlfn.SWITCH(P11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF11" s="4" t="e">
+        <f>_xlfn.SWITCH(B11:F11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG11" s="4">
+        <f t="array" ref="AG11:AV11">_xlfn.SWITCH(B11:P11,2,0,1,3,TRUE,2,1,1,-1,6,2.3,5,,3,"ciao",99,7)</f>
+        <v>3</v>
+      </c>
+      <c r="AH11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="4">
+        <v>5</v>
+      </c>
+      <c r="AJ11" s="4">
+        <v>7</v>
+      </c>
+      <c r="AK11" s="4">
+        <v>6</v>
+      </c>
+      <c r="AL11" s="4">
+        <v>3</v>
+      </c>
+      <c r="AM11" s="4">
+        <v>99</v>
+      </c>
+      <c r="AN11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AO11" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP11" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ11" s="4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR11" s="4" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS11" s="4" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT11" s="4" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU11" s="4" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV11" s="4" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
feat(stat), #35: Add `MINA`, `AVERAGEA`, `MAXA` functions.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90890B43-7A9E-F747-9153-2880E8D2AD60}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0630FE57-8A62-2740-B24F-AA257D4AE981}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="770" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="770" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="429">
   <si>
     <t>ca</t>
   </si>
@@ -1496,13 +1495,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1844,70 +1843,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="33"/>
+      <c r="AV1" s="33"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -1917,22 +1916,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -1942,36 +1941,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="32" t="s">
+      <c r="Y2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="32" t="s">
+      <c r="AG2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
@@ -12206,7 +12205,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AT81">
+  <sortState ref="A3:AT81">
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="8">
@@ -12265,70 +12264,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="33"/>
+      <c r="AV1" s="33"/>
     </row>
     <row r="2" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="26" t="s">
         <v>38</v>
       </c>
@@ -12338,22 +12337,22 @@
       <c r="I2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="26" t="s">
         <v>38</v>
       </c>
@@ -12363,36 +12362,36 @@
       <c r="X2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="32" t="s">
+      <c r="Y2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
       <c r="AF2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="32" t="s">
+      <c r="AG2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
     </row>
     <row r="3" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="28" t="s">
@@ -14875,70 +14874,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="33"/>
+      <c r="AV1" s="33"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="27" t="s">
         <v>38</v>
       </c>
@@ -14948,22 +14947,22 @@
       <c r="I2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="27" t="s">
         <v>38</v>
       </c>
@@ -14973,36 +14972,36 @@
       <c r="X2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="32" t="s">
+      <c r="Y2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
       <c r="AF2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="32" t="s">
+      <c r="AG2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -16749,70 +16748,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="33"/>
+      <c r="AV1" s="33"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -16822,22 +16821,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -16847,36 +16846,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="32" t="s">
+      <c r="Y2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="32" t="s">
+      <c r="AG2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -17505,70 +17504,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="33"/>
+      <c r="AV1" s="33"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -17578,22 +17577,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -17603,36 +17602,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="32" t="s">
+      <c r="Y2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="32" t="s">
+      <c r="AG2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -19448,7 +19447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AV113"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -19459,7 +19458,7 @@
     <col min="3" max="6" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
@@ -19468,7 +19467,7 @@
     <col min="15" max="15" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="21" width="2.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -19479,76 +19478,77 @@
     <col min="30" max="30" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="38" width="2.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="38" width="2.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="39" max="48" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="49" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="33"/>
+      <c r="AV1" s="33"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -19558,22 +19558,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -19583,36 +19583,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="32" t="s">
+      <c r="Y2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="32" t="s">
+      <c r="AG2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -19782,8 +19782,165 @@
       </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>101</v>
+      </c>
+      <c r="B5" s="14">
+        <v>0</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="14">
+        <v>-0.1</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K5" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L5" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M5" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N5" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O5" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P5" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q5" s="6">
+        <f>AVERAGEA(B5:C5,C5:D5,D5:E5)</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="R5" s="6">
+        <f t="shared" ref="R5:T5" si="1">AVERAGEA(C5:D5,D5:E5,E5:F5)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="S5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.12000000000000002</v>
+      </c>
+      <c r="T5" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4999999999999994E-2</v>
+      </c>
+      <c r="U5" s="6">
+        <f>AVERAGEA(F5:G5,G5:H5,H5:I5)</f>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="V5" s="6" t="e">
+        <f>AVERAGEA(G4:G5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W5" s="6">
+        <f>AVERAGEA(H5,F5:G5)</f>
+        <v>-0.05</v>
+      </c>
+      <c r="X5" s="6">
+        <f>AVERAGEA(I5,G5:H5)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Y5" s="6" t="e">
+        <f>AVERAGEA(J5:K5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z5" s="6" t="e">
+        <f t="shared" ref="Z5:AE5" si="2">AVERAGEA(K5:L5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA5" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB5" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC5" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD5" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE5" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF5" s="6">
+        <f>AVERAGEA(G5:I5)</f>
+        <v>0.5</v>
+      </c>
+      <c r="AG5" s="6">
+        <f t="array" ref="AG5:AL5">AVERAGEA(B5:I5)</f>
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="AH5" s="6">
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="AI5" s="6">
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="AJ5" s="6">
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="AK5" s="6">
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="AL5" s="6">
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="AM5" s="6" t="e">
+        <f t="array" ref="AM5:AV5">AVERAGEA(I5:P5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN5" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO5" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP5" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ5" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR5" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS5" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT5" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AU5" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AV5" s="4" t="e">
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.15">
@@ -20113,19 +20270,19 @@
         <v>0.3</v>
       </c>
       <c r="R61" s="6">
-        <f t="shared" ref="R61:U61" si="1">MAX(C61:D61,D61:E61,E61:F61)</f>
+        <f t="shared" ref="R61:U61" si="3">MAX(C61:D61,D61:E61,E61:F61)</f>
         <v>0.3</v>
       </c>
       <c r="S61" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
       <c r="T61" s="6">
-        <f t="shared" si="1"/>
-        <v>0.3</v>
+        <f>MAX(G61)</f>
+        <v>0</v>
       </c>
       <c r="U61" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-0.1</v>
       </c>
       <c r="V61" s="6">
@@ -20145,27 +20302,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z61" s="6" t="e">
-        <f t="shared" ref="Z61:AE61" si="2">MAX(K61:L61)</f>
+        <f t="shared" ref="Z61:AE61" si="4">MAX(K61:L61)</f>
         <v>#N/A</v>
       </c>
       <c r="AA61" s="6" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB61" s="6" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
       <c r="AC61" s="6" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#NULL!</v>
       </c>
       <c r="AD61" s="6" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
       <c r="AE61" s="6" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="AF61" s="6">
@@ -20224,8 +20381,165 @@
       </c>
     </row>
     <row r="62" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="17" t="s">
         <v>157</v>
+      </c>
+      <c r="B62" s="14">
+        <v>0</v>
+      </c>
+      <c r="C62" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="D62" s="14">
+        <v>-2</v>
+      </c>
+      <c r="E62" s="14">
+        <v>-3</v>
+      </c>
+      <c r="F62" s="14">
+        <v>4</v>
+      </c>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I62" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J62" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K62" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L62" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M62" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N62" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O62" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P62" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q62" s="6">
+        <f>MAXA(B62:C62,C62:D62,D62:E62)</f>
+        <v>0.1</v>
+      </c>
+      <c r="R62" s="6">
+        <f>MAXA(C62:D62,D62:E62,E62:F62)</f>
+        <v>4</v>
+      </c>
+      <c r="S62" s="6">
+        <f>MAXA(D62,E62,I62)</f>
+        <v>1</v>
+      </c>
+      <c r="T62" s="6">
+        <f>MAXA(G62)</f>
+        <v>0</v>
+      </c>
+      <c r="U62" s="6">
+        <f>MAXA(F62,G62,H62)</f>
+        <v>4</v>
+      </c>
+      <c r="V62" s="6">
+        <f>MAXA(G62,H62,I62)</f>
+        <v>1</v>
+      </c>
+      <c r="W62" s="6">
+        <f>MAXA(H62,E62)</f>
+        <v>0</v>
+      </c>
+      <c r="X62" s="6">
+        <f>MAXA(G62,E62)</f>
+        <v>-3</v>
+      </c>
+      <c r="Y62" s="6" t="e">
+        <f>MAXA(J62:K62)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z62" s="6" t="e">
+        <f>MAXA(K62:L62)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA62" s="6" t="e">
+        <f>MAXA(L62:M62)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB62" s="6" t="e">
+        <f t="shared" ref="AB62:AE62" si="5">MAXA(M62:N62)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC62" s="6" t="e">
+        <f t="shared" si="5"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD62" s="6" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE62" s="6" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF62" s="6">
+        <f>MAXA(G62:I62)</f>
+        <v>1</v>
+      </c>
+      <c r="AG62" s="6">
+        <f t="array" ref="AG62:AL62">MAXA(B62:I62)</f>
+        <v>4</v>
+      </c>
+      <c r="AH62" s="6">
+        <v>4</v>
+      </c>
+      <c r="AI62" s="6">
+        <v>4</v>
+      </c>
+      <c r="AJ62" s="6">
+        <v>4</v>
+      </c>
+      <c r="AK62" s="6">
+        <v>4</v>
+      </c>
+      <c r="AL62" s="6">
+        <v>4</v>
+      </c>
+      <c r="AM62" s="6" t="e">
+        <f t="array" ref="AM62:AV62">MAXA(I62:P62)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN62" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO62" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP62" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ62" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR62" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS62" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT62" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AU62" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AV62" s="4" t="e">
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="63" spans="1:48" x14ac:dyDescent="0.15">
@@ -20298,8 +20612,8 @@
         <v>-0.3</v>
       </c>
       <c r="T65" s="6">
-        <f>MIN(E65:F65,F65:G65,G65:H65)</f>
-        <v>-0.3</v>
+        <f>MIN(G65)</f>
+        <v>0</v>
       </c>
       <c r="U65" s="6">
         <f>MIN(F65:G65,G65:H65,H65:I65)</f>
@@ -20318,31 +20632,31 @@
         <v>0.1</v>
       </c>
       <c r="Y65" s="6" t="e">
-        <f t="shared" ref="Y65:AE65" si="3">MIN(J65:K65)</f>
+        <f t="shared" ref="Y65:AE65" si="6">MIN(J65:K65)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z65" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="AA65" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB65" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#NAME?</v>
       </c>
       <c r="AC65" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#NULL!</v>
       </c>
       <c r="AD65" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
       <c r="AE65" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="AF65" s="6">
@@ -20406,8 +20720,165 @@
       </c>
     </row>
     <row r="67" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="17" t="s">
         <v>161</v>
+      </c>
+      <c r="B67" s="14">
+        <v>0</v>
+      </c>
+      <c r="C67" s="14">
+        <v>-0.1</v>
+      </c>
+      <c r="D67" s="14">
+        <v>2</v>
+      </c>
+      <c r="E67" s="14">
+        <v>3</v>
+      </c>
+      <c r="F67" s="14">
+        <v>4</v>
+      </c>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I67" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J67" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K67" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L67" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M67" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N67" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O67" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P67" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q67" s="6">
+        <f>MINA(B67:C67,C67:D67,D67:E67)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="R67" s="6">
+        <f>MINA(C67:D67,D67:E67,E67:F67)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="S67" s="6">
+        <f>MINA(D67,E67,I67)</f>
+        <v>1</v>
+      </c>
+      <c r="T67" s="6">
+        <f>MINA(G67)</f>
+        <v>0</v>
+      </c>
+      <c r="U67" s="6">
+        <f>MINA(F67,G67,H67)</f>
+        <v>0</v>
+      </c>
+      <c r="V67" s="6">
+        <f>MINA(G67,H67,I67)</f>
+        <v>0</v>
+      </c>
+      <c r="W67" s="6">
+        <f>MINA(H67,F67)</f>
+        <v>0</v>
+      </c>
+      <c r="X67" s="6">
+        <f>MINA(I67,F67)</f>
+        <v>1</v>
+      </c>
+      <c r="Y67" s="6" t="e">
+        <f t="shared" ref="Y67:AE67" si="7">MINA(J67:K67)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z67" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA67" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB67" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC67" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD67" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE67" s="6" t="e">
+        <f t="shared" si="7"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF67" s="6">
+        <f>MINA(G67:I67)</f>
+        <v>0</v>
+      </c>
+      <c r="AG67" s="6">
+        <f t="array" ref="AG67:AL67">MINA(B67:I67)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="AH67" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="AI67" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="AJ67" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="AK67" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="AL67" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="AM67" s="6" t="e">
+        <f t="array" ref="AM67:AV67">MINA(I67:P67)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN67" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO67" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP67" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ67" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR67" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS67" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT67" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AU67" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AV67" s="4" t="e">
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="68" spans="1:48" x14ac:dyDescent="0.15">
@@ -20698,70 +21169,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="33"/>
+      <c r="AV1" s="33"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -20771,22 +21242,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -20796,36 +21267,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="32" t="s">
+      <c r="Y2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="32" t="s">
+      <c r="AG2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -21258,7 +21729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BJ74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="AA2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="AO13" sqref="AO13"/>
     </sheetView>
   </sheetViews>
@@ -21307,70 +21778,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="33"/>
+      <c r="AV1" s="33"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="19" t="s">
         <v>38</v>
       </c>
@@ -21380,22 +21851,22 @@
       <c r="I2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="19" t="s">
         <v>38</v>
       </c>
@@ -21405,36 +21876,36 @@
       <c r="X2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="32" t="s">
+      <c r="Y2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
       <c r="AF2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="32" t="s">
+      <c r="AG2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -21452,7 +21923,7 @@
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>334</v>
       </c>
       <c r="B6" s="22">
@@ -21618,7 +22089,7 @@
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A7" s="33"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
@@ -21748,7 +22219,7 @@
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A8" s="33"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -22000,7 +22471,7 @@
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="34" t="s">
         <v>338</v>
       </c>
       <c r="B12" s="22">
@@ -22158,7 +22629,7 @@
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A13" s="33"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -22265,7 +22736,7 @@
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A14" s="33"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -22377,7 +22848,7 @@
       </c>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>340</v>
       </c>
       <c r="B16" s="22">
@@ -22445,7 +22916,7 @@
         <v>0</v>
       </c>
       <c r="V16" s="4" t="str">
-        <f t="shared" ref="U16:AE16" si="15">INDEX(G16:I17,1,2)</f>
+        <f t="shared" ref="V16:AE16" si="15">INDEX(G16:I17,1,2)</f>
         <v>b</v>
       </c>
       <c r="W16" s="4" t="b">
@@ -22536,7 +23007,7 @@
       </c>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A17" s="33"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="22">
         <v>-2</v>
       </c>
@@ -22652,7 +23123,7 @@
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A18" s="33"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="22">
         <v>-2.9</v>
       </c>
@@ -22765,7 +23236,7 @@
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="34" t="s">
         <v>342</v>
       </c>
       <c r="B20" s="22">
@@ -22927,7 +23398,7 @@
       </c>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A21" s="33"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -23058,7 +23529,7 @@
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A22" s="33"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
@@ -23189,7 +23660,7 @@
       </c>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A23" s="33"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
@@ -23320,7 +23791,7 @@
       </c>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A24" s="33"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
@@ -23451,7 +23922,7 @@
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A25" s="33"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
@@ -23582,7 +24053,7 @@
       </c>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A26" s="33"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
@@ -23713,7 +24184,7 @@
       </c>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A27" s="33"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
@@ -23844,7 +24315,7 @@
       </c>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A28" s="33"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -23974,7 +24445,7 @@
       </c>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="34" t="s">
         <v>352</v>
       </c>
       <c r="B29" s="22">
@@ -24099,7 +24570,7 @@
       <c r="AU29" s="6"/>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A30" s="33"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="22">
         <v>-2</v>
       </c>
@@ -24208,7 +24679,7 @@
       <c r="AG30" s="6"/>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A31" s="33"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="22">
         <v>-2</v>
       </c>
@@ -24317,7 +24788,7 @@
       <c r="AG31" s="6"/>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A32" s="33"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="22">
         <v>-2</v>
       </c>
@@ -24426,7 +24897,7 @@
       <c r="AG32" s="6"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A33" s="33"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="22">
         <v>-2</v>
       </c>
@@ -24535,7 +25006,7 @@
       <c r="AG33" s="6"/>
     </row>
     <row r="34" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A34" s="33"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="22">
         <v>-2</v>
       </c>
@@ -24644,7 +25115,7 @@
       <c r="AG34" s="6"/>
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A35" s="33"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="22">
         <v>-2</v>
       </c>
@@ -24753,7 +25224,7 @@
       <c r="AG35" s="6"/>
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A36" s="33"/>
+      <c r="A36" s="34"/>
       <c r="B36" s="22">
         <v>-2</v>
       </c>
@@ -24862,7 +25333,7 @@
       <c r="AG36" s="6"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A37" s="33"/>
+      <c r="A37" s="34"/>
       <c r="B37" s="22">
         <v>-2</v>
       </c>
@@ -24971,7 +25442,7 @@
       <c r="AG37" s="6"/>
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A38" s="33" t="s">
+      <c r="A38" s="34" t="s">
         <v>351</v>
       </c>
       <c r="B38" s="22">
@@ -25096,7 +25567,7 @@
       <c r="AU38" s="6"/>
     </row>
     <row r="39" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A39" s="33"/>
+      <c r="A39" s="34"/>
       <c r="B39" s="22">
         <v>-2</v>
       </c>
@@ -25205,7 +25676,7 @@
       <c r="AG39" s="6"/>
     </row>
     <row r="40" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A40" s="33"/>
+      <c r="A40" s="34"/>
       <c r="B40" s="22">
         <v>-2</v>
       </c>
@@ -25314,7 +25785,7 @@
       <c r="AG40" s="6"/>
     </row>
     <row r="41" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A41" s="33"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="22">
         <v>-2</v>
       </c>
@@ -25423,7 +25894,7 @@
       <c r="AG41" s="6"/>
     </row>
     <row r="42" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A42" s="33"/>
+      <c r="A42" s="34"/>
       <c r="B42" s="22">
         <v>-2</v>
       </c>
@@ -25532,7 +26003,7 @@
       <c r="AG42" s="6"/>
     </row>
     <row r="43" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A43" s="33"/>
+      <c r="A43" s="34"/>
       <c r="B43" s="22">
         <v>-2</v>
       </c>
@@ -25641,7 +26112,7 @@
       <c r="AG43" s="6"/>
     </row>
     <row r="44" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A44" s="33"/>
+      <c r="A44" s="34"/>
       <c r="B44" s="22">
         <v>-2</v>
       </c>
@@ -25750,7 +26221,7 @@
       <c r="AG44" s="6"/>
     </row>
     <row r="45" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A45" s="33"/>
+      <c r="A45" s="34"/>
       <c r="B45" s="22">
         <v>-2</v>
       </c>
@@ -25859,7 +26330,7 @@
       <c r="AG45" s="6"/>
     </row>
     <row r="46" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A46" s="33"/>
+      <c r="A46" s="34"/>
       <c r="B46" s="22">
         <v>-2</v>
       </c>
@@ -25968,7 +26439,7 @@
       <c r="AG46" s="6"/>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="34" t="s">
         <v>353</v>
       </c>
       <c r="B47" s="22">
@@ -26093,7 +26564,7 @@
       <c r="AU47" s="6"/>
     </row>
     <row r="48" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A48" s="33"/>
+      <c r="A48" s="34"/>
       <c r="B48" s="22">
         <v>-2</v>
       </c>
@@ -26202,7 +26673,7 @@
       <c r="AG48" s="6"/>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A49" s="33"/>
+      <c r="A49" s="34"/>
       <c r="B49" s="22">
         <v>-2</v>
       </c>
@@ -26311,7 +26782,7 @@
       <c r="AG49" s="6"/>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A50" s="33"/>
+      <c r="A50" s="34"/>
       <c r="B50" s="22">
         <v>-2</v>
       </c>
@@ -26420,7 +26891,7 @@
       <c r="AG50" s="6"/>
     </row>
     <row r="51" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A51" s="33"/>
+      <c r="A51" s="34"/>
       <c r="B51" s="22">
         <v>-2</v>
       </c>
@@ -26529,7 +27000,7 @@
       <c r="AG51" s="6"/>
     </row>
     <row r="52" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A52" s="33"/>
+      <c r="A52" s="34"/>
       <c r="B52" s="22">
         <v>-2</v>
       </c>
@@ -26638,7 +27109,7 @@
       <c r="AG52" s="6"/>
     </row>
     <row r="53" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A53" s="33"/>
+      <c r="A53" s="34"/>
       <c r="B53" s="22">
         <v>-2</v>
       </c>
@@ -26747,7 +27218,7 @@
       <c r="AG53" s="6"/>
     </row>
     <row r="54" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A54" s="33"/>
+      <c r="A54" s="34"/>
       <c r="B54" s="22">
         <v>-2</v>
       </c>
@@ -26856,7 +27327,7 @@
       <c r="AG54" s="6"/>
     </row>
     <row r="55" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A55" s="33"/>
+      <c r="A55" s="34"/>
       <c r="B55" s="22">
         <v>-2</v>
       </c>
@@ -26995,7 +27466,7 @@
       <c r="AE56" s="6"/>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A57" s="33" t="s">
+      <c r="A57" s="34" t="s">
         <v>344</v>
       </c>
       <c r="B57" s="22">
@@ -27161,7 +27632,7 @@
       </c>
     </row>
     <row r="58" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A58" s="33"/>
+      <c r="A58" s="34"/>
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22"/>
@@ -27291,7 +27762,7 @@
       </c>
     </row>
     <row r="59" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A59" s="33"/>
+      <c r="A59" s="34"/>
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
       <c r="D59" s="22"/>
@@ -27526,7 +27997,7 @@
       <c r="AE62" s="6"/>
     </row>
     <row r="63" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A63" s="33" t="s">
+      <c r="A63" s="34" t="s">
         <v>348</v>
       </c>
       <c r="B63" s="22">
@@ -27635,7 +28106,7 @@
       </c>
     </row>
     <row r="64" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A64" s="33"/>
+      <c r="A64" s="34"/>
       <c r="B64" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -27742,7 +28213,7 @@
       </c>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.15">
-      <c r="A65" s="33"/>
+      <c r="A65" s="34"/>
       <c r="B65" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -28213,70 +28684,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32"/>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="33"/>
+      <c r="AV1" s="33"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -28286,22 +28757,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -28311,36 +28782,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="32" t="s">
+      <c r="Y2" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="32" t="s">
+      <c r="AG2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
@@ -28362,7 +28833,7 @@
         <v>-1</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="32" t="s">
         <v>428</v>
       </c>
       <c r="I3" s="6" t="b">
@@ -28973,7 +29444,7 @@
         <v>-1</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="32" t="s">
         <v>428</v>
       </c>
       <c r="I9" s="6" t="b">

</xml_diff>

<commit_message>
fix(excel,date), #21, #35: Add custom Excel Reader to parse raw datetime.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E26513-B695-1E42-B2A7-134ACFAF4A17}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17503C1B-31BC-1B47-B861-08F606B83C7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1440,8 +1440,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="180" formatCode="0.00000000000000"/>
-    <numFmt numFmtId="184" formatCode="0.000000000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000000000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1538,7 +1538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1595,12 +1595,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1609,8 +1603,16 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="184" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1952,70 +1954,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="34"/>
-      <c r="AV1" s="34"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AQ1" s="44"/>
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -2025,22 +2027,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -2050,36 +2052,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="34" t="s">
+      <c r="Y2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="34" t="s">
+      <c r="AG2" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
@@ -12408,70 +12410,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="44" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="34"/>
-      <c r="AV1" s="34"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AQ1" s="44"/>
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
     </row>
     <row r="2" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
       <c r="G2" s="26" t="s">
         <v>38</v>
       </c>
@@ -12481,22 +12483,22 @@
       <c r="I2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
       <c r="V2" s="26" t="s">
         <v>38</v>
       </c>
@@ -12506,36 +12508,36 @@
       <c r="X2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="34" t="s">
+      <c r="Y2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
       <c r="AF2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="34" t="s">
+      <c r="AG2" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
     </row>
     <row r="3" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="28" t="s">
@@ -15018,70 +15020,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="34"/>
-      <c r="AV1" s="34"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AQ1" s="44"/>
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
       <c r="G2" s="27" t="s">
         <v>38</v>
       </c>
@@ -15091,22 +15093,22 @@
       <c r="I2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
       <c r="V2" s="27" t="s">
         <v>38</v>
       </c>
@@ -15116,36 +15118,36 @@
       <c r="X2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="34" t="s">
+      <c r="Y2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
       <c r="AF2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="34" t="s">
+      <c r="AG2" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -16892,70 +16894,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="34"/>
-      <c r="AV1" s="34"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AQ1" s="44"/>
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -16965,22 +16967,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -16990,36 +16992,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="34" t="s">
+      <c r="Y2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="34" t="s">
+      <c r="AG2" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -17648,70 +17650,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="34"/>
-      <c r="AV1" s="34"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AQ1" s="44"/>
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -17721,22 +17723,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -17746,36 +17748,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="34" t="s">
+      <c r="Y2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="34" t="s">
+      <c r="AG2" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -19629,70 +19631,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="34"/>
-      <c r="AV1" s="34"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AQ1" s="44"/>
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -19702,22 +19704,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -19727,36 +19729,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="34" t="s">
+      <c r="Y2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="34" t="s">
+      <c r="AG2" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -21273,13 +21275,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7D9E77-BF90-2E45-87C2-E9C169025282}">
-  <dimension ref="A1:AV113"/>
+  <dimension ref="A1:AV34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="237" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+    <sheetView tabSelected="1" zoomScale="237" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -21322,71 +21324,71 @@
     <col min="49" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="11" x14ac:dyDescent="0.15">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="A1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="34"/>
-      <c r="AV1" s="34"/>
-    </row>
-    <row r="2" spans="1:48" ht="11" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34" t="s">
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AQ1" s="44"/>
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
       <c r="G2" s="33" t="s">
         <v>38</v>
       </c>
@@ -21396,22 +21398,22 @@
       <c r="I2" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
       <c r="V2" s="33" t="s">
         <v>38</v>
       </c>
@@ -21421,58 +21423,58 @@
       <c r="X2" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="34" t="s">
+      <c r="Y2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
       <c r="AF2" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="34" t="s">
+      <c r="AG2" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
-    </row>
-    <row r="3" spans="1:48" s="7" customFormat="1" ht="11" x14ac:dyDescent="0.15">
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
+    </row>
+    <row r="3" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>429</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="34">
         <v>1987</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="34">
         <v>8</v>
       </c>
-      <c r="D3" s="36">
-        <v>1</v>
-      </c>
-      <c r="E3" s="36">
+      <c r="D3" s="34">
+        <v>1</v>
+      </c>
+      <c r="E3" s="34">
         <v>0.7</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="34">
         <v>0</v>
       </c>
       <c r="G3" s="11"/>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="39" t="s">
         <v>454</v>
       </c>
       <c r="I3" s="11" t="b">
@@ -21484,19 +21486,19 @@
       <c r="K3" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L3" s="37" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M3" s="37" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N3" s="37" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O3" s="37" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P3" s="37" t="e">
+      <c r="L3" s="35" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M3" s="35" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N3" s="35" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O3" s="35" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P3" s="35" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q3" s="11">
@@ -21536,7 +21538,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z3" s="11" t="e">
-        <f t="shared" ref="Y3:AE3" si="0">DATE(F3,G3,K3)</f>
+        <f t="shared" ref="Z3:AA3" si="0">DATE(F3,G3,K3)</f>
         <v>#N/A</v>
       </c>
       <c r="AA3" s="11" t="e">
@@ -21611,29 +21613,29 @@
       <c r="AU3" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="AV3" s="38" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="4" spans="1:48" s="7" customFormat="1" ht="11" x14ac:dyDescent="0.15">
+      <c r="AV3" s="36" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="30" t="s">
         <v>430</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
@@ -21666,27 +21668,27 @@
       <c r="AT4" s="11"/>
       <c r="AU4" s="11"/>
     </row>
-    <row r="5" spans="1:48" s="7" customFormat="1" ht="11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>431</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="34">
         <v>1987</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="34">
         <v>8</v>
       </c>
-      <c r="D5" s="36">
-        <v>1</v>
-      </c>
-      <c r="E5" s="36">
+      <c r="D5" s="34">
+        <v>1</v>
+      </c>
+      <c r="E5" s="34">
         <v>0.7</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="34">
         <v>0</v>
       </c>
       <c r="G5" s="11"/>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="39" t="s">
         <v>459</v>
       </c>
       <c r="I5" s="11" t="b">
@@ -21698,19 +21700,19 @@
       <c r="K5" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L5" s="37" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M5" s="37" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N5" s="37" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O5" s="37" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P5" s="37" t="e">
+      <c r="L5" s="35" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M5" s="35" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N5" s="35" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O5" s="35" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P5" s="35" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q5" s="11" t="e">
@@ -21827,27 +21829,27 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
         <v>432</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="34">
         <v>1987</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="34">
         <v>-1</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="34">
         <v>2958466</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>0.7</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="34">
         <v>0</v>
       </c>
       <c r="G6" s="11"/>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="39" t="s">
         <v>456</v>
       </c>
       <c r="I6" s="11" t="b">
@@ -21859,19 +21861,19 @@
       <c r="K6" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L6" s="37" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M6" s="37" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N6" s="37" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O6" s="37" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P6" s="37" t="e">
+      <c r="L6" s="35" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M6" s="35" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N6" s="35" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O6" s="35" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P6" s="35" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q6" s="11">
@@ -21988,33 +21990,33 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>433</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="40"/>
-      <c r="S7" s="39"/>
-    </row>
-    <row r="8" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+      <c r="B7" s="37"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="37"/>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>434</v>
       </c>
-      <c r="B8" s="39"/>
+      <c r="B8" s="37"/>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="10" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="11" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
         <v>437</v>
       </c>
@@ -22033,7 +22035,7 @@
       <c r="F11" s="4">
         <v>0</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="41" t="s">
         <v>457</v>
       </c>
       <c r="I11" s="4" t="b">
@@ -22045,19 +22047,19 @@
       <c r="K11" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L11" s="37" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M11" s="37" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N11" s="37" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O11" s="37" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P11" s="37" t="e">
+      <c r="L11" s="35" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="35" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N11" s="35" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O11" s="35" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P11" s="35" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q11" s="4">
@@ -22174,12 +22176,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="13" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>439</v>
       </c>
@@ -22198,7 +22200,7 @@
       <c r="F13" s="4">
         <v>0</v>
       </c>
-      <c r="H13" s="43" t="s">
+      <c r="H13" s="41" t="s">
         <v>457</v>
       </c>
       <c r="I13" s="4" t="b">
@@ -22210,19 +22212,19 @@
       <c r="K13" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L13" s="37" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M13" s="37" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N13" s="37" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O13" s="37" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P13" s="37" t="e">
+      <c r="L13" s="35" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" s="35" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N13" s="35" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O13" s="35" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P13" s="35" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q13" s="4">
@@ -22339,27 +22341,27 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
         <v>440</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="34">
         <v>1987</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="34">
         <v>8</v>
       </c>
-      <c r="D14" s="36">
-        <v>1</v>
-      </c>
-      <c r="E14" s="36">
+      <c r="D14" s="34">
+        <v>1</v>
+      </c>
+      <c r="E14" s="34">
         <v>0.7</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="34">
         <v>0</v>
       </c>
       <c r="G14" s="11"/>
-      <c r="H14" s="41" t="s">
+      <c r="H14" s="39" t="s">
         <v>456</v>
       </c>
       <c r="I14" s="11" t="b">
@@ -22371,19 +22373,19 @@
       <c r="K14" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L14" s="37" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M14" s="37" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N14" s="37" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O14" s="37" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P14" s="37" t="e">
+      <c r="L14" s="35" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M14" s="35" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N14" s="35" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O14" s="35" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P14" s="35" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q14" s="11">
@@ -22500,17 +22502,17 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="16" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="17" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
         <v>443</v>
       </c>
@@ -22520,7 +22522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
         <v>444</v>
       </c>
@@ -22539,7 +22541,7 @@
       <c r="F18" s="4">
         <v>0</v>
       </c>
-      <c r="H18" s="43" t="s">
+      <c r="H18" s="41" t="s">
         <v>457</v>
       </c>
       <c r="I18" s="4" t="b">
@@ -22551,19 +22553,19 @@
       <c r="K18" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L18" s="37" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M18" s="37" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N18" s="37" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O18" s="37" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P18" s="37" t="e">
+      <c r="L18" s="35" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" s="35" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N18" s="35" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O18" s="35" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P18" s="35" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q18" s="4">
@@ -22680,27 +22682,27 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>445</v>
       </c>
-      <c r="B19" s="36">
+      <c r="B19" s="34">
         <v>32767.99</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C19" s="34">
         <v>-1</v>
       </c>
-      <c r="D19" s="36">
+      <c r="D19" s="34">
         <v>67</v>
       </c>
-      <c r="E19" s="36">
+      <c r="E19" s="34">
         <v>0.7</v>
       </c>
-      <c r="F19" s="36">
+      <c r="F19" s="34">
         <v>0</v>
       </c>
       <c r="G19" s="11"/>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="39" t="s">
         <v>455</v>
       </c>
       <c r="I19" s="11" t="b">
@@ -22712,19 +22714,19 @@
       <c r="K19" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L19" s="37" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M19" s="37" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N19" s="37" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O19" s="37" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P19" s="37" t="e">
+      <c r="L19" s="35" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19" s="35" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N19" s="35" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O19" s="35" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P19" s="35" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q19" s="11">
@@ -22739,7 +22741,7 @@
         <f>TIME(0.9,0.9,0.9)</f>
         <v>0</v>
       </c>
-      <c r="T19" s="42">
+      <c r="T19" s="40">
         <f>TIME(0,1,0)</f>
         <v>6.9444444444444447E-4</v>
       </c>
@@ -22748,31 +22750,31 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="V19" s="11">
-        <f>TIME(B19,C19,G19)</f>
+        <f t="shared" ref="V19:AB19" si="7">TIME(B19,C19,G19)</f>
         <v>0.29097222222230812</v>
       </c>
       <c r="W19" s="11">
-        <f>TIME(C19,D19,H19)</f>
+        <f t="shared" si="7"/>
         <v>5.555555555555554E-3</v>
       </c>
       <c r="X19" s="11">
-        <f>TIME(D19,E19,I19)</f>
+        <f t="shared" si="7"/>
         <v>0.79167824074074078</v>
       </c>
       <c r="Y19" s="11" t="e">
-        <f>TIME(E19,F19,J19)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z19" s="11" t="e">
-        <f>TIME(F19,G19,K19)</f>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="AA19" s="11" t="e">
-        <f>TIME(G19,H19,L19)</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB19" s="11" t="e">
-        <f>TIME(H19,I19,M19)</f>
+        <f t="shared" si="7"/>
         <v>#NAME?</v>
       </c>
       <c r="AC19" s="11" t="e">
@@ -22839,31 +22841,31 @@
       <c r="AU19" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="AV19" s="38" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="20" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+      <c r="AV19" s="36" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
         <v>446</v>
       </c>
-      <c r="B20" s="36">
+      <c r="B20" s="34">
         <v>1987</v>
       </c>
-      <c r="C20" s="36">
+      <c r="C20" s="34">
         <v>8</v>
       </c>
-      <c r="D20" s="36">
-        <v>1</v>
-      </c>
-      <c r="E20" s="36">
+      <c r="D20" s="34">
+        <v>1</v>
+      </c>
+      <c r="E20" s="34">
         <v>0.7</v>
       </c>
-      <c r="F20" s="36">
+      <c r="F20" s="34">
         <v>0</v>
       </c>
       <c r="G20" s="11"/>
-      <c r="H20" s="41" t="s">
+      <c r="H20" s="39" t="s">
         <v>458</v>
       </c>
       <c r="I20" s="11" t="b">
@@ -22875,19 +22877,19 @@
       <c r="K20" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L20" s="37" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M20" s="37" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N20" s="37" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O20" s="37" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P20" s="37" t="e">
+      <c r="L20" s="35" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M20" s="35" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N20" s="35" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O20" s="35" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P20" s="35" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q20" s="11" t="e">
@@ -22895,23 +22897,23 @@
         <v>#VALUE!</v>
       </c>
       <c r="R20" s="11" t="e">
-        <f t="shared" ref="R20:AE20" si="7">TIMEVALUE(C20)</f>
+        <f t="shared" ref="R20:AE20" si="8">TIMEVALUE(C20)</f>
         <v>#VALUE!</v>
       </c>
       <c r="S20" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="T20" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="U20" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="V20" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="W20" s="11">
@@ -22923,31 +22925,31 @@
         <v>#VALUE!</v>
       </c>
       <c r="Y20" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z20" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AA20" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB20" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#NAME?</v>
       </c>
       <c r="AC20" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#NULL!</v>
       </c>
       <c r="AD20" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AE20" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
       <c r="AF20" s="11">
@@ -23004,57 +23006,57 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
         <v>447</v>
       </c>
-      <c r="B21" s="39"/>
+      <c r="B21" s="37"/>
       <c r="V21" s="14">
         <f ca="1">IF(TODAY(),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A22" s="16" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="23" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A23" s="16" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="24" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A24" s="16" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="25" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A25" s="16" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="26" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A26" s="17" t="s">
         <v>452</v>
       </c>
-      <c r="B26" s="36">
+      <c r="B26" s="34">
         <v>1987</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C26" s="34">
         <v>8</v>
       </c>
-      <c r="D26" s="36">
-        <v>1</v>
-      </c>
-      <c r="E26" s="36">
+      <c r="D26" s="34">
+        <v>1</v>
+      </c>
+      <c r="E26" s="34">
         <v>0.7</v>
       </c>
-      <c r="F26" s="36">
+      <c r="F26" s="34">
         <v>0</v>
       </c>
       <c r="G26" s="11"/>
-      <c r="H26" s="41" t="s">
+      <c r="H26" s="39" t="s">
         <v>456</v>
       </c>
       <c r="I26" s="11" t="b">
@@ -23066,19 +23068,19 @@
       <c r="K26" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L26" s="37" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M26" s="37" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N26" s="37" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O26" s="37" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P26" s="37" t="e">
+      <c r="L26" s="35" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M26" s="35" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N26" s="35" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O26" s="35" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P26" s="35" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q26" s="11">
@@ -23086,59 +23088,59 @@
         <v>1905</v>
       </c>
       <c r="R26" s="11">
-        <f t="shared" ref="R26:AE26" si="8">YEAR(C26)</f>
+        <f t="shared" ref="R26:AE26" si="9">YEAR(C26)</f>
         <v>1900</v>
       </c>
       <c r="S26" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1900</v>
       </c>
       <c r="T26" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1900</v>
       </c>
       <c r="U26" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1900</v>
       </c>
       <c r="V26" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1900</v>
       </c>
       <c r="W26" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1901</v>
       </c>
       <c r="X26" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1900</v>
       </c>
       <c r="Y26" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z26" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#N/A</v>
       </c>
       <c r="AA26" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB26" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#NAME?</v>
       </c>
       <c r="AC26" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#NULL!</v>
       </c>
       <c r="AD26" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#NUM!</v>
       </c>
       <c r="AE26" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
       <c r="AF26" s="11">
@@ -23195,11 +23197,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A27" s="17" t="s">
         <v>453</v>
       </c>
-      <c r="B27" s="36">
+      <c r="B27" s="34">
         <v>1987</v>
       </c>
       <c r="C27" s="4">
@@ -23214,7 +23216,7 @@
       <c r="F27" s="4">
         <v>4</v>
       </c>
-      <c r="H27" s="41" t="s">
+      <c r="H27" s="39" t="s">
         <v>458</v>
       </c>
       <c r="I27" s="4" t="b">
@@ -23226,19 +23228,19 @@
       <c r="K27" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L27" s="37" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M27" s="37" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N27" s="37" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O27" s="37" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P27" s="37" t="e">
+      <c r="L27" s="35" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M27" s="35" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N27" s="35" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O27" s="35" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P27" s="35" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q27" s="4">
@@ -23246,7 +23248,7 @@
         <v>4.4965769055225921</v>
       </c>
       <c r="R27" s="4">
-        <f t="shared" ref="R27:U27" si="9">YEARFRAC(C27,345,D27)</f>
+        <f t="shared" ref="R27" si="10">YEARFRAC(C27,345,D27)</f>
         <v>0.9555555555555556</v>
       </c>
       <c r="S27" s="4">
@@ -23282,19 +23284,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AA27" s="4" t="e">
-        <f t="shared" ref="AA27" si="10">YEARFRAC(L27,345,M27)</f>
+        <f t="shared" ref="AA27" si="11">YEARFRAC(L27,345,M27)</f>
         <v>#NAME?</v>
       </c>
       <c r="AB27" s="4" t="e">
-        <f t="shared" ref="AB27:AC27" si="11">YEARFRAC(M27,345,N27)</f>
+        <f t="shared" ref="AB27:AC27" si="12">YEARFRAC(M27,345,N27)</f>
         <v>#NULL!</v>
       </c>
       <c r="AC27" s="4" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>#NUM!</v>
       </c>
       <c r="AD27" s="4" t="e">
-        <f t="shared" ref="AD27" si="12">YEARFRAC(O27,345,P27)</f>
+        <f t="shared" ref="AD27" si="13">YEARFRAC(O27,345,P27)</f>
         <v>#REF!</v>
       </c>
       <c r="AE27" s="4" t="e">
@@ -23355,109 +23357,30 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="28" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A28" s="16"/>
     </row>
-    <row r="29" spans="1:48" ht="11" x14ac:dyDescent="0.15">
-      <c r="A29" s="39"/>
-      <c r="B29" s="39"/>
-    </row>
-    <row r="30" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="A29" s="37"/>
+      <c r="B29" s="37"/>
+    </row>
+    <row r="30" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A30" s="16"/>
-      <c r="B30" s="45"/>
-    </row>
-    <row r="31" spans="1:48" ht="11" x14ac:dyDescent="0.15">
+      <c r="B30" s="43"/>
+    </row>
+    <row r="31" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A31" s="16"/>
-      <c r="B31" s="44"/>
-    </row>
-    <row r="32" spans="1:48" ht="11" x14ac:dyDescent="0.15">
-      <c r="B32" s="44"/>
-    </row>
-    <row r="33" spans="2:2" ht="11" x14ac:dyDescent="0.15">
-      <c r="B33" s="44"/>
-    </row>
-    <row r="34" spans="2:2" ht="11" x14ac:dyDescent="0.15">
-      <c r="B34" s="44"/>
-    </row>
-    <row r="35" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="36" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="37" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="38" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="39" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="40" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="41" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="42" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="43" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="44" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="45" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="46" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="47" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="48" spans="2:2" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="50" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="51" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="52" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="53" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="54" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="55" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="56" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="57" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="58" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="59" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="60" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="61" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="62" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="63" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="64" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="65" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="66" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="67" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="68" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="69" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="70" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="71" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="72" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="73" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="74" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="75" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="76" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="77" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="78" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="79" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="80" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="81" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="82" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="83" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="84" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="85" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="86" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="87" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="88" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="89" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="90" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="91" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="92" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="93" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="94" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="95" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="96" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="97" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="98" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="99" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="100" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="101" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="102" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="103" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="104" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="105" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="106" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="107" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="108" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="109" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="110" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="111" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="112" ht="11" x14ac:dyDescent="0.15"/>
-    <row r="113" ht="11" x14ac:dyDescent="0.15"/>
+      <c r="B31" s="42"/>
+    </row>
+    <row r="32" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="B32" s="42"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B33" s="42"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B34" s="42"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A1:A2"/>
@@ -23516,70 +23439,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="34"/>
-      <c r="AV1" s="34"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AQ1" s="44"/>
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -23589,22 +23512,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -23614,36 +23537,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="34" t="s">
+      <c r="Y2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="34" t="s">
+      <c r="AG2" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -24076,8 +23999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BJ74"/>
   <sheetViews>
-    <sheetView topLeftCell="AA2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="AO13" sqref="AO13"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -24125,70 +24048,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="34"/>
-      <c r="AV1" s="34"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AQ1" s="44"/>
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
       <c r="G2" s="19" t="s">
         <v>38</v>
       </c>
@@ -24198,22 +24121,22 @@
       <c r="I2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
       <c r="V2" s="19" t="s">
         <v>38</v>
       </c>
@@ -24223,36 +24146,36 @@
       <c r="X2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="34" t="s">
+      <c r="Y2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
       <c r="AF2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="34" t="s">
+      <c r="AG2" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -24270,7 +24193,7 @@
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>334</v>
       </c>
       <c r="B6" s="22">
@@ -24436,7 +24359,7 @@
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A7" s="35"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
@@ -24566,7 +24489,7 @@
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A8" s="35"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -24818,7 +24741,7 @@
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="45" t="s">
         <v>338</v>
       </c>
       <c r="B12" s="22">
@@ -24976,7 +24899,7 @@
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A13" s="35"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -25083,7 +25006,7 @@
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A14" s="35"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -25195,7 +25118,7 @@
       </c>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="45" t="s">
         <v>340</v>
       </c>
       <c r="B16" s="22">
@@ -25354,7 +25277,7 @@
       </c>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A17" s="35"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="22">
         <v>-2</v>
       </c>
@@ -25470,7 +25393,7 @@
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A18" s="35"/>
+      <c r="A18" s="45"/>
       <c r="B18" s="22">
         <v>-2.9</v>
       </c>
@@ -25583,7 +25506,7 @@
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="45" t="s">
         <v>342</v>
       </c>
       <c r="B20" s="22">
@@ -25745,7 +25668,7 @@
       </c>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A21" s="35"/>
+      <c r="A21" s="45"/>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -25876,7 +25799,7 @@
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A22" s="35"/>
+      <c r="A22" s="45"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
@@ -26007,7 +25930,7 @@
       </c>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A23" s="35"/>
+      <c r="A23" s="45"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
@@ -26138,7 +26061,7 @@
       </c>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A24" s="35"/>
+      <c r="A24" s="45"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
@@ -26269,7 +26192,7 @@
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A25" s="35"/>
+      <c r="A25" s="45"/>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
@@ -26400,7 +26323,7 @@
       </c>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A26" s="35"/>
+      <c r="A26" s="45"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
@@ -26531,7 +26454,7 @@
       </c>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A27" s="35"/>
+      <c r="A27" s="45"/>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
@@ -26662,7 +26585,7 @@
       </c>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A28" s="35"/>
+      <c r="A28" s="45"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -26792,7 +26715,7 @@
       </c>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="45" t="s">
         <v>352</v>
       </c>
       <c r="B29" s="22">
@@ -26917,7 +26840,7 @@
       <c r="AU29" s="6"/>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A30" s="35"/>
+      <c r="A30" s="45"/>
       <c r="B30" s="22">
         <v>-2</v>
       </c>
@@ -27026,7 +26949,7 @@
       <c r="AG30" s="6"/>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A31" s="35"/>
+      <c r="A31" s="45"/>
       <c r="B31" s="22">
         <v>-2</v>
       </c>
@@ -27135,7 +27058,7 @@
       <c r="AG31" s="6"/>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A32" s="35"/>
+      <c r="A32" s="45"/>
       <c r="B32" s="22">
         <v>-2</v>
       </c>
@@ -27244,7 +27167,7 @@
       <c r="AG32" s="6"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A33" s="35"/>
+      <c r="A33" s="45"/>
       <c r="B33" s="22">
         <v>-2</v>
       </c>
@@ -27353,7 +27276,7 @@
       <c r="AG33" s="6"/>
     </row>
     <row r="34" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A34" s="35"/>
+      <c r="A34" s="45"/>
       <c r="B34" s="22">
         <v>-2</v>
       </c>
@@ -27462,7 +27385,7 @@
       <c r="AG34" s="6"/>
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A35" s="35"/>
+      <c r="A35" s="45"/>
       <c r="B35" s="22">
         <v>-2</v>
       </c>
@@ -27571,7 +27494,7 @@
       <c r="AG35" s="6"/>
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A36" s="35"/>
+      <c r="A36" s="45"/>
       <c r="B36" s="22">
         <v>-2</v>
       </c>
@@ -27680,7 +27603,7 @@
       <c r="AG36" s="6"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A37" s="35"/>
+      <c r="A37" s="45"/>
       <c r="B37" s="22">
         <v>-2</v>
       </c>
@@ -27789,7 +27712,7 @@
       <c r="AG37" s="6"/>
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="45" t="s">
         <v>351</v>
       </c>
       <c r="B38" s="22">
@@ -27914,7 +27837,7 @@
       <c r="AU38" s="6"/>
     </row>
     <row r="39" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A39" s="35"/>
+      <c r="A39" s="45"/>
       <c r="B39" s="22">
         <v>-2</v>
       </c>
@@ -28023,7 +27946,7 @@
       <c r="AG39" s="6"/>
     </row>
     <row r="40" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A40" s="35"/>
+      <c r="A40" s="45"/>
       <c r="B40" s="22">
         <v>-2</v>
       </c>
@@ -28132,7 +28055,7 @@
       <c r="AG40" s="6"/>
     </row>
     <row r="41" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A41" s="35"/>
+      <c r="A41" s="45"/>
       <c r="B41" s="22">
         <v>-2</v>
       </c>
@@ -28241,7 +28164,7 @@
       <c r="AG41" s="6"/>
     </row>
     <row r="42" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A42" s="35"/>
+      <c r="A42" s="45"/>
       <c r="B42" s="22">
         <v>-2</v>
       </c>
@@ -28350,7 +28273,7 @@
       <c r="AG42" s="6"/>
     </row>
     <row r="43" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A43" s="35"/>
+      <c r="A43" s="45"/>
       <c r="B43" s="22">
         <v>-2</v>
       </c>
@@ -28459,7 +28382,7 @@
       <c r="AG43" s="6"/>
     </row>
     <row r="44" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A44" s="35"/>
+      <c r="A44" s="45"/>
       <c r="B44" s="22">
         <v>-2</v>
       </c>
@@ -28568,7 +28491,7 @@
       <c r="AG44" s="6"/>
     </row>
     <row r="45" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A45" s="35"/>
+      <c r="A45" s="45"/>
       <c r="B45" s="22">
         <v>-2</v>
       </c>
@@ -28677,7 +28600,7 @@
       <c r="AG45" s="6"/>
     </row>
     <row r="46" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A46" s="35"/>
+      <c r="A46" s="45"/>
       <c r="B46" s="22">
         <v>-2</v>
       </c>
@@ -28786,7 +28709,7 @@
       <c r="AG46" s="6"/>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="45" t="s">
         <v>353</v>
       </c>
       <c r="B47" s="22">
@@ -28911,7 +28834,7 @@
       <c r="AU47" s="6"/>
     </row>
     <row r="48" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A48" s="35"/>
+      <c r="A48" s="45"/>
       <c r="B48" s="22">
         <v>-2</v>
       </c>
@@ -29020,7 +28943,7 @@
       <c r="AG48" s="6"/>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A49" s="35"/>
+      <c r="A49" s="45"/>
       <c r="B49" s="22">
         <v>-2</v>
       </c>
@@ -29129,7 +29052,7 @@
       <c r="AG49" s="6"/>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A50" s="35"/>
+      <c r="A50" s="45"/>
       <c r="B50" s="22">
         <v>-2</v>
       </c>
@@ -29238,7 +29161,7 @@
       <c r="AG50" s="6"/>
     </row>
     <row r="51" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A51" s="35"/>
+      <c r="A51" s="45"/>
       <c r="B51" s="22">
         <v>-2</v>
       </c>
@@ -29347,7 +29270,7 @@
       <c r="AG51" s="6"/>
     </row>
     <row r="52" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A52" s="35"/>
+      <c r="A52" s="45"/>
       <c r="B52" s="22">
         <v>-2</v>
       </c>
@@ -29456,7 +29379,7 @@
       <c r="AG52" s="6"/>
     </row>
     <row r="53" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A53" s="35"/>
+      <c r="A53" s="45"/>
       <c r="B53" s="22">
         <v>-2</v>
       </c>
@@ -29565,7 +29488,7 @@
       <c r="AG53" s="6"/>
     </row>
     <row r="54" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A54" s="35"/>
+      <c r="A54" s="45"/>
       <c r="B54" s="22">
         <v>-2</v>
       </c>
@@ -29674,7 +29597,7 @@
       <c r="AG54" s="6"/>
     </row>
     <row r="55" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A55" s="35"/>
+      <c r="A55" s="45"/>
       <c r="B55" s="22">
         <v>-2</v>
       </c>
@@ -29813,7 +29736,7 @@
       <c r="AE56" s="6"/>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="45" t="s">
         <v>344</v>
       </c>
       <c r="B57" s="22">
@@ -29979,7 +29902,7 @@
       </c>
     </row>
     <row r="58" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A58" s="35"/>
+      <c r="A58" s="45"/>
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22"/>
@@ -30109,7 +30032,7 @@
       </c>
     </row>
     <row r="59" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A59" s="35"/>
+      <c r="A59" s="45"/>
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
       <c r="D59" s="22"/>
@@ -30344,7 +30267,7 @@
       <c r="AE62" s="6"/>
     </row>
     <row r="63" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A63" s="35" t="s">
+      <c r="A63" s="45" t="s">
         <v>348</v>
       </c>
       <c r="B63" s="22">
@@ -30453,7 +30376,7 @@
       </c>
     </row>
     <row r="64" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A64" s="35"/>
+      <c r="A64" s="45"/>
       <c r="B64" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -30560,7 +30483,7 @@
       </c>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.15">
-      <c r="A65" s="35"/>
+      <c r="A65" s="45"/>
       <c r="B65" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -30956,6 +30879,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -30967,12 +30896,6 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -31031,70 +30954,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="34"/>
-      <c r="AV1" s="34"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AQ1" s="44"/>
+      <c r="AR1" s="44"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -31104,22 +31027,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -31129,36 +31052,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="34" t="s">
+      <c r="Y2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="34" t="s">
+      <c r="AG2" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
@@ -32887,6 +32810,13 @@
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C22" s="46">
+        <v>60</v>
+      </c>
+      <c r="D22" s="47">
+        <f>C22+1</f>
+        <v>61</v>
+      </c>
       <c r="H22">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
feat(info), #21: Add `NA` function.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17503C1B-31BC-1B47-B861-08F606B83C7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946AF576-9C20-694F-B332-F15C310B5842}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -1605,14 +1605,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1954,70 +1954,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -2027,22 +2027,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -2052,36 +2052,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="44" t="s">
+      <c r="Y2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="46"/>
+      <c r="AB2" s="46"/>
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="46"/>
+      <c r="AE2" s="46"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AG2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="44"/>
-      <c r="AP2" s="44"/>
-      <c r="AQ2" s="44"/>
-      <c r="AR2" s="44"/>
-      <c r="AS2" s="44"/>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="44"/>
-      <c r="AV2" s="44"/>
+      <c r="AH2" s="46"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
+      <c r="AL2" s="46"/>
+      <c r="AM2" s="46"/>
+      <c r="AN2" s="46"/>
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="46"/>
+      <c r="AR2" s="46"/>
+      <c r="AS2" s="46"/>
+      <c r="AT2" s="46"/>
+      <c r="AU2" s="46"/>
+      <c r="AV2" s="46"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
@@ -12410,70 +12410,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
     </row>
     <row r="2" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="26" t="s">
         <v>38</v>
       </c>
@@ -12483,22 +12483,22 @@
       <c r="I2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
       <c r="V2" s="26" t="s">
         <v>38</v>
       </c>
@@ -12508,36 +12508,36 @@
       <c r="X2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="44" t="s">
+      <c r="Y2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="46"/>
+      <c r="AB2" s="46"/>
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="46"/>
+      <c r="AE2" s="46"/>
       <c r="AF2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AG2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="44"/>
-      <c r="AP2" s="44"/>
-      <c r="AQ2" s="44"/>
-      <c r="AR2" s="44"/>
-      <c r="AS2" s="44"/>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="44"/>
-      <c r="AV2" s="44"/>
+      <c r="AH2" s="46"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
+      <c r="AL2" s="46"/>
+      <c r="AM2" s="46"/>
+      <c r="AN2" s="46"/>
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="46"/>
+      <c r="AR2" s="46"/>
+      <c r="AS2" s="46"/>
+      <c r="AT2" s="46"/>
+      <c r="AU2" s="46"/>
+      <c r="AV2" s="46"/>
     </row>
     <row r="3" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="28" t="s">
@@ -15020,70 +15020,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="27" t="s">
         <v>38</v>
       </c>
@@ -15093,22 +15093,22 @@
       <c r="I2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
       <c r="V2" s="27" t="s">
         <v>38</v>
       </c>
@@ -15118,36 +15118,36 @@
       <c r="X2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="44" t="s">
+      <c r="Y2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="46"/>
+      <c r="AB2" s="46"/>
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="46"/>
+      <c r="AE2" s="46"/>
       <c r="AF2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AG2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="44"/>
-      <c r="AP2" s="44"/>
-      <c r="AQ2" s="44"/>
-      <c r="AR2" s="44"/>
-      <c r="AS2" s="44"/>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="44"/>
-      <c r="AV2" s="44"/>
+      <c r="AH2" s="46"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
+      <c r="AL2" s="46"/>
+      <c r="AM2" s="46"/>
+      <c r="AN2" s="46"/>
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="46"/>
+      <c r="AR2" s="46"/>
+      <c r="AS2" s="46"/>
+      <c r="AT2" s="46"/>
+      <c r="AU2" s="46"/>
+      <c r="AV2" s="46"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -16894,70 +16894,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -16967,22 +16967,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -16992,36 +16992,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="44" t="s">
+      <c r="Y2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="46"/>
+      <c r="AB2" s="46"/>
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="46"/>
+      <c r="AE2" s="46"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AG2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="44"/>
-      <c r="AP2" s="44"/>
-      <c r="AQ2" s="44"/>
-      <c r="AR2" s="44"/>
-      <c r="AS2" s="44"/>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="44"/>
-      <c r="AV2" s="44"/>
+      <c r="AH2" s="46"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
+      <c r="AL2" s="46"/>
+      <c r="AM2" s="46"/>
+      <c r="AN2" s="46"/>
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="46"/>
+      <c r="AR2" s="46"/>
+      <c r="AS2" s="46"/>
+      <c r="AT2" s="46"/>
+      <c r="AU2" s="46"/>
+      <c r="AV2" s="46"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -17650,70 +17650,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -17723,22 +17723,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -17748,36 +17748,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="44" t="s">
+      <c r="Y2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="46"/>
+      <c r="AB2" s="46"/>
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="46"/>
+      <c r="AE2" s="46"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AG2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="44"/>
-      <c r="AP2" s="44"/>
-      <c r="AQ2" s="44"/>
-      <c r="AR2" s="44"/>
-      <c r="AS2" s="44"/>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="44"/>
-      <c r="AV2" s="44"/>
+      <c r="AH2" s="46"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
+      <c r="AL2" s="46"/>
+      <c r="AM2" s="46"/>
+      <c r="AN2" s="46"/>
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="46"/>
+      <c r="AR2" s="46"/>
+      <c r="AS2" s="46"/>
+      <c r="AT2" s="46"/>
+      <c r="AU2" s="46"/>
+      <c r="AV2" s="46"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -19631,70 +19631,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -19704,22 +19704,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -19729,36 +19729,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="44" t="s">
+      <c r="Y2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="46"/>
+      <c r="AB2" s="46"/>
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="46"/>
+      <c r="AE2" s="46"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AG2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="44"/>
-      <c r="AP2" s="44"/>
-      <c r="AQ2" s="44"/>
-      <c r="AR2" s="44"/>
-      <c r="AS2" s="44"/>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="44"/>
-      <c r="AV2" s="44"/>
+      <c r="AH2" s="46"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
+      <c r="AL2" s="46"/>
+      <c r="AM2" s="46"/>
+      <c r="AN2" s="46"/>
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="46"/>
+      <c r="AR2" s="46"/>
+      <c r="AS2" s="46"/>
+      <c r="AT2" s="46"/>
+      <c r="AU2" s="46"/>
+      <c r="AV2" s="46"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -21277,7 +21277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7D9E77-BF90-2E45-87C2-E9C169025282}">
   <dimension ref="A1:AV34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="237" workbookViewId="0">
+    <sheetView zoomScale="237" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -21325,70 +21325,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="33" t="s">
         <v>38</v>
       </c>
@@ -21398,22 +21398,22 @@
       <c r="I2" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
       <c r="V2" s="33" t="s">
         <v>38</v>
       </c>
@@ -21423,36 +21423,36 @@
       <c r="X2" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="44" t="s">
+      <c r="Y2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="46"/>
+      <c r="AB2" s="46"/>
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="46"/>
+      <c r="AE2" s="46"/>
       <c r="AF2" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AG2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="44"/>
-      <c r="AP2" s="44"/>
-      <c r="AQ2" s="44"/>
-      <c r="AR2" s="44"/>
-      <c r="AS2" s="44"/>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="44"/>
-      <c r="AV2" s="44"/>
+      <c r="AH2" s="46"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
+      <c r="AL2" s="46"/>
+      <c r="AM2" s="46"/>
+      <c r="AN2" s="46"/>
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="46"/>
+      <c r="AR2" s="46"/>
+      <c r="AS2" s="46"/>
+      <c r="AT2" s="46"/>
+      <c r="AU2" s="46"/>
+      <c r="AV2" s="46"/>
     </row>
     <row r="3" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
@@ -23401,7 +23401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AV22"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -23439,70 +23439,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -23512,22 +23512,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -23537,36 +23537,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="44" t="s">
+      <c r="Y2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="46"/>
+      <c r="AB2" s="46"/>
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="46"/>
+      <c r="AE2" s="46"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AG2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="44"/>
-      <c r="AP2" s="44"/>
-      <c r="AQ2" s="44"/>
-      <c r="AR2" s="44"/>
-      <c r="AS2" s="44"/>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="44"/>
-      <c r="AV2" s="44"/>
+      <c r="AH2" s="46"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
+      <c r="AL2" s="46"/>
+      <c r="AM2" s="46"/>
+      <c r="AN2" s="46"/>
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="46"/>
+      <c r="AR2" s="46"/>
+      <c r="AS2" s="46"/>
+      <c r="AT2" s="46"/>
+      <c r="AU2" s="46"/>
+      <c r="AV2" s="46"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -23950,32 +23950,85 @@
         <v>219</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="A19" s="17" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="V19" s="4" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AG19" s="4" t="e">
+        <f t="array" ref="AG19:AV19">NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AH19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AI19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AK19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AL19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AM19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AN19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AO19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AP19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AR19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AS19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AT19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AU19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AV19" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A21" s="16" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A22" s="16" t="s">
         <v>225</v>
       </c>
@@ -24048,70 +24101,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="19" t="s">
         <v>38</v>
       </c>
@@ -24121,22 +24174,22 @@
       <c r="I2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
       <c r="V2" s="19" t="s">
         <v>38</v>
       </c>
@@ -24146,36 +24199,36 @@
       <c r="X2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="44" t="s">
+      <c r="Y2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="46"/>
+      <c r="AB2" s="46"/>
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="46"/>
+      <c r="AE2" s="46"/>
       <c r="AF2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AG2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="44"/>
-      <c r="AP2" s="44"/>
-      <c r="AQ2" s="44"/>
-      <c r="AR2" s="44"/>
-      <c r="AS2" s="44"/>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="44"/>
-      <c r="AV2" s="44"/>
+      <c r="AH2" s="46"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
+      <c r="AL2" s="46"/>
+      <c r="AM2" s="46"/>
+      <c r="AN2" s="46"/>
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="46"/>
+      <c r="AR2" s="46"/>
+      <c r="AS2" s="46"/>
+      <c r="AT2" s="46"/>
+      <c r="AU2" s="46"/>
+      <c r="AV2" s="46"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -24193,7 +24246,7 @@
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="47" t="s">
         <v>334</v>
       </c>
       <c r="B6" s="22">
@@ -24359,7 +24412,7 @@
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A7" s="45"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
@@ -24489,7 +24542,7 @@
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A8" s="45"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -24741,7 +24794,7 @@
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="47" t="s">
         <v>338</v>
       </c>
       <c r="B12" s="22">
@@ -24899,7 +24952,7 @@
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A13" s="45"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -25006,7 +25059,7 @@
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A14" s="45"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -25118,7 +25171,7 @@
       </c>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="47" t="s">
         <v>340</v>
       </c>
       <c r="B16" s="22">
@@ -25277,7 +25330,7 @@
       </c>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A17" s="45"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="22">
         <v>-2</v>
       </c>
@@ -25393,7 +25446,7 @@
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A18" s="45"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="22">
         <v>-2.9</v>
       </c>
@@ -25506,7 +25559,7 @@
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="47" t="s">
         <v>342</v>
       </c>
       <c r="B20" s="22">
@@ -25668,7 +25721,7 @@
       </c>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A21" s="45"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -25799,7 +25852,7 @@
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A22" s="45"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
@@ -25930,7 +25983,7 @@
       </c>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A23" s="45"/>
+      <c r="A23" s="47"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
@@ -26061,7 +26114,7 @@
       </c>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A24" s="45"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
@@ -26192,7 +26245,7 @@
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A25" s="45"/>
+      <c r="A25" s="47"/>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
@@ -26323,7 +26376,7 @@
       </c>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A26" s="45"/>
+      <c r="A26" s="47"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
@@ -26454,7 +26507,7 @@
       </c>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A27" s="45"/>
+      <c r="A27" s="47"/>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
@@ -26585,7 +26638,7 @@
       </c>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A28" s="45"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -26715,7 +26768,7 @@
       </c>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="47" t="s">
         <v>352</v>
       </c>
       <c r="B29" s="22">
@@ -26840,7 +26893,7 @@
       <c r="AU29" s="6"/>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A30" s="45"/>
+      <c r="A30" s="47"/>
       <c r="B30" s="22">
         <v>-2</v>
       </c>
@@ -26949,7 +27002,7 @@
       <c r="AG30" s="6"/>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A31" s="45"/>
+      <c r="A31" s="47"/>
       <c r="B31" s="22">
         <v>-2</v>
       </c>
@@ -27058,7 +27111,7 @@
       <c r="AG31" s="6"/>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A32" s="45"/>
+      <c r="A32" s="47"/>
       <c r="B32" s="22">
         <v>-2</v>
       </c>
@@ -27167,7 +27220,7 @@
       <c r="AG32" s="6"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A33" s="45"/>
+      <c r="A33" s="47"/>
       <c r="B33" s="22">
         <v>-2</v>
       </c>
@@ -27276,7 +27329,7 @@
       <c r="AG33" s="6"/>
     </row>
     <row r="34" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A34" s="45"/>
+      <c r="A34" s="47"/>
       <c r="B34" s="22">
         <v>-2</v>
       </c>
@@ -27385,7 +27438,7 @@
       <c r="AG34" s="6"/>
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A35" s="45"/>
+      <c r="A35" s="47"/>
       <c r="B35" s="22">
         <v>-2</v>
       </c>
@@ -27494,7 +27547,7 @@
       <c r="AG35" s="6"/>
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A36" s="45"/>
+      <c r="A36" s="47"/>
       <c r="B36" s="22">
         <v>-2</v>
       </c>
@@ -27603,7 +27656,7 @@
       <c r="AG36" s="6"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A37" s="45"/>
+      <c r="A37" s="47"/>
       <c r="B37" s="22">
         <v>-2</v>
       </c>
@@ -27712,7 +27765,7 @@
       <c r="AG37" s="6"/>
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="47" t="s">
         <v>351</v>
       </c>
       <c r="B38" s="22">
@@ -27837,7 +27890,7 @@
       <c r="AU38" s="6"/>
     </row>
     <row r="39" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A39" s="45"/>
+      <c r="A39" s="47"/>
       <c r="B39" s="22">
         <v>-2</v>
       </c>
@@ -27946,7 +27999,7 @@
       <c r="AG39" s="6"/>
     </row>
     <row r="40" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A40" s="45"/>
+      <c r="A40" s="47"/>
       <c r="B40" s="22">
         <v>-2</v>
       </c>
@@ -28055,7 +28108,7 @@
       <c r="AG40" s="6"/>
     </row>
     <row r="41" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A41" s="45"/>
+      <c r="A41" s="47"/>
       <c r="B41" s="22">
         <v>-2</v>
       </c>
@@ -28164,7 +28217,7 @@
       <c r="AG41" s="6"/>
     </row>
     <row r="42" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A42" s="45"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="22">
         <v>-2</v>
       </c>
@@ -28273,7 +28326,7 @@
       <c r="AG42" s="6"/>
     </row>
     <row r="43" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A43" s="45"/>
+      <c r="A43" s="47"/>
       <c r="B43" s="22">
         <v>-2</v>
       </c>
@@ -28382,7 +28435,7 @@
       <c r="AG43" s="6"/>
     </row>
     <row r="44" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A44" s="45"/>
+      <c r="A44" s="47"/>
       <c r="B44" s="22">
         <v>-2</v>
       </c>
@@ -28491,7 +28544,7 @@
       <c r="AG44" s="6"/>
     </row>
     <row r="45" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A45" s="45"/>
+      <c r="A45" s="47"/>
       <c r="B45" s="22">
         <v>-2</v>
       </c>
@@ -28600,7 +28653,7 @@
       <c r="AG45" s="6"/>
     </row>
     <row r="46" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A46" s="45"/>
+      <c r="A46" s="47"/>
       <c r="B46" s="22">
         <v>-2</v>
       </c>
@@ -28709,7 +28762,7 @@
       <c r="AG46" s="6"/>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="47" t="s">
         <v>353</v>
       </c>
       <c r="B47" s="22">
@@ -28834,7 +28887,7 @@
       <c r="AU47" s="6"/>
     </row>
     <row r="48" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A48" s="45"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="22">
         <v>-2</v>
       </c>
@@ -28943,7 +28996,7 @@
       <c r="AG48" s="6"/>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A49" s="45"/>
+      <c r="A49" s="47"/>
       <c r="B49" s="22">
         <v>-2</v>
       </c>
@@ -29052,7 +29105,7 @@
       <c r="AG49" s="6"/>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A50" s="45"/>
+      <c r="A50" s="47"/>
       <c r="B50" s="22">
         <v>-2</v>
       </c>
@@ -29161,7 +29214,7 @@
       <c r="AG50" s="6"/>
     </row>
     <row r="51" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A51" s="45"/>
+      <c r="A51" s="47"/>
       <c r="B51" s="22">
         <v>-2</v>
       </c>
@@ -29270,7 +29323,7 @@
       <c r="AG51" s="6"/>
     </row>
     <row r="52" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A52" s="45"/>
+      <c r="A52" s="47"/>
       <c r="B52" s="22">
         <v>-2</v>
       </c>
@@ -29379,7 +29432,7 @@
       <c r="AG52" s="6"/>
     </row>
     <row r="53" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A53" s="45"/>
+      <c r="A53" s="47"/>
       <c r="B53" s="22">
         <v>-2</v>
       </c>
@@ -29488,7 +29541,7 @@
       <c r="AG53" s="6"/>
     </row>
     <row r="54" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A54" s="45"/>
+      <c r="A54" s="47"/>
       <c r="B54" s="22">
         <v>-2</v>
       </c>
@@ -29597,7 +29650,7 @@
       <c r="AG54" s="6"/>
     </row>
     <row r="55" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A55" s="45"/>
+      <c r="A55" s="47"/>
       <c r="B55" s="22">
         <v>-2</v>
       </c>
@@ -29736,7 +29789,7 @@
       <c r="AE56" s="6"/>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A57" s="45" t="s">
+      <c r="A57" s="47" t="s">
         <v>344</v>
       </c>
       <c r="B57" s="22">
@@ -29902,7 +29955,7 @@
       </c>
     </row>
     <row r="58" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A58" s="45"/>
+      <c r="A58" s="47"/>
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22"/>
@@ -30032,7 +30085,7 @@
       </c>
     </row>
     <row r="59" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A59" s="45"/>
+      <c r="A59" s="47"/>
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
       <c r="D59" s="22"/>
@@ -30267,7 +30320,7 @@
       <c r="AE62" s="6"/>
     </row>
     <row r="63" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A63" s="45" t="s">
+      <c r="A63" s="47" t="s">
         <v>348</v>
       </c>
       <c r="B63" s="22">
@@ -30376,7 +30429,7 @@
       </c>
     </row>
     <row r="64" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A64" s="45"/>
+      <c r="A64" s="47"/>
       <c r="B64" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -30483,7 +30536,7 @@
       </c>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.15">
-      <c r="A65" s="45"/>
+      <c r="A65" s="47"/>
       <c r="B65" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -30879,12 +30932,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -30896,6 +30943,12 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -30907,7 +30960,7 @@
   <dimension ref="A1:BJ22"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -30954,70 +31007,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -31027,22 +31080,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -31052,36 +31105,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="44" t="s">
+      <c r="Y2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="46"/>
+      <c r="AB2" s="46"/>
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="46"/>
+      <c r="AE2" s="46"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AG2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="44"/>
-      <c r="AP2" s="44"/>
-      <c r="AQ2" s="44"/>
-      <c r="AR2" s="44"/>
-      <c r="AS2" s="44"/>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="44"/>
-      <c r="AV2" s="44"/>
+      <c r="AH2" s="46"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
+      <c r="AL2" s="46"/>
+      <c r="AM2" s="46"/>
+      <c r="AN2" s="46"/>
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="46"/>
+      <c r="AR2" s="46"/>
+      <c r="AS2" s="46"/>
+      <c r="AT2" s="46"/>
+      <c r="AU2" s="46"/>
+      <c r="AV2" s="46"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
@@ -32810,10 +32863,10 @@
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C22" s="46">
+      <c r="C22" s="44">
         <v>60</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="45">
         <f>C22+1</f>
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
feat(math), #21: Add `SUMIF` function.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946AF576-9C20-694F-B332-F15C310B5842}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D550AB63-9932-1146-8B67-E38BE5C0DF15}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="460">
   <si>
     <t>ca</t>
   </si>
@@ -1919,7 +1919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV81"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -11375,55 +11375,165 @@
       </c>
     </row>
     <row r="72" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
+      <c r="B72" s="14">
+        <v>0</v>
+      </c>
+      <c r="C72" s="14">
+        <v>1</v>
+      </c>
+      <c r="D72" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E72" s="14">
+        <v>10</v>
+      </c>
+      <c r="F72" s="14">
+        <v>-1</v>
+      </c>
       <c r="G72" s="6"/>
-      <c r="H72" s="6"/>
-      <c r="I72" s="6"/>
-      <c r="J72" s="6"/>
-      <c r="K72" s="6"/>
-      <c r="L72" s="6"/>
-      <c r="M72" s="6"/>
-      <c r="N72" s="6"/>
-      <c r="O72" s="6"/>
-      <c r="P72" s="6"/>
-      <c r="Q72" s="6"/>
-      <c r="R72" s="6"/>
-      <c r="S72" s="6"/>
-      <c r="T72" s="6"/>
-      <c r="U72" s="6"/>
-      <c r="V72" s="6"/>
-      <c r="W72" s="6"/>
-      <c r="X72" s="6"/>
-      <c r="Y72" s="6"/>
-      <c r="Z72" s="6"/>
-      <c r="AA72" s="6"/>
-      <c r="AB72" s="6"/>
-      <c r="AC72" s="6"/>
-      <c r="AD72" s="6"/>
-      <c r="AE72" s="6"/>
-      <c r="AF72" s="10"/>
-      <c r="AG72" s="6"/>
-      <c r="AH72" s="6"/>
-      <c r="AI72" s="6"/>
-      <c r="AJ72" s="6"/>
-      <c r="AK72" s="6"/>
-      <c r="AL72" s="6"/>
-      <c r="AM72" s="6"/>
-      <c r="AN72" s="6"/>
-      <c r="AO72" s="6"/>
-      <c r="AP72" s="6"/>
-      <c r="AQ72" s="6"/>
-      <c r="AR72" s="6"/>
-      <c r="AS72" s="6"/>
-      <c r="AT72" s="6"/>
-      <c r="AU72" s="6"/>
+      <c r="H72" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I72" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J72" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K72" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L72" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M72" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N72" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O72" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P72" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q72" s="6">
+        <f>SUMIF(B72:C72,1,D72:E72)</f>
+        <v>10</v>
+      </c>
+      <c r="R72" s="6">
+        <f>SUMIF(C72:D72,"1",E72:F72)</f>
+        <v>10</v>
+      </c>
+      <c r="S72" s="6">
+        <f>SUMIF(D72:E72,"&gt;1",F72:G72)</f>
+        <v>-1</v>
+      </c>
+      <c r="T72" s="6">
+        <f>SUMIF(E72:F72,"&lt;&gt;-1",F72:G72)</f>
+        <v>-1</v>
+      </c>
+      <c r="U72" s="6">
+        <f>SUMIF(F72:G72,1,H72:I72)</f>
+        <v>0</v>
+      </c>
+      <c r="V72" s="6">
+        <f>SUMIF(G72:H72,G72,C72:D72)</f>
+        <v>0</v>
+      </c>
+      <c r="W72" s="6">
+        <f>SUMIF(H72:I72,H72,D72:E72)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X72" s="6">
+        <f>SUMIF(H72:I72,"&lt;=TRUE",E72:F72)</f>
+        <v>-1</v>
+      </c>
+      <c r="Y72" s="6" t="e">
+        <f>SUMIF(H72:I72,H72,J72:K72)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z72" s="6" t="e">
+        <f t="shared" ref="Z72:AE72" si="65">SUMIF(I72:J72,I72,K72:L72)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA72" s="6" t="e">
+        <f t="shared" si="65"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB72" s="6" t="e">
+        <f t="shared" si="65"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC72" s="6" t="e">
+        <f t="shared" si="65"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD72" s="6" t="e">
+        <f t="shared" si="65"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE72" s="6" t="e">
+        <f t="shared" si="65"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF72" s="11">
+        <f t="array" ref="AF72">SUMIF(C72:G72,{1,"&gt;3"},D72:H72)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AG72" s="6">
+        <f t="array" ref="AG72:AV72">SUMIF(E72:I72,{"*ao","","TRUE",TRUE,"*a?"},B72:F72)</f>
+        <v>10</v>
+      </c>
+      <c r="AH72" s="6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AI72" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AJ72" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AK72" s="6">
+        <v>10</v>
+      </c>
+      <c r="AL72" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AM72" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AN72" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AO72" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AP72" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ72" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AR72" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AS72" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AT72" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AU72" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AV72" s="4" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="73" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A73" s="4" t="s">
@@ -11889,63 +11999,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q79" s="6">
-        <f t="shared" ref="Q79:AE79" si="65">TAN(B79)</f>
+        <f t="shared" ref="Q79:AE79" si="66">TAN(B79)</f>
         <v>0</v>
       </c>
       <c r="R79" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1.5574077246549023</v>
       </c>
       <c r="S79" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-1.1192136417341325</v>
       </c>
       <c r="T79" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>0.64836082745908663</v>
       </c>
       <c r="U79" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-1.5574077246549023</v>
       </c>
       <c r="V79" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="W79" s="6" t="e">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>#VALUE!</v>
       </c>
       <c r="X79" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1.5574077246549023</v>
       </c>
       <c r="Y79" s="6" t="e">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z79" s="6" t="e">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>#N/A</v>
       </c>
       <c r="AA79" s="6" t="e">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB79" s="6" t="e">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>#NAME?</v>
       </c>
       <c r="AC79" s="6" t="e">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>#NULL!</v>
       </c>
       <c r="AD79" s="6" t="e">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>#NUM!</v>
       </c>
       <c r="AE79" s="6" t="e">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>#REF!</v>
       </c>
       <c r="AF79" s="10"/>
@@ -12047,63 +12157,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q80" s="6">
-        <f t="shared" ref="Q80:AE80" si="66">TANH(B80)</f>
+        <f t="shared" ref="Q80:AE80" si="67">TANH(B80)</f>
         <v>0</v>
       </c>
       <c r="R80" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>0.76159415595576485</v>
       </c>
       <c r="S80" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>0.98009639626619138</v>
       </c>
       <c r="T80" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>0.99999999587769262</v>
       </c>
       <c r="U80" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>-0.76159415595576485</v>
       </c>
       <c r="V80" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="W80" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#VALUE!</v>
       </c>
       <c r="X80" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>0.76159415595576485</v>
       </c>
       <c r="Y80" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z80" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#N/A</v>
       </c>
       <c r="AA80" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB80" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#NAME?</v>
       </c>
       <c r="AC80" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#NULL!</v>
       </c>
       <c r="AD80" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#NUM!</v>
       </c>
       <c r="AE80" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#REF!</v>
       </c>
       <c r="AF80" s="10"/>
@@ -12237,31 +12347,31 @@
         <v>1</v>
       </c>
       <c r="Y81" s="6" t="e">
-        <f t="shared" ref="Y81:AE81" si="67">TRUNC(J81,I81)</f>
+        <f t="shared" ref="Y81:AE81" si="68">TRUNC(J81,I81)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z81" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#N/A</v>
       </c>
       <c r="AA81" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB81" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#NAME?</v>
       </c>
       <c r="AC81" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#NULL!</v>
       </c>
       <c r="AD81" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#NUM!</v>
       </c>
       <c r="AE81" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#REF!</v>
       </c>
       <c r="AF81" s="10"/>
@@ -23401,7 +23511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AV22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -30932,6 +31042,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -30943,12 +31059,6 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat(stat), #21: Add `AVERAGEIF`, `COUNT`, `COUNTA`, `COUNTIF` functions.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D550AB63-9932-1146-8B67-E38BE5C0DF15}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1795F26-2899-7242-8358-C12458D4585F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="461">
   <si>
     <t>ca</t>
   </si>
@@ -1432,6 +1432,9 @@
   </si>
   <si>
     <t>26/8/1987 02:00 AM</t>
+  </si>
+  <si>
+    <t>29/02/1900</t>
   </si>
 </sst>
 </file>
@@ -1538,7 +1541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1607,12 +1610,14 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1919,7 +1924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1954,70 +1959,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="47"/>
+      <c r="AQ1" s="47"/>
+      <c r="AR1" s="47"/>
+      <c r="AS1" s="47"/>
+      <c r="AT1" s="47"/>
+      <c r="AU1" s="47"/>
+      <c r="AV1" s="47"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -2027,22 +2032,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -2052,36 +2057,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="46" t="s">
+      <c r="Y2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="46" t="s">
+      <c r="AG2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="46"/>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="46"/>
-      <c r="AL2" s="46"/>
-      <c r="AM2" s="46"/>
-      <c r="AN2" s="46"/>
-      <c r="AO2" s="46"/>
-      <c r="AP2" s="46"/>
-      <c r="AQ2" s="46"/>
-      <c r="AR2" s="46"/>
-      <c r="AS2" s="46"/>
-      <c r="AT2" s="46"/>
-      <c r="AU2" s="46"/>
-      <c r="AV2" s="46"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
@@ -12520,70 +12525,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="47"/>
+      <c r="AQ1" s="47"/>
+      <c r="AR1" s="47"/>
+      <c r="AS1" s="47"/>
+      <c r="AT1" s="47"/>
+      <c r="AU1" s="47"/>
+      <c r="AV1" s="47"/>
     </row>
     <row r="2" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="26" t="s">
         <v>38</v>
       </c>
@@ -12593,22 +12598,22 @@
       <c r="I2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
       <c r="V2" s="26" t="s">
         <v>38</v>
       </c>
@@ -12618,36 +12623,36 @@
       <c r="X2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="46" t="s">
+      <c r="Y2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
       <c r="AF2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="46" t="s">
+      <c r="AG2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="46"/>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="46"/>
-      <c r="AL2" s="46"/>
-      <c r="AM2" s="46"/>
-      <c r="AN2" s="46"/>
-      <c r="AO2" s="46"/>
-      <c r="AP2" s="46"/>
-      <c r="AQ2" s="46"/>
-      <c r="AR2" s="46"/>
-      <c r="AS2" s="46"/>
-      <c r="AT2" s="46"/>
-      <c r="AU2" s="46"/>
-      <c r="AV2" s="46"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
     </row>
     <row r="3" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="28" t="s">
@@ -12975,7 +12980,7 @@
       </c>
     </row>
     <row r="5" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="49" t="s">
         <v>357</v>
       </c>
       <c r="B5" s="14">
@@ -13136,7 +13141,7 @@
       </c>
     </row>
     <row r="6" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="49" t="s">
         <v>358</v>
       </c>
       <c r="B6" s="14">
@@ -14854,7 +14859,7 @@
       <c r="AV17" s="4"/>
     </row>
     <row r="18" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="28"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -14904,7 +14909,7 @@
       <c r="AV18" s="4"/>
     </row>
     <row r="19" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="28"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -14954,7 +14959,7 @@
       <c r="AV19" s="4"/>
     </row>
     <row r="20" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="28"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -15130,70 +15135,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="47"/>
+      <c r="AQ1" s="47"/>
+      <c r="AR1" s="47"/>
+      <c r="AS1" s="47"/>
+      <c r="AT1" s="47"/>
+      <c r="AU1" s="47"/>
+      <c r="AV1" s="47"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="27" t="s">
         <v>38</v>
       </c>
@@ -15203,22 +15208,22 @@
       <c r="I2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
       <c r="V2" s="27" t="s">
         <v>38</v>
       </c>
@@ -15228,36 +15233,36 @@
       <c r="X2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="46" t="s">
+      <c r="Y2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
       <c r="AF2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="46" t="s">
+      <c r="AG2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="46"/>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="46"/>
-      <c r="AL2" s="46"/>
-      <c r="AM2" s="46"/>
-      <c r="AN2" s="46"/>
-      <c r="AO2" s="46"/>
-      <c r="AP2" s="46"/>
-      <c r="AQ2" s="46"/>
-      <c r="AR2" s="46"/>
-      <c r="AS2" s="46"/>
-      <c r="AT2" s="46"/>
-      <c r="AU2" s="46"/>
-      <c r="AV2" s="46"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -17004,70 +17009,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="47"/>
+      <c r="AQ1" s="47"/>
+      <c r="AR1" s="47"/>
+      <c r="AS1" s="47"/>
+      <c r="AT1" s="47"/>
+      <c r="AU1" s="47"/>
+      <c r="AV1" s="47"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -17077,22 +17082,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -17102,36 +17107,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="46" t="s">
+      <c r="Y2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="46" t="s">
+      <c r="AG2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="46"/>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="46"/>
-      <c r="AL2" s="46"/>
-      <c r="AM2" s="46"/>
-      <c r="AN2" s="46"/>
-      <c r="AO2" s="46"/>
-      <c r="AP2" s="46"/>
-      <c r="AQ2" s="46"/>
-      <c r="AR2" s="46"/>
-      <c r="AS2" s="46"/>
-      <c r="AT2" s="46"/>
-      <c r="AU2" s="46"/>
-      <c r="AV2" s="46"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -17760,70 +17765,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="47"/>
+      <c r="AQ1" s="47"/>
+      <c r="AR1" s="47"/>
+      <c r="AS1" s="47"/>
+      <c r="AT1" s="47"/>
+      <c r="AU1" s="47"/>
+      <c r="AV1" s="47"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -17833,22 +17838,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -17858,36 +17863,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="46" t="s">
+      <c r="Y2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="46" t="s">
+      <c r="AG2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="46"/>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="46"/>
-      <c r="AL2" s="46"/>
-      <c r="AM2" s="46"/>
-      <c r="AN2" s="46"/>
-      <c r="AO2" s="46"/>
-      <c r="AP2" s="46"/>
-      <c r="AQ2" s="46"/>
-      <c r="AR2" s="46"/>
-      <c r="AS2" s="46"/>
-      <c r="AT2" s="46"/>
-      <c r="AU2" s="46"/>
-      <c r="AV2" s="46"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -19711,19 +19716,23 @@
   <cols>
     <col min="1" max="1" width="16.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="1.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="21" width="2.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -19734,77 +19743,78 @@
     <col min="30" max="30" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="38" width="2.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="48" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="48" width="6" style="4" bestFit="1" customWidth="1"/>
     <col min="49" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="47"/>
+      <c r="AQ1" s="47"/>
+      <c r="AR1" s="47"/>
+      <c r="AS1" s="47"/>
+      <c r="AT1" s="47"/>
+      <c r="AU1" s="47"/>
+      <c r="AV1" s="47"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -19814,22 +19824,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -19839,36 +19849,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="46" t="s">
+      <c r="Y2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="46" t="s">
+      <c r="AG2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="46"/>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="46"/>
-      <c r="AL2" s="46"/>
-      <c r="AM2" s="46"/>
-      <c r="AN2" s="46"/>
-      <c r="AO2" s="46"/>
-      <c r="AP2" s="46"/>
-      <c r="AQ2" s="46"/>
-      <c r="AR2" s="46"/>
-      <c r="AS2" s="46"/>
-      <c r="AT2" s="46"/>
-      <c r="AU2" s="46"/>
-      <c r="AV2" s="46"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -19895,8 +19905,8 @@
         <v>-0.1</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="6" t="s">
-        <v>32</v>
+      <c r="H4" s="32" t="s">
+        <v>460</v>
       </c>
       <c r="I4" s="6" t="b">
         <v>1</v>
@@ -19926,13 +19936,13 @@
         <f>AVERAGE(B4:C4,C4:D4,D4:E4)</f>
         <v>0.15000000000000002</v>
       </c>
-      <c r="R4" s="6">
-        <f>AVERAGE(C4:D4,D4:E4,E4:F4)</f>
-        <v>0.16666666666666666</v>
+      <c r="R4" s="6" t="e">
+        <f>AVERAGE(C4:D4,D4:E4,E4:F4,"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="S4" s="6">
-        <f>AVERAGE(D4:E4,E4:F4,F4:G4)</f>
-        <v>0.12000000000000002</v>
+        <f>AVERAGE(D4:E4,E4:F4,F4:G4,"29/02/1900")</f>
+        <v>10.1</v>
       </c>
       <c r="T4" s="6">
         <f>AVERAGE(E4:F4,F4:G4,G4:H4)</f>
@@ -20057,8 +20067,8 @@
         <v>-0.1</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="6" t="s">
-        <v>32</v>
+      <c r="H5" s="32" t="s">
+        <v>460</v>
       </c>
       <c r="I5" s="6" t="b">
         <v>1</v>
@@ -20088,16 +20098,16 @@
         <f>AVERAGEA(B5:C5,C5:D5,D5:E5)</f>
         <v>0.15000000000000002</v>
       </c>
-      <c r="R5" s="6">
-        <f t="shared" ref="R5:T5" si="1">AVERAGEA(C5:D5,D5:E5,E5:F5)</f>
-        <v>0.16666666666666666</v>
+      <c r="R5" s="6" t="e">
+        <f>AVERAGEA(C5:D5,D5:E5,E5:F5,"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="S5" s="6">
-        <f t="shared" si="1"/>
-        <v>0.12000000000000002</v>
+        <f>AVERAGEA(D5:E5,E5:F5,F5:G5,"29/02/1900")</f>
+        <v>10.1</v>
       </c>
       <c r="T5" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="T5" si="1">AVERAGEA(E5:F5,F5:G5,G5:H5)</f>
         <v>2.4999999999999994E-2</v>
       </c>
       <c r="U5" s="6">
@@ -20200,8 +20210,164 @@
       </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>102</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E6" s="14">
+        <v>10</v>
+      </c>
+      <c r="F6" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K6" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M6" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N6" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O6" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P6" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q6" s="6">
+        <f>AVERAGEIF(B6:C6,1,D6:E6)</f>
+        <v>6.15</v>
+      </c>
+      <c r="R6" s="6">
+        <f>AVERAGEIF(C6:D6,"1",E6:F6)</f>
+        <v>10</v>
+      </c>
+      <c r="S6" s="6">
+        <f>AVERAGEIF(D6:E6,"&gt;1",F6:G6)</f>
+        <v>-1</v>
+      </c>
+      <c r="T6" s="6">
+        <f>AVERAGEIF(E6:F6,"&lt;&gt;-1",F6:G6)</f>
+        <v>-1</v>
+      </c>
+      <c r="U6" s="6" t="e">
+        <f>AVERAGEIF(F6:G6,1,H6:I6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V6" s="6" t="e">
+        <f>AVERAGEIF(G6:H6,G6,C6:D6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W6" s="6">
+        <f>AVERAGEIF(H6:I6,H6,D6:E6)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X6" s="6">
+        <f>AVERAGEIF(H6:I6,"&lt;=TRUE",E6:F6)</f>
+        <v>-1</v>
+      </c>
+      <c r="Y6" s="6" t="e">
+        <f>AVERAGEIF(H6:I6,H6,J6:K6)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z6" s="6" t="e">
+        <f>AVERAGEIF(I6:J6,I6,K6:L6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA6" s="6" t="e">
+        <f t="shared" ref="AA6:AE6" si="3">AVERAGEIF(J6:K6,J6,L6:M6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB6" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC6" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD6" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE6" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF6" s="11">
+        <f t="array" ref="AF6">AVERAGEIF(C6:G6,{1,"&gt;3"},D6:H6)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AG6" s="6">
+        <f t="array" ref="AG6:AV6">AVERAGEIF(E6:I6,{"*ao","","TRUE",TRUE,"*a?"},B6:F6)</f>
+        <v>10</v>
+      </c>
+      <c r="AH6" s="6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AI6" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AJ6" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AK6" s="6">
+        <v>10</v>
+      </c>
+      <c r="AL6" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AM6" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AN6" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AO6" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AP6" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ6" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AR6" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AS6" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AT6" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AU6" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AV6" s="4" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.15">
@@ -20254,82 +20420,553 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="A21" s="17" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A22" s="16" t="s">
+      <c r="B21" s="14">
+        <v>0</v>
+      </c>
+      <c r="C21" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="D21" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="E21" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="F21" s="14">
+        <v>-0.1</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="32" t="s">
+        <v>460</v>
+      </c>
+      <c r="I21" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K21" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L21" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M21" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N21" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O21" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P21" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q21" s="6">
+        <f>COUNT(B21:C21,C21:D21,D21:E21,TRUE,"26/08")</f>
+        <v>8</v>
+      </c>
+      <c r="R21" s="6">
+        <f>COUNT(C21:D21,D21:E21,E21:F21)</f>
+        <v>6</v>
+      </c>
+      <c r="S21" s="6">
+        <f>COUNT(D21:E21,E21:F21,F21:G21)</f>
+        <v>5</v>
+      </c>
+      <c r="T21" s="6">
+        <f>COUNT(G21)</f>
+        <v>0</v>
+      </c>
+      <c r="U21" s="6">
+        <f>COUNT(F21:G21,G21:H21,H21:I21)</f>
+        <v>1</v>
+      </c>
+      <c r="V21" s="6">
+        <f>COUNT(F21:G21)</f>
+        <v>1</v>
+      </c>
+      <c r="W21" s="6">
+        <f>COUNT(H21,F21)</f>
+        <v>1</v>
+      </c>
+      <c r="X21" s="6">
+        <f t="shared" ref="X21:AE21" si="4">COUNT(I21,G21)</f>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="6">
+        <f>COUNT(J21,H21)</f>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AB21" s="6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AC21" s="6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AD21" s="6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AE21" s="6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AF21" s="6">
+        <f>COUNT(G21:I21)</f>
+        <v>0</v>
+      </c>
+      <c r="AG21" s="6">
+        <f t="array" ref="AG21:AL21">COUNT(B21:I21)</f>
+        <v>5</v>
+      </c>
+      <c r="AH21" s="6">
+        <v>5</v>
+      </c>
+      <c r="AI21" s="6">
+        <v>5</v>
+      </c>
+      <c r="AJ21" s="6">
+        <v>5</v>
+      </c>
+      <c r="AK21" s="6">
+        <v>5</v>
+      </c>
+      <c r="AL21" s="6">
+        <v>5</v>
+      </c>
+      <c r="AM21" s="6">
+        <f t="array" ref="AM21:AV21">COUNT(I21:P21)</f>
+        <v>0</v>
+      </c>
+      <c r="AN21" s="6">
+        <v>0</v>
+      </c>
+      <c r="AO21" s="6">
+        <v>0</v>
+      </c>
+      <c r="AP21" s="6">
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="6">
+        <v>0</v>
+      </c>
+      <c r="AR21" s="6">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="6">
+        <v>0</v>
+      </c>
+      <c r="AT21" s="6">
+        <v>0</v>
+      </c>
+      <c r="AU21" s="6">
+        <v>0</v>
+      </c>
+      <c r="AV21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="A22" s="17" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B22" s="14">
+        <v>0</v>
+      </c>
+      <c r="C22" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="D22" s="14">
+        <v>-2</v>
+      </c>
+      <c r="E22" s="14">
+        <v>-3</v>
+      </c>
+      <c r="F22" s="14">
+        <v>4</v>
+      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" s="32" t="s">
+        <v>460</v>
+      </c>
+      <c r="I22" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K22" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L22" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M22" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N22" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O22" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P22" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q22" s="6">
+        <f>COUNTA(B22:C22,C22:D22,D22:E22,TRUE,"26/08")</f>
+        <v>8</v>
+      </c>
+      <c r="R22" s="6">
+        <f>COUNTA(C22:D22,D22:E22,E22:F22)</f>
+        <v>6</v>
+      </c>
+      <c r="S22" s="6">
+        <f>COUNTA(D22:E22,E22:F22,F22:G22)</f>
+        <v>5</v>
+      </c>
+      <c r="T22" s="6">
+        <f>COUNTA(G22)</f>
+        <v>0</v>
+      </c>
+      <c r="U22" s="6">
+        <f>COUNTA(F22:G22,G22:H22,H22:I22)</f>
+        <v>4</v>
+      </c>
+      <c r="V22" s="6">
+        <f>COUNTA(F22:G22)</f>
+        <v>1</v>
+      </c>
+      <c r="W22" s="6">
+        <f t="shared" ref="W22:AE22" si="5">COUNTA(H22,F22)</f>
+        <v>2</v>
+      </c>
+      <c r="X22" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Y22" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Z22" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AA22" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AB22" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AC22" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AD22" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AE22" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AF22" s="6">
+        <f>COUNTA(G22:I22)</f>
+        <v>2</v>
+      </c>
+      <c r="AG22" s="6">
+        <f t="array" ref="AG22:AL22">COUNTA(B22:I22)</f>
+        <v>7</v>
+      </c>
+      <c r="AH22" s="6">
+        <v>7</v>
+      </c>
+      <c r="AI22" s="6">
+        <v>7</v>
+      </c>
+      <c r="AJ22" s="6">
+        <v>7</v>
+      </c>
+      <c r="AK22" s="6">
+        <v>7</v>
+      </c>
+      <c r="AL22" s="6">
+        <v>7</v>
+      </c>
+      <c r="AM22" s="6">
+        <f t="array" ref="AM22:AV22">COUNTA(I22:P22)</f>
+        <v>8</v>
+      </c>
+      <c r="AN22" s="6">
+        <v>8</v>
+      </c>
+      <c r="AO22" s="6">
+        <v>8</v>
+      </c>
+      <c r="AP22" s="6">
+        <v>8</v>
+      </c>
+      <c r="AQ22" s="6">
+        <v>8</v>
+      </c>
+      <c r="AR22" s="6">
+        <v>8</v>
+      </c>
+      <c r="AS22" s="6">
+        <v>8</v>
+      </c>
+      <c r="AT22" s="6">
+        <v>8</v>
+      </c>
+      <c r="AU22" s="6">
+        <v>8</v>
+      </c>
+      <c r="AV22" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A23" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A24" s="16" t="s">
+      <c r="G23" s="46"/>
+    </row>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="A24" s="17" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B24" s="14">
+        <v>0</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
+      <c r="D24" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E24" s="14">
+        <v>10</v>
+      </c>
+      <c r="F24" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" s="32" t="s">
+        <v>460</v>
+      </c>
+      <c r="I24" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K24" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L24" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M24" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N24" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O24" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P24" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q24" s="6">
+        <f>COUNTIF(B24:C24,1)</f>
+        <v>1</v>
+      </c>
+      <c r="R24" s="6">
+        <f>COUNTIF(C24:D24,"1")</f>
+        <v>1</v>
+      </c>
+      <c r="S24" s="6">
+        <f>COUNTIF(D24:E24,"&gt;1")</f>
+        <v>2</v>
+      </c>
+      <c r="T24" s="6">
+        <f>COUNTIF(E24:F24,"&lt;&gt;-1")</f>
+        <v>1</v>
+      </c>
+      <c r="U24" s="6">
+        <f>COUNTIF(F24:G24,1)</f>
+        <v>0</v>
+      </c>
+      <c r="V24" s="6">
+        <f>COUNTIF(G24:H24,G24)</f>
+        <v>0</v>
+      </c>
+      <c r="W24" s="6">
+        <f>COUNTIF(H24:I24,H24)</f>
+        <v>1</v>
+      </c>
+      <c r="X24" s="6">
+        <f>COUNTIF(H24:I24,"&lt;=TRUE")</f>
+        <v>1</v>
+      </c>
+      <c r="Y24" s="6">
+        <f t="shared" ref="Y24:AE24" si="6">COUNTIF(H24:I24,H24)</f>
+        <v>1</v>
+      </c>
+      <c r="Z24" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AA24" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AB24" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AC24" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AD24" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AE24" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AF24" s="11">
+        <f t="array" ref="AF24">COUNTIF(C24:G24,{1,"&gt;3"})</f>
+        <v>1</v>
+      </c>
+      <c r="AG24" s="6">
+        <f t="array" ref="AG24:AV24">COUNTIF(E24:I24,{"*ao","","TRUE",TRUE,"*a?"})</f>
+        <v>0</v>
+      </c>
+      <c r="AH24" s="6">
+        <v>1</v>
+      </c>
+      <c r="AI24" s="6">
+        <v>1</v>
+      </c>
+      <c r="AJ24" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK24" s="6">
+        <v>0</v>
+      </c>
+      <c r="AL24" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AM24" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AN24" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AO24" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AP24" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ24" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AR24" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AS24" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AT24" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AU24" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AV24" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A25" s="16" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A26" s="16" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A28" s="16" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A29" s="16" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A30" s="16" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A31" s="16" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A32" s="16" t="s">
         <v>128</v>
       </c>
@@ -20494,8 +21131,8 @@
         <v>-0.1</v>
       </c>
       <c r="G61" s="6"/>
-      <c r="H61" s="6" t="s">
-        <v>32</v>
+      <c r="H61" s="32" t="s">
+        <v>460</v>
       </c>
       <c r="I61" s="6" t="b">
         <v>1</v>
@@ -20522,23 +21159,23 @@
         <v>#REF!</v>
       </c>
       <c r="Q61" s="6">
-        <f>MAX(B61:C61,C61:D61,D61:E61)</f>
-        <v>0.3</v>
-      </c>
-      <c r="R61" s="6">
-        <f t="shared" ref="R61:U61" si="3">MAX(C61:D61,D61:E61,E61:F61)</f>
-        <v>0.3</v>
+        <f>MAX(B61:C61,C61:D61,D61:E61,"2")</f>
+        <v>2</v>
+      </c>
+      <c r="R61" s="6" t="e">
+        <f>MAX(C61:D61,D61:E61,E61:F61,"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="S61" s="6">
-        <f t="shared" si="3"/>
-        <v>0.3</v>
+        <f>MAX(D61:E61,E61:F61,F61:G61,"29/02/1900")</f>
+        <v>60</v>
       </c>
       <c r="T61" s="6">
         <f>MAX(G61)</f>
         <v>0</v>
       </c>
       <c r="U61" s="6">
-        <f t="shared" si="3"/>
+        <f>MAX(F61:G61,G61:H61,H61:I61)</f>
         <v>-0.1</v>
       </c>
       <c r="V61" s="6">
@@ -20558,27 +21195,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z61" s="6" t="e">
-        <f t="shared" ref="Z61:AE61" si="4">MAX(K61:L61)</f>
+        <f t="shared" ref="Z61:AE61" si="7">MAX(K61:L61)</f>
         <v>#N/A</v>
       </c>
       <c r="AA61" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB61" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#NAME?</v>
       </c>
       <c r="AC61" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#NULL!</v>
       </c>
       <c r="AD61" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#NUM!</v>
       </c>
       <c r="AE61" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
       <c r="AF61" s="6">
@@ -20656,8 +21293,8 @@
         <v>4</v>
       </c>
       <c r="G62" s="6"/>
-      <c r="H62" s="6" t="s">
-        <v>32</v>
+      <c r="H62" s="32" t="s">
+        <v>460</v>
       </c>
       <c r="I62" s="6" t="b">
         <v>1</v>
@@ -20687,13 +21324,13 @@
         <f>MAXA(B62:C62,C62:D62,D62:E62)</f>
         <v>0.1</v>
       </c>
-      <c r="R62" s="6">
-        <f>MAXA(C62:D62,D62:E62,E62:F62)</f>
-        <v>4</v>
+      <c r="R62" s="6" t="e">
+        <f>MAXA(C62:D62,D62:E62,E62:F62,"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="S62" s="6">
-        <f>MAXA(D62,E62,I62)</f>
-        <v>1</v>
+        <f>MAXA(D62,E62,I62,"29/02/1900")</f>
+        <v>60</v>
       </c>
       <c r="T62" s="6">
         <f>MAXA(G62)</f>
@@ -20728,19 +21365,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AB62" s="6" t="e">
-        <f t="shared" ref="AB62:AE62" si="5">MAXA(M62:N62)</f>
+        <f t="shared" ref="AB62:AE62" si="8">MAXA(M62:N62)</f>
         <v>#NAME?</v>
       </c>
       <c r="AC62" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>#NULL!</v>
       </c>
       <c r="AD62" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AE62" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
       <c r="AF62" s="6">
@@ -20828,8 +21465,8 @@
         <v>0.1</v>
       </c>
       <c r="G65" s="6"/>
-      <c r="H65" s="6" t="s">
-        <v>32</v>
+      <c r="H65" s="32" t="s">
+        <v>460</v>
       </c>
       <c r="I65" s="6" t="b">
         <v>1</v>
@@ -20859,12 +21496,12 @@
         <f>MIN(B65:C65,C65:D65,D65:E65)</f>
         <v>-0.3</v>
       </c>
-      <c r="R65" s="6">
-        <f>MIN(C65:D65,D65:E65,E65:F65)</f>
-        <v>-0.3</v>
+      <c r="R65" s="6" t="e">
+        <f>MIN(C65:D65,D65:E65,E65:F65,"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="S65" s="6">
-        <f>MIN(D65:E65,E65:F65,F65:G65)</f>
+        <f>MIN(D65:E65,E65:F65,F65:G65,"29/02/1900")</f>
         <v>-0.3</v>
       </c>
       <c r="T65" s="6">
@@ -20888,31 +21525,31 @@
         <v>0.1</v>
       </c>
       <c r="Y65" s="6" t="e">
-        <f t="shared" ref="Y65:AE65" si="6">MIN(J65:K65)</f>
+        <f t="shared" ref="Y65:AE65" si="9">MIN(J65:K65)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z65" s="6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>#N/A</v>
       </c>
       <c r="AA65" s="6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB65" s="6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>#NAME?</v>
       </c>
       <c r="AC65" s="6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>#NULL!</v>
       </c>
       <c r="AD65" s="6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>#NUM!</v>
       </c>
       <c r="AE65" s="6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
       <c r="AF65" s="6">
@@ -20995,8 +21632,8 @@
         <v>4</v>
       </c>
       <c r="G67" s="6"/>
-      <c r="H67" s="6" t="s">
-        <v>32</v>
+      <c r="H67" s="32" t="s">
+        <v>460</v>
       </c>
       <c r="I67" s="6" t="b">
         <v>1</v>
@@ -21026,12 +21663,12 @@
         <f>MINA(B67:C67,C67:D67,D67:E67)</f>
         <v>-0.1</v>
       </c>
-      <c r="R67" s="6">
-        <f>MINA(C67:D67,D67:E67,E67:F67)</f>
-        <v>-0.1</v>
+      <c r="R67" s="6" t="e">
+        <f>MINA(C67:D67,D67:E67,E67:F67,"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="S67" s="6">
-        <f>MINA(D67,E67,I67)</f>
+        <f>MINA(D67,E67,I67,"29/02/1900")</f>
         <v>1</v>
       </c>
       <c r="T67" s="6">
@@ -21055,31 +21692,31 @@
         <v>1</v>
       </c>
       <c r="Y67" s="6" t="e">
-        <f t="shared" ref="Y67:AE67" si="7">MINA(J67:K67)</f>
+        <f t="shared" ref="Y67:AE67" si="10">MINA(J67:K67)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z67" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
       <c r="AA67" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB67" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>#NAME?</v>
       </c>
       <c r="AC67" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>#NULL!</v>
       </c>
       <c r="AD67" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>#NUM!</v>
       </c>
       <c r="AE67" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>#REF!</v>
       </c>
       <c r="AF67" s="6">
@@ -21378,6 +22015,7 @@
     <mergeCell ref="Y2:AE2"/>
     <mergeCell ref="AG2:AV2"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -21387,7 +22025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7D9E77-BF90-2E45-87C2-E9C169025282}">
   <dimension ref="A1:AV34"/>
   <sheetViews>
-    <sheetView zoomScale="237" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="237" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -21435,70 +22073,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="47"/>
+      <c r="AQ1" s="47"/>
+      <c r="AR1" s="47"/>
+      <c r="AS1" s="47"/>
+      <c r="AT1" s="47"/>
+      <c r="AU1" s="47"/>
+      <c r="AV1" s="47"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="33" t="s">
         <v>38</v>
       </c>
@@ -21508,22 +22146,22 @@
       <c r="I2" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
       <c r="V2" s="33" t="s">
         <v>38</v>
       </c>
@@ -21533,36 +22171,36 @@
       <c r="X2" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="46" t="s">
+      <c r="Y2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
       <c r="AF2" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="46" t="s">
+      <c r="AG2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="46"/>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="46"/>
-      <c r="AL2" s="46"/>
-      <c r="AM2" s="46"/>
-      <c r="AN2" s="46"/>
-      <c r="AO2" s="46"/>
-      <c r="AP2" s="46"/>
-      <c r="AQ2" s="46"/>
-      <c r="AR2" s="46"/>
-      <c r="AS2" s="46"/>
-      <c r="AT2" s="46"/>
-      <c r="AU2" s="46"/>
-      <c r="AV2" s="46"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
     </row>
     <row r="3" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
@@ -23549,70 +24187,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="47"/>
+      <c r="AQ1" s="47"/>
+      <c r="AR1" s="47"/>
+      <c r="AS1" s="47"/>
+      <c r="AT1" s="47"/>
+      <c r="AU1" s="47"/>
+      <c r="AV1" s="47"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -23622,22 +24260,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -23647,36 +24285,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="46" t="s">
+      <c r="Y2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="46" t="s">
+      <c r="AG2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="46"/>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="46"/>
-      <c r="AL2" s="46"/>
-      <c r="AM2" s="46"/>
-      <c r="AN2" s="46"/>
-      <c r="AO2" s="46"/>
-      <c r="AP2" s="46"/>
-      <c r="AQ2" s="46"/>
-      <c r="AR2" s="46"/>
-      <c r="AS2" s="46"/>
-      <c r="AT2" s="46"/>
-      <c r="AU2" s="46"/>
-      <c r="AV2" s="46"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -24168,7 +24806,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -24211,70 +24849,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="47"/>
+      <c r="AQ1" s="47"/>
+      <c r="AR1" s="47"/>
+      <c r="AS1" s="47"/>
+      <c r="AT1" s="47"/>
+      <c r="AU1" s="47"/>
+      <c r="AV1" s="47"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="19" t="s">
         <v>38</v>
       </c>
@@ -24284,22 +24922,22 @@
       <c r="I2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
       <c r="V2" s="19" t="s">
         <v>38</v>
       </c>
@@ -24309,36 +24947,36 @@
       <c r="X2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="46" t="s">
+      <c r="Y2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
       <c r="AF2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="46" t="s">
+      <c r="AG2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="46"/>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="46"/>
-      <c r="AL2" s="46"/>
-      <c r="AM2" s="46"/>
-      <c r="AN2" s="46"/>
-      <c r="AO2" s="46"/>
-      <c r="AP2" s="46"/>
-      <c r="AQ2" s="46"/>
-      <c r="AR2" s="46"/>
-      <c r="AS2" s="46"/>
-      <c r="AT2" s="46"/>
-      <c r="AU2" s="46"/>
-      <c r="AV2" s="46"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -24356,7 +24994,7 @@
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="48" t="s">
         <v>334</v>
       </c>
       <c r="B6" s="22">
@@ -24522,7 +25160,7 @@
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A7" s="47"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
@@ -24652,7 +25290,7 @@
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A8" s="47"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -24904,7 +25542,7 @@
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="48" t="s">
         <v>338</v>
       </c>
       <c r="B12" s="22">
@@ -25062,7 +25700,7 @@
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A13" s="47"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -25169,7 +25807,7 @@
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A14" s="47"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -25281,7 +25919,7 @@
       </c>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="48" t="s">
         <v>340</v>
       </c>
       <c r="B16" s="22">
@@ -25440,7 +26078,7 @@
       </c>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A17" s="47"/>
+      <c r="A17" s="48"/>
       <c r="B17" s="22">
         <v>-2</v>
       </c>
@@ -25556,7 +26194,7 @@
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A18" s="47"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="22">
         <v>-2.9</v>
       </c>
@@ -25669,7 +26307,7 @@
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="48" t="s">
         <v>342</v>
       </c>
       <c r="B20" s="22">
@@ -25831,7 +26469,7 @@
       </c>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A21" s="47"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -25962,7 +26600,7 @@
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A22" s="47"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
@@ -26093,7 +26731,7 @@
       </c>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A23" s="47"/>
+      <c r="A23" s="48"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
@@ -26224,7 +26862,7 @@
       </c>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A24" s="47"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
@@ -26355,7 +26993,7 @@
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A25" s="47"/>
+      <c r="A25" s="48"/>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
@@ -26486,7 +27124,7 @@
       </c>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A26" s="47"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
@@ -26617,7 +27255,7 @@
       </c>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A27" s="47"/>
+      <c r="A27" s="48"/>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
@@ -26748,7 +27386,7 @@
       </c>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A28" s="47"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -26878,7 +27516,7 @@
       </c>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="48" t="s">
         <v>352</v>
       </c>
       <c r="B29" s="22">
@@ -27003,7 +27641,7 @@
       <c r="AU29" s="6"/>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A30" s="47"/>
+      <c r="A30" s="48"/>
       <c r="B30" s="22">
         <v>-2</v>
       </c>
@@ -27112,7 +27750,7 @@
       <c r="AG30" s="6"/>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A31" s="47"/>
+      <c r="A31" s="48"/>
       <c r="B31" s="22">
         <v>-2</v>
       </c>
@@ -27221,7 +27859,7 @@
       <c r="AG31" s="6"/>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A32" s="47"/>
+      <c r="A32" s="48"/>
       <c r="B32" s="22">
         <v>-2</v>
       </c>
@@ -27330,7 +27968,7 @@
       <c r="AG32" s="6"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A33" s="47"/>
+      <c r="A33" s="48"/>
       <c r="B33" s="22">
         <v>-2</v>
       </c>
@@ -27439,7 +28077,7 @@
       <c r="AG33" s="6"/>
     </row>
     <row r="34" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A34" s="47"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="22">
         <v>-2</v>
       </c>
@@ -27548,7 +28186,7 @@
       <c r="AG34" s="6"/>
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A35" s="47"/>
+      <c r="A35" s="48"/>
       <c r="B35" s="22">
         <v>-2</v>
       </c>
@@ -27657,7 +28295,7 @@
       <c r="AG35" s="6"/>
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A36" s="47"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="22">
         <v>-2</v>
       </c>
@@ -27766,7 +28404,7 @@
       <c r="AG36" s="6"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A37" s="47"/>
+      <c r="A37" s="48"/>
       <c r="B37" s="22">
         <v>-2</v>
       </c>
@@ -27875,7 +28513,7 @@
       <c r="AG37" s="6"/>
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="48" t="s">
         <v>351</v>
       </c>
       <c r="B38" s="22">
@@ -28000,7 +28638,7 @@
       <c r="AU38" s="6"/>
     </row>
     <row r="39" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A39" s="47"/>
+      <c r="A39" s="48"/>
       <c r="B39" s="22">
         <v>-2</v>
       </c>
@@ -28109,7 +28747,7 @@
       <c r="AG39" s="6"/>
     </row>
     <row r="40" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A40" s="47"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="22">
         <v>-2</v>
       </c>
@@ -28218,7 +28856,7 @@
       <c r="AG40" s="6"/>
     </row>
     <row r="41" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A41" s="47"/>
+      <c r="A41" s="48"/>
       <c r="B41" s="22">
         <v>-2</v>
       </c>
@@ -28327,7 +28965,7 @@
       <c r="AG41" s="6"/>
     </row>
     <row r="42" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A42" s="47"/>
+      <c r="A42" s="48"/>
       <c r="B42" s="22">
         <v>-2</v>
       </c>
@@ -28436,7 +29074,7 @@
       <c r="AG42" s="6"/>
     </row>
     <row r="43" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A43" s="47"/>
+      <c r="A43" s="48"/>
       <c r="B43" s="22">
         <v>-2</v>
       </c>
@@ -28545,7 +29183,7 @@
       <c r="AG43" s="6"/>
     </row>
     <row r="44" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A44" s="47"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="22">
         <v>-2</v>
       </c>
@@ -28654,7 +29292,7 @@
       <c r="AG44" s="6"/>
     </row>
     <row r="45" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A45" s="47"/>
+      <c r="A45" s="48"/>
       <c r="B45" s="22">
         <v>-2</v>
       </c>
@@ -28763,7 +29401,7 @@
       <c r="AG45" s="6"/>
     </row>
     <row r="46" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A46" s="47"/>
+      <c r="A46" s="48"/>
       <c r="B46" s="22">
         <v>-2</v>
       </c>
@@ -28872,7 +29510,7 @@
       <c r="AG46" s="6"/>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A47" s="47" t="s">
+      <c r="A47" s="48" t="s">
         <v>353</v>
       </c>
       <c r="B47" s="22">
@@ -28997,7 +29635,7 @@
       <c r="AU47" s="6"/>
     </row>
     <row r="48" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A48" s="47"/>
+      <c r="A48" s="48"/>
       <c r="B48" s="22">
         <v>-2</v>
       </c>
@@ -29106,7 +29744,7 @@
       <c r="AG48" s="6"/>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A49" s="47"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="22">
         <v>-2</v>
       </c>
@@ -29215,7 +29853,7 @@
       <c r="AG49" s="6"/>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A50" s="47"/>
+      <c r="A50" s="48"/>
       <c r="B50" s="22">
         <v>-2</v>
       </c>
@@ -29324,7 +29962,7 @@
       <c r="AG50" s="6"/>
     </row>
     <row r="51" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A51" s="47"/>
+      <c r="A51" s="48"/>
       <c r="B51" s="22">
         <v>-2</v>
       </c>
@@ -29433,7 +30071,7 @@
       <c r="AG51" s="6"/>
     </row>
     <row r="52" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A52" s="47"/>
+      <c r="A52" s="48"/>
       <c r="B52" s="22">
         <v>-2</v>
       </c>
@@ -29542,7 +30180,7 @@
       <c r="AG52" s="6"/>
     </row>
     <row r="53" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A53" s="47"/>
+      <c r="A53" s="48"/>
       <c r="B53" s="22">
         <v>-2</v>
       </c>
@@ -29651,7 +30289,7 @@
       <c r="AG53" s="6"/>
     </row>
     <row r="54" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A54" s="47"/>
+      <c r="A54" s="48"/>
       <c r="B54" s="22">
         <v>-2</v>
       </c>
@@ -29760,7 +30398,7 @@
       <c r="AG54" s="6"/>
     </row>
     <row r="55" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A55" s="47"/>
+      <c r="A55" s="48"/>
       <c r="B55" s="22">
         <v>-2</v>
       </c>
@@ -29899,7 +30537,7 @@
       <c r="AE56" s="6"/>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A57" s="47" t="s">
+      <c r="A57" s="48" t="s">
         <v>344</v>
       </c>
       <c r="B57" s="22">
@@ -30065,7 +30703,7 @@
       </c>
     </row>
     <row r="58" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A58" s="47"/>
+      <c r="A58" s="48"/>
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22"/>
@@ -30195,7 +30833,7 @@
       </c>
     </row>
     <row r="59" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A59" s="47"/>
+      <c r="A59" s="48"/>
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
       <c r="D59" s="22"/>
@@ -30430,7 +31068,7 @@
       <c r="AE62" s="6"/>
     </row>
     <row r="63" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A63" s="47" t="s">
+      <c r="A63" s="48" t="s">
         <v>348</v>
       </c>
       <c r="B63" s="22">
@@ -30539,7 +31177,7 @@
       </c>
     </row>
     <row r="64" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A64" s="47"/>
+      <c r="A64" s="48"/>
       <c r="B64" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -30646,7 +31284,7 @@
       </c>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.15">
-      <c r="A65" s="47"/>
+      <c r="A65" s="48"/>
       <c r="B65" s="22">
         <v>-1.1000000000000001</v>
       </c>
@@ -31070,7 +31708,7 @@
   <dimension ref="A1:BJ22"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -31117,70 +31755,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="47"/>
+      <c r="AQ1" s="47"/>
+      <c r="AR1" s="47"/>
+      <c r="AS1" s="47"/>
+      <c r="AT1" s="47"/>
+      <c r="AU1" s="47"/>
+      <c r="AV1" s="47"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -31190,22 +31828,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -31215,36 +31853,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="46" t="s">
+      <c r="Y2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="46" t="s">
+      <c r="AG2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="46"/>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="46"/>
-      <c r="AL2" s="46"/>
-      <c r="AM2" s="46"/>
-      <c r="AN2" s="46"/>
-      <c r="AO2" s="46"/>
-      <c r="AP2" s="46"/>
-      <c r="AQ2" s="46"/>
-      <c r="AR2" s="46"/>
-      <c r="AS2" s="46"/>
-      <c r="AT2" s="46"/>
-      <c r="AU2" s="46"/>
-      <c r="AV2" s="46"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">

</xml_diff>

<commit_message>
feat(stat), #21: Add `COUNTBLANK`, `LARGE`, `SMALL` functions.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE52709F-89D9-7C44-8F41-84696B23EDFA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59DCFEE-3E43-AB4E-AC67-C31CC64343D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="465">
   <si>
     <t>ca</t>
   </si>
@@ -1438,6 +1438,15 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>01/01/1900</t>
+  </si>
+  <si>
+    <t>1/01/1900</t>
   </si>
 </sst>
 </file>
@@ -1615,13 +1624,13 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -12993,7 +13002,7 @@
       </c>
     </row>
     <row r="5" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="45" t="s">
         <v>357</v>
       </c>
       <c r="B5" s="14">
@@ -13154,7 +13163,7 @@
       </c>
     </row>
     <row r="6" spans="1:48" ht="11" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="45" t="s">
         <v>358</v>
       </c>
       <c r="B6" s="14">
@@ -16973,7 +16982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BJ61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -17477,7 +17486,7 @@
         <f>IRR({-7,2,-1,4,-3;7,2,-1,4,#REF!})</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AF26" s="48">
+      <c r="AF26" s="47">
         <f t="array" ref="AF26">IRR({-7,2,-1,4,-3;7,2,-1,4,4},B54:D54)</f>
         <v>0.19086464188385843</v>
       </c>
@@ -17857,13 +17866,13 @@
       <c r="A34" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="Q34" s="50"/>
+      <c r="Q34" s="49"/>
     </row>
     <row r="35" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A35" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="H35" s="51"/>
+      <c r="H35" s="50"/>
     </row>
     <row r="36" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A36" s="16" t="s">
@@ -17960,14 +17969,14 @@
       <c r="A51" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="Q51" s="48"/>
+      <c r="Q51" s="47"/>
     </row>
     <row r="52" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A52" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="Q52" s="48"/>
-      <c r="R52" s="49"/>
+      <c r="Q52" s="47"/>
+      <c r="R52" s="48"/>
       <c r="AC52" s="4" t="e">
         <f>XNPV(AC54,$B$55:G$55,$B$54:G$54)</f>
         <v>#NUM!</v>
@@ -17978,7 +17987,7 @@
         <v>286</v>
       </c>
       <c r="Q53" s="42"/>
-      <c r="R53" s="49"/>
+      <c r="R53" s="48"/>
     </row>
     <row r="54" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A54" s="53" t="s">
@@ -18051,7 +18060,7 @@
         <f>XIRR($B$55:$F$55,$B$54:$F$54,H56)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="W54" s="47">
+      <c r="W54" s="46">
         <f>XIRR($B$55:$F$55,$B$54:$F$54,"26/08/1987")</f>
         <v>0.59931975404310833</v>
       </c>
@@ -18150,7 +18159,7 @@
         <v>0.59931974858045578</v>
       </c>
       <c r="T55" s="6">
-        <f t="shared" ref="T55:U55" si="3">XIRR($B$55:$F$55,$B$54:$F$54,D56)</f>
+        <f t="shared" ref="T55" si="3">XIRR($B$55:$F$55,$B$54:$F$54,D56)</f>
         <v>0.59931975585937503</v>
       </c>
       <c r="U55" s="6">
@@ -18417,7 +18426,7 @@
       <c r="A57" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="R57" s="50"/>
+      <c r="R57" s="49"/>
     </row>
     <row r="58" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A58" s="16" t="s">
@@ -20447,7 +20456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AV113"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -20467,12 +20476,11 @@
     <col min="13" max="14" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="2.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -20482,10 +20490,11 @@
     <col min="30" max="30" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="48" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="3.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="48" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="49" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
@@ -21504,10 +21513,166 @@
       </c>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="G23" s="45"/>
+      <c r="B23" s="14">
+        <v>0</v>
+      </c>
+      <c r="C23" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="D23" s="14">
+        <v>-2</v>
+      </c>
+      <c r="E23" s="14">
+        <v>-3</v>
+      </c>
+      <c r="F23" s="14">
+        <v>4</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" s="31" t="s">
+        <v>462</v>
+      </c>
+      <c r="I23" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K23" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L23" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M23" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N23" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O23" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P23" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q23" s="6">
+        <f>COUNTBLANK(B23:C23)</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="6">
+        <f t="shared" ref="R23:AE23" si="6">COUNTBLANK(C23:D23)</f>
+        <v>0</v>
+      </c>
+      <c r="S23" s="6">
+        <f>COUNTBLANK(B23)</f>
+        <v>0</v>
+      </c>
+      <c r="T23" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V23" s="6">
+        <f>COUNTBLANK(G23:H23)</f>
+        <v>2</v>
+      </c>
+      <c r="W23" s="6">
+        <f>COUNTBLANK(H23:I23)</f>
+        <v>1</v>
+      </c>
+      <c r="X23" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z23" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AA23" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AB23" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC23" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AD23" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AE23" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AF23" s="6">
+        <f>COUNTA(G23:I23)</f>
+        <v>2</v>
+      </c>
+      <c r="AG23" s="6">
+        <f t="array" ref="AG23:AL23">COUNTA(B23:I23)</f>
+        <v>7</v>
+      </c>
+      <c r="AH23" s="6">
+        <v>7</v>
+      </c>
+      <c r="AI23" s="6">
+        <v>7</v>
+      </c>
+      <c r="AJ23" s="6">
+        <v>7</v>
+      </c>
+      <c r="AK23" s="6">
+        <v>7</v>
+      </c>
+      <c r="AL23" s="6">
+        <v>7</v>
+      </c>
+      <c r="AM23" s="6">
+        <f t="array" ref="AM23:AV23">COUNTA(I23:P23)</f>
+        <v>8</v>
+      </c>
+      <c r="AN23" s="6">
+        <v>8</v>
+      </c>
+      <c r="AO23" s="6">
+        <v>8</v>
+      </c>
+      <c r="AP23" s="6">
+        <v>8</v>
+      </c>
+      <c r="AQ23" s="6">
+        <v>8</v>
+      </c>
+      <c r="AR23" s="6">
+        <v>8</v>
+      </c>
+      <c r="AS23" s="6">
+        <v>8</v>
+      </c>
+      <c r="AT23" s="6">
+        <v>8</v>
+      </c>
+      <c r="AU23" s="6">
+        <v>8</v>
+      </c>
+      <c r="AV23" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A24" s="17" t="s">
@@ -21589,31 +21754,31 @@
         <v>1</v>
       </c>
       <c r="Y24" s="6">
-        <f t="shared" ref="Y24:AE24" si="6">COUNTIF(H24:I24,H24)</f>
+        <f t="shared" ref="Y24:AE24" si="7">COUNTIF(H24:I24,H24)</f>
         <v>1</v>
       </c>
       <c r="Z24" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AA24" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AB24" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AC24" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AD24" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AE24" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AF24" s="11">
@@ -21824,10 +21989,181 @@
       <c r="A55" s="16" t="s">
         <v>151</v>
       </c>
+      <c r="AG55" s="51"/>
+      <c r="AH55" s="51"/>
+      <c r="AI55" s="51"/>
+      <c r="AJ55" s="51"/>
+      <c r="AK55" s="51"/>
+      <c r="AL55" s="13"/>
+      <c r="AM55" s="13"/>
+      <c r="AN55" s="13"/>
+      <c r="AO55" s="13"/>
+      <c r="AP55" s="13"/>
+      <c r="AQ55" s="9"/>
+      <c r="AR55" s="9"/>
+      <c r="AS55" s="9"/>
+      <c r="AT55" s="9"/>
+      <c r="AU55" s="9"/>
     </row>
     <row r="56" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="17" t="s">
         <v>152</v>
+      </c>
+      <c r="B56" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="C56" s="14">
+        <v>-10</v>
+      </c>
+      <c r="D56" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="E56" s="14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F56" s="14">
+        <v>-0.1</v>
+      </c>
+      <c r="G56" s="6"/>
+      <c r="H56" s="31" t="s">
+        <v>463</v>
+      </c>
+      <c r="I56" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J56" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K56" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L56" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M56" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N56" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O56" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P56" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q56" s="6">
+        <f>LARGE($B56:$I56,"1")</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R56" s="6">
+        <f>LARGE($B56:$I56,2)</f>
+        <v>0.9</v>
+      </c>
+      <c r="S56" s="6">
+        <f>LARGE($B56:$I56,3)</f>
+        <v>0.1</v>
+      </c>
+      <c r="T56" s="6">
+        <f>LARGE($B56:$I56,3)</f>
+        <v>0.1</v>
+      </c>
+      <c r="U56" s="6">
+        <f>LARGE($B56:$I56,4)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="V56" s="6" t="e">
+        <f>LARGE($B56:$I56,G56)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="W56" s="6" t="e">
+        <f>LARGE($B56:$I56,"c")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X56" s="6">
+        <f t="shared" ref="X56" si="8">LARGE($B56:$I56,I56)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Y56" s="6" t="e">
+        <f>LARGE($B56:$J56,J56)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z56" s="6" t="e">
+        <f t="shared" ref="Z56:AE56" si="9">LARGE($B56:$J56,K56)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA56" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB56" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC56" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD56" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE56" s="6" t="e">
+        <f t="shared" si="9"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF56" s="6" t="e">
+        <f t="array" ref="AF56">LARGE($B56:$I56,D56:E56)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AG56" s="6" t="e">
+        <f t="array" ref="AG56:AV56">LARGE($B56:$I56,B56:P56)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AH56" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AI56" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AJ56" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="AK56" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AL56" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AM56" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AN56" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AO56" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP56" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ56" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR56" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS56" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT56" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU56" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV56" s="4" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.15">
@@ -21934,27 +22270,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z61" s="6" t="e">
-        <f t="shared" ref="Z61:AE61" si="7">MAX(K61:L61)</f>
+        <f t="shared" ref="Z61:AE61" si="10">MAX(K61:L61)</f>
         <v>#N/A</v>
       </c>
       <c r="AA61" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB61" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>#NAME?</v>
       </c>
       <c r="AC61" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>#NULL!</v>
       </c>
       <c r="AD61" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>#NUM!</v>
       </c>
       <c r="AE61" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>#REF!</v>
       </c>
       <c r="AF61" s="6">
@@ -22104,19 +22440,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AB62" s="6" t="e">
-        <f t="shared" ref="AB62:AE62" si="8">MAXA(M62:N62)</f>
+        <f t="shared" ref="AB62:AE62" si="11">MAXA(M62:N62)</f>
         <v>#NAME?</v>
       </c>
       <c r="AC62" s="6" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>#NULL!</v>
       </c>
       <c r="AD62" s="6" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
       <c r="AE62" s="6" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>#REF!</v>
       </c>
       <c r="AF62" s="6">
@@ -22264,31 +22600,31 @@
         <v>0.1</v>
       </c>
       <c r="Y65" s="6" t="e">
-        <f t="shared" ref="Y65:AE65" si="9">MIN(J65:K65)</f>
+        <f t="shared" ref="Y65:AE65" si="12">MIN(J65:K65)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z65" s="6" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="AA65" s="6" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB65" s="6" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>#NAME?</v>
       </c>
       <c r="AC65" s="6" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>#NULL!</v>
       </c>
       <c r="AD65" s="6" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>#NUM!</v>
       </c>
       <c r="AE65" s="6" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>#REF!</v>
       </c>
       <c r="AF65" s="6">
@@ -22431,31 +22767,31 @@
         <v>1</v>
       </c>
       <c r="Y67" s="6" t="e">
-        <f t="shared" ref="Y67:AE67" si="10">MINA(J67:K67)</f>
+        <f t="shared" ref="Y67:AE67" si="13">MINA(J67:K67)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z67" s="6" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="AA67" s="6" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB67" s="6" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>#NAME?</v>
       </c>
       <c r="AC67" s="6" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>#NULL!</v>
       </c>
       <c r="AD67" s="6" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
       <c r="AE67" s="6" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>#REF!</v>
       </c>
       <c r="AF67" s="6">
@@ -22578,82 +22914,238 @@
         <v>174</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A81" s="16" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A82" s="16" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A83" s="16" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A84" s="16" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A85" s="16" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A86" s="16" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A87" s="16" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A88" s="16" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A89" s="16" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A90" s="16" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A91" s="16" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A92" s="16" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A93" s="16" t="s">
+    <row r="93" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="A93" s="17" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B93" s="14">
+        <v>0</v>
+      </c>
+      <c r="C93" s="14">
+        <v>-10</v>
+      </c>
+      <c r="D93" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="E93" s="14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F93" s="14">
+        <v>-0.1</v>
+      </c>
+      <c r="G93" s="6"/>
+      <c r="H93" s="31" t="s">
+        <v>464</v>
+      </c>
+      <c r="I93" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J93" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K93" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L93" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M93" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N93" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O93" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P93" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q93" s="6">
+        <f>SMALL($B93:$I93,"1")</f>
+        <v>-10</v>
+      </c>
+      <c r="R93" s="6">
+        <f>SMALL($B93:$I93,2)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="S93" s="6">
+        <f>SMALL($B93:$I93,3)</f>
+        <v>0</v>
+      </c>
+      <c r="T93" s="6">
+        <f>SMALL($B93:$I93,3)</f>
+        <v>0</v>
+      </c>
+      <c r="U93" s="6">
+        <f>SMALL($B93:$I93,4)</f>
+        <v>0.9</v>
+      </c>
+      <c r="V93" s="6" t="e">
+        <f>SMALL($B93:$I93,G93)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="W93" s="6" t="e">
+        <f>SMALL($B93:$I93,"c")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X93" s="6">
+        <f>SMALL($B93:$I93,I93)</f>
+        <v>-10</v>
+      </c>
+      <c r="Y93" s="6" t="e">
+        <f t="shared" ref="Y93:AE93" si="14">SMALL($B93:$J93,J93)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z93" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA93" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB93" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC93" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD93" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE93" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF93" s="6" t="e">
+        <f t="array" ref="AF93">SMALL($B93:$I93,D93:E93)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AG93" s="6" t="e">
+        <f t="array" ref="AG93:AV93">SMALL($B93:$I93,B93:P93)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AH93" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AI93" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AJ93" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="AK93" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AL93" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AM93" s="6">
+        <v>-10</v>
+      </c>
+      <c r="AN93" s="6">
+        <v>-10</v>
+      </c>
+      <c r="AO93" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP93" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ93" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR93" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS93" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT93" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU93" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV93" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="94" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A94" s="16" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A95" s="16" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A96" s="16" t="s">
         <v>190</v>
       </c>
@@ -32419,12 +32911,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -32436,6 +32922,12 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat(logic), #38: Add TRUE/FALSE functions.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD7E319-D15B-1A4C-B2D8-92E75F887FEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE0A08A-8127-9B43-81EF-F43C8120D4F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -32981,6 +32981,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -32992,12 +32998,6 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -33008,7 +33008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BJ22"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -33038,20 +33038,19 @@
     <col min="29" max="30" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="49" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
@@ -33345,6 +33344,60 @@
       </c>
       <c r="I4" s="6" t="b">
         <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="4" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AG4" s="4" t="b">
+        <f t="array" ref="AG4:AN4">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AH4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="4" t="b">
+        <f t="array" ref="AO4:AV4">FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="AP4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -34280,6 +34333,60 @@
       <c r="I12" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="V12" s="4" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AG12" s="4" t="b">
+        <f t="array" ref="AG12:AN12">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AH12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO12" s="4" t="b">
+        <f t="array" ref="AO12:AV12">TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="AP12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV12" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
@@ -34488,8 +34595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
test(logic, core), #39: Update test cases.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE0A08A-8127-9B43-81EF-F43C8120D4F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6C5B4B-E3B4-A942-8C48-8176F842EBAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="465">
   <si>
     <t>ca</t>
   </si>
@@ -18536,19 +18536,15 @@
     <col min="29" max="29" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="2.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="3.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="42" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="35" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="42" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="49" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
@@ -18830,59 +18826,328 @@
       <c r="BJ7" s="6"/>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="B8" s="14">
+        <v>0</v>
+      </c>
+      <c r="C8" s="14">
+        <v>2</v>
+      </c>
+      <c r="D8" s="14">
+        <v>3</v>
+      </c>
+      <c r="E8" s="14">
+        <v>10</v>
+      </c>
+      <c r="F8" s="14">
+        <v>-1</v>
+      </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="6"/>
-      <c r="AE8" s="6"/>
-      <c r="AF8" s="6"/>
-      <c r="AG8" s="6"/>
-      <c r="AH8" s="6"/>
-      <c r="AI8" s="6"/>
-      <c r="AJ8" s="6"/>
-      <c r="AK8" s="6"/>
-      <c r="AL8" s="6"/>
-      <c r="AM8" s="6"/>
-      <c r="AN8" s="6"/>
-      <c r="AO8" s="6"/>
-      <c r="AP8" s="6"/>
-      <c r="AQ8" s="6"/>
-      <c r="AR8" s="6"/>
-      <c r="AS8" s="6"/>
-      <c r="AT8" s="6"/>
-      <c r="AU8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K8" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L8" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N8" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O8" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P8" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q8" s="6" t="str">
+        <f>_xlfn.CONCAT(B8,C8,D8)</f>
+        <v>023</v>
+      </c>
+      <c r="R8" s="6" t="str">
+        <f t="shared" ref="R8:U8" si="0">_xlfn.CONCAT(C8,D8,E8)</f>
+        <v>2310</v>
+      </c>
+      <c r="S8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>310-1</v>
+      </c>
+      <c r="T8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>10-1</v>
+      </c>
+      <c r="U8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>-1ciao</v>
+      </c>
+      <c r="V8" s="6" t="str">
+        <f>_xlfn.CONCAT(G8,H8,I8)</f>
+        <v>ciaoTRUE</v>
+      </c>
+      <c r="W8" s="6" t="e">
+        <f t="shared" ref="W8" si="1">_xlfn.CONCAT(H8,I8,J8)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X8" s="6" t="e">
+        <f t="shared" ref="X8" si="2">_xlfn.CONCAT(I8,J8,K8)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y8" s="6" t="e">
+        <f t="shared" ref="Y8" si="3">_xlfn.CONCAT(J8,K8,L8)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z8" s="6" t="e">
+        <f t="shared" ref="Z8" si="4">_xlfn.CONCAT(K8,L8,M8)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA8" s="6" t="e">
+        <f t="shared" ref="AA8" si="5">_xlfn.CONCAT(L8,M8,N8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB8" s="6" t="e">
+        <f t="shared" ref="AB8" si="6">_xlfn.CONCAT(M8,N8,O8)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC8" s="6" t="e">
+        <f t="shared" ref="AC8" si="7">_xlfn.CONCAT(N8,O8,P8)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD8" s="6" t="e">
+        <f t="shared" ref="AD8" si="8">_xlfn.CONCAT(O8,P8,Q8)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE8" s="6" t="e">
+        <f t="shared" ref="AE8" si="9">_xlfn.CONCAT(P8,Q8,R8)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF8" s="6" t="str">
+        <f>_xlfn.CONCAT(B8:I8)</f>
+        <v>02310-1ciaoTRUE</v>
+      </c>
+      <c r="AG8" s="4" t="str">
+        <f t="array" ref="AG8:AJ8">_xlfn.CONCAT(B8:E8,C8:D8)</f>
+        <v>0231023</v>
+      </c>
+      <c r="AH8" s="6" t="str">
+        <v>0231023</v>
+      </c>
+      <c r="AI8" s="6" t="str">
+        <v>0231023</v>
+      </c>
+      <c r="AJ8" s="6" t="str">
+        <v>0231023</v>
+      </c>
+      <c r="AK8" s="6" t="e">
+        <f t="array" ref="AK8:AV8">_xlfn.CONCAT(L8:O8,I8:J8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL8" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM8" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AN8" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AO8" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AP8" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AQ8" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR8" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS8" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AT8" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AU8" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AV8" s="4" t="e">
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>298</v>
+      </c>
+      <c r="B9" s="14">
+        <v>0</v>
+      </c>
+      <c r="C9" s="14">
+        <v>2</v>
+      </c>
+      <c r="D9" s="14">
+        <v>3</v>
+      </c>
+      <c r="E9" s="14">
+        <v>10</v>
+      </c>
+      <c r="F9" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K9" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L9" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N9" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O9" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P9" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q9" s="6" t="str">
+        <f>CONCATENATE(B9,C9,D9)</f>
+        <v>023</v>
+      </c>
+      <c r="R9" s="6" t="str">
+        <f t="shared" ref="R9:X9" si="10">CONCATENATE(C9,D9,E9)</f>
+        <v>2310</v>
+      </c>
+      <c r="S9" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v>310-1</v>
+      </c>
+      <c r="T9" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v>10-1</v>
+      </c>
+      <c r="U9" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v>-1ciao</v>
+      </c>
+      <c r="V9" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v>ciaoTRUE</v>
+      </c>
+      <c r="W9" s="6" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X9" s="6" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y9" s="6" t="e">
+        <f t="shared" ref="Y9" si="11">CONCATENATE(J9,K9,L9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z9" s="6" t="e">
+        <f t="shared" ref="Z9" si="12">CONCATENATE(K9,L9,M9)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA9" s="6" t="e">
+        <f t="shared" ref="AA9" si="13">CONCATENATE(L9,M9,N9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB9" s="6" t="e">
+        <f t="shared" ref="AB9" si="14">CONCATENATE(M9,N9,O9)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC9" s="6" t="e">
+        <f t="shared" ref="AC9" si="15">CONCATENATE(N9,O9,P9)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD9" s="6" t="e">
+        <f t="shared" ref="AD9" si="16">CONCATENATE(O9,P9,Q9)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE9" s="6" t="e">
+        <f t="shared" ref="AE9" si="17">CONCATENATE(P9,Q9,R9)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF9" s="6" t="e">
+        <f>CONCATENATE(B9:I9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG9" s="4" t="str">
+        <f t="array" ref="AG9:AV9">CONCATENATE(B9:O9,C9:P9)</f>
+        <v>02</v>
+      </c>
+      <c r="AH9" s="4" t="str">
+        <v>23</v>
+      </c>
+      <c r="AI9" s="4" t="str">
+        <v>310</v>
+      </c>
+      <c r="AJ9" s="4" t="str">
+        <v>10-1</v>
+      </c>
+      <c r="AK9" s="4" t="str">
+        <v>-1</v>
+      </c>
+      <c r="AL9" s="4" t="str">
+        <v>ciao</v>
+      </c>
+      <c r="AM9" s="4" t="str">
+        <v>ciaoTRUE</v>
+      </c>
+      <c r="AN9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP9" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ9" s="4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR9" s="4" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS9" s="4" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT9" s="4" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU9" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AV9" s="4" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.15">
@@ -18977,35 +19242,35 @@
         <v>#VALUE!</v>
       </c>
       <c r="X13" s="4">
-        <f t="shared" ref="X13:AE13" si="0">FIND("ia","ciao",I13)</f>
+        <f t="shared" ref="X13:AE13" si="18">FIND("ia","ciao",I13)</f>
         <v>2</v>
       </c>
       <c r="Y13" s="4" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z13" s="4" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="AA13" s="4" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB13" s="4" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="18"/>
         <v>#NAME?</v>
       </c>
       <c r="AC13" s="4" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="18"/>
         <v>#NULL!</v>
       </c>
       <c r="AD13" s="4" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="18"/>
         <v>#NUM!</v>
       </c>
       <c r="AE13" s="4" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="18"/>
         <v>#REF!</v>
       </c>
       <c r="AF13" s="4">
@@ -19139,7 +19404,7 @@
         <v/>
       </c>
       <c r="R16" s="4" t="str">
-        <f t="shared" ref="R16:U16" si="1">LEFT("ciao",C16)</f>
+        <f t="shared" ref="R16:U16" si="19">LEFT("ciao",C16)</f>
         <v>c</v>
       </c>
       <c r="S16" s="4" t="str">
@@ -19147,11 +19412,11 @@
         <v>2.</v>
       </c>
       <c r="T16" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="19"/>
         <v>ciao</v>
       </c>
       <c r="U16" s="4" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="V16" s="4" t="str">
@@ -19167,31 +19432,31 @@
         <v>c</v>
       </c>
       <c r="Y16" s="4" t="e">
-        <f t="shared" ref="Y16:AE16" si="2">LEFT("ciao",J16)</f>
+        <f t="shared" ref="Y16:AE16" si="20">LEFT("ciao",J16)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z16" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="20"/>
         <v>#N/A</v>
       </c>
       <c r="AA16" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB16" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="20"/>
         <v>#NAME?</v>
       </c>
       <c r="AC16" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="20"/>
         <v>#NULL!</v>
       </c>
       <c r="AD16" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AE16" s="4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="20"/>
         <v>#REF!</v>
       </c>
       <c r="AF16" s="4" t="str">
@@ -19307,59 +19572,59 @@
         <v>1</v>
       </c>
       <c r="R18" s="4">
-        <f t="shared" ref="R18:AE18" si="3">LEN(C18)</f>
+        <f t="shared" ref="R18:AE18" si="21">LEN(C18)</f>
         <v>3</v>
       </c>
       <c r="S18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
       <c r="T18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="U18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="V18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="W18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
       <c r="X18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
       <c r="Y18" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z18" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="AA18" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB18" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>#NAME?</v>
       </c>
       <c r="AC18" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>#NULL!</v>
       </c>
       <c r="AD18" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>#NUM!</v>
       </c>
       <c r="AE18" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>#REF!</v>
       </c>
       <c r="AF18" s="4" t="e">
@@ -19474,59 +19739,59 @@
         <v>0</v>
       </c>
       <c r="R20" s="4" t="str">
-        <f t="shared" ref="R20:AE20" si="4">LOWER(C20)</f>
+        <f t="shared" ref="R20:AE20" si="22">LOWER(C20)</f>
         <v>1.9</v>
       </c>
       <c r="S20" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>2.3</v>
       </c>
       <c r="T20" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="U20" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>-1</v>
       </c>
       <c r="V20" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="W20" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>ciao</v>
       </c>
       <c r="X20" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>true</v>
       </c>
       <c r="Y20" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z20" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>#N/A</v>
       </c>
       <c r="AA20" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB20" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>#NAME?</v>
       </c>
       <c r="AC20" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>#NULL!</v>
       </c>
       <c r="AD20" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>#NUM!</v>
       </c>
       <c r="AE20" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>#REF!</v>
       </c>
       <c r="AF20" s="4" t="e">
@@ -19668,27 +19933,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z21" s="4" t="e">
-        <f t="shared" ref="Z21:AE21" si="5">MID("ciao",K21,2)</f>
+        <f t="shared" ref="Z21:AE21" si="23">MID("ciao",K21,2)</f>
         <v>#N/A</v>
       </c>
       <c r="AA21" s="4" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB21" s="4" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="23"/>
         <v>#NAME?</v>
       </c>
       <c r="AC21" s="4" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="23"/>
         <v>#NULL!</v>
       </c>
       <c r="AD21" s="4" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="23"/>
         <v>#NUM!</v>
       </c>
       <c r="AE21" s="4" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="23"/>
         <v>#REF!</v>
       </c>
       <c r="AF21" s="4" t="str">
@@ -19851,27 +20116,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z26" s="4" t="e">
-        <f t="shared" ref="Z26:AE26" si="6">REPLACE("ciao",K26,2,"vv")</f>
+        <f t="shared" ref="Z26:AE26" si="24">REPLACE("ciao",K26,2,"vv")</f>
         <v>#N/A</v>
       </c>
       <c r="AA26" s="4" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB26" s="4" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="24"/>
         <v>#NAME?</v>
       </c>
       <c r="AC26" s="4" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="24"/>
         <v>#NULL!</v>
       </c>
       <c r="AD26" s="4" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="24"/>
         <v>#NUM!</v>
       </c>
       <c r="AE26" s="4" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="24"/>
         <v>#REF!</v>
       </c>
       <c r="AF26" s="4" t="str">
@@ -20000,51 +20265,51 @@
         <v>3</v>
       </c>
       <c r="T29" s="4" t="str">
-        <f t="shared" ref="T29:AE29" si="7">RIGHT("ciao",E29)</f>
+        <f t="shared" ref="T29:AE29" si="25">RIGHT("ciao",E29)</f>
         <v>ciao</v>
       </c>
       <c r="U29" s="4" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>#VALUE!</v>
       </c>
       <c r="V29" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="W29" s="4" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>#VALUE!</v>
       </c>
       <c r="X29" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>o</v>
       </c>
       <c r="Y29" s="4" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z29" s="4" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>#N/A</v>
       </c>
       <c r="AA29" s="4" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB29" s="4" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>#NAME?</v>
       </c>
       <c r="AC29" s="4" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>#NULL!</v>
       </c>
       <c r="AD29" s="4" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>#NUM!</v>
       </c>
       <c r="AE29" s="4" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="25"/>
         <v>#REF!</v>
       </c>
       <c r="AF29" s="4" t="str">
@@ -20190,59 +20455,59 @@
         <v>0</v>
       </c>
       <c r="R37" s="4" t="str">
-        <f t="shared" ref="R37:AE37" si="8">TRIM(C37)</f>
+        <f t="shared" ref="R37:AE37" si="26">TRIM(C37)</f>
         <v>1.9</v>
       </c>
       <c r="S37" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="26"/>
         <v>2.3</v>
       </c>
       <c r="T37" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="U37" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="26"/>
         <v>-1</v>
       </c>
       <c r="V37" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="W37" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="26"/>
         <v>ciao</v>
       </c>
       <c r="X37" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="26"/>
         <v>TRUE</v>
       </c>
       <c r="Y37" s="4" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="26"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z37" s="4" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="26"/>
         <v>#N/A</v>
       </c>
       <c r="AA37" s="4" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB37" s="4" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="26"/>
         <v>#NAME?</v>
       </c>
       <c r="AC37" s="4" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="26"/>
         <v>#NULL!</v>
       </c>
       <c r="AD37" s="4" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
       <c r="AE37" s="4" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="26"/>
         <v>#REF!</v>
       </c>
       <c r="AF37" s="4" t="e">
@@ -20362,59 +20627,59 @@
         <v>0</v>
       </c>
       <c r="R40" s="4" t="str">
-        <f t="shared" ref="R40:AE40" si="9">UPPER(C40)</f>
+        <f t="shared" ref="R40:AE40" si="27">UPPER(C40)</f>
         <v>1.9</v>
       </c>
       <c r="S40" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>2.3</v>
       </c>
       <c r="T40" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>10</v>
       </c>
       <c r="U40" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>-1</v>
       </c>
       <c r="V40" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="W40" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>CIAO</v>
       </c>
       <c r="X40" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>TRUE</v>
       </c>
       <c r="Y40" s="4" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z40" s="4" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="AA40" s="4" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB40" s="4" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>#NAME?</v>
       </c>
       <c r="AC40" s="4" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>#NULL!</v>
       </c>
       <c r="AD40" s="4" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>#NUM!</v>
       </c>
       <c r="AE40" s="4" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>#REF!</v>
       </c>
       <c r="AF40" s="4" t="e">
@@ -32981,12 +33246,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -32998,6 +33257,12 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -33008,7 +33273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -34595,8 +34860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:T60"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35064,6 +35329,14 @@
         <f>ISERR(J16)</f>
         <v>0</v>
       </c>
+      <c r="N23" t="e">
+        <f ca="1">MYFUNCTION(M21)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O23" t="e">
+        <f ca="1">MYFUNCTION()</f>
+        <v>#NAME?</v>
+      </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="H24" t="e">

</xml_diff>

<commit_message>
fix(excel): Skip function compilation for string cells.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD18F2B-BE31-1E42-8B91-2C49C65755DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E93CBE-C26D-5744-98BC-E623267831D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
     <definedName name="NAMEDCELL123">"'ciao"</definedName>
     <definedName name="QF_SYS_LISTPRICECURRENCY">CORE!$F$12</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateCount="1" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="504">
   <si>
     <t>ca</t>
   </si>
@@ -1568,6 +1568,9 @@
   </si>
   <si>
     <t>ZTEST</t>
+  </si>
+  <si>
+    <t>=SUM(D2:D5)</t>
   </si>
 </sst>
 </file>
@@ -36275,6 +36278,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -36286,12 +36295,6 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -38377,6 +38380,13 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="D25" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="E25" t="e">
+        <f>REF!#REF!</f>
+        <v>#REF!</v>
+      </c>
       <c r="M25" s="56" t="str">
         <f>"Exchange(1 "&amp;NAMEDCELL123&amp;"=)"</f>
         <v>Exchange(1 'ciao=)</v>

</xml_diff>

<commit_message>
fix(excel): Correct invalid range definition and missing sheet or files.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E93CBE-C26D-5744-98BC-E623267831D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC36242D-A963-8141-B355-A0CC79039647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -29,6 +29,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <definedNames>
     <definedName name="a">CORE!$B$2:$C$3</definedName>
@@ -1842,6 +1843,19 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="MISSING"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2107,7 +2121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -37892,8 +37906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:T60"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38274,7 +38288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17">
         <f>[1]Sheet1!$A$1+1</f>
         <v>3</v>
@@ -38289,8 +38303,12 @@
       <c r="J17" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P17" t="e">
+        <f>[2]MISSING!A1</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B18">
         <f>[1]Sheet1!$A$1+[1]Sheet1!$A$2</f>
         <v>4</v>
@@ -38308,14 +38326,18 @@
         <f ca="1">IFERROR(INDIRECT("ab")+1, 33)</f>
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P18" t="e">
+        <f>A2:'[2]MISSING'!A2</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
       <c r="E19">
         <f>D16*3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
       <c r="H20">
         <f t="array" ref="H20:H24">IF(G9:G12&lt;&gt;H10:H13,1,0)</f>
         <v>0</v>
@@ -38324,7 +38346,7 @@
       <c r="N20" s="57"/>
       <c r="O20" s="57"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="F21">
         <f>C19+1</f>
         <v>1</v>
@@ -38341,7 +38363,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C22" s="43">
         <v>60</v>
       </c>
@@ -38353,7 +38375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="H23">
         <v>1</v>
       </c>
@@ -38370,7 +38392,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="H24" t="e">
         <v>#N/A</v>
       </c>
@@ -38379,7 +38401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D25" s="1" t="s">
         <v>503</v>
       </c>

</xml_diff>

<commit_message>
Links B17 & B18 of CORE sheet of test.xlsx had to be updated with absolute paths for testing to complete.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Widdershins\OneDrive\Documents\Python_Projects\formulas_check\formulas\test\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C724D7-CBF6-4C1B-AAF8-3DA8F1A297AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B892589C-C5B0-4776-ACC3-FD25A4F84BE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="45" windowWidth="24180" windowHeight="9098" tabRatio="770" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15945" tabRatio="770" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId14"/>
-    <externalReference r:id="rId15"/>
   </externalReferences>
   <definedNames>
     <definedName name="a">CORE!$B$2:$C$3</definedName>
@@ -1848,22 +1847,24 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
+      <sheetName val="test_link"/>
       <sheetName val="MISSING"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2135,7 +2136,7 @@
   <dimension ref="A1:AV81"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="10.5"/>
@@ -36332,7 +36333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
@@ -38034,8 +38035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:T60"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -38417,9 +38418,9 @@
       </c>
     </row>
     <row r="17" spans="2:16">
-      <c r="B17" t="e">
+      <c r="B17">
         <f>[1]Sheet1!$A$1+1</f>
-        <v>#REF!</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1"/>
       <c r="H17">
@@ -38431,15 +38432,15 @@
       <c r="J17" t="e">
         <v>#N/A</v>
       </c>
-      <c r="P17" t="e">
-        <f>[2]MISSING!A1</f>
-        <v>#REF!</v>
+      <c r="P17">
+        <f>[1]Sheet1!A1</f>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:16">
-      <c r="B18" t="e">
+      <c r="B18">
         <f>[1]Sheet1!$A$1+[1]Sheet1!$A$2</f>
-        <v>#REF!</v>
+        <v>4</v>
       </c>
       <c r="H18" t="e">
         <v>#N/A</v>
@@ -38455,7 +38456,7 @@
         <v>33</v>
       </c>
       <c r="P18" t="e">
-        <f>A2:'[2]MISSING'!A2</f>
+        <f>A2:'[1]Sheet1'!A2</f>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(parser), #61: Skip `\n` in formula expression.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC36242D-A963-8141-B355-A0CC79039647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D105DE2E-1275-9249-A92F-0CD926D778B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,12 +46,6 @@
   </definedNames>
   <calcPr calcId="191029" iterateCount="1" calcOnSave="0"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -36292,12 +36286,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -36309,6 +36297,12 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -37907,7 +37901,7 @@
   <dimension ref="B1:T60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38379,6 +38373,13 @@
       <c r="H23">
         <v>1</v>
       </c>
+      <c r="J23">
+        <f>IF(
+B2=1,
+1,
+2 )</f>
+        <v>1</v>
+      </c>
       <c r="L23" t="b">
         <f>ISERR(J16)</f>
         <v>0</v>

</xml_diff>

<commit_message>
fix(math), #59: Convert string to number in math operations.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D105DE2E-1275-9249-A92F-0CD926D778B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE5BCD1-0D04-EA47-ADB5-2BDEB35C2083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="11400" tabRatio="770" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="505">
   <si>
     <t>ca</t>
   </si>
@@ -1566,6 +1566,9 @@
   </si>
   <si>
     <t>=SUM(D2:D5)</t>
+  </si>
+  <si>
+    <t>= text</t>
   </si>
 </sst>
 </file>
@@ -1582,7 +1585,7 @@
     <numFmt numFmtId="170" formatCode="0.0000000000000000000000"/>
     <numFmt numFmtId="171" formatCode="&quot;€&quot;#,##0.00000;[Red]\-&quot;€&quot;#,##0.00000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1633,6 +1636,12 @@
       <sz val="9"/>
       <color indexed="0"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF24292E"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1704,7 +1713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1780,6 +1789,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2115,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV81"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A69" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="W71" sqref="W71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -2150,70 +2160,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -2223,22 +2233,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -2248,36 +2258,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="53" t="s">
+      <c r="AG2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="53"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="54"/>
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="54"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
@@ -6486,7 +6496,7 @@
         <v>1</v>
       </c>
       <c r="R32" s="6">
-        <f t="shared" ref="R32:AE32" si="35">FACTDOUBLE(C32)</f>
+        <f>FACTDOUBLE("2.3")</f>
         <v>2</v>
       </c>
       <c r="S32" s="6" t="e">
@@ -6510,7 +6520,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="X32" s="6" t="e">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="X32:AE32" si="35">FACTDOUBLE(I32)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Y32" s="6" t="e">
@@ -8509,7 +8519,7 @@
         <v>#REF!</v>
       </c>
       <c r="Q47" s="6">
-        <f>MROUND(B47,1.4)</f>
+        <f>MROUND(B47,"1.4")</f>
         <v>2.8</v>
       </c>
       <c r="R47" s="6">
@@ -12686,70 +12696,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="52" t="s">
         <v>38</v>
       </c>
@@ -12759,22 +12769,22 @@
       <c r="I2" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="52" t="s">
         <v>38</v>
       </c>
@@ -12784,36 +12794,36 @@
       <c r="X2" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
       <c r="AF2" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="53" t="s">
+      <c r="AG2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="53"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="54"/>
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="54"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="29" t="s">
@@ -14280,70 +14290,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
     </row>
     <row r="2" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="25" t="s">
         <v>38</v>
       </c>
@@ -14353,22 +14363,22 @@
       <c r="I2" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="25" t="s">
         <v>38</v>
       </c>
@@ -14378,36 +14388,36 @@
       <c r="X2" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
       <c r="AF2" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="53" t="s">
+      <c r="AG2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="53"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="54"/>
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="54"/>
     </row>
     <row r="3" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="27" t="s">
@@ -16890,70 +16900,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="26" t="s">
         <v>38</v>
       </c>
@@ -16963,22 +16973,22 @@
       <c r="I2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="26" t="s">
         <v>38</v>
       </c>
@@ -16988,36 +16998,36 @@
       <c r="X2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
       <c r="AF2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="53" t="s">
+      <c r="AG2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="53"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="54"/>
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="54"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -18746,70 +18756,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -18819,22 +18829,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -18844,36 +18854,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="53" t="s">
+      <c r="AG2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="53"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="54"/>
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="54"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -19113,7 +19123,7 @@
       </c>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="55" t="s">
         <v>260</v>
       </c>
       <c r="B26" s="4">
@@ -19244,7 +19254,7 @@
       </c>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A27" s="54"/>
+      <c r="A27" s="55"/>
       <c r="B27" s="14">
         <v>-0.1</v>
       </c>
@@ -19723,7 +19733,7 @@
       <c r="R53" s="48"/>
     </row>
     <row r="54" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A54" s="54" t="s">
+      <c r="A54" s="55" t="s">
         <v>287</v>
       </c>
       <c r="B54" s="4">
@@ -19835,7 +19845,7 @@
       </c>
     </row>
     <row r="55" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A55" s="54"/>
+      <c r="A55" s="55"/>
       <c r="B55" s="4">
         <v>-10</v>
       </c>
@@ -20242,70 +20252,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -20315,22 +20325,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -20340,36 +20350,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="53" t="s">
+      <c r="AG2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="53"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="54"/>
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="54"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -22495,70 +22505,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -22568,22 +22578,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -22593,36 +22603,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="53" t="s">
+      <c r="AG2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="53"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="54"/>
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="54"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -26649,70 +26659,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="32" t="s">
         <v>38</v>
       </c>
@@ -26722,22 +26732,22 @@
       <c r="I2" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="32" t="s">
         <v>38</v>
       </c>
@@ -26747,36 +26757,36 @@
       <c r="X2" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
       <c r="AF2" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="53" t="s">
+      <c r="AG2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="53"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="54"/>
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="54"/>
     </row>
     <row r="3" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
@@ -28763,70 +28773,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -28836,22 +28846,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -28861,36 +28871,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="53" t="s">
+      <c r="AG2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="53"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="54"/>
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="54"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -29455,70 +29465,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="19" t="s">
         <v>38</v>
       </c>
@@ -29528,22 +29538,22 @@
       <c r="I2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="19" t="s">
         <v>38</v>
       </c>
@@ -29553,36 +29563,36 @@
       <c r="X2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
       <c r="AF2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="53" t="s">
+      <c r="AG2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="53"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="54"/>
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="54"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -29600,7 +29610,7 @@
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="56" t="s">
         <v>334</v>
       </c>
       <c r="B6" s="21">
@@ -29766,7 +29776,7 @@
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A7" s="55"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
@@ -29896,7 +29906,7 @@
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A8" s="55"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
@@ -30148,7 +30158,7 @@
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="56" t="s">
         <v>338</v>
       </c>
       <c r="B12" s="21">
@@ -30306,7 +30316,7 @@
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A13" s="55"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="21">
         <v>-1.1000000000000001</v>
       </c>
@@ -30413,7 +30423,7 @@
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A14" s="55"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="21">
         <v>-1.1000000000000001</v>
       </c>
@@ -30525,7 +30535,7 @@
       </c>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="56" t="s">
         <v>340</v>
       </c>
       <c r="B16" s="21">
@@ -30684,7 +30694,7 @@
       </c>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A17" s="55"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="21">
         <v>-2</v>
       </c>
@@ -30800,7 +30810,7 @@
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A18" s="55"/>
+      <c r="A18" s="56"/>
       <c r="B18" s="21">
         <v>-2.9</v>
       </c>
@@ -30913,7 +30923,7 @@
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="56" t="s">
         <v>342</v>
       </c>
       <c r="B20" s="21">
@@ -31075,7 +31085,7 @@
       </c>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A21" s="55"/>
+      <c r="A21" s="56"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -31206,7 +31216,7 @@
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A22" s="55"/>
+      <c r="A22" s="56"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
@@ -31337,7 +31347,7 @@
       </c>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A23" s="55"/>
+      <c r="A23" s="56"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -31468,7 +31478,7 @@
       </c>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A24" s="55"/>
+      <c r="A24" s="56"/>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
@@ -31599,7 +31609,7 @@
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A25" s="55"/>
+      <c r="A25" s="56"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
@@ -31730,7 +31740,7 @@
       </c>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A26" s="55"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -31861,7 +31871,7 @@
       </c>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A27" s="55"/>
+      <c r="A27" s="56"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
       <c r="D27" s="21"/>
@@ -31992,7 +32002,7 @@
       </c>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A28" s="55"/>
+      <c r="A28" s="56"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -32122,7 +32132,7 @@
       </c>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="56" t="s">
         <v>352</v>
       </c>
       <c r="B29" s="21">
@@ -32247,7 +32257,7 @@
       <c r="AU29" s="6"/>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A30" s="55"/>
+      <c r="A30" s="56"/>
       <c r="B30" s="21">
         <v>-2</v>
       </c>
@@ -32356,7 +32366,7 @@
       <c r="AG30" s="6"/>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A31" s="55"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="21">
         <v>-2</v>
       </c>
@@ -32465,7 +32475,7 @@
       <c r="AG31" s="6"/>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A32" s="55"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="21">
         <v>-2</v>
       </c>
@@ -32574,7 +32584,7 @@
       <c r="AG32" s="6"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A33" s="55"/>
+      <c r="A33" s="56"/>
       <c r="B33" s="21">
         <v>-2</v>
       </c>
@@ -32683,7 +32693,7 @@
       <c r="AG33" s="6"/>
     </row>
     <row r="34" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A34" s="55"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="21">
         <v>-2</v>
       </c>
@@ -32792,7 +32802,7 @@
       <c r="AG34" s="6"/>
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A35" s="55"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="21">
         <v>-2</v>
       </c>
@@ -32901,7 +32911,7 @@
       <c r="AG35" s="6"/>
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A36" s="55"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="21">
         <v>-2</v>
       </c>
@@ -33010,7 +33020,7 @@
       <c r="AG36" s="6"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A37" s="55"/>
+      <c r="A37" s="56"/>
       <c r="B37" s="21">
         <v>-2</v>
       </c>
@@ -33119,7 +33129,7 @@
       <c r="AG37" s="6"/>
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A38" s="55" t="s">
+      <c r="A38" s="56" t="s">
         <v>351</v>
       </c>
       <c r="B38" s="21">
@@ -33244,7 +33254,7 @@
       <c r="AU38" s="6"/>
     </row>
     <row r="39" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A39" s="55"/>
+      <c r="A39" s="56"/>
       <c r="B39" s="21">
         <v>-2</v>
       </c>
@@ -33353,7 +33363,7 @@
       <c r="AG39" s="6"/>
     </row>
     <row r="40" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A40" s="55"/>
+      <c r="A40" s="56"/>
       <c r="B40" s="21">
         <v>-2</v>
       </c>
@@ -33462,7 +33472,7 @@
       <c r="AG40" s="6"/>
     </row>
     <row r="41" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A41" s="55"/>
+      <c r="A41" s="56"/>
       <c r="B41" s="21">
         <v>-2</v>
       </c>
@@ -33571,7 +33581,7 @@
       <c r="AG41" s="6"/>
     </row>
     <row r="42" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A42" s="55"/>
+      <c r="A42" s="56"/>
       <c r="B42" s="21">
         <v>-2</v>
       </c>
@@ -33680,7 +33690,7 @@
       <c r="AG42" s="6"/>
     </row>
     <row r="43" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A43" s="55"/>
+      <c r="A43" s="56"/>
       <c r="B43" s="21">
         <v>-2</v>
       </c>
@@ -33789,7 +33799,7 @@
       <c r="AG43" s="6"/>
     </row>
     <row r="44" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A44" s="55"/>
+      <c r="A44" s="56"/>
       <c r="B44" s="21">
         <v>-2</v>
       </c>
@@ -33898,7 +33908,7 @@
       <c r="AG44" s="6"/>
     </row>
     <row r="45" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A45" s="55"/>
+      <c r="A45" s="56"/>
       <c r="B45" s="21">
         <v>-2</v>
       </c>
@@ -34007,7 +34017,7 @@
       <c r="AG45" s="6"/>
     </row>
     <row r="46" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A46" s="55"/>
+      <c r="A46" s="56"/>
       <c r="B46" s="21">
         <v>-2</v>
       </c>
@@ -34116,7 +34126,7 @@
       <c r="AG46" s="6"/>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A47" s="55" t="s">
+      <c r="A47" s="56" t="s">
         <v>353</v>
       </c>
       <c r="B47" s="21">
@@ -34241,7 +34251,7 @@
       <c r="AU47" s="6"/>
     </row>
     <row r="48" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A48" s="55"/>
+      <c r="A48" s="56"/>
       <c r="B48" s="21">
         <v>-2</v>
       </c>
@@ -34350,7 +34360,7 @@
       <c r="AG48" s="6"/>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A49" s="55"/>
+      <c r="A49" s="56"/>
       <c r="B49" s="21">
         <v>-2</v>
       </c>
@@ -34459,7 +34469,7 @@
       <c r="AG49" s="6"/>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A50" s="55"/>
+      <c r="A50" s="56"/>
       <c r="B50" s="21">
         <v>-2</v>
       </c>
@@ -34568,7 +34578,7 @@
       <c r="AG50" s="6"/>
     </row>
     <row r="51" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A51" s="55"/>
+      <c r="A51" s="56"/>
       <c r="B51" s="21">
         <v>-2</v>
       </c>
@@ -34677,7 +34687,7 @@
       <c r="AG51" s="6"/>
     </row>
     <row r="52" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A52" s="55"/>
+      <c r="A52" s="56"/>
       <c r="B52" s="21">
         <v>-2</v>
       </c>
@@ -34786,7 +34796,7 @@
       <c r="AG52" s="6"/>
     </row>
     <row r="53" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A53" s="55"/>
+      <c r="A53" s="56"/>
       <c r="B53" s="21">
         <v>-2</v>
       </c>
@@ -34895,7 +34905,7 @@
       <c r="AG53" s="6"/>
     </row>
     <row r="54" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A54" s="55"/>
+      <c r="A54" s="56"/>
       <c r="B54" s="21">
         <v>-2</v>
       </c>
@@ -35004,7 +35014,7 @@
       <c r="AG54" s="6"/>
     </row>
     <row r="55" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A55" s="55"/>
+      <c r="A55" s="56"/>
       <c r="B55" s="21">
         <v>-2</v>
       </c>
@@ -35143,7 +35153,7 @@
       <c r="AE56" s="6"/>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A57" s="55" t="s">
+      <c r="A57" s="56" t="s">
         <v>344</v>
       </c>
       <c r="B57" s="21">
@@ -35309,7 +35319,7 @@
       </c>
     </row>
     <row r="58" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A58" s="55"/>
+      <c r="A58" s="56"/>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
       <c r="D58" s="21"/>
@@ -35439,7 +35449,7 @@
       </c>
     </row>
     <row r="59" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A59" s="55"/>
+      <c r="A59" s="56"/>
       <c r="B59" s="21"/>
       <c r="C59" s="21"/>
       <c r="D59" s="21"/>
@@ -35674,7 +35684,7 @@
       <c r="AE62" s="6"/>
     </row>
     <row r="63" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A63" s="55" t="s">
+      <c r="A63" s="56" t="s">
         <v>348</v>
       </c>
       <c r="B63" s="21">
@@ -35783,7 +35793,7 @@
       </c>
     </row>
     <row r="64" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A64" s="55"/>
+      <c r="A64" s="56"/>
       <c r="B64" s="21">
         <v>-1.1000000000000001</v>
       </c>
@@ -35890,7 +35900,7 @@
       </c>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.15">
-      <c r="A65" s="55"/>
+      <c r="A65" s="56"/>
       <c r="B65" s="21">
         <v>-1.1000000000000001</v>
       </c>
@@ -36286,6 +36296,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -36297,12 +36313,6 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -36360,70 +36370,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
-      <c r="AU1" s="53"/>
-      <c r="AV1" s="53"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="54"/>
+      <c r="AT1" s="54"/>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -36433,22 +36443,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -36458,36 +36468,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="53" t="s">
+      <c r="AG2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="53"/>
-      <c r="AS2" s="53"/>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="53"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="54"/>
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="54"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
@@ -37900,8 +37910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38234,6 +38244,18 @@
         <f>"ciao"&amp;B13&amp;" cc" &amp;C13</f>
         <v>ciao ccca</v>
       </c>
+      <c r="H14">
+        <f>SUM("2","4", Q8:Q9)</f>
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <f>SUM("2","4", TRUE)</f>
+        <v>7</v>
+      </c>
+      <c r="J14" t="e">
+        <f>SUM("2","4", "ciao")</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="K14">
         <f>IFERROR(K12,3)</f>
         <v>3</v>
@@ -38252,6 +38274,18 @@
       </c>
       <c r="C15" s="1">
         <v>0</v>
+      </c>
+      <c r="H15">
+        <f>SUM("2","4", H14)</f>
+        <v>12</v>
+      </c>
+      <c r="I15">
+        <f>SUM("2","4", E13)</f>
+        <v>6</v>
+      </c>
+      <c r="J15" t="e">
+        <f>SUM("2","4", "")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="K15">
         <f>IFERROR(K14,1)</f>
@@ -38336,11 +38370,11 @@
         <f t="array" ref="H20:H24">IF(G9:G12&lt;&gt;H10:H13,1,0)</f>
         <v>0</v>
       </c>
-      <c r="M20" s="57"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="57"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="M20" s="58"/>
+      <c r="N20" s="58"/>
+      <c r="O20" s="58"/>
+    </row>
+    <row r="21" spans="2:16" ht="18" x14ac:dyDescent="0.2">
       <c r="F21">
         <f>C19+1</f>
         <v>1</v>
@@ -38348,6 +38382,7 @@
       <c r="H21">
         <v>1</v>
       </c>
+      <c r="J21" s="53"/>
       <c r="L21" t="b">
         <f>ISERROR(J18)</f>
         <v>1</v>
@@ -38367,6 +38402,9 @@
       </c>
       <c r="H22">
         <v>0</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
@@ -38410,12 +38448,12 @@
         <f>REF!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="M25" s="56" t="str">
+      <c r="M25" s="57" t="str">
         <f>"Exchange(1 "&amp;NAMEDCELL123&amp;"=)"</f>
         <v>Exchange(1 'ciao=)</v>
       </c>
-      <c r="N25" s="56"/>
-      <c r="O25" s="56"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="57"/>
     </row>
     <row r="48" spans="20:20" ht="17" x14ac:dyDescent="0.25">
       <c r="T48" s="3"/>

</xml_diff>

<commit_message>
fix(text), #61: Convert float as int when stringify if it is an integer.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE5BCD1-0D04-EA47-ADB5-2BDEB35C2083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044D3181-586F-5C49-AF4E-E41C7A848A9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="11400" tabRatio="770" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36296,12 +36296,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -36313,6 +36307,12 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -37910,8 +37910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38205,6 +38205,10 @@
       <c r="H11">
         <v>9</v>
       </c>
+      <c r="M11" t="str">
+        <f>"\n" &amp; SUM(3,4)</f>
+        <v>\n7</v>
+      </c>
       <c r="R11" t="e">
         <f>SUM(H16:K18)</f>
         <v>#N/A</v>

</xml_diff>

<commit_message>
feat(core): Update range definition with path file.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044D3181-586F-5C49-AF4E-E41C7A848A9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0CCB60-184E-0D43-91F9-AE395E0E5405}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="11400" tabRatio="770" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="11400" tabRatio="770" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -1853,6 +1853,9 @@
     <sheetNames>
       <sheetName val="MISSING"/>
     </sheetNames>
+    <definedNames>
+      <definedName name="A"/>
+    </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
@@ -36296,6 +36299,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -36307,12 +36316,6 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -37910,8 +37913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38319,6 +38322,10 @@
       <c r="N16">
         <v>1</v>
       </c>
+      <c r="P16" t="e">
+        <f>[2]!A</f>
+        <v>#NAME?</v>
+      </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17">

</xml_diff>

<commit_message>
fix(excel), #48: Correct reference pointing to different workbooks.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E35009-026A-E848-9526-E66B5545C9E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427D70E7-CD4C-964A-AF8C-9C6B1479D305}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="13760" tabRatio="770" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="13760" tabRatio="770" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -41,6 +41,7 @@
     <definedName name="h">CORE!$K$4:$K$6 CORE!$J$5:$L$5</definedName>
     <definedName name="i">SUM(CORE!$M$4:$N$5,h)</definedName>
     <definedName name="l">h+i</definedName>
+    <definedName name="m">[2]Sheet1!$A$1</definedName>
     <definedName name="NAMEDCELL123">"'ciao"</definedName>
     <definedName name="QF_SYS_LISTPRICECURRENCY">CORE!$F$12</definedName>
   </definedNames>
@@ -36299,12 +36300,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -36316,6 +36311,12 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -36326,7 +36327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="AS8" sqref="AS8:AV8"/>
     </sheetView>
   </sheetViews>
@@ -38030,8 +38031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:T60"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38358,6 +38359,10 @@
         <f>"ciao"&amp;B13&amp;" cc" &amp;C13</f>
         <v>ciao ccca</v>
       </c>
+      <c r="O13">
+        <f>m</f>
+        <v>2</v>
+      </c>
       <c r="R13" t="e">
         <f>SUMPRODUCT(H16:J18)</f>
         <v>#N/A</v>

</xml_diff>

<commit_message>
feat(functions): Add `SEARCH`, `ISNUMBER`, and `EDATE` functions.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427D70E7-CD4C-964A-AF8C-9C6B1479D305}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A66A67F-E8BE-1348-93C1-59F1CFFA971E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="13760" tabRatio="770" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="13760" tabRatio="770" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -41,12 +41,19 @@
     <definedName name="h">CORE!$K$4:$K$6 CORE!$J$5:$L$5</definedName>
     <definedName name="i">SUM(CORE!$M$4:$N$5,h)</definedName>
     <definedName name="l">h+i</definedName>
-    <definedName name="m">[2]Sheet1!$A$1</definedName>
+    <definedName name="m">[1]Sheet1!$A$1</definedName>
     <definedName name="NAMEDCELL123">"'ciao"</definedName>
     <definedName name="QF_SYS_LISTPRICECURRENCY">CORE!$F$12</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateCount="1" calcOnSave="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -55,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="505">
   <si>
     <t>ca</t>
   </si>
@@ -1576,7 +1583,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;#,##0.00;[Red]\-&quot;€&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.00000000000000"/>
@@ -1585,6 +1592,7 @@
     <numFmt numFmtId="169" formatCode="0.0000000000000000000"/>
     <numFmt numFmtId="170" formatCode="0.0000000000000000000000"/>
     <numFmt numFmtId="171" formatCode="&quot;€&quot;#,##0.00000;[Red]\-&quot;€&quot;#,##0.00000"/>
+    <numFmt numFmtId="172" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1714,7 +1722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1791,6 +1799,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1828,22 +1839,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="MISSING"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="A"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
@@ -1859,6 +1854,22 @@
           </cell>
         </row>
       </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="MISSING"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="A"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2164,70 +2175,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -2237,22 +2248,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -2262,36 +2273,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
@@ -12700,70 +12711,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="52" t="s">
         <v>38</v>
       </c>
@@ -12773,22 +12784,22 @@
       <c r="I2" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="52" t="s">
         <v>38</v>
       </c>
@@ -12798,36 +12809,36 @@
       <c r="X2" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="29" t="s">
@@ -14294,70 +14305,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="25" t="s">
         <v>38</v>
       </c>
@@ -14367,22 +14378,22 @@
       <c r="I2" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="25" t="s">
         <v>38</v>
       </c>
@@ -14392,36 +14403,36 @@
       <c r="X2" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="27" t="s">
@@ -16904,70 +16915,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="26" t="s">
         <v>38</v>
       </c>
@@ -16977,22 +16988,22 @@
       <c r="I2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="26" t="s">
         <v>38</v>
       </c>
@@ -17002,36 +17013,36 @@
       <c r="X2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -18760,70 +18771,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -18833,22 +18844,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -18858,36 +18869,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -19127,7 +19138,7 @@
       </c>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="58" t="s">
         <v>260</v>
       </c>
       <c r="B26" s="4">
@@ -19258,7 +19269,7 @@
       </c>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A27" s="55"/>
+      <c r="A27" s="58"/>
       <c r="B27" s="14">
         <v>-0.1</v>
       </c>
@@ -19737,7 +19748,7 @@
       <c r="R53" s="48"/>
     </row>
     <row r="54" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A54" s="55" t="s">
+      <c r="A54" s="58" t="s">
         <v>287</v>
       </c>
       <c r="B54" s="4">
@@ -19849,7 +19860,7 @@
       </c>
     </row>
     <row r="55" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A55" s="55"/>
+      <c r="A55" s="58"/>
       <c r="B55" s="4">
         <v>-10</v>
       </c>
@@ -20212,7 +20223,7 @@
   <dimension ref="A1:BJ41"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:AV41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -20256,70 +20267,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -20329,22 +20340,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -20354,36 +20365,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -22080,8 +22091,167 @@
       </c>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="17" t="s">
         <v>320</v>
+      </c>
+      <c r="B31" s="14">
+        <v>0</v>
+      </c>
+      <c r="C31" s="14">
+        <v>1.9</v>
+      </c>
+      <c r="D31" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E31" s="14">
+        <v>10</v>
+      </c>
+      <c r="F31" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I31" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K31" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L31" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M31" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N31" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O31" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P31" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q31" s="4" t="e">
+        <f>SEARCH("BASE","database",B31)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R31" s="4">
+        <f t="shared" ref="R31:Z31" si="26">SEARCH("BASE","database",C31)</f>
+        <v>5</v>
+      </c>
+      <c r="S31" s="4">
+        <f t="shared" si="26"/>
+        <v>5</v>
+      </c>
+      <c r="T31" s="4" t="e">
+        <f>SEARCH("BASE","database",E31)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U31" s="4" t="e">
+        <f>SEARCH("BASE","database",F31)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V31" s="4" t="e">
+        <f>SEARCH("BASE","database",G31)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W31" s="4" t="e">
+        <f>SEARCH("BASE","database",H31)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X31" s="4">
+        <f t="shared" si="26"/>
+        <v>5</v>
+      </c>
+      <c r="Y31" s="4" t="e">
+        <f t="shared" si="26"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z31" s="4" t="e">
+        <f t="shared" si="26"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA31" s="4" t="e">
+        <f t="shared" ref="AA31" si="27">SEARCH("BASE","database",L31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB31" s="4" t="e">
+        <f t="shared" ref="AB31" si="28">SEARCH("BASE","database",M31)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC31" s="4" t="e">
+        <f t="shared" ref="AC31" si="29">SEARCH("BASE","database",N31)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD31" s="4" t="e">
+        <f t="shared" ref="AD31" si="30">SEARCH("BASE","database",O31)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE31" s="4" t="e">
+        <f>SEARCH("BASE","database",P31)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF31" s="4">
+        <f>SEARCH({"BASE","bau"},"database")</f>
+        <v>5</v>
+      </c>
+      <c r="AG31" s="4">
+        <f t="array" ref="AG31:AI31">SEARCH({"BASE","bau"},"database")</f>
+        <v>5</v>
+      </c>
+      <c r="AH31" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI31" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ31" s="4" t="e">
+        <f t="array" ref="AJ31:AL31">SEARCH({"bau","BASE"},"database",B31:C31)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AK31" s="4">
+        <v>5</v>
+      </c>
+      <c r="AL31" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AM31" s="4" t="e">
+        <f t="array" ref="AM31:AV31">SEARCH({"bau","BASE",3},"database",B31:D31)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN31" s="4">
+        <v>5</v>
+      </c>
+      <c r="AO31" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP31" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ31" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AR31" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AS31" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AT31" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AU31" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AV31" s="4" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.15">
@@ -22162,59 +22332,59 @@
         <v>0</v>
       </c>
       <c r="R37" s="4" t="str">
-        <f t="shared" ref="R37:AE37" si="26">TRIM(C37)</f>
+        <f t="shared" ref="R37:AE37" si="31">TRIM(C37)</f>
         <v>1.9</v>
       </c>
       <c r="S37" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>2.3</v>
       </c>
       <c r="T37" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>10</v>
       </c>
       <c r="U37" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>-1</v>
       </c>
       <c r="V37" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="W37" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>ciao</v>
       </c>
       <c r="X37" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>TRUE</v>
       </c>
       <c r="Y37" s="4" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z37" s="4" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#N/A</v>
       </c>
       <c r="AA37" s="4" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB37" s="4" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#NAME?</v>
       </c>
       <c r="AC37" s="4" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#NULL!</v>
       </c>
       <c r="AD37" s="4" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#NUM!</v>
       </c>
       <c r="AE37" s="4" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#REF!</v>
       </c>
       <c r="AF37" s="4" t="e">
@@ -22334,59 +22504,59 @@
         <v>0</v>
       </c>
       <c r="R40" s="4" t="str">
-        <f t="shared" ref="R40:AE40" si="27">UPPER(C40)</f>
+        <f t="shared" ref="R40:AE40" si="32">UPPER(C40)</f>
         <v>1.9</v>
       </c>
       <c r="S40" s="4" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>2.3</v>
       </c>
       <c r="T40" s="4" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>10</v>
       </c>
       <c r="U40" s="4" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>-1</v>
       </c>
       <c r="V40" s="4" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="W40" s="4" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>CIAO</v>
       </c>
       <c r="X40" s="4" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>TRUE</v>
       </c>
       <c r="Y40" s="4" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z40" s="4" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>#N/A</v>
       </c>
       <c r="AA40" s="4" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB40" s="4" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>#NAME?</v>
       </c>
       <c r="AC40" s="4" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>#NULL!</v>
       </c>
       <c r="AD40" s="4" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>#NUM!</v>
       </c>
       <c r="AE40" s="4" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>#REF!</v>
       </c>
       <c r="AF40" s="4" t="e">
@@ -22509,70 +22679,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -22582,22 +22752,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -22607,36 +22777,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -26613,32 +26783,32 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7D9E77-BF90-2E45-87C2-E9C169025282}">
-  <dimension ref="A1:AV34"/>
+  <dimension ref="A1:AV106"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:AV27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.5" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -26663,70 +26833,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="32" t="s">
         <v>38</v>
       </c>
@@ -26736,22 +26906,22 @@
       <c r="I2" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="32" t="s">
         <v>38</v>
       </c>
@@ -26761,36 +26931,36 @@
       <c r="X2" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
@@ -26961,7 +27131,7 @@
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="33"/>
       <c r="F4" s="33"/>
       <c r="G4" s="11"/>
@@ -27345,14 +27515,174 @@
       <c r="Q8" s="14"/>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>435</v>
+      </c>
+      <c r="B9" s="33">
+        <v>1987</v>
+      </c>
+      <c r="C9" s="33">
+        <v>8</v>
+      </c>
+      <c r="D9" s="33">
+        <v>1</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0.7</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="38" t="s">
+        <v>459</v>
+      </c>
+      <c r="I9" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="11" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K9" s="11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L9" s="34" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="34" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N9" s="34" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O9" s="34" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P9" s="34" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q9" s="4">
+        <f>EDATE(B9,C9)</f>
+        <v>2232</v>
+      </c>
+      <c r="R9" s="4">
+        <f>EDATE(C9,"2")</f>
+        <v>68</v>
+      </c>
+      <c r="S9" s="4">
+        <f>EDATE(D9,".55")</f>
+        <v>1</v>
+      </c>
+      <c r="T9" s="4" t="e">
+        <f>EDATE(I9,F9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U9" s="4">
+        <f>EDATE(F9,G9)</f>
+        <v>0</v>
+      </c>
+      <c r="V9" s="4">
+        <f>EDATE(E9,H9)</f>
+        <v>974437</v>
+      </c>
+      <c r="W9" s="4">
+        <f>EDATE(H9,G9)</f>
+        <v>32015</v>
+      </c>
+      <c r="X9" s="4" t="e">
+        <f>EDATE(H9,I9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y9" s="4" t="e">
+        <f t="shared" ref="Y9:AE9" si="3">EDATE(J9,K9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z9" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA9" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB9" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC9" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD9" s="4" t="e">
+        <f>EDATE(O9,P9)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE9" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF9" s="4" t="e">
+        <f t="array" ref="AF9">EDATE(H9,B9:F9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG9" s="4" t="e">
+        <f t="array" ref="AG9:AV9">EDATE(D9:H9,B9:F9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AH9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AJ9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AK9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AU9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AV9" s="4" t="e">
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>436</v>
       </c>
+      <c r="R10" s="14">
+        <f>EDATE(1, "2")</f>
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
@@ -27405,11 +27735,11 @@
         <v>10</v>
       </c>
       <c r="R11" s="4" t="e">
-        <f t="shared" ref="R11:AE11" si="3">HOUR(C11)</f>
+        <f t="shared" ref="R11:AE11" si="4">HOUR(C11)</f>
         <v>#NUM!</v>
       </c>
       <c r="S11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="T11" s="4">
@@ -27417,47 +27747,47 @@
         <v>9</v>
       </c>
       <c r="U11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="X11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Y11" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z11" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="AA11" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB11" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
       <c r="AC11" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#NULL!</v>
       </c>
       <c r="AD11" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
       <c r="AE11" s="4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
       <c r="AF11" s="4">
@@ -27570,11 +27900,11 @@
         <v>33</v>
       </c>
       <c r="R13" s="4" t="e">
-        <f t="shared" ref="R13:AE13" si="4">MINUTE(C13)</f>
+        <f t="shared" ref="R13:AE13" si="5">MINUTE(C13)</f>
         <v>#NUM!</v>
       </c>
       <c r="S13" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>55</v>
       </c>
       <c r="T13" s="4">
@@ -27582,47 +27912,47 @@
         <v>36</v>
       </c>
       <c r="U13" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V13" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W13" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X13" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y13" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z13" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="AA13" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB13" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#NAME?</v>
       </c>
       <c r="AC13" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#NULL!</v>
       </c>
       <c r="AD13" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AE13" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
       <c r="AF13" s="4">
@@ -27731,11 +28061,11 @@
         <v>6</v>
       </c>
       <c r="R14" s="11">
-        <f t="shared" ref="R14:AE14" si="5">MONTH(C14)</f>
+        <f t="shared" ref="R14:AE14" si="6">MONTH(C14)</f>
         <v>1</v>
       </c>
       <c r="S14" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="T14" s="11">
@@ -27743,47 +28073,47 @@
         <v>1</v>
       </c>
       <c r="U14" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="V14" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="W14" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="X14" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Y14" s="11" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z14" s="11" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="AA14" s="11" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB14" s="11" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#NAME?</v>
       </c>
       <c r="AC14" s="11" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#NULL!</v>
       </c>
       <c r="AD14" s="11" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
       <c r="AE14" s="11" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
       <c r="AF14" s="11">
@@ -27911,59 +28241,59 @@
         <v>36</v>
       </c>
       <c r="R18" s="4" t="e">
-        <f t="shared" ref="R18:AE18" si="6">SECOND(C18)</f>
+        <f t="shared" ref="R18:AE18" si="7">SECOND(C18)</f>
         <v>#NUM!</v>
       </c>
       <c r="S18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="T18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="X18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y18" s="4" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z18" s="4" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="AA18" s="4" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB18" s="4" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#NAME?</v>
       </c>
       <c r="AC18" s="4" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#NULL!</v>
       </c>
       <c r="AD18" s="4" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#NUM!</v>
       </c>
       <c r="AE18" s="4" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
       <c r="AF18" s="4">
@@ -28088,31 +28418,31 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="V19" s="11">
-        <f t="shared" ref="V19:AB19" si="7">TIME(B19,C19,G19)</f>
+        <f t="shared" ref="V19:AB19" si="8">TIME(B19,C19,G19)</f>
         <v>0.29097222222230812</v>
       </c>
       <c r="W19" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.555555555555554E-3</v>
       </c>
       <c r="X19" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.79167824074074078</v>
       </c>
       <c r="Y19" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z19" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="AA19" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB19" s="11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#NAME?</v>
       </c>
       <c r="AC19" s="11" t="e">
@@ -28235,23 +28565,23 @@
         <v>#VALUE!</v>
       </c>
       <c r="R20" s="11" t="e">
-        <f t="shared" ref="R20:AE20" si="8">TIMEVALUE(C20)</f>
+        <f t="shared" ref="R20:AE20" si="9">TIMEVALUE(C20)</f>
         <v>#VALUE!</v>
       </c>
       <c r="S20" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="T20" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="U20" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="V20" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="W20" s="11">
@@ -28263,31 +28593,31 @@
         <v>#VALUE!</v>
       </c>
       <c r="Y20" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z20" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#N/A</v>
       </c>
       <c r="AA20" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB20" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#NAME?</v>
       </c>
       <c r="AC20" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#NULL!</v>
       </c>
       <c r="AD20" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#NUM!</v>
       </c>
       <c r="AE20" s="11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
       <c r="AF20" s="11">
@@ -28426,59 +28756,59 @@
         <v>1905</v>
       </c>
       <c r="R26" s="11">
-        <f t="shared" ref="R26:AE26" si="9">YEAR(C26)</f>
+        <f t="shared" ref="R26:AE26" si="10">YEAR(C26)</f>
         <v>1900</v>
       </c>
       <c r="S26" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1900</v>
       </c>
       <c r="T26" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1900</v>
       </c>
       <c r="U26" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1900</v>
       </c>
       <c r="V26" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1900</v>
       </c>
       <c r="W26" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1901</v>
       </c>
       <c r="X26" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1900</v>
       </c>
       <c r="Y26" s="11" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z26" s="11" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
       <c r="AA26" s="11" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB26" s="11" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>#NAME?</v>
       </c>
       <c r="AC26" s="11" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>#NULL!</v>
       </c>
       <c r="AD26" s="11" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>#NUM!</v>
       </c>
       <c r="AE26" s="11" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>#REF!</v>
       </c>
       <c r="AF26" s="11">
@@ -28586,7 +28916,7 @@
         <v>4.4965769055225921</v>
       </c>
       <c r="R27" s="4">
-        <f t="shared" ref="R27" si="10">YEARFRAC(C27,345,D27)</f>
+        <f t="shared" ref="R27" si="11">YEARFRAC(C27,345,D27)</f>
         <v>0.9555555555555556</v>
       </c>
       <c r="S27" s="4">
@@ -28622,19 +28952,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AA27" s="4" t="e">
-        <f t="shared" ref="AA27" si="11">YEARFRAC(L27,345,M27)</f>
+        <f t="shared" ref="AA27" si="12">YEARFRAC(L27,345,M27)</f>
         <v>#NAME?</v>
       </c>
       <c r="AB27" s="4" t="e">
-        <f t="shared" ref="AB27:AC27" si="12">YEARFRAC(M27,345,N27)</f>
+        <f t="shared" ref="AB27:AC27" si="13">YEARFRAC(M27,345,N27)</f>
         <v>#NULL!</v>
       </c>
       <c r="AC27" s="4" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
       <c r="AD27" s="4" t="e">
-        <f t="shared" ref="AD27" si="13">YEARFRAC(O27,345,P27)</f>
+        <f t="shared" ref="AD27" si="14">YEARFRAC(O27,345,P27)</f>
         <v>#REF!</v>
       </c>
       <c r="AE27" s="4" t="e">
@@ -28704,20 +29034,241 @@
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A30" s="16"/>
-      <c r="B30" s="42"/>
+      <c r="B30" s="37"/>
+      <c r="K30" s="55"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="54"/>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A31" s="16"/>
-      <c r="B31" s="41"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="36"/>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="B32" s="41"/>
+      <c r="B32" s="37"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B33" s="41"/>
+      <c r="B33" s="37"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B34" s="41"/>
+      <c r="B34" s="37"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B35" s="37"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B36" s="37"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B37" s="37"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B38" s="37"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B39" s="37"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B40" s="37"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B41" s="37"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B42" s="37"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B43" s="37"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B44" s="37"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B45" s="37"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B46" s="37"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B47" s="37"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B48" s="37"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B49" s="37"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B50" s="37"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B51" s="37"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B52" s="37"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B53" s="37"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B54" s="37"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B55" s="37"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B56" s="37"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B57" s="37"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B58" s="37"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B59" s="37"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B60" s="37"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B61" s="37"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B62" s="37"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B63" s="37"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B64" s="37"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B65" s="37"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B66" s="37"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B67" s="37"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B68" s="37"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B69" s="37"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B70" s="37"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B71" s="37"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B72" s="37"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B73" s="37"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B74" s="37"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B75" s="37"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B76" s="37"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B77" s="37"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B78" s="37"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B79" s="37"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B80" s="37"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B81" s="37"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B82" s="37"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B83" s="37"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B84" s="37"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B85" s="37"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B86" s="37"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B87" s="37"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B88" s="37"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B89" s="37"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B90" s="37"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B91" s="37"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B92" s="37"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B93" s="37"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B94" s="37"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B95" s="37"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B96" s="37"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B97" s="37"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B98" s="37"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B99" s="37"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B100" s="37"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B101" s="37"/>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B102" s="37"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B103" s="37"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B104" s="37"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B105" s="37"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B106" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -28739,8 +29290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AV22"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:AV22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -28768,79 +29319,79 @@
     <col min="26" max="26" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="27" max="31" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="40" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="47" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="40" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="47" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="49" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -28850,22 +29401,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -28875,36 +29426,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -29038,68 +29589,53 @@
         <v>1</v>
       </c>
       <c r="AG7" s="6" t="b">
-        <f t="shared" ref="AG7:AV7" si="1">ISERR(B7:P7)</f>
-        <v>1</v>
+        <f t="array" ref="AG7:AV7">ISERR(B7:P7)</f>
+        <v>0</v>
       </c>
       <c r="AH7" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI7" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ7" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL7" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM7" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN7" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO7" s="6" t="b">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AP7" s="6" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ7" s="6" t="b">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AR7" s="6" t="b">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AS7" s="6" t="b">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AT7" s="6" t="b">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AU7" s="6" t="b">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AV7" s="4" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.15">
@@ -29150,63 +29686,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q8" s="6" t="b">
-        <f t="shared" ref="Q8:AE8" si="2">ISERROR(B8)</f>
+        <f t="shared" ref="Q8:AE8" si="1">ISERROR(B8)</f>
         <v>0</v>
       </c>
       <c r="R8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Z8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AA8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AB8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AD8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AE8" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AF8" s="6" t="b">
@@ -29214,67 +29750,52 @@
         <v>1</v>
       </c>
       <c r="AG8" s="6" t="b">
-        <f t="shared" ref="AG8:AV8" si="3">ISERROR(B8:P8)</f>
-        <v>1</v>
+        <f t="array" ref="AG8:AV8">ISERROR(B8:P8)</f>
+        <v>0</v>
       </c>
       <c r="AH8" s="6" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI8" s="6" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ8" s="6" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK8" s="6" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL8" s="6" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM8" s="6" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN8" s="6" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO8" s="6" t="b">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AP8" s="6" t="b">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AQ8" s="6" t="b">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AR8" s="6" t="b">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AS8" s="6" t="b">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AT8" s="6" t="b">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AU8" s="6" t="b">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AV8" s="4" t="b">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -29304,8 +29825,164 @@
       </c>
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>217</v>
+      </c>
+      <c r="B14" s="14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E14" s="14">
+        <v>10</v>
+      </c>
+      <c r="F14" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K14" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L14" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M14" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N14" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O14" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P14" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q14" s="4" t="b">
+        <f>ISNUMBER(B14)</f>
+        <v>1</v>
+      </c>
+      <c r="R14" s="4" t="b">
+        <f t="shared" ref="R14:AE14" si="2">ISNUMBER(C14)</f>
+        <v>1</v>
+      </c>
+      <c r="S14" s="4" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T14" s="4" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U14" s="4" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V14" s="4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W14" s="4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X14" s="4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AD14" s="4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AE14" s="4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AF14" s="4" t="b">
+        <f>ISNUMBER(B14:P14)</f>
+        <v>0</v>
+      </c>
+      <c r="AG14" s="4" t="b">
+        <f t="array" ref="AG14:AV14">ISNUMBER(B14:O14)</f>
+        <v>1</v>
+      </c>
+      <c r="AH14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.15">
@@ -29421,7 +30098,7 @@
   <dimension ref="A1:BJ74"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:AV65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -29469,70 +30146,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="19" t="s">
         <v>38</v>
       </c>
@@ -29542,22 +30219,22 @@
       <c r="I2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="19" t="s">
         <v>38</v>
       </c>
@@ -29567,36 +30244,36 @@
       <c r="X2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -29614,7 +30291,7 @@
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="59" t="s">
         <v>334</v>
       </c>
       <c r="B6" s="21">
@@ -29780,7 +30457,7 @@
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A7" s="56"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
@@ -29910,7 +30587,7 @@
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A8" s="56"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
@@ -30162,7 +30839,7 @@
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="59" t="s">
         <v>338</v>
       </c>
       <c r="B12" s="21">
@@ -30320,7 +30997,7 @@
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A13" s="56"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="21">
         <v>-1.1000000000000001</v>
       </c>
@@ -30427,7 +31104,7 @@
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A14" s="56"/>
+      <c r="A14" s="59"/>
       <c r="B14" s="21">
         <v>-1.1000000000000001</v>
       </c>
@@ -30539,7 +31216,7 @@
       </c>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="59" t="s">
         <v>340</v>
       </c>
       <c r="B16" s="21">
@@ -30698,7 +31375,7 @@
       </c>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A17" s="56"/>
+      <c r="A17" s="59"/>
       <c r="B17" s="21">
         <v>-2</v>
       </c>
@@ -30814,7 +31491,7 @@
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A18" s="56"/>
+      <c r="A18" s="59"/>
       <c r="B18" s="21">
         <v>-2.9</v>
       </c>
@@ -30927,7 +31604,7 @@
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="59" t="s">
         <v>342</v>
       </c>
       <c r="B20" s="21">
@@ -31089,7 +31766,7 @@
       </c>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A21" s="56"/>
+      <c r="A21" s="59"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -31220,7 +31897,7 @@
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A22" s="56"/>
+      <c r="A22" s="59"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
@@ -31351,7 +32028,7 @@
       </c>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A23" s="56"/>
+      <c r="A23" s="59"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -31482,7 +32159,7 @@
       </c>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A24" s="56"/>
+      <c r="A24" s="59"/>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
@@ -31613,7 +32290,7 @@
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A25" s="56"/>
+      <c r="A25" s="59"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
@@ -31744,7 +32421,7 @@
       </c>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A26" s="56"/>
+      <c r="A26" s="59"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -31875,7 +32552,7 @@
       </c>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A27" s="56"/>
+      <c r="A27" s="59"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
       <c r="D27" s="21"/>
@@ -32006,7 +32683,7 @@
       </c>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A28" s="56"/>
+      <c r="A28" s="59"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -32136,7 +32813,7 @@
       </c>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="59" t="s">
         <v>352</v>
       </c>
       <c r="B29" s="21">
@@ -32261,7 +32938,7 @@
       <c r="AU29" s="6"/>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A30" s="56"/>
+      <c r="A30" s="59"/>
       <c r="B30" s="21">
         <v>-2</v>
       </c>
@@ -32370,7 +33047,7 @@
       <c r="AG30" s="6"/>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A31" s="56"/>
+      <c r="A31" s="59"/>
       <c r="B31" s="21">
         <v>-2</v>
       </c>
@@ -32479,7 +33156,7 @@
       <c r="AG31" s="6"/>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A32" s="56"/>
+      <c r="A32" s="59"/>
       <c r="B32" s="21">
         <v>-2</v>
       </c>
@@ -32588,7 +33265,7 @@
       <c r="AG32" s="6"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A33" s="56"/>
+      <c r="A33" s="59"/>
       <c r="B33" s="21">
         <v>-2</v>
       </c>
@@ -32697,7 +33374,7 @@
       <c r="AG33" s="6"/>
     </row>
     <row r="34" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A34" s="56"/>
+      <c r="A34" s="59"/>
       <c r="B34" s="21">
         <v>-2</v>
       </c>
@@ -32806,7 +33483,7 @@
       <c r="AG34" s="6"/>
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A35" s="56"/>
+      <c r="A35" s="59"/>
       <c r="B35" s="21">
         <v>-2</v>
       </c>
@@ -32915,7 +33592,7 @@
       <c r="AG35" s="6"/>
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A36" s="56"/>
+      <c r="A36" s="59"/>
       <c r="B36" s="21">
         <v>-2</v>
       </c>
@@ -33024,7 +33701,7 @@
       <c r="AG36" s="6"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A37" s="56"/>
+      <c r="A37" s="59"/>
       <c r="B37" s="21">
         <v>-2</v>
       </c>
@@ -33133,7 +33810,7 @@
       <c r="AG37" s="6"/>
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A38" s="56" t="s">
+      <c r="A38" s="59" t="s">
         <v>351</v>
       </c>
       <c r="B38" s="21">
@@ -33258,7 +33935,7 @@
       <c r="AU38" s="6"/>
     </row>
     <row r="39" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A39" s="56"/>
+      <c r="A39" s="59"/>
       <c r="B39" s="21">
         <v>-2</v>
       </c>
@@ -33367,7 +34044,7 @@
       <c r="AG39" s="6"/>
     </row>
     <row r="40" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A40" s="56"/>
+      <c r="A40" s="59"/>
       <c r="B40" s="21">
         <v>-2</v>
       </c>
@@ -33476,7 +34153,7 @@
       <c r="AG40" s="6"/>
     </row>
     <row r="41" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A41" s="56"/>
+      <c r="A41" s="59"/>
       <c r="B41" s="21">
         <v>-2</v>
       </c>
@@ -33585,7 +34262,7 @@
       <c r="AG41" s="6"/>
     </row>
     <row r="42" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A42" s="56"/>
+      <c r="A42" s="59"/>
       <c r="B42" s="21">
         <v>-2</v>
       </c>
@@ -33694,7 +34371,7 @@
       <c r="AG42" s="6"/>
     </row>
     <row r="43" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A43" s="56"/>
+      <c r="A43" s="59"/>
       <c r="B43" s="21">
         <v>-2</v>
       </c>
@@ -33803,7 +34480,7 @@
       <c r="AG43" s="6"/>
     </row>
     <row r="44" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A44" s="56"/>
+      <c r="A44" s="59"/>
       <c r="B44" s="21">
         <v>-2</v>
       </c>
@@ -33912,7 +34589,7 @@
       <c r="AG44" s="6"/>
     </row>
     <row r="45" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A45" s="56"/>
+      <c r="A45" s="59"/>
       <c r="B45" s="21">
         <v>-2</v>
       </c>
@@ -34021,7 +34698,7 @@
       <c r="AG45" s="6"/>
     </row>
     <row r="46" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A46" s="56"/>
+      <c r="A46" s="59"/>
       <c r="B46" s="21">
         <v>-2</v>
       </c>
@@ -34130,7 +34807,7 @@
       <c r="AG46" s="6"/>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A47" s="56" t="s">
+      <c r="A47" s="59" t="s">
         <v>353</v>
       </c>
       <c r="B47" s="21">
@@ -34255,7 +34932,7 @@
       <c r="AU47" s="6"/>
     </row>
     <row r="48" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A48" s="56"/>
+      <c r="A48" s="59"/>
       <c r="B48" s="21">
         <v>-2</v>
       </c>
@@ -34364,7 +35041,7 @@
       <c r="AG48" s="6"/>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A49" s="56"/>
+      <c r="A49" s="59"/>
       <c r="B49" s="21">
         <v>-2</v>
       </c>
@@ -34473,7 +35150,7 @@
       <c r="AG49" s="6"/>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A50" s="56"/>
+      <c r="A50" s="59"/>
       <c r="B50" s="21">
         <v>-2</v>
       </c>
@@ -34582,7 +35259,7 @@
       <c r="AG50" s="6"/>
     </row>
     <row r="51" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A51" s="56"/>
+      <c r="A51" s="59"/>
       <c r="B51" s="21">
         <v>-2</v>
       </c>
@@ -34691,7 +35368,7 @@
       <c r="AG51" s="6"/>
     </row>
     <row r="52" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A52" s="56"/>
+      <c r="A52" s="59"/>
       <c r="B52" s="21">
         <v>-2</v>
       </c>
@@ -34800,7 +35477,7 @@
       <c r="AG52" s="6"/>
     </row>
     <row r="53" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A53" s="56"/>
+      <c r="A53" s="59"/>
       <c r="B53" s="21">
         <v>-2</v>
       </c>
@@ -34909,7 +35586,7 @@
       <c r="AG53" s="6"/>
     </row>
     <row r="54" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A54" s="56"/>
+      <c r="A54" s="59"/>
       <c r="B54" s="21">
         <v>-2</v>
       </c>
@@ -35018,7 +35695,7 @@
       <c r="AG54" s="6"/>
     </row>
     <row r="55" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A55" s="56"/>
+      <c r="A55" s="59"/>
       <c r="B55" s="21">
         <v>-2</v>
       </c>
@@ -35157,7 +35834,7 @@
       <c r="AE56" s="6"/>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A57" s="56" t="s">
+      <c r="A57" s="59" t="s">
         <v>344</v>
       </c>
       <c r="B57" s="21">
@@ -35323,7 +36000,7 @@
       </c>
     </row>
     <row r="58" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A58" s="56"/>
+      <c r="A58" s="59"/>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
       <c r="D58" s="21"/>
@@ -35453,7 +36130,7 @@
       </c>
     </row>
     <row r="59" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A59" s="56"/>
+      <c r="A59" s="59"/>
       <c r="B59" s="21"/>
       <c r="C59" s="21"/>
       <c r="D59" s="21"/>
@@ -35688,7 +36365,7 @@
       <c r="AE62" s="6"/>
     </row>
     <row r="63" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A63" s="56" t="s">
+      <c r="A63" s="59" t="s">
         <v>348</v>
       </c>
       <c r="B63" s="21">
@@ -35797,7 +36474,7 @@
       </c>
     </row>
     <row r="64" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A64" s="56"/>
+      <c r="A64" s="59"/>
       <c r="B64" s="21">
         <v>-1.1000000000000001</v>
       </c>
@@ -35904,7 +36581,7 @@
       </c>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.15">
-      <c r="A65" s="56"/>
+      <c r="A65" s="59"/>
       <c r="B65" s="21">
         <v>-1.1000000000000001</v>
       </c>
@@ -36300,6 +36977,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -36311,12 +36994,6 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -36375,70 +37052,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -36448,22 +37125,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -36473,36 +37150,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="54" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
@@ -38031,7 +38708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="E7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
@@ -38445,13 +39122,13 @@
         <v>1</v>
       </c>
       <c r="P16" t="e">
-        <f>[1]!A</f>
+        <f>[2]!A</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17">
-        <f>[2]Sheet1!$A$1+1</f>
+        <f>[1]Sheet1!$A$1+1</f>
         <v>3</v>
       </c>
       <c r="C17" s="1"/>
@@ -38465,13 +39142,13 @@
         <v>#N/A</v>
       </c>
       <c r="P17" t="e">
-        <f>[1]MISSING!A1</f>
+        <f>[2]MISSING!A1</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B18">
-        <f>[2]Sheet1!$A$1+[2]Sheet1!$A$2</f>
+        <f>[1]Sheet1!$A$1+[1]Sheet1!$A$2</f>
         <v>4</v>
       </c>
       <c r="H18" t="e">
@@ -38488,7 +39165,7 @@
         <v>33</v>
       </c>
       <c r="P18" t="e">
-        <f>A2:'[1]MISSING'!A2</f>
+        <f>A2:'[2]MISSING'!A2</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -38503,9 +39180,9 @@
         <f t="array" ref="H20:H24">IF(G9:G12&lt;&gt;H10:H13,1,0)</f>
         <v>0</v>
       </c>
-      <c r="M20" s="58"/>
-      <c r="N20" s="58"/>
-      <c r="O20" s="58"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="61"/>
     </row>
     <row r="21" spans="2:16" ht="18" x14ac:dyDescent="0.2">
       <c r="F21">
@@ -38581,12 +39258,12 @@
         <f>REF!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="M25" s="57" t="str">
+      <c r="M25" s="60" t="str">
         <f>"Exchange(1 "&amp;NAMEDCELL123&amp;"=)"</f>
         <v>Exchange(1 'ciao=)</v>
       </c>
-      <c r="N25" s="57"/>
-      <c r="O25" s="57"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="60"/>
     </row>
     <row r="48" spans="20:20" ht="17" x14ac:dyDescent="0.25">
       <c r="T48" s="3"/>

</xml_diff>

<commit_message>
feat(look), #87: Add `ADDRESS` function.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896DA910-0919-8145-9475-4438E6BD02B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173A5E89-9319-C445-A7AB-B5D00AC12900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19200" tabRatio="770" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="505">
   <si>
     <t>ca</t>
   </si>
@@ -1584,9 +1584,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="172" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="174" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1731,14 +1731,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1755,10 +1755,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1771,16 +1771,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1794,9 +1794,23 @@
     <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="174" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1808,20 +1822,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2180,70 +2180,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="51"/>
-      <c r="AR1" s="51"/>
-      <c r="AS1" s="51"/>
-      <c r="AT1" s="51"/>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -2253,22 +2253,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -2278,36 +2278,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="51" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="51" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="51"/>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
@@ -12828,70 +12828,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="51"/>
-      <c r="AR1" s="51"/>
-      <c r="AS1" s="51"/>
-      <c r="AT1" s="51"/>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="44" t="s">
         <v>38</v>
       </c>
@@ -12901,22 +12901,22 @@
       <c r="I2" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="44" t="s">
         <v>38</v>
       </c>
@@ -12926,36 +12926,36 @@
       <c r="X2" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="51" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="51" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="51"/>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="28" t="s">
@@ -14425,70 +14425,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="51"/>
-      <c r="AR1" s="51"/>
-      <c r="AS1" s="51"/>
-      <c r="AT1" s="51"/>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="24" t="s">
         <v>38</v>
       </c>
@@ -14498,22 +14498,22 @@
       <c r="I2" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="24" t="s">
         <v>38</v>
       </c>
@@ -14523,36 +14523,36 @@
       <c r="X2" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="51" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="51" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="51"/>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="26" t="s">
@@ -17035,70 +17035,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="51"/>
-      <c r="AR1" s="51"/>
-      <c r="AS1" s="51"/>
-      <c r="AT1" s="51"/>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="25" t="s">
         <v>38</v>
       </c>
@@ -17108,22 +17108,22 @@
       <c r="I2" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="25" t="s">
         <v>38</v>
       </c>
@@ -17133,36 +17133,36 @@
       <c r="X2" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="51" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="51" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="51"/>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -18860,7 +18860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AV59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection activeCell="AG32" sqref="AG32:AV32"/>
     </sheetView>
   </sheetViews>
@@ -18896,208 +18896,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
-      <c r="AI1" s="55"/>
-      <c r="AJ1" s="55"/>
-      <c r="AK1" s="55"/>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="55"/>
-      <c r="AN1" s="55"/>
-      <c r="AO1" s="55"/>
-      <c r="AP1" s="55"/>
-      <c r="AQ1" s="55"/>
-      <c r="AR1" s="55"/>
-      <c r="AS1" s="55"/>
-      <c r="AT1" s="55"/>
-      <c r="AU1" s="55"/>
-      <c r="AV1" s="55"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="59"/>
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59"/>
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="59"/>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="59"/>
+      <c r="AK1" s="59"/>
+      <c r="AL1" s="59"/>
+      <c r="AM1" s="59"/>
+      <c r="AN1" s="59"/>
+      <c r="AO1" s="59"/>
+      <c r="AP1" s="59"/>
+      <c r="AQ1" s="59"/>
+      <c r="AR1" s="59"/>
+      <c r="AS1" s="59"/>
+      <c r="AT1" s="59"/>
+      <c r="AU1" s="59"/>
+      <c r="AV1" s="59"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55" t="s">
+      <c r="A2" s="59"/>
+      <c r="B2" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="56" t="s">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="56" t="s">
+      <c r="I2" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="56" t="s">
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="56" t="s">
+      <c r="W2" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="56" t="s">
+      <c r="X2" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="55" t="s">
+      <c r="Y2" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="55"/>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="55"/>
-      <c r="AD2" s="55"/>
-      <c r="AE2" s="55"/>
-      <c r="AF2" s="56" t="s">
+      <c r="Z2" s="59"/>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="59"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="59"/>
+      <c r="AF2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="55" t="s">
+      <c r="AG2" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="55"/>
-      <c r="AI2" s="55"/>
-      <c r="AJ2" s="55"/>
-      <c r="AK2" s="55"/>
-      <c r="AL2" s="55"/>
-      <c r="AM2" s="55"/>
-      <c r="AN2" s="55"/>
-      <c r="AO2" s="55"/>
-      <c r="AP2" s="55"/>
-      <c r="AQ2" s="55"/>
-      <c r="AR2" s="55"/>
-      <c r="AS2" s="55"/>
-      <c r="AT2" s="55"/>
-      <c r="AU2" s="55"/>
-      <c r="AV2" s="55"/>
+      <c r="AH2" s="59"/>
+      <c r="AI2" s="59"/>
+      <c r="AJ2" s="59"/>
+      <c r="AK2" s="59"/>
+      <c r="AL2" s="59"/>
+      <c r="AM2" s="59"/>
+      <c r="AN2" s="59"/>
+      <c r="AO2" s="59"/>
+      <c r="AP2" s="59"/>
+      <c r="AQ2" s="59"/>
+      <c r="AR2" s="59"/>
+      <c r="AS2" s="59"/>
+      <c r="AT2" s="59"/>
+      <c r="AU2" s="59"/>
+      <c r="AV2" s="59"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="52" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="52" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="52" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="52" t="s">
         <v>240</v>
       </c>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="53"/>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="52" t="s">
         <v>241</v>
       </c>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58"/>
-      <c r="AQ7" s="58"/>
-      <c r="AR7" s="58"/>
-      <c r="AS7" s="58"/>
-      <c r="AT7" s="58"/>
-      <c r="AU7" s="58"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="53"/>
+      <c r="AQ7" s="53"/>
+      <c r="AR7" s="53"/>
+      <c r="AS7" s="53"/>
+      <c r="AT7" s="53"/>
+      <c r="AU7" s="53"/>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="52" t="s">
         <v>242</v>
       </c>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="58"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="53"/>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="52" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="52" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="52" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:48" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="52" t="s">
         <v>246</v>
       </c>
-      <c r="R12" s="59"/>
+      <c r="R12" s="54"/>
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="55" t="s">
         <v>247</v>
       </c>
       <c r="B13" s="14">
@@ -19128,19 +19128,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L13" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M13" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N13" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O13" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P13" s="58" t="e">
+      <c r="L13" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N13" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O13" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P13" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q13" s="14">
@@ -19258,54 +19258,54 @@
       </c>
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="52" t="s">
         <v>248</v>
       </c>
-      <c r="Q14" s="61"/>
+      <c r="Q14" s="56"/>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="52" t="s">
         <v>249</v>
       </c>
-      <c r="Q15" s="61"/>
+      <c r="Q15" s="56"/>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="52" t="s">
         <v>250</v>
       </c>
-      <c r="Q16" s="61"/>
+      <c r="Q16" s="56"/>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="52" t="s">
         <v>251</v>
       </c>
-      <c r="Q17" s="61"/>
+      <c r="Q17" s="56"/>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="52" t="s">
         <v>252</v>
       </c>
-      <c r="Q18" s="61"/>
+      <c r="Q18" s="56"/>
     </row>
     <row r="19" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="52" t="s">
         <v>253</v>
       </c>
-      <c r="Q19" s="61"/>
+      <c r="Q19" s="56"/>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="52" t="s">
         <v>254</v>
       </c>
-      <c r="Q20" s="61"/>
+      <c r="Q20" s="56"/>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="52" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A22" s="60" t="s">
+      <c r="A22" s="55" t="s">
         <v>256</v>
       </c>
       <c r="B22" s="14">
@@ -19336,19 +19336,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L22" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M22" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N22" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O22" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P22" s="58" t="e">
+      <c r="L22" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M22" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N22" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O22" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P22" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q22" s="14">
@@ -19356,7 +19356,7 @@
         <v>2.1871014779833633</v>
       </c>
       <c r="R22" s="14">
-        <f t="shared" ref="R22:AE22" si="1">FV(C22, -D22, E22)</f>
+        <f t="shared" ref="R22:AD22" si="1">FV(C22, -D22, E22)</f>
         <v>0.66666585715621407</v>
       </c>
       <c r="S22" s="14">
@@ -19466,18 +19466,18 @@
       </c>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="52" t="s">
         <v>257</v>
       </c>
-      <c r="Q23" s="61"/>
+      <c r="Q23" s="56"/>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A24" s="57" t="s">
+      <c r="A24" s="52" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A25" s="60" t="s">
+      <c r="A25" s="55" t="s">
         <v>259</v>
       </c>
       <c r="B25" s="14">
@@ -19508,19 +19508,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L25" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M25" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N25" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O25" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P25" s="58" t="e">
+      <c r="L25" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M25" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N25" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O25" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P25" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q25" s="14">
@@ -19638,7 +19638,7 @@
       </c>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A26" s="62" t="s">
+      <c r="A26" s="58" t="s">
         <v>260</v>
       </c>
       <c r="B26" s="14">
@@ -19669,19 +19669,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L26" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M26" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N26" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O26" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P26" s="58" t="e">
+      <c r="L26" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M26" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N26" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O26" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P26" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q26" s="14" t="e">
@@ -19799,7 +19799,7 @@
       </c>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A27" s="62"/>
+      <c r="A27" s="58"/>
       <c r="B27" s="14">
         <v>-0.1</v>
       </c>
@@ -19828,19 +19828,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L27" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M27" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N27" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O27" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P27" s="58" t="e">
+      <c r="L27" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M27" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N27" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O27" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P27" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q27" s="14">
@@ -19958,27 +19958,27 @@
       </c>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="52" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A29" s="57" t="s">
+      <c r="A29" s="52" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A30" s="57" t="s">
+      <c r="A30" s="52" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A31" s="57" t="s">
+      <c r="A31" s="52" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A32" s="60" t="s">
+      <c r="A32" s="55" t="s">
         <v>265</v>
       </c>
       <c r="B32" s="14">
@@ -20009,19 +20009,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L32" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M32" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N32" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O32" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P32" s="58" t="e">
+      <c r="L32" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M32" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N32" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O32" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P32" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q32" s="14">
@@ -20041,7 +20041,7 @@
         <v>40.019613898255479</v>
       </c>
       <c r="U32" s="14" t="e">
-        <f t="shared" ref="R32:AE32" si="4">NPER(F32/12,G32,H32,10000,1)</f>
+        <f t="shared" ref="U32:AE32" si="4">NPER(F32/12,G32,H32,10000,1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="V32" s="14" t="e">
@@ -20139,7 +20139,7 @@
       </c>
     </row>
     <row r="33" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A33" s="60" t="s">
+      <c r="A33" s="55" t="s">
         <v>266</v>
       </c>
       <c r="B33" s="14">
@@ -20170,19 +20170,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L33" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M33" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N33" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O33" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P33" s="58" t="e">
+      <c r="L33" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M33" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N33" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O33" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P33" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q33" s="14">
@@ -20300,32 +20300,32 @@
       </c>
     </row>
     <row r="34" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A34" s="57" t="s">
+      <c r="A34" s="52" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="35" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="52" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="36" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="52" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="37" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A37" s="57" t="s">
+      <c r="A37" s="52" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="38" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="52" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="39" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A39" s="60" t="s">
+      <c r="A39" s="55" t="s">
         <v>272</v>
       </c>
       <c r="B39" s="14">
@@ -20356,19 +20356,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L39" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M39" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N39" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O39" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P39" s="58" t="e">
+      <c r="L39" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M39" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N39" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O39" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P39" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q39" s="14">
@@ -20486,7 +20486,7 @@
       </c>
     </row>
     <row r="40" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A40" s="60" t="s">
+      <c r="A40" s="55" t="s">
         <v>273</v>
       </c>
       <c r="B40" s="14">
@@ -20517,19 +20517,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L40" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M40" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N40" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O40" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P40" s="58" t="e">
+      <c r="L40" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M40" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N40" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O40" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P40" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q40" s="14">
@@ -20647,22 +20647,22 @@
       </c>
     </row>
     <row r="41" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A41" s="57" t="s">
+      <c r="A41" s="52" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="42" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A42" s="57" t="s">
+      <c r="A42" s="52" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="43" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A43" s="57" t="s">
+      <c r="A43" s="52" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="44" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A44" s="60" t="s">
+      <c r="A44" s="55" t="s">
         <v>277</v>
       </c>
       <c r="B44" s="14">
@@ -20693,19 +20693,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L44" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M44" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N44" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O44" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P44" s="58" t="e">
+      <c r="L44" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M44" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N44" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O44" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P44" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q44" s="14">
@@ -20823,7 +20823,7 @@
       </c>
     </row>
     <row r="45" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A45" s="60" t="s">
+      <c r="A45" s="55" t="s">
         <v>278</v>
       </c>
       <c r="B45" s="14">
@@ -20854,19 +20854,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L45" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M45" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N45" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O45" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P45" s="58" t="e">
+      <c r="L45" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M45" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N45" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O45" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P45" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q45" s="14" t="e">
@@ -20984,47 +20984,47 @@
       </c>
     </row>
     <row r="46" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="52" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="47" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A47" s="57" t="s">
+      <c r="A47" s="52" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="48" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A48" s="57" t="s">
+      <c r="A48" s="52" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A49" s="57" t="s">
+      <c r="A49" s="52" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A50" s="57" t="s">
+      <c r="A50" s="52" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="51" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A51" s="57" t="s">
+      <c r="A51" s="52" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="52" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A52" s="57" t="s">
+      <c r="A52" s="52" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="53" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A53" s="57" t="s">
+      <c r="A53" s="52" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="54" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A54" s="62" t="s">
+      <c r="A54" s="58" t="s">
         <v>287</v>
       </c>
       <c r="B54" s="14">
@@ -21039,7 +21039,7 @@
       <c r="E54" s="14">
         <v>4</v>
       </c>
-      <c r="F54" s="61">
+      <c r="F54" s="56">
         <v>9</v>
       </c>
       <c r="H54" s="14">
@@ -21055,19 +21055,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L54" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M54" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N54" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O54" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P54" s="58" t="e">
+      <c r="L54" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M54" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N54" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O54" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P54" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q54" s="14">
@@ -21185,7 +21185,7 @@
       </c>
     </row>
     <row r="55" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A55" s="62"/>
+      <c r="A55" s="58"/>
       <c r="B55" s="14">
         <v>-10</v>
       </c>
@@ -21201,7 +21201,7 @@
       <c r="F55" s="14">
         <v>4.5</v>
       </c>
-      <c r="H55" s="61" t="s">
+      <c r="H55" s="56" t="s">
         <v>461</v>
       </c>
       <c r="I55" s="14" t="b">
@@ -21214,19 +21214,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L55" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M55" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N55" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O55" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P55" s="58" t="e">
+      <c r="L55" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M55" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N55" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O55" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P55" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q55" s="14" t="e">
@@ -21344,7 +21344,7 @@
       </c>
     </row>
     <row r="56" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A56" s="60" t="s">
+      <c r="A56" s="55" t="s">
         <v>288</v>
       </c>
       <c r="B56" s="14">
@@ -21375,19 +21375,19 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L56" s="58" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M56" s="58" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N56" s="58" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O56" s="58" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P56" s="58" t="e">
+      <c r="L56" s="53" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M56" s="53" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N56" s="53" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O56" s="53" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P56" s="53" t="e">
         <v>#REF!</v>
       </c>
       <c r="Q56" s="14">
@@ -21505,17 +21505,17 @@
       </c>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A57" s="57" t="s">
+      <c r="A57" s="52" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="58" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A58" s="57" t="s">
+      <c r="A58" s="52" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="59" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A59" s="57" t="s">
+      <c r="A59" s="52" t="s">
         <v>291</v>
       </c>
     </row>
@@ -21587,70 +21587,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="51"/>
-      <c r="AR1" s="51"/>
-      <c r="AS1" s="51"/>
-      <c r="AT1" s="51"/>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -21660,22 +21660,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -21685,36 +21685,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="51" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="51" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="51"/>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -23994,70 +23994,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="51"/>
-      <c r="AR1" s="51"/>
-      <c r="AS1" s="51"/>
-      <c r="AT1" s="51"/>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -24067,22 +24067,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -24092,36 +24092,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="51" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="51" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="51"/>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -25803,6 +25803,10 @@
     <row r="38" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A38" s="16" t="s">
         <v>134</v>
+      </c>
+      <c r="Q38" s="4">
+        <f>FORECAST(0.21,  {0.0217,0.0474,0.050457757,0.062},{0.21,0.291,0.328,0.396})</f>
+        <v>2.4828332054633209E-2</v>
       </c>
     </row>
     <row r="39" spans="1:48" x14ac:dyDescent="0.15">
@@ -28778,70 +28782,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="51"/>
-      <c r="AR1" s="51"/>
-      <c r="AS1" s="51"/>
-      <c r="AT1" s="51"/>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="31" t="s">
         <v>38</v>
       </c>
@@ -28851,22 +28855,22 @@
       <c r="I2" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="31" t="s">
         <v>38</v>
       </c>
@@ -28876,36 +28880,36 @@
       <c r="X2" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="51" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="51" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="51"/>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
@@ -32940,70 +32944,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="51"/>
-      <c r="AR1" s="51"/>
-      <c r="AS1" s="51"/>
-      <c r="AT1" s="51"/>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -33013,22 +33017,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -33038,36 +33042,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="51" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="51" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="51"/>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
@@ -33865,15 +33869,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BJ74"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:AV65"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.5" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="1.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
@@ -33884,100 +33890,95 @@
     <col min="14" max="14" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="35" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="49" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="51"/>
-      <c r="AR1" s="51"/>
-      <c r="AS1" s="51"/>
-      <c r="AT1" s="51"/>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="19" t="s">
         <v>38</v>
       </c>
@@ -33987,22 +33988,22 @@
       <c r="I2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="19" t="s">
         <v>38</v>
       </c>
@@ -34012,40 +34013,197 @@
       <c r="X2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="51" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="51" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="51"/>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>331</v>
+      </c>
+      <c r="B3" s="20">
+        <v>-2</v>
+      </c>
+      <c r="C3" s="20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D3" s="20">
+        <v>3</v>
+      </c>
+      <c r="E3" s="21">
+        <v>4</v>
+      </c>
+      <c r="F3" s="21">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="I3" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="22" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K3" s="22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L3" s="23" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M3" s="23" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N3" s="23" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O3" s="23" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P3" s="23" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q3" s="4" t="e">
+        <f>ADDRESS(B3,C3,D3,E3,F3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R3" s="4" t="str">
+        <f>ADDRESS(C3,D3,E3,F3,G3)</f>
+        <v>!C1</v>
+      </c>
+      <c r="S3" s="4" t="str">
+        <f>ADDRESS(D3,E3,F3,G3,H3)</f>
+        <v>'*b?u*'!R[3]C[4]</v>
+      </c>
+      <c r="T3" s="4" t="e">
+        <f t="shared" ref="S3:AE3" si="0">ADDRESS(E3,F3,G3,H3,I3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U3" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V3" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W3" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X3" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y3" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z3" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA3" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB3" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC3" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD3" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE3" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF3" s="4" t="e">
+        <f>ADDRESS(C3:P3,D3,E3,F3,G3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG3" s="4" t="str">
+        <f t="array" ref="AG3:AV3">ADDRESS(C3:P3,D3,E3,F3,G3)</f>
+        <v>!C1</v>
+      </c>
+      <c r="AH3" s="4" t="str">
+        <v>!C3</v>
+      </c>
+      <c r="AI3" s="4" t="str">
+        <v>!C4</v>
+      </c>
+      <c r="AJ3" s="4" t="str">
+        <v>!C4</v>
+      </c>
+      <c r="AK3" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL3" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM3" s="4" t="str">
+        <v>!C1</v>
+      </c>
+      <c r="AN3" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO3" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AP3" s="4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AQ3" s="4" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AR3" s="4" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AS3" s="4" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AT3" s="4" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AU3" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AV3" s="4" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.15">
@@ -34059,7 +34217,7 @@
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="60" t="s">
         <v>334</v>
       </c>
       <c r="B6" s="20">
@@ -34111,19 +34269,19 @@
         <v>2</v>
       </c>
       <c r="R6" s="6">
-        <f t="shared" ref="R6:AE6" si="0">COLUMN(C6)</f>
+        <f t="shared" ref="R6:AE6" si="1">COLUMN(C6)</f>
         <v>3</v>
       </c>
       <c r="S6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="T6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="U6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="V6" s="6">
@@ -34131,39 +34289,39 @@
         <v>22</v>
       </c>
       <c r="W6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="Y6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="Z6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="AA6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="AB6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="AC6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="AD6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="AE6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="AF6" s="4">
@@ -34225,7 +34383,7 @@
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A7" s="52"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
@@ -34242,23 +34400,23 @@
       <c r="O7" s="23"/>
       <c r="P7" s="23"/>
       <c r="Q7" s="6">
-        <f t="shared" ref="Q7:Q8" si="1">COLUMN(B7)</f>
+        <f t="shared" ref="Q7:Q8" si="2">COLUMN(B7)</f>
         <v>2</v>
       </c>
       <c r="R7" s="6">
-        <f t="shared" ref="R7:R8" si="2">COLUMN(C7)</f>
+        <f t="shared" ref="R7:R8" si="3">COLUMN(C7)</f>
         <v>3</v>
       </c>
       <c r="S7" s="6">
-        <f t="shared" ref="S7:S8" si="3">COLUMN(D7)</f>
+        <f t="shared" ref="S7:S8" si="4">COLUMN(D7)</f>
         <v>4</v>
       </c>
       <c r="T7" s="6">
-        <f t="shared" ref="T7:T8" si="4">COLUMN(E7)</f>
+        <f t="shared" ref="T7:T8" si="5">COLUMN(E7)</f>
         <v>5</v>
       </c>
       <c r="U7" s="6">
-        <f t="shared" ref="U7:U8" si="5">COLUMN(F7)</f>
+        <f t="shared" ref="U7:U8" si="6">COLUMN(F7)</f>
         <v>6</v>
       </c>
       <c r="V7" s="6">
@@ -34266,39 +34424,39 @@
         <v>22</v>
       </c>
       <c r="W7" s="6">
-        <f t="shared" ref="W7:W8" si="6">COLUMN(H7)</f>
+        <f t="shared" ref="W7:W8" si="7">COLUMN(H7)</f>
         <v>8</v>
       </c>
       <c r="X7" s="6">
-        <f t="shared" ref="X7:X8" si="7">COLUMN(I7)</f>
+        <f t="shared" ref="X7:X8" si="8">COLUMN(I7)</f>
         <v>9</v>
       </c>
       <c r="Y7" s="6">
-        <f t="shared" ref="Y7:Y8" si="8">COLUMN(J7)</f>
+        <f t="shared" ref="Y7:Y8" si="9">COLUMN(J7)</f>
         <v>10</v>
       </c>
       <c r="Z7" s="6">
-        <f t="shared" ref="Z7:Z8" si="9">COLUMN(K7)</f>
+        <f t="shared" ref="Z7:Z8" si="10">COLUMN(K7)</f>
         <v>11</v>
       </c>
       <c r="AA7" s="6">
-        <f t="shared" ref="AA7:AA8" si="10">COLUMN(L7)</f>
+        <f t="shared" ref="AA7:AA8" si="11">COLUMN(L7)</f>
         <v>12</v>
       </c>
       <c r="AB7" s="6">
-        <f t="shared" ref="AB7:AB8" si="11">COLUMN(M7)</f>
+        <f t="shared" ref="AB7:AB8" si="12">COLUMN(M7)</f>
         <v>13</v>
       </c>
       <c r="AC7" s="6">
-        <f t="shared" ref="AC7:AC8" si="12">COLUMN(N7)</f>
+        <f t="shared" ref="AC7:AC8" si="13">COLUMN(N7)</f>
         <v>14</v>
       </c>
       <c r="AD7" s="6">
-        <f t="shared" ref="AD7:AD8" si="13">COLUMN(O7)</f>
+        <f t="shared" ref="AD7:AD8" si="14">COLUMN(O7)</f>
         <v>15</v>
       </c>
       <c r="AE7" s="6">
-        <f t="shared" ref="AE7:AE8" si="14">COLUMN(P7)</f>
+        <f t="shared" ref="AE7:AE8" si="15">COLUMN(P7)</f>
         <v>16</v>
       </c>
       <c r="AF7" s="4" t="e">
@@ -34355,7 +34513,7 @@
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A8" s="52"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
@@ -34372,23 +34530,23 @@
       <c r="O8" s="23"/>
       <c r="P8" s="23"/>
       <c r="Q8" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="R8" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="S8" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="T8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="U8" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="V8" s="6">
@@ -34396,39 +34554,39 @@
         <v>22</v>
       </c>
       <c r="W8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="X8" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="Y8" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="Z8" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
       <c r="AA8" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="AB8" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="AC8" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
       <c r="AD8" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="AE8" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
       <c r="AF8" s="4">
@@ -34607,7 +34765,7 @@
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="60" t="s">
         <v>338</v>
       </c>
       <c r="B12" s="20">
@@ -34765,7 +34923,7 @@
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A13" s="52"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="20">
         <v>-1.1000000000000001</v>
       </c>
@@ -34872,7 +35030,7 @@
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A14" s="52"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="20">
         <v>-1.1000000000000001</v>
       </c>
@@ -34984,7 +35142,7 @@
       </c>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="60" t="s">
         <v>340</v>
       </c>
       <c r="B16" s="20">
@@ -35052,43 +35210,43 @@
         <v>0</v>
       </c>
       <c r="V16" s="4" t="str">
-        <f t="shared" ref="V16:AE16" si="15">INDEX(G16:I17,1,2)</f>
+        <f t="shared" ref="V16:AE16" si="16">INDEX(G16:I17,1,2)</f>
         <v>b</v>
       </c>
       <c r="W16" s="4" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="X16" s="4" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y16" s="4" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#N/A</v>
       </c>
       <c r="Z16" s="4" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA16" s="4" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NAME?</v>
       </c>
       <c r="AB16" s="4" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NULL!</v>
       </c>
       <c r="AC16" s="4" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="AD16" s="4" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#REF!</v>
       </c>
       <c r="AE16" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.1</v>
       </c>
       <c r="AG16" s="4">
@@ -35143,7 +35301,7 @@
       </c>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A17" s="52"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="20">
         <v>-2</v>
       </c>
@@ -35259,7 +35417,7 @@
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A18" s="52"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="20">
         <v>-2.9</v>
       </c>
@@ -35372,7 +35530,7 @@
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="60" t="s">
         <v>342</v>
       </c>
       <c r="B20" s="20">
@@ -35534,7 +35692,7 @@
       </c>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A21" s="52"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
@@ -35665,7 +35823,7 @@
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A22" s="52"/>
+      <c r="A22" s="60"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
@@ -35796,7 +35954,7 @@
       </c>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A23" s="52"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
@@ -35927,7 +36085,7 @@
       </c>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A24" s="52"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
@@ -36058,7 +36216,7 @@
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A25" s="52"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
@@ -36189,7 +36347,7 @@
       </c>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A26" s="52"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
@@ -36320,7 +36478,7 @@
       </c>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A27" s="52"/>
+      <c r="A27" s="60"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
@@ -36451,7 +36609,7 @@
       </c>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A28" s="52"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -36581,7 +36739,7 @@
       </c>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A29" s="52" t="s">
+      <c r="A29" s="60" t="s">
         <v>352</v>
       </c>
       <c r="B29" s="20">
@@ -36706,7 +36864,7 @@
       <c r="AU29" s="6"/>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A30" s="52"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="20">
         <v>-2</v>
       </c>
@@ -36815,7 +36973,7 @@
       <c r="AG30" s="6"/>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A31" s="52"/>
+      <c r="A31" s="60"/>
       <c r="B31" s="20">
         <v>-2</v>
       </c>
@@ -36924,7 +37082,7 @@
       <c r="AG31" s="6"/>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A32" s="52"/>
+      <c r="A32" s="60"/>
       <c r="B32" s="20">
         <v>-2</v>
       </c>
@@ -37033,7 +37191,7 @@
       <c r="AG32" s="6"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A33" s="52"/>
+      <c r="A33" s="60"/>
       <c r="B33" s="20">
         <v>-2</v>
       </c>
@@ -37142,7 +37300,7 @@
       <c r="AG33" s="6"/>
     </row>
     <row r="34" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A34" s="52"/>
+      <c r="A34" s="60"/>
       <c r="B34" s="20">
         <v>-2</v>
       </c>
@@ -37251,7 +37409,7 @@
       <c r="AG34" s="6"/>
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A35" s="52"/>
+      <c r="A35" s="60"/>
       <c r="B35" s="20">
         <v>-2</v>
       </c>
@@ -37360,7 +37518,7 @@
       <c r="AG35" s="6"/>
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A36" s="52"/>
+      <c r="A36" s="60"/>
       <c r="B36" s="20">
         <v>-2</v>
       </c>
@@ -37469,7 +37627,7 @@
       <c r="AG36" s="6"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A37" s="52"/>
+      <c r="A37" s="60"/>
       <c r="B37" s="20">
         <v>-2</v>
       </c>
@@ -37578,7 +37736,7 @@
       <c r="AG37" s="6"/>
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A38" s="52" t="s">
+      <c r="A38" s="60" t="s">
         <v>351</v>
       </c>
       <c r="B38" s="20">
@@ -37703,7 +37861,7 @@
       <c r="AU38" s="6"/>
     </row>
     <row r="39" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A39" s="52"/>
+      <c r="A39" s="60"/>
       <c r="B39" s="20">
         <v>-2</v>
       </c>
@@ -37812,7 +37970,7 @@
       <c r="AG39" s="6"/>
     </row>
     <row r="40" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A40" s="52"/>
+      <c r="A40" s="60"/>
       <c r="B40" s="20">
         <v>-2</v>
       </c>
@@ -37921,7 +38079,7 @@
       <c r="AG40" s="6"/>
     </row>
     <row r="41" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A41" s="52"/>
+      <c r="A41" s="60"/>
       <c r="B41" s="20">
         <v>-2</v>
       </c>
@@ -38030,7 +38188,7 @@
       <c r="AG41" s="6"/>
     </row>
     <row r="42" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A42" s="52"/>
+      <c r="A42" s="60"/>
       <c r="B42" s="20">
         <v>-2</v>
       </c>
@@ -38139,7 +38297,7 @@
       <c r="AG42" s="6"/>
     </row>
     <row r="43" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A43" s="52"/>
+      <c r="A43" s="60"/>
       <c r="B43" s="20">
         <v>-2</v>
       </c>
@@ -38248,7 +38406,7 @@
       <c r="AG43" s="6"/>
     </row>
     <row r="44" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A44" s="52"/>
+      <c r="A44" s="60"/>
       <c r="B44" s="20">
         <v>-2</v>
       </c>
@@ -38357,7 +38515,7 @@
       <c r="AG44" s="6"/>
     </row>
     <row r="45" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A45" s="52"/>
+      <c r="A45" s="60"/>
       <c r="B45" s="20">
         <v>-2</v>
       </c>
@@ -38466,7 +38624,7 @@
       <c r="AG45" s="6"/>
     </row>
     <row r="46" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A46" s="52"/>
+      <c r="A46" s="60"/>
       <c r="B46" s="20">
         <v>-2</v>
       </c>
@@ -38575,7 +38733,7 @@
       <c r="AG46" s="6"/>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A47" s="52" t="s">
+      <c r="A47" s="60" t="s">
         <v>353</v>
       </c>
       <c r="B47" s="20">
@@ -38700,7 +38858,7 @@
       <c r="AU47" s="6"/>
     </row>
     <row r="48" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A48" s="52"/>
+      <c r="A48" s="60"/>
       <c r="B48" s="20">
         <v>-2</v>
       </c>
@@ -38809,7 +38967,7 @@
       <c r="AG48" s="6"/>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A49" s="52"/>
+      <c r="A49" s="60"/>
       <c r="B49" s="20">
         <v>-2</v>
       </c>
@@ -38918,7 +39076,7 @@
       <c r="AG49" s="6"/>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A50" s="52"/>
+      <c r="A50" s="60"/>
       <c r="B50" s="20">
         <v>-2</v>
       </c>
@@ -39027,7 +39185,7 @@
       <c r="AG50" s="6"/>
     </row>
     <row r="51" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A51" s="52"/>
+      <c r="A51" s="60"/>
       <c r="B51" s="20">
         <v>-2</v>
       </c>
@@ -39136,7 +39294,7 @@
       <c r="AG51" s="6"/>
     </row>
     <row r="52" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A52" s="52"/>
+      <c r="A52" s="60"/>
       <c r="B52" s="20">
         <v>-2</v>
       </c>
@@ -39245,7 +39403,7 @@
       <c r="AG52" s="6"/>
     </row>
     <row r="53" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A53" s="52"/>
+      <c r="A53" s="60"/>
       <c r="B53" s="20">
         <v>-2</v>
       </c>
@@ -39354,7 +39512,7 @@
       <c r="AG53" s="6"/>
     </row>
     <row r="54" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A54" s="52"/>
+      <c r="A54" s="60"/>
       <c r="B54" s="20">
         <v>-2</v>
       </c>
@@ -39463,7 +39621,7 @@
       <c r="AG54" s="6"/>
     </row>
     <row r="55" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A55" s="52"/>
+      <c r="A55" s="60"/>
       <c r="B55" s="20">
         <v>-2</v>
       </c>
@@ -39602,7 +39760,7 @@
       <c r="AE56" s="6"/>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A57" s="52" t="s">
+      <c r="A57" s="60" t="s">
         <v>344</v>
       </c>
       <c r="B57" s="20">
@@ -39654,19 +39812,19 @@
         <v>57</v>
       </c>
       <c r="R57" s="6">
-        <f t="shared" ref="R57:AE57" si="16">ROW(C57)</f>
+        <f t="shared" ref="R57:AE57" si="17">ROW(C57)</f>
         <v>57</v>
       </c>
       <c r="S57" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>57</v>
       </c>
       <c r="T57" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>57</v>
       </c>
       <c r="U57" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>57</v>
       </c>
       <c r="V57" s="6">
@@ -39674,39 +39832,39 @@
         <v>57</v>
       </c>
       <c r="W57" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>57</v>
       </c>
       <c r="X57" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>57</v>
       </c>
       <c r="Y57" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>57</v>
       </c>
       <c r="Z57" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>57</v>
       </c>
       <c r="AA57" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>57</v>
       </c>
       <c r="AB57" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>57</v>
       </c>
       <c r="AC57" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>57</v>
       </c>
       <c r="AD57" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>57</v>
       </c>
       <c r="AE57" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>57</v>
       </c>
       <c r="AF57" s="4">
@@ -39768,7 +39926,7 @@
       </c>
     </row>
     <row r="58" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A58" s="52"/>
+      <c r="A58" s="60"/>
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
       <c r="D58" s="20"/>
@@ -39785,23 +39943,23 @@
       <c r="O58" s="23"/>
       <c r="P58" s="23"/>
       <c r="Q58" s="6">
-        <f t="shared" ref="Q58:Q59" si="17">ROW(B58)</f>
+        <f t="shared" ref="Q58:Q59" si="18">ROW(B58)</f>
         <v>58</v>
       </c>
       <c r="R58" s="6">
-        <f t="shared" ref="R58:R59" si="18">ROW(C58)</f>
+        <f t="shared" ref="R58:R59" si="19">ROW(C58)</f>
         <v>58</v>
       </c>
       <c r="S58" s="6">
-        <f t="shared" ref="S58:S59" si="19">ROW(D58)</f>
+        <f t="shared" ref="S58:S59" si="20">ROW(D58)</f>
         <v>58</v>
       </c>
       <c r="T58" s="6">
-        <f t="shared" ref="T58:T59" si="20">ROW(E58)</f>
+        <f t="shared" ref="T58:T59" si="21">ROW(E58)</f>
         <v>58</v>
       </c>
       <c r="U58" s="6">
-        <f t="shared" ref="U58:U59" si="21">ROW(F58)</f>
+        <f t="shared" ref="U58:U59" si="22">ROW(F58)</f>
         <v>58</v>
       </c>
       <c r="V58" s="6">
@@ -39813,35 +39971,35 @@
         <v>58</v>
       </c>
       <c r="X58" s="6">
-        <f t="shared" ref="X58:X59" si="22">ROW(I58)</f>
+        <f t="shared" ref="X58:X59" si="23">ROW(I58)</f>
         <v>58</v>
       </c>
       <c r="Y58" s="6">
-        <f t="shared" ref="Y58:Y59" si="23">ROW(J58)</f>
+        <f t="shared" ref="Y58:Y59" si="24">ROW(J58)</f>
         <v>58</v>
       </c>
       <c r="Z58" s="6">
-        <f t="shared" ref="Z58:Z59" si="24">ROW(K58)</f>
+        <f t="shared" ref="Z58:Z59" si="25">ROW(K58)</f>
         <v>58</v>
       </c>
       <c r="AA58" s="6">
-        <f t="shared" ref="AA58:AA59" si="25">ROW(L58)</f>
+        <f t="shared" ref="AA58:AA59" si="26">ROW(L58)</f>
         <v>58</v>
       </c>
       <c r="AB58" s="6">
-        <f t="shared" ref="AB58:AB59" si="26">ROW(M58)</f>
+        <f t="shared" ref="AB58:AB59" si="27">ROW(M58)</f>
         <v>58</v>
       </c>
       <c r="AC58" s="6">
-        <f t="shared" ref="AC58:AC59" si="27">ROW(N58)</f>
+        <f t="shared" ref="AC58:AC59" si="28">ROW(N58)</f>
         <v>58</v>
       </c>
       <c r="AD58" s="6">
-        <f t="shared" ref="AD58:AD59" si="28">ROW(O58)</f>
+        <f t="shared" ref="AD58:AD59" si="29">ROW(O58)</f>
         <v>58</v>
       </c>
       <c r="AE58" s="6">
-        <f t="shared" ref="AE58:AE59" si="29">ROW(P58)</f>
+        <f t="shared" ref="AE58:AE59" si="30">ROW(P58)</f>
         <v>58</v>
       </c>
       <c r="AF58" s="4" t="e">
@@ -39898,7 +40056,7 @@
       </c>
     </row>
     <row r="59" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A59" s="52"/>
+      <c r="A59" s="60"/>
       <c r="B59" s="20"/>
       <c r="C59" s="20"/>
       <c r="D59" s="20"/>
@@ -39915,23 +40073,23 @@
       <c r="O59" s="23"/>
       <c r="P59" s="23"/>
       <c r="Q59" s="6">
-        <f t="shared" si="17"/>
-        <v>59</v>
-      </c>
-      <c r="R59" s="6">
         <f t="shared" si="18"/>
         <v>59</v>
       </c>
-      <c r="S59" s="6">
+      <c r="R59" s="6">
         <f t="shared" si="19"/>
         <v>59</v>
       </c>
-      <c r="T59" s="6">
+      <c r="S59" s="6">
         <f t="shared" si="20"/>
         <v>59</v>
       </c>
+      <c r="T59" s="6">
+        <f t="shared" si="21"/>
+        <v>59</v>
+      </c>
       <c r="U59" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>59</v>
       </c>
       <c r="V59" s="6">
@@ -39939,39 +40097,39 @@
         <v>59</v>
       </c>
       <c r="W59" s="6">
-        <f t="shared" ref="W59" si="30">ROW(H59)</f>
+        <f t="shared" ref="W59" si="31">ROW(H59)</f>
         <v>59</v>
       </c>
       <c r="X59" s="6">
-        <f t="shared" si="22"/>
-        <v>59</v>
-      </c>
-      <c r="Y59" s="6">
         <f t="shared" si="23"/>
         <v>59</v>
       </c>
-      <c r="Z59" s="6">
+      <c r="Y59" s="6">
         <f t="shared" si="24"/>
         <v>59</v>
       </c>
-      <c r="AA59" s="6">
+      <c r="Z59" s="6">
         <f t="shared" si="25"/>
         <v>59</v>
       </c>
-      <c r="AB59" s="6">
+      <c r="AA59" s="6">
         <f t="shared" si="26"/>
         <v>59</v>
       </c>
-      <c r="AC59" s="6">
+      <c r="AB59" s="6">
         <f t="shared" si="27"/>
         <v>59</v>
       </c>
-      <c r="AD59" s="6">
+      <c r="AC59" s="6">
         <f t="shared" si="28"/>
         <v>59</v>
       </c>
+      <c r="AD59" s="6">
+        <f t="shared" si="29"/>
+        <v>59</v>
+      </c>
       <c r="AE59" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>59</v>
       </c>
       <c r="AF59" s="4">
@@ -40133,7 +40291,7 @@
       <c r="AE62" s="6"/>
     </row>
     <row r="63" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A63" s="52" t="s">
+      <c r="A63" s="60" t="s">
         <v>348</v>
       </c>
       <c r="B63" s="20">
@@ -40242,7 +40400,7 @@
       </c>
     </row>
     <row r="64" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A64" s="52"/>
+      <c r="A64" s="60"/>
       <c r="B64" s="20">
         <v>-1.1000000000000001</v>
       </c>
@@ -40349,7 +40507,7 @@
       </c>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.15">
-      <c r="A65" s="52"/>
+      <c r="A65" s="60"/>
       <c r="B65" s="20">
         <v>-1.1000000000000001</v>
       </c>
@@ -40745,6 +40903,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -40756,12 +40920,6 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -40823,70 +40981,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="51"/>
-      <c r="AR1" s="51"/>
-      <c r="AS1" s="51"/>
-      <c r="AT1" s="51"/>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
+      <c r="AU1" s="57"/>
+      <c r="AV1" s="57"/>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="18" t="s">
         <v>38</v>
       </c>
@@ -40896,22 +41054,22 @@
       <c r="I2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="18" t="s">
         <v>38</v>
       </c>
@@ -40921,36 +41079,36 @@
       <c r="X2" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="51" t="s">
+      <c r="Y2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="51" t="s">
+      <c r="AG2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="51"/>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="57"/>
+      <c r="AR2" s="57"/>
+      <c r="AS2" s="57"/>
+      <c r="AT2" s="57"/>
+      <c r="AU2" s="57"/>
+      <c r="AV2" s="57"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
@@ -43063,9 +43221,9 @@
         <f t="array" ref="H20:H24">IF(G9:G12&lt;&gt;H10:H13,1,0)</f>
         <v>0</v>
       </c>
-      <c r="M20" s="54"/>
-      <c r="N20" s="54"/>
-      <c r="O20" s="54"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="62"/>
     </row>
     <row r="21" spans="2:16" ht="18" x14ac:dyDescent="0.2">
       <c r="F21">
@@ -43141,12 +43299,12 @@
         <f>REF!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="M25" s="53" t="str">
+      <c r="M25" s="61" t="str">
         <f>"Exchange(1 "&amp;NAMEDCELL123&amp;"=)"</f>
         <v>Exchange(1 'ciao=)</v>
       </c>
-      <c r="N25" s="53"/>
-      <c r="O25" s="53"/>
+      <c r="N25" s="61"/>
+      <c r="O25" s="61"/>
     </row>
     <row r="48" spans="20:20" ht="17" x14ac:dyDescent="0.25">
       <c r="T48" s="3"/>

</xml_diff>

<commit_message>
feat(info): Add `ISODD`, `ISEVEN`, `ISBLANK`, `ISTEXT`, `ISNONTEXT`, and `ISLOGICAL` functions.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173A5E89-9319-C445-A7AB-B5D00AC12900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00852B2C-F7D2-4649-B727-132912553120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19200" tabRatio="770" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19200" tabRatio="770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="506">
   <si>
     <t>ca</t>
   </si>
@@ -1577,6 +1577,9 @@
   </si>
   <si>
     <t>= text</t>
+  </si>
+  <si>
+    <t>1/1/1900</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +1725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1823,6 +1826,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2145,7 +2150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV81"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:AV81"/>
     </sheetView>
   </sheetViews>
@@ -18861,7 +18866,7 @@
   <dimension ref="A1:AV59"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="AG32" sqref="AG32:AV32"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -21543,7 +21548,7 @@
   <dimension ref="A1:BJ41"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:AV41"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -32929,17 +32934,16 @@
     <col min="16" max="16" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="21" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="31" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="40" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="47" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="48" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="49" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
@@ -33089,8 +33093,165 @@
       </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>211</v>
+      </c>
+      <c r="B6" s="14">
+        <v>0</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E6" s="14">
+        <v>10</v>
+      </c>
+      <c r="F6" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K6" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M6" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N6" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O6" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P6" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q6" s="6" t="b">
+        <f>ISBLANK(B6)</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="6" t="b">
+        <f t="shared" ref="R6:AE6" si="0">ISBLANK(C6)</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="6" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W6" s="6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X6" s="6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE6" s="6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="6" t="b">
+        <f>ISBLANK(B6:P6)</f>
+        <v>0</v>
+      </c>
+      <c r="AG6" s="6" t="b">
+        <f>ISBLANK(G6:P6)</f>
+        <v>0</v>
+      </c>
+      <c r="AH6" s="4" t="b">
+        <f t="array" ref="AH6:AV6">ISBLANK(C6:P6)</f>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.15">
@@ -33141,63 +33302,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q7" s="6" t="b">
-        <f t="shared" ref="Q7:AE7" si="0">ISERR(B7)</f>
+        <f t="shared" ref="Q6:AE7" si="1">ISERR(B7)</f>
         <v>0</v>
       </c>
       <c r="R7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Z7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AB7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AD7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AE7" s="6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AF7" s="6" t="b">
@@ -33302,63 +33463,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q8" s="6" t="b">
-        <f t="shared" ref="Q8:AE8" si="1">ISERROR(B8)</f>
+        <f t="shared" ref="Q8:AE8" si="2">ISERROR(B8)</f>
         <v>0</v>
       </c>
       <c r="R8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Z8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AA8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AB8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AC8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AE8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AF8" s="6" t="b">
@@ -33416,18 +33577,364 @@
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>212</v>
+      </c>
+      <c r="B9" s="14">
+        <v>0</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E9" s="14">
+        <v>10</v>
+      </c>
+      <c r="F9" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="30" t="s">
+        <v>505</v>
+      </c>
+      <c r="I9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K9" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L9" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N9" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O9" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P9" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q9" s="6" t="b">
+        <f>ISEVEN(B9)</f>
+        <v>1</v>
+      </c>
+      <c r="R9" s="6" t="b">
+        <f t="shared" ref="R9:AE9" si="3">ISEVEN(C9)</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="6" t="b">
+        <f>ISEVEN(D9)</f>
+        <v>1</v>
+      </c>
+      <c r="T9" s="6" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U9" s="6" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V9" s="6" t="b">
+        <f>ISEVEN(G9)</f>
+        <v>1</v>
+      </c>
+      <c r="W9" s="6" t="b">
+        <f>ISEVEN(H9)</f>
+        <v>0</v>
+      </c>
+      <c r="X9" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y9" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z9" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA9" s="6" t="e">
+        <f>ISEVEN(L9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB9" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC9" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD9" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE9" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF9" s="4" t="e">
+        <f>ISEVEN(B9:P9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG9" s="4" t="e">
+        <f t="array" ref="AG9:AI9">ISEVEN(B9:P9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AH9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AJ9" s="4" t="e">
+        <f t="array" ref="AJ9:AM9">ISEVEN(B9:F9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AK9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN9" s="4" t="e">
+        <f t="array" ref="AN9:AV9">ISEVEN(L9:P9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AU9" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AV9" s="4" t="e">
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>213</v>
       </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="17" t="s">
         <v>214</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E11" s="14">
+        <v>10</v>
+      </c>
+      <c r="F11" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="30" t="s">
+        <v>505</v>
+      </c>
+      <c r="I11" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K11" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L11" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N11" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O11" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P11" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q11" s="6" t="b">
+        <f>ISLOGICAL(B11)</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="6" t="b">
+        <f t="shared" ref="R11:AE11" si="4">ISLOGICAL(C11)</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U11" s="6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X11" s="6" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y11" s="6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AB11" s="6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AE11" s="6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AF11" s="4" t="b">
+        <f>ISLOGICAL(I11:P11)</f>
+        <v>0</v>
+      </c>
+      <c r="AG11" s="4" t="b">
+        <f t="array" ref="AG11:AI11">ISLOGICAL(B11:P11)</f>
+        <v>0</v>
+      </c>
+      <c r="AH11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="4" t="b">
+        <f t="array" ref="AJ11:AM11">ISLOGICAL(G11:K11)</f>
+        <v>0</v>
+      </c>
+      <c r="AK11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN11" s="4" t="b">
+        <f t="array" ref="AN11:AV11">ISLOGICAL(L11:P11)</f>
+        <v>0</v>
+      </c>
+      <c r="AO11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV11" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.15">
@@ -33482,59 +33989,59 @@
         <v>0</v>
       </c>
       <c r="R12" s="6" t="b">
-        <f t="shared" ref="R12:AE12" si="2">ISNA(C12)</f>
+        <f t="shared" ref="R12:AE12" si="5">ISNA(C12)</f>
         <v>0</v>
       </c>
       <c r="S12" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T12" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U12" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V12" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W12" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X12" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y12" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z12" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AA12" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB12" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC12" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AD12" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE12" s="6" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AF12" s="6" t="b">
@@ -33592,8 +34099,166 @@
       </c>
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="17" t="s">
         <v>216</v>
+      </c>
+      <c r="B13" s="14">
+        <v>0</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E13" s="14">
+        <v>10</v>
+      </c>
+      <c r="F13" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="30" t="s">
+        <v>505</v>
+      </c>
+      <c r="I13" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K13" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L13" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N13" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O13" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P13" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q13" s="6" t="b">
+        <f>ISNONTEXT(B13)</f>
+        <v>1</v>
+      </c>
+      <c r="R13" s="6" t="b">
+        <f t="shared" ref="R13:AE13" si="6">ISNONTEXT(C13)</f>
+        <v>1</v>
+      </c>
+      <c r="S13" s="6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T13" s="6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="U13" s="6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V13" s="6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="W13" s="6" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X13" s="6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Y13" s="6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Z13" s="6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AA13" s="6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AB13" s="6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AC13" s="6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AD13" s="6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AE13" s="6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AF13" s="4" t="b">
+        <f>ISNONTEXT(H13:P13)</f>
+        <v>1</v>
+      </c>
+      <c r="AG13" s="4" t="b">
+        <f t="array" ref="AG13:AI13">ISNONTEXT(B13:P13)</f>
+        <v>1</v>
+      </c>
+      <c r="AH13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="4" t="b">
+        <f t="array" ref="AJ13:AM13">ISNONTEXT(E13:I13)</f>
+        <v>1</v>
+      </c>
+      <c r="AK13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="4" t="b">
+        <f t="array" ref="AN13:AV13">ISNONTEXT(L13:P13)</f>
+        <v>1</v>
+      </c>
+      <c r="AO13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV13" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.15">
@@ -33648,59 +34313,59 @@
         <v>1</v>
       </c>
       <c r="R14" s="4" t="b">
-        <f t="shared" ref="R14:AE14" si="3">ISNUMBER(C14)</f>
+        <f t="shared" ref="R14:AE14" si="7">ISNUMBER(C14)</f>
         <v>1</v>
       </c>
       <c r="S14" s="4" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="T14" s="4" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="U14" s="4" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V14" s="4" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W14" s="4" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="X14" s="4" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y14" s="4" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z14" s="4" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AA14" s="4" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB14" s="4" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC14" s="4" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD14" s="4" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AE14" s="4" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AF14" s="4" t="b">
@@ -33758,18 +34423,364 @@
       </c>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="17" t="s">
         <v>218</v>
       </c>
+      <c r="B15" s="14">
+        <v>0</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1</v>
+      </c>
+      <c r="D15" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E15" s="14">
+        <v>10</v>
+      </c>
+      <c r="F15" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="30" t="s">
+        <v>505</v>
+      </c>
+      <c r="I15" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K15" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L15" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N15" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O15" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P15" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q15" s="6" t="b">
+        <f>ISODD(B15)</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="6" t="b">
+        <f t="shared" ref="R15:AE15" si="8">ISODD(C15)</f>
+        <v>1</v>
+      </c>
+      <c r="S15" s="6" t="b">
+        <f>ISODD(D15)</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="6" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U15" s="6" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="V15" s="6" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W15" s="6" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="X15" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y15" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z15" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA15" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB15" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC15" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD15" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE15" s="6" t="e">
+        <f t="shared" si="8"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF15" s="4" t="e">
+        <f>ISODD(B15:P15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG15" s="4" t="e">
+        <f t="array" ref="AG15:AI15">ISODD(B15:P15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AH15" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI15" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AJ15" s="4" t="e">
+        <f t="array" ref="AJ15:AM15">ISODD(B15:F15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AK15" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL15" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM15" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN15" s="4" t="e">
+        <f t="array" ref="AN15:AV15">ISODD(L15:P15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO15" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP15" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ15" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR15" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS15" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT15" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AU15" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AV15" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="28" t="s">
         <v>219</v>
       </c>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="63"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="63"/>
+      <c r="R16" s="63"/>
+      <c r="S16" s="63"/>
+      <c r="T16" s="63"/>
+      <c r="U16" s="63"/>
+      <c r="V16" s="63"/>
+      <c r="W16" s="63"/>
+      <c r="X16" s="63"/>
+      <c r="Y16" s="63"/>
+      <c r="Z16" s="63"/>
+      <c r="AA16" s="63"/>
+      <c r="AB16" s="63"/>
+      <c r="AC16" s="63"/>
+      <c r="AD16" s="63"/>
+      <c r="AE16" s="63"/>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="17" t="s">
         <v>220</v>
+      </c>
+      <c r="B17" s="14">
+        <v>0</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E17" s="14">
+        <v>10</v>
+      </c>
+      <c r="F17" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="30" t="s">
+        <v>505</v>
+      </c>
+      <c r="I17" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K17" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L17" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="9" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N17" s="9" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O17" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P17" s="9" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q17" s="6" t="b">
+        <f>ISTEXT(B17)</f>
+        <v>0</v>
+      </c>
+      <c r="R17" s="6" t="b">
+        <f t="shared" ref="R17:AE17" si="9">ISTEXT(C17)</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="6" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T17" s="6" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U17" s="6" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="V17" s="6" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="W17" s="6" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="X17" s="6" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="6" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z17" s="6" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA17" s="6" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB17" s="6" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AC17" s="6" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AD17" s="6" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE17" s="6" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF17" s="4" t="b">
+        <f>ISTEXT(H17:P17)</f>
+        <v>0</v>
+      </c>
+      <c r="AG17" s="4" t="b">
+        <f t="array" ref="AG17:AI17">ISTEXT(B17:P17)</f>
+        <v>0</v>
+      </c>
+      <c r="AH17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="4" t="b">
+        <f t="array" ref="AJ17:AM17">ISTEXT(E17:I17)</f>
+        <v>0</v>
+      </c>
+      <c r="AK17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN17" s="4" t="b">
+        <f t="array" ref="AN17:AV17">ISTEXT(L17:P17)</f>
+        <v>0</v>
+      </c>
+      <c r="AO17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV17" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.15">
@@ -33869,7 +34880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BJ74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -34105,7 +35116,7 @@
         <v>'*b?u*'!R[3]C[4]</v>
       </c>
       <c r="T3" s="4" t="e">
-        <f t="shared" ref="S3:AE3" si="0">ADDRESS(E3,F3,G3,H3,I3)</f>
+        <f t="shared" ref="T3:AE3" si="0">ADDRESS(E3,F3,G3,H3,I3)</f>
         <v>#VALUE!</v>
       </c>
       <c r="U3" s="4" t="e">
@@ -40903,12 +41914,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -40920,6 +41925,12 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat(logic): Update logic functions according to new excel logic.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F11F1FA-8D63-624C-998F-8BEE0FA604B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7CB1C1-AD4C-6C4B-B385-3BD881F13DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" tabRatio="770" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="506">
   <si>
     <t>ca</t>
   </si>
@@ -1584,9 +1584,6 @@
   </si>
   <si>
     <t>1/1/1900</t>
-  </si>
-  <si>
-    <t>26/08/1987</t>
   </si>
 </sst>
 </file>
@@ -21348,8 +21345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BJ41"/>
   <sheetViews>
-    <sheetView topLeftCell="T23" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="AF41" sqref="AF41"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -21371,7 +21368,9 @@
     <col min="16" max="16" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="25" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="23" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -23372,50 +23371,6 @@
       <c r="A35" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="B35" s="4">
-        <v>0</v>
-      </c>
-      <c r="C35" s="4">
-        <v>1.9</v>
-      </c>
-      <c r="D35" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E35" s="4">
-        <v>10</v>
-      </c>
-      <c r="F35" s="4">
-        <v>-1</v>
-      </c>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I35" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J35" s="6" t="e">
-        <f>#VALUE!</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K35" s="6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L35" s="8" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M35" s="8" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N35" s="8" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O35" s="8" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P35" s="8" t="e">
-        <v>#REF!</v>
-      </c>
     </row>
     <row r="36" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A36" s="12" t="s">
@@ -23659,7 +23614,7 @@
         <v>10</v>
       </c>
       <c r="U40" s="4" t="str">
-        <f>UPPER(F40)</f>
+        <f t="shared" si="32"/>
         <v>-1</v>
       </c>
       <c r="V40" s="4" t="str">
@@ -23757,165 +23712,8 @@
       </c>
     </row>
     <row r="41" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="12" t="s">
         <v>330</v>
-      </c>
-      <c r="B41" s="4">
-        <v>0</v>
-      </c>
-      <c r="C41" s="4">
-        <v>1.9</v>
-      </c>
-      <c r="D41" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E41" s="4">
-        <v>10</v>
-      </c>
-      <c r="F41" s="4">
-        <v>-1</v>
-      </c>
-      <c r="G41" s="6"/>
-      <c r="H41" s="20" t="s">
-        <v>506</v>
-      </c>
-      <c r="I41" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J41" s="6" t="e">
-        <f>#VALUE!</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K41" s="6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L41" s="8" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M41" s="8" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="N41" s="8" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="O41" s="8" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="P41" s="8" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="Q41" s="4">
-        <f t="shared" ref="Q41:AE41" si="33">VALUE(B41)</f>
-        <v>0</v>
-      </c>
-      <c r="R41" s="4">
-        <f t="shared" si="33"/>
-        <v>1.9</v>
-      </c>
-      <c r="S41" s="4">
-        <f t="shared" si="33"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="T41" s="4">
-        <f t="shared" si="33"/>
-        <v>10</v>
-      </c>
-      <c r="U41" s="4">
-        <f t="shared" si="33"/>
-        <v>-1</v>
-      </c>
-      <c r="V41" s="4">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="W41" s="4">
-        <f t="shared" si="33"/>
-        <v>32015</v>
-      </c>
-      <c r="X41" s="4" t="e">
-        <f t="shared" si="33"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Y41" s="4" t="e">
-        <f t="shared" si="33"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Z41" s="4" t="e">
-        <f t="shared" si="33"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AA41" s="4" t="e">
-        <f t="shared" si="33"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB41" s="4" t="e">
-        <f t="shared" si="33"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="AC41" s="4" t="e">
-        <f t="shared" si="33"/>
-        <v>#NULL!</v>
-      </c>
-      <c r="AD41" s="4" t="e">
-        <f t="shared" si="33"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="AE41" s="4" t="e">
-        <f t="shared" si="33"/>
-        <v>#REF!</v>
-      </c>
-      <c r="AF41" s="4" t="e">
-        <f>VALUE(B41:C41)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AG41" s="4">
-        <f t="array" ref="AG41:AV41">VALUE(B41:P41)</f>
-        <v>0</v>
-      </c>
-      <c r="AH41" s="4">
-        <v>1.9</v>
-      </c>
-      <c r="AI41" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="AJ41" s="4">
-        <v>10</v>
-      </c>
-      <c r="AK41" s="4">
-        <v>-1</v>
-      </c>
-      <c r="AL41" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM41" s="4">
-        <v>32015</v>
-      </c>
-      <c r="AN41" s="4" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="AO41" s="4" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="AP41" s="4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AQ41" s="4" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AR41" s="4" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="AS41" s="4" t="e">
-        <v>#NULL!</v>
-      </c>
-      <c r="AT41" s="4" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="AU41" s="4" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="AV41" s="4" t="e">
-        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -40561,6 +40359,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -40572,12 +40376,6 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -40591,8 +40389,8 @@
   </sheetPr>
   <dimension ref="A1:BJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="AQ10" sqref="AQ10"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="AJ11" sqref="AJ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -40921,6 +40719,14 @@
         <f>AND(G3:H3)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="AR3" s="4" t="e">
+        <f>AND(TRUE,"ciao",#REF!,"0")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AS3" s="4" t="b">
+        <f>AND(TRUE,"0")</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">

</xml_diff>

<commit_message>
fix(excel), #132: Correction on how to handle the empty values used within a formula
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10320"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49F5A2F-6539-494D-9A1C-6AA646F77AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F860A0-6244-0446-9D55-62E2C82DB977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" tabRatio="770" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15800" tabRatio="770" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <definedName name="NAMEDCELL123">"'ciao"</definedName>
     <definedName name="QF_SYS_LISTPRICECURRENCY">CORE!$F$12</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateCount="1" calcOnSave="0"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -12696,7 +12696,7 @@
   <dimension ref="B1:T60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13252,12 +13252,36 @@
       <c r="N25" s="39"/>
       <c r="O25" s="39"/>
     </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="H26">
+        <f>VAL1</f>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f>J26</f>
+        <v>0</v>
+      </c>
+      <c r="J26" cm="1">
+        <f t="array" ref="J26:J29">G26:G29</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D27" t="b">
         <v>0</v>
       </c>
       <c r="E27">
         <v>5</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ref="I27:I29" si="0">J27</f>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
@@ -13268,16 +13292,44 @@
       <c r="E28">
         <v>6</v>
       </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28">
+        <f>H28</f>
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D29" t="b" cm="1">
         <f t="array" ref="D29:D30">_xlfn.IFS(C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,TRUE,D27:D28)</f>
         <v>0</v>
       </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D30">
         <v>7</v>
+      </c>
+      <c r="H30">
+        <f>AVERAGE(H26:H29)</f>
+        <v>1.5</v>
+      </c>
+      <c r="I30">
+        <f>AVERAGE(I26:I29, VAL1)</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="48" spans="20:20" ht="17" x14ac:dyDescent="0.25">
@@ -24713,7 +24765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6C48B-2D77-2542-8BB6-71EF8476BBAF}">
   <dimension ref="A1:E160"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat(text): Add `CHAR` function.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10320"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F860A0-6244-0446-9D55-62E2C82DB977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A6D8CF-003B-BC45-AAE1-A91C032D79C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15800" tabRatio="770" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15800" tabRatio="770" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <definedName name="NAMEDCELL123">"'ciao"</definedName>
     <definedName name="QF_SYS_LISTPRICECURRENCY">CORE!$F$12</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="507">
   <si>
     <t>ca</t>
   </si>
@@ -2139,8 +2139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV81"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="Q60" sqref="Q60"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -12693,10 +12693,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="B1:T60"/>
+  <dimension ref="A1:T286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13113,7 +13113,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B17">
         <f>[1]Sheet1!$A$1+1</f>
         <v>3</v>
@@ -13133,7 +13133,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B18">
         <f>[1]Sheet1!$A$1+[1]Sheet1!$A$2</f>
         <v>4</v>
@@ -13156,13 +13156,13 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E19">
         <f>D16*3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H20">
         <f t="array" ref="H20:H24">IF(G9:G12&lt;&gt;H10:H13,1,0)</f>
         <v>0</v>
@@ -13171,7 +13171,7 @@
       <c r="N20" s="37"/>
       <c r="O20" s="37"/>
     </row>
-    <row r="21" spans="2:16" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="F21">
         <f>C19+1</f>
         <v>1</v>
@@ -13189,7 +13189,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C22" s="24">
         <v>60</v>
       </c>
@@ -13204,7 +13204,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H23">
         <v>1</v>
       </c>
@@ -13228,7 +13228,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H24" t="e">
         <v>#N/A</v>
       </c>
@@ -13237,7 +13237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D25" s="1" t="s">
         <v>503</v>
       </c>
@@ -13252,7 +13252,7 @@
       <c r="N25" s="39"/>
       <c r="O25" s="39"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H26">
         <f>VAL1</f>
         <v>0</v>
@@ -13266,7 +13266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D27" t="b">
         <v>0</v>
       </c>
@@ -13284,7 +13284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D28" cm="1">
         <f t="array" ref="D28">_xlfn.IFS(D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,D27,E27,TRUE,7)</f>
         <v>7</v>
@@ -13303,7 +13303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D29" t="b" cm="1">
         <f t="array" ref="D29:D30">_xlfn.IFS(C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,TRUE,D27:D28)</f>
         <v>0</v>
@@ -13319,7 +13319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D30">
         <v>7</v>
       </c>
@@ -13332,43 +13332,2319 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="20:20" ht="17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="str">
+        <f>CHAR(A32)</f>
+        <v>_x0001_</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" ref="B33:B96" si="1">CHAR(A33)</f>
+        <v>_x0002_</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0003_</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0004_</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0005_</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0006_</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0007_</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0008_</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">	</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">
+</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>11</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="1"/>
+        <v>_x000B_</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>12</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="1"/>
+        <v>_x000C_</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>13</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="1"/>
+        <v>_x000D_</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>14</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="1"/>
+        <v>_x000E_</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>15</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="1"/>
+        <v>_x000F_</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>16</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0010_</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>17</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0011_</v>
+      </c>
       <c r="T48" s="3"/>
     </row>
-    <row r="52" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>18</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0012_</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>19</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0013_</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>20</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0014_</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>21</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0015_</v>
+      </c>
       <c r="F52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>22</v>
+      </c>
+      <c r="B53" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0016_</v>
+      </c>
       <c r="F53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>23</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0017_</v>
+      </c>
       <c r="F54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>24</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0018_</v>
+      </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>25</v>
+      </c>
+      <c r="B56" t="str">
+        <f t="shared" si="1"/>
+        <v>_x0019_</v>
+      </c>
       <c r="F56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>26</v>
+      </c>
+      <c r="B57" t="str">
+        <f t="shared" si="1"/>
+        <v>_x001A_</v>
+      </c>
       <c r="F57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>27</v>
+      </c>
+      <c r="B58" t="str">
+        <f t="shared" si="1"/>
+        <v>_x001B_</v>
+      </c>
       <c r="F58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>28</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="1"/>
+        <v>_x001C_</v>
+      </c>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>29</v>
+      </c>
+      <c r="B60" t="str">
+        <f t="shared" si="1"/>
+        <v>_x001D_</v>
+      </c>
       <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>30</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="1"/>
+        <v>_x001E_</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>31</v>
+      </c>
+      <c r="B62" t="str">
+        <f t="shared" si="1"/>
+        <v>_x001F_</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>32</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>33</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="1"/>
+        <v>!</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>34</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="1"/>
+        <v>"</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>35</v>
+      </c>
+      <c r="B66" t="str">
+        <f t="shared" si="1"/>
+        <v>#</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>36</v>
+      </c>
+      <c r="B67" t="str">
+        <f t="shared" si="1"/>
+        <v>$</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>37</v>
+      </c>
+      <c r="B68" t="str">
+        <f t="shared" si="1"/>
+        <v>%</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>38</v>
+      </c>
+      <c r="B69" t="str">
+        <f t="shared" si="1"/>
+        <v>&amp;</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>39</v>
+      </c>
+      <c r="B70" t="str">
+        <f t="shared" si="1"/>
+        <v>'</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>40</v>
+      </c>
+      <c r="B71" t="str">
+        <f t="shared" si="1"/>
+        <v>(</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>41</v>
+      </c>
+      <c r="B72" t="str">
+        <f t="shared" si="1"/>
+        <v>)</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>42</v>
+      </c>
+      <c r="B73" t="str">
+        <f t="shared" si="1"/>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>43</v>
+      </c>
+      <c r="B74" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>44</v>
+      </c>
+      <c r="B75" t="str">
+        <f t="shared" si="1"/>
+        <v>,</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>45</v>
+      </c>
+      <c r="B76" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>46</v>
+      </c>
+      <c r="B77" t="str">
+        <f t="shared" si="1"/>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>47</v>
+      </c>
+      <c r="B78" t="str">
+        <f t="shared" si="1"/>
+        <v>/</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>48</v>
+      </c>
+      <c r="B79" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>49</v>
+      </c>
+      <c r="B80" t="str">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>50</v>
+      </c>
+      <c r="B81" t="str">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>51</v>
+      </c>
+      <c r="B82" t="str">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>52</v>
+      </c>
+      <c r="B83" t="str">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>53</v>
+      </c>
+      <c r="B84" t="str">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>54</v>
+      </c>
+      <c r="B85" t="str">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>55</v>
+      </c>
+      <c r="B86" t="str">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>56</v>
+      </c>
+      <c r="B87" t="str">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>57</v>
+      </c>
+      <c r="B88" t="str">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>58</v>
+      </c>
+      <c r="B89" t="str">
+        <f t="shared" si="1"/>
+        <v>:</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>59</v>
+      </c>
+      <c r="B90" t="str">
+        <f t="shared" si="1"/>
+        <v>;</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>60</v>
+      </c>
+      <c r="B91" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>61</v>
+      </c>
+      <c r="B92" t="str">
+        <f t="shared" si="1"/>
+        <v>=</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>62</v>
+      </c>
+      <c r="B93" t="str">
+        <f t="shared" si="1"/>
+        <v>&gt;</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>63</v>
+      </c>
+      <c r="B94" t="str">
+        <f t="shared" si="1"/>
+        <v>?</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>64</v>
+      </c>
+      <c r="B95" t="str">
+        <f t="shared" si="1"/>
+        <v>@</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>65</v>
+      </c>
+      <c r="B96" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>66</v>
+      </c>
+      <c r="B97" t="str">
+        <f t="shared" ref="B97:B160" si="2">CHAR(A97)</f>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>67</v>
+      </c>
+      <c r="B98" t="str">
+        <f t="shared" si="2"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>68</v>
+      </c>
+      <c r="B99" t="str">
+        <f t="shared" si="2"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>69</v>
+      </c>
+      <c r="B100" t="str">
+        <f t="shared" si="2"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>70</v>
+      </c>
+      <c r="B101" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>71</v>
+      </c>
+      <c r="B102" t="str">
+        <f t="shared" si="2"/>
+        <v>G</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>72</v>
+      </c>
+      <c r="B103" t="str">
+        <f t="shared" si="2"/>
+        <v>H</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>73</v>
+      </c>
+      <c r="B104" t="str">
+        <f t="shared" si="2"/>
+        <v>I</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>74</v>
+      </c>
+      <c r="B105" t="str">
+        <f t="shared" si="2"/>
+        <v>J</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>75</v>
+      </c>
+      <c r="B106" t="str">
+        <f t="shared" si="2"/>
+        <v>K</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>76</v>
+      </c>
+      <c r="B107" t="str">
+        <f t="shared" si="2"/>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>77</v>
+      </c>
+      <c r="B108" t="str">
+        <f t="shared" si="2"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>78</v>
+      </c>
+      <c r="B109" t="str">
+        <f t="shared" si="2"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>79</v>
+      </c>
+      <c r="B110" t="str">
+        <f t="shared" si="2"/>
+        <v>O</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>80</v>
+      </c>
+      <c r="B111" t="str">
+        <f t="shared" si="2"/>
+        <v>P</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>81</v>
+      </c>
+      <c r="B112" t="str">
+        <f t="shared" si="2"/>
+        <v>Q</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>82</v>
+      </c>
+      <c r="B113" t="str">
+        <f t="shared" si="2"/>
+        <v>R</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>83</v>
+      </c>
+      <c r="B114" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>84</v>
+      </c>
+      <c r="B115" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>85</v>
+      </c>
+      <c r="B116" t="str">
+        <f t="shared" si="2"/>
+        <v>U</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>86</v>
+      </c>
+      <c r="B117" t="str">
+        <f t="shared" si="2"/>
+        <v>V</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>87</v>
+      </c>
+      <c r="B118" t="str">
+        <f t="shared" si="2"/>
+        <v>W</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>88</v>
+      </c>
+      <c r="B119" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>89</v>
+      </c>
+      <c r="B120" t="str">
+        <f t="shared" si="2"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>90</v>
+      </c>
+      <c r="B121" t="str">
+        <f t="shared" si="2"/>
+        <v>Z</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>91</v>
+      </c>
+      <c r="B122" t="str">
+        <f t="shared" si="2"/>
+        <v>[</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>92</v>
+      </c>
+      <c r="B123" t="str">
+        <f t="shared" si="2"/>
+        <v>\</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>93</v>
+      </c>
+      <c r="B124" t="str">
+        <f t="shared" si="2"/>
+        <v>]</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>94</v>
+      </c>
+      <c r="B125" t="str">
+        <f t="shared" si="2"/>
+        <v>^</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>95</v>
+      </c>
+      <c r="B126" t="str">
+        <f t="shared" si="2"/>
+        <v>_</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>96</v>
+      </c>
+      <c r="B127" t="str">
+        <f t="shared" si="2"/>
+        <v>`</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>97</v>
+      </c>
+      <c r="B128" t="str">
+        <f t="shared" si="2"/>
+        <v>a</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>98</v>
+      </c>
+      <c r="B129" t="str">
+        <f t="shared" si="2"/>
+        <v>b</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>99</v>
+      </c>
+      <c r="B130" t="str">
+        <f t="shared" si="2"/>
+        <v>c</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>100</v>
+      </c>
+      <c r="B131" t="str">
+        <f t="shared" si="2"/>
+        <v>d</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>101</v>
+      </c>
+      <c r="B132" t="str">
+        <f t="shared" si="2"/>
+        <v>e</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>102</v>
+      </c>
+      <c r="B133" t="str">
+        <f t="shared" si="2"/>
+        <v>f</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>103</v>
+      </c>
+      <c r="B134" t="str">
+        <f t="shared" si="2"/>
+        <v>g</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>104</v>
+      </c>
+      <c r="B135" t="str">
+        <f t="shared" si="2"/>
+        <v>h</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>105</v>
+      </c>
+      <c r="B136" t="str">
+        <f t="shared" si="2"/>
+        <v>i</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>106</v>
+      </c>
+      <c r="B137" t="str">
+        <f t="shared" si="2"/>
+        <v>j</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>107</v>
+      </c>
+      <c r="B138" t="str">
+        <f t="shared" si="2"/>
+        <v>k</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>108</v>
+      </c>
+      <c r="B139" t="str">
+        <f t="shared" si="2"/>
+        <v>l</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>109</v>
+      </c>
+      <c r="B140" t="str">
+        <f t="shared" si="2"/>
+        <v>m</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>110</v>
+      </c>
+      <c r="B141" t="str">
+        <f t="shared" si="2"/>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>111</v>
+      </c>
+      <c r="B142" t="str">
+        <f t="shared" si="2"/>
+        <v>o</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>112</v>
+      </c>
+      <c r="B143" t="str">
+        <f t="shared" si="2"/>
+        <v>p</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>113</v>
+      </c>
+      <c r="B144" t="str">
+        <f t="shared" si="2"/>
+        <v>q</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>114</v>
+      </c>
+      <c r="B145" t="str">
+        <f t="shared" si="2"/>
+        <v>r</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>115</v>
+      </c>
+      <c r="B146" t="str">
+        <f t="shared" si="2"/>
+        <v>s</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>116</v>
+      </c>
+      <c r="B147" t="str">
+        <f t="shared" si="2"/>
+        <v>t</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>117</v>
+      </c>
+      <c r="B148" t="str">
+        <f t="shared" si="2"/>
+        <v>u</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>118</v>
+      </c>
+      <c r="B149" t="str">
+        <f t="shared" si="2"/>
+        <v>v</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>119</v>
+      </c>
+      <c r="B150" t="str">
+        <f t="shared" si="2"/>
+        <v>w</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>120</v>
+      </c>
+      <c r="B151" t="str">
+        <f t="shared" si="2"/>
+        <v>x</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>121</v>
+      </c>
+      <c r="B152" t="str">
+        <f t="shared" si="2"/>
+        <v>y</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>122</v>
+      </c>
+      <c r="B153" t="str">
+        <f t="shared" si="2"/>
+        <v>z</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>123</v>
+      </c>
+      <c r="B154" t="str">
+        <f t="shared" si="2"/>
+        <v>{</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>124</v>
+      </c>
+      <c r="B155" t="str">
+        <f t="shared" si="2"/>
+        <v>|</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>125</v>
+      </c>
+      <c r="B156" t="str">
+        <f t="shared" si="2"/>
+        <v>}</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>126</v>
+      </c>
+      <c r="B157" t="str">
+        <f t="shared" si="2"/>
+        <v>~</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>127</v>
+      </c>
+      <c r="B158" t="str">
+        <f t="shared" si="2"/>
+        <v></v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>128</v>
+      </c>
+      <c r="B159" t="str">
+        <f t="shared" si="2"/>
+        <v>Ä</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>129</v>
+      </c>
+      <c r="B160" t="str">
+        <f t="shared" si="2"/>
+        <v>Å</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>130</v>
+      </c>
+      <c r="B161" t="str">
+        <f t="shared" ref="B161:B224" si="3">CHAR(A161)</f>
+        <v>Ç</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>131</v>
+      </c>
+      <c r="B162" t="str">
+        <f t="shared" si="3"/>
+        <v>É</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>132</v>
+      </c>
+      <c r="B163" t="str">
+        <f t="shared" si="3"/>
+        <v>Ñ</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>133</v>
+      </c>
+      <c r="B164" t="str">
+        <f t="shared" si="3"/>
+        <v>Ö</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>134</v>
+      </c>
+      <c r="B165" t="str">
+        <f t="shared" si="3"/>
+        <v>Ü</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>135</v>
+      </c>
+      <c r="B166" t="str">
+        <f t="shared" si="3"/>
+        <v>á</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>136</v>
+      </c>
+      <c r="B167" t="str">
+        <f t="shared" si="3"/>
+        <v>à</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>137</v>
+      </c>
+      <c r="B168" t="str">
+        <f t="shared" si="3"/>
+        <v>â</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>138</v>
+      </c>
+      <c r="B169" t="str">
+        <f t="shared" si="3"/>
+        <v>ä</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>139</v>
+      </c>
+      <c r="B170" t="str">
+        <f t="shared" si="3"/>
+        <v>ã</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>140</v>
+      </c>
+      <c r="B171" t="str">
+        <f t="shared" si="3"/>
+        <v>å</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>141</v>
+      </c>
+      <c r="B172" t="str">
+        <f t="shared" si="3"/>
+        <v>ç</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>142</v>
+      </c>
+      <c r="B173" t="str">
+        <f t="shared" si="3"/>
+        <v>é</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>143</v>
+      </c>
+      <c r="B174" t="str">
+        <f t="shared" si="3"/>
+        <v>è</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>144</v>
+      </c>
+      <c r="B175" t="str">
+        <f t="shared" si="3"/>
+        <v>ê</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>145</v>
+      </c>
+      <c r="B176" t="str">
+        <f t="shared" si="3"/>
+        <v>ë</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>146</v>
+      </c>
+      <c r="B177" t="str">
+        <f t="shared" si="3"/>
+        <v>í</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>147</v>
+      </c>
+      <c r="B178" t="str">
+        <f t="shared" si="3"/>
+        <v>ì</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>148</v>
+      </c>
+      <c r="B179" t="str">
+        <f t="shared" si="3"/>
+        <v>î</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>149</v>
+      </c>
+      <c r="B180" t="str">
+        <f t="shared" si="3"/>
+        <v>ï</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>150</v>
+      </c>
+      <c r="B181" t="str">
+        <f t="shared" si="3"/>
+        <v>ñ</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>151</v>
+      </c>
+      <c r="B182" t="str">
+        <f t="shared" si="3"/>
+        <v>ó</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>152</v>
+      </c>
+      <c r="B183" t="str">
+        <f t="shared" si="3"/>
+        <v>ò</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>153</v>
+      </c>
+      <c r="B184" t="str">
+        <f t="shared" si="3"/>
+        <v>ô</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>154</v>
+      </c>
+      <c r="B185" t="str">
+        <f t="shared" si="3"/>
+        <v>ö</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>155</v>
+      </c>
+      <c r="B186" t="str">
+        <f t="shared" si="3"/>
+        <v>õ</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>156</v>
+      </c>
+      <c r="B187" t="str">
+        <f t="shared" si="3"/>
+        <v>ú</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>157</v>
+      </c>
+      <c r="B188" t="str">
+        <f t="shared" si="3"/>
+        <v>ù</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>158</v>
+      </c>
+      <c r="B189" t="str">
+        <f t="shared" si="3"/>
+        <v>û</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>159</v>
+      </c>
+      <c r="B190" t="str">
+        <f t="shared" si="3"/>
+        <v>ü</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>160</v>
+      </c>
+      <c r="B191" t="str">
+        <f t="shared" si="3"/>
+        <v>†</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>161</v>
+      </c>
+      <c r="B192" t="str">
+        <f t="shared" si="3"/>
+        <v>°</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>162</v>
+      </c>
+      <c r="B193" t="str">
+        <f t="shared" si="3"/>
+        <v>¢</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>163</v>
+      </c>
+      <c r="B194" t="str">
+        <f t="shared" si="3"/>
+        <v>£</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>164</v>
+      </c>
+      <c r="B195" t="str">
+        <f t="shared" si="3"/>
+        <v>§</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>165</v>
+      </c>
+      <c r="B196" t="str">
+        <f t="shared" si="3"/>
+        <v>•</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>166</v>
+      </c>
+      <c r="B197" t="str">
+        <f t="shared" si="3"/>
+        <v>¶</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>167</v>
+      </c>
+      <c r="B198" t="str">
+        <f t="shared" si="3"/>
+        <v>ß</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>168</v>
+      </c>
+      <c r="B199" t="str">
+        <f t="shared" si="3"/>
+        <v>®</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>169</v>
+      </c>
+      <c r="B200" t="str">
+        <f t="shared" si="3"/>
+        <v>©</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>170</v>
+      </c>
+      <c r="B201" t="str">
+        <f t="shared" si="3"/>
+        <v>™</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>171</v>
+      </c>
+      <c r="B202" t="str">
+        <f t="shared" si="3"/>
+        <v>´</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>172</v>
+      </c>
+      <c r="B203" t="str">
+        <f t="shared" si="3"/>
+        <v>¨</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>173</v>
+      </c>
+      <c r="B204" t="str">
+        <f t="shared" si="3"/>
+        <v>≠</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>174</v>
+      </c>
+      <c r="B205" t="str">
+        <f t="shared" si="3"/>
+        <v>Æ</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>175</v>
+      </c>
+      <c r="B206" t="str">
+        <f t="shared" si="3"/>
+        <v>Ø</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>176</v>
+      </c>
+      <c r="B207" t="str">
+        <f t="shared" si="3"/>
+        <v>∞</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>177</v>
+      </c>
+      <c r="B208" t="str">
+        <f t="shared" si="3"/>
+        <v>±</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>178</v>
+      </c>
+      <c r="B209" t="str">
+        <f t="shared" si="3"/>
+        <v>≤</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>179</v>
+      </c>
+      <c r="B210" t="str">
+        <f t="shared" si="3"/>
+        <v>≥</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>180</v>
+      </c>
+      <c r="B211" t="str">
+        <f t="shared" si="3"/>
+        <v>¥</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>181</v>
+      </c>
+      <c r="B212" t="str">
+        <f t="shared" si="3"/>
+        <v>µ</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>182</v>
+      </c>
+      <c r="B213" t="str">
+        <f t="shared" si="3"/>
+        <v>∂</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>183</v>
+      </c>
+      <c r="B214" t="str">
+        <f t="shared" si="3"/>
+        <v>∑</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>184</v>
+      </c>
+      <c r="B215" t="str">
+        <f t="shared" si="3"/>
+        <v>∏</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>185</v>
+      </c>
+      <c r="B216" t="str">
+        <f t="shared" si="3"/>
+        <v>π</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>186</v>
+      </c>
+      <c r="B217" t="str">
+        <f t="shared" si="3"/>
+        <v>∫</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>187</v>
+      </c>
+      <c r="B218" t="str">
+        <f t="shared" si="3"/>
+        <v>ª</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>188</v>
+      </c>
+      <c r="B219" t="str">
+        <f t="shared" si="3"/>
+        <v>º</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>189</v>
+      </c>
+      <c r="B220" t="str">
+        <f t="shared" si="3"/>
+        <v>Ω</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>190</v>
+      </c>
+      <c r="B221" t="str">
+        <f t="shared" si="3"/>
+        <v>æ</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>191</v>
+      </c>
+      <c r="B222" t="str">
+        <f t="shared" si="3"/>
+        <v>ø</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>192</v>
+      </c>
+      <c r="B223" t="str">
+        <f t="shared" si="3"/>
+        <v>¿</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>193</v>
+      </c>
+      <c r="B224" t="str">
+        <f t="shared" si="3"/>
+        <v>¡</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>194</v>
+      </c>
+      <c r="B225" t="str">
+        <f t="shared" ref="B225:B286" si="4">CHAR(A225)</f>
+        <v>¬</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>195</v>
+      </c>
+      <c r="B226" t="str">
+        <f t="shared" si="4"/>
+        <v>√</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>196</v>
+      </c>
+      <c r="B227" t="str">
+        <f t="shared" si="4"/>
+        <v>ƒ</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>197</v>
+      </c>
+      <c r="B228" t="str">
+        <f t="shared" si="4"/>
+        <v>≈</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>198</v>
+      </c>
+      <c r="B229" t="str">
+        <f t="shared" si="4"/>
+        <v>∆</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>199</v>
+      </c>
+      <c r="B230" t="str">
+        <f t="shared" si="4"/>
+        <v>«</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>200</v>
+      </c>
+      <c r="B231" t="str">
+        <f t="shared" si="4"/>
+        <v>»</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>201</v>
+      </c>
+      <c r="B232" t="str">
+        <f t="shared" si="4"/>
+        <v>…</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>202</v>
+      </c>
+      <c r="B233" t="str">
+        <f t="shared" si="4"/>
+        <v> </v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>203</v>
+      </c>
+      <c r="B234" t="str">
+        <f t="shared" si="4"/>
+        <v>À</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>204</v>
+      </c>
+      <c r="B235" t="str">
+        <f t="shared" si="4"/>
+        <v>Ã</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>205</v>
+      </c>
+      <c r="B236" t="str">
+        <f t="shared" si="4"/>
+        <v>Õ</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>206</v>
+      </c>
+      <c r="B237" t="str">
+        <f t="shared" si="4"/>
+        <v>Œ</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>207</v>
+      </c>
+      <c r="B238" t="str">
+        <f t="shared" si="4"/>
+        <v>œ</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>208</v>
+      </c>
+      <c r="B239" t="str">
+        <f t="shared" si="4"/>
+        <v>–</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>209</v>
+      </c>
+      <c r="B240" t="str">
+        <f t="shared" si="4"/>
+        <v>—</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>210</v>
+      </c>
+      <c r="B241" t="str">
+        <f t="shared" si="4"/>
+        <v>“</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>211</v>
+      </c>
+      <c r="B242" t="str">
+        <f t="shared" si="4"/>
+        <v>”</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>212</v>
+      </c>
+      <c r="B243" t="str">
+        <f t="shared" si="4"/>
+        <v>‘</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>213</v>
+      </c>
+      <c r="B244" t="str">
+        <f t="shared" si="4"/>
+        <v>’</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>214</v>
+      </c>
+      <c r="B245" t="str">
+        <f t="shared" si="4"/>
+        <v>÷</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>215</v>
+      </c>
+      <c r="B246" t="str">
+        <f t="shared" si="4"/>
+        <v>◊</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>216</v>
+      </c>
+      <c r="B247" t="str">
+        <f t="shared" si="4"/>
+        <v>ÿ</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>217</v>
+      </c>
+      <c r="B248" t="str">
+        <f t="shared" si="4"/>
+        <v>Ÿ</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>218</v>
+      </c>
+      <c r="B249" t="str">
+        <f t="shared" si="4"/>
+        <v>⁄</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>219</v>
+      </c>
+      <c r="B250" t="str">
+        <f t="shared" si="4"/>
+        <v>€</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>220</v>
+      </c>
+      <c r="B251" t="str">
+        <f t="shared" si="4"/>
+        <v>‹</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>221</v>
+      </c>
+      <c r="B252" t="str">
+        <f t="shared" si="4"/>
+        <v>›</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>222</v>
+      </c>
+      <c r="B253" t="str">
+        <f t="shared" si="4"/>
+        <v>ﬁ</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>223</v>
+      </c>
+      <c r="B254" t="str">
+        <f t="shared" si="4"/>
+        <v>ﬂ</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>224</v>
+      </c>
+      <c r="B255" t="str">
+        <f t="shared" si="4"/>
+        <v>‡</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>225</v>
+      </c>
+      <c r="B256" t="str">
+        <f t="shared" si="4"/>
+        <v>·</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>226</v>
+      </c>
+      <c r="B257" t="str">
+        <f t="shared" si="4"/>
+        <v>‚</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>227</v>
+      </c>
+      <c r="B258" t="str">
+        <f t="shared" si="4"/>
+        <v>„</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>228</v>
+      </c>
+      <c r="B259" t="str">
+        <f t="shared" si="4"/>
+        <v>‰</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>229</v>
+      </c>
+      <c r="B260" t="str">
+        <f t="shared" si="4"/>
+        <v>Â</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>230</v>
+      </c>
+      <c r="B261" t="str">
+        <f t="shared" si="4"/>
+        <v>Ê</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>231</v>
+      </c>
+      <c r="B262" t="str">
+        <f t="shared" si="4"/>
+        <v>Á</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>232</v>
+      </c>
+      <c r="B263" t="str">
+        <f t="shared" si="4"/>
+        <v>Ë</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>233</v>
+      </c>
+      <c r="B264" t="str">
+        <f t="shared" si="4"/>
+        <v>È</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>234</v>
+      </c>
+      <c r="B265" t="str">
+        <f t="shared" si="4"/>
+        <v>Í</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>235</v>
+      </c>
+      <c r="B266" t="str">
+        <f t="shared" si="4"/>
+        <v>Î</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>236</v>
+      </c>
+      <c r="B267" t="str">
+        <f t="shared" si="4"/>
+        <v>Ï</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>237</v>
+      </c>
+      <c r="B268" t="str">
+        <f t="shared" si="4"/>
+        <v>Ì</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>238</v>
+      </c>
+      <c r="B269" t="str">
+        <f t="shared" si="4"/>
+        <v>Ó</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>239</v>
+      </c>
+      <c r="B270" t="str">
+        <f t="shared" si="4"/>
+        <v>Ô</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>240</v>
+      </c>
+      <c r="B271" t="str">
+        <f t="shared" si="4"/>
+        <v></v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>241</v>
+      </c>
+      <c r="B272" t="str">
+        <f t="shared" si="4"/>
+        <v>Ò</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>242</v>
+      </c>
+      <c r="B273" t="str">
+        <f t="shared" si="4"/>
+        <v>Ú</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>243</v>
+      </c>
+      <c r="B274" t="str">
+        <f t="shared" si="4"/>
+        <v>Û</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>244</v>
+      </c>
+      <c r="B275" t="str">
+        <f t="shared" si="4"/>
+        <v>Ù</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>245</v>
+      </c>
+      <c r="B276" t="str">
+        <f t="shared" si="4"/>
+        <v>ı</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>246</v>
+      </c>
+      <c r="B277" t="str">
+        <f t="shared" si="4"/>
+        <v>ˆ</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>247</v>
+      </c>
+      <c r="B278" t="str">
+        <f t="shared" si="4"/>
+        <v>˜</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>248</v>
+      </c>
+      <c r="B279" t="str">
+        <f t="shared" si="4"/>
+        <v>¯</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>249</v>
+      </c>
+      <c r="B280" t="str">
+        <f t="shared" si="4"/>
+        <v>˘</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>250</v>
+      </c>
+      <c r="B281" t="str">
+        <f t="shared" si="4"/>
+        <v>˙</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <v>251</v>
+      </c>
+      <c r="B282" t="str">
+        <f t="shared" si="4"/>
+        <v>˚</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <v>252</v>
+      </c>
+      <c r="B283" t="str">
+        <f t="shared" si="4"/>
+        <v>¸</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <v>253</v>
+      </c>
+      <c r="B284" t="str">
+        <f t="shared" si="4"/>
+        <v>˝</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A285">
+        <v>254</v>
+      </c>
+      <c r="B285" t="str">
+        <f t="shared" si="4"/>
+        <v>˛</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A286">
+        <v>255</v>
+      </c>
+      <c r="B286" t="str">
+        <f t="shared" si="4"/>
+        <v>ˇ</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -17511,8 +19787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:BJ56"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A34" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -19378,7 +21654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AV59"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="200" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -22061,7 +24337,7 @@
   <dimension ref="A1:BJ41"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -22245,50 +24521,166 @@
       </c>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.15">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="6"/>
-      <c r="AI5" s="6"/>
-      <c r="AJ5" s="6"/>
-      <c r="AK5" s="6"/>
-      <c r="AL5" s="6"/>
-      <c r="AM5" s="6"/>
-      <c r="AN5" s="6"/>
-      <c r="AO5" s="6"/>
-      <c r="AP5" s="6"/>
-      <c r="AQ5" s="6"/>
-      <c r="AR5" s="6"/>
-      <c r="AS5" s="6"/>
-      <c r="AT5" s="6"/>
-      <c r="AU5" s="6"/>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>157</v>
+      </c>
+      <c r="D5" s="4">
+        <v>65</v>
+      </c>
+      <c r="E5" s="4">
+        <v>65.8</v>
+      </c>
+      <c r="F5" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6" t="e">
+        <f>#VALUE!</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K5" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L5" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M5" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N5" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O5" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P5" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q5" s="6" t="e">
+        <f>CHAR(B5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R5" s="6" t="str">
+        <f>CHAR(C5)</f>
+        <v>ù</v>
+      </c>
+      <c r="S5" s="6" t="str">
+        <f t="shared" ref="R5:U5" si="0">CHAR(D5)</f>
+        <v>A</v>
+      </c>
+      <c r="T5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="U5" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V5" s="6" t="e">
+        <f t="shared" ref="V5" si="1">CHAR(G5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W5" s="6" t="e">
+        <f t="shared" ref="W5" si="2">CHAR(H5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X5" s="6" t="str">
+        <f>CHAR(I5)</f>
+        <v>_x0001_</v>
+      </c>
+      <c r="Y5" s="6" t="e">
+        <f t="shared" ref="Y5" si="3">CHAR(J5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z5" s="6" t="e">
+        <f t="shared" ref="Z5" si="4">CHAR(K5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA5" s="6" t="e">
+        <f t="shared" ref="AA5" si="5">CHAR(L5)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB5" s="6" t="e">
+        <f t="shared" ref="AB5" si="6">CHAR(M5)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC5" s="6" t="e">
+        <f t="shared" ref="AC5" si="7">CHAR(N5)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD5" s="6" t="e">
+        <f t="shared" ref="AD5" si="8">CHAR(O5)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE5" s="6" t="e">
+        <f t="shared" ref="AE5:AF5" si="9">CHAR(P5)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF5" s="6" t="e">
+        <f>CHAR(B5:P5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG5" s="6" t="e">
+        <f t="array" ref="AG5:AV5">CHAR(B5:P5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AH5" s="6" t="str">
+        <v>ù</v>
+      </c>
+      <c r="AI5" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="AJ5" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="AK5" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL5" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM5" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN5" s="6" t="str">
+        <v>_x0001_</v>
+      </c>
+      <c r="AO5" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP5" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ5" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR5" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS5" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT5" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU5" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV5" s="4" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
@@ -22414,19 +24806,19 @@
         <v>023</v>
       </c>
       <c r="R8" s="6" t="str">
-        <f t="shared" ref="R8:U8" si="0">_xlfn.CONCAT(C8,D8,E8)</f>
+        <f t="shared" ref="R8:U8" si="10">_xlfn.CONCAT(C8,D8,E8)</f>
         <v>2310</v>
       </c>
       <c r="S8" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>310-1</v>
       </c>
       <c r="T8" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>10-1</v>
       </c>
       <c r="U8" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>-1ciao</v>
       </c>
       <c r="V8" s="6" t="str">
@@ -22434,39 +24826,39 @@
         <v>ciaoTRUE</v>
       </c>
       <c r="W8" s="6" t="e">
-        <f t="shared" ref="W8" si="1">_xlfn.CONCAT(H8,I8,J8)</f>
+        <f t="shared" ref="W8" si="11">_xlfn.CONCAT(H8,I8,J8)</f>
         <v>#VALUE!</v>
       </c>
       <c r="X8" s="6" t="e">
-        <f t="shared" ref="X8" si="2">_xlfn.CONCAT(I8,J8,K8)</f>
+        <f t="shared" ref="X8" si="12">_xlfn.CONCAT(I8,J8,K8)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Y8" s="6" t="e">
-        <f t="shared" ref="Y8" si="3">_xlfn.CONCAT(J8,K8,L8)</f>
+        <f t="shared" ref="Y8" si="13">_xlfn.CONCAT(J8,K8,L8)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z8" s="6" t="e">
-        <f t="shared" ref="Z8" si="4">_xlfn.CONCAT(K8,L8,M8)</f>
+        <f t="shared" ref="Z8" si="14">_xlfn.CONCAT(K8,L8,M8)</f>
         <v>#N/A</v>
       </c>
       <c r="AA8" s="6" t="e">
-        <f t="shared" ref="AA8" si="5">_xlfn.CONCAT(L8,M8,N8)</f>
+        <f t="shared" ref="AA8" si="15">_xlfn.CONCAT(L8,M8,N8)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB8" s="6" t="e">
-        <f t="shared" ref="AB8" si="6">_xlfn.CONCAT(M8,N8,O8)</f>
+        <f t="shared" ref="AB8" si="16">_xlfn.CONCAT(M8,N8,O8)</f>
         <v>#NAME?</v>
       </c>
       <c r="AC8" s="6" t="e">
-        <f t="shared" ref="AC8" si="7">_xlfn.CONCAT(N8,O8,P8)</f>
+        <f t="shared" ref="AC8" si="17">_xlfn.CONCAT(N8,O8,P8)</f>
         <v>#NULL!</v>
       </c>
       <c r="AD8" s="6" t="e">
-        <f t="shared" ref="AD8" si="8">_xlfn.CONCAT(O8,P8,Q8)</f>
+        <f t="shared" ref="AD8" si="18">_xlfn.CONCAT(O8,P8,Q8)</f>
         <v>#NUM!</v>
       </c>
       <c r="AE8" s="6" t="e">
-        <f t="shared" ref="AE8" si="9">_xlfn.CONCAT(P8,Q8,R8)</f>
+        <f t="shared" ref="AE8" si="19">_xlfn.CONCAT(P8,Q8,R8)</f>
         <v>#REF!</v>
       </c>
       <c r="AF8" s="6" t="str">
@@ -22577,59 +24969,59 @@
         <v>023</v>
       </c>
       <c r="R9" s="6" t="str">
-        <f t="shared" ref="R9:X9" si="10">CONCATENATE(C9,D9,E9)</f>
+        <f t="shared" ref="R9:X9" si="20">CONCATENATE(C9,D9,E9)</f>
         <v>2310</v>
       </c>
       <c r="S9" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="20"/>
         <v>310-1</v>
       </c>
       <c r="T9" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="20"/>
         <v>10-1</v>
       </c>
       <c r="U9" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="20"/>
         <v>-1ciao</v>
       </c>
       <c r="V9" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="20"/>
         <v>ciaoTRUE</v>
       </c>
       <c r="W9" s="6" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="X9" s="6" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y9" s="6" t="e">
-        <f t="shared" ref="Y9" si="11">CONCATENATE(J9,K9,L9)</f>
+        <f t="shared" ref="Y9" si="21">CONCATENATE(J9,K9,L9)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z9" s="6" t="e">
-        <f t="shared" ref="Z9" si="12">CONCATENATE(K9,L9,M9)</f>
+        <f t="shared" ref="Z9" si="22">CONCATENATE(K9,L9,M9)</f>
         <v>#N/A</v>
       </c>
       <c r="AA9" s="6" t="e">
-        <f t="shared" ref="AA9" si="13">CONCATENATE(L9,M9,N9)</f>
+        <f t="shared" ref="AA9" si="23">CONCATENATE(L9,M9,N9)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB9" s="6" t="e">
-        <f t="shared" ref="AB9" si="14">CONCATENATE(M9,N9,O9)</f>
+        <f t="shared" ref="AB9" si="24">CONCATENATE(M9,N9,O9)</f>
         <v>#NAME?</v>
       </c>
       <c r="AC9" s="6" t="e">
-        <f t="shared" ref="AC9" si="15">CONCATENATE(N9,O9,P9)</f>
+        <f t="shared" ref="AC9" si="25">CONCATENATE(N9,O9,P9)</f>
         <v>#NULL!</v>
       </c>
       <c r="AD9" s="6" t="e">
-        <f t="shared" ref="AD9" si="16">CONCATENATE(O9,P9,Q9)</f>
+        <f t="shared" ref="AD9" si="26">CONCATENATE(O9,P9,Q9)</f>
         <v>#NUM!</v>
       </c>
       <c r="AE9" s="6" t="e">
-        <f t="shared" ref="AE9" si="17">CONCATENATE(P9,Q9,R9)</f>
+        <f t="shared" ref="AE9" si="27">CONCATENATE(P9,Q9,R9)</f>
         <v>#REF!</v>
       </c>
       <c r="AF9" s="6" t="e">
@@ -22778,35 +25170,35 @@
         <v>#VALUE!</v>
       </c>
       <c r="X13" s="4">
-        <f t="shared" ref="X13:AE13" si="18">FIND("ia","ciao",I13)</f>
+        <f t="shared" ref="X13:AE13" si="28">FIND("ia","ciao",I13)</f>
         <v>2</v>
       </c>
       <c r="Y13" s="4" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z13" s="4" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>#N/A</v>
       </c>
       <c r="AA13" s="4" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB13" s="4" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>#NAME?</v>
       </c>
       <c r="AC13" s="4" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>#NULL!</v>
       </c>
       <c r="AD13" s="4" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>#NUM!</v>
       </c>
       <c r="AE13" s="4" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>#REF!</v>
       </c>
       <c r="AF13" s="4">
@@ -22935,7 +25327,7 @@
         <v/>
       </c>
       <c r="R16" s="4" t="str">
-        <f t="shared" ref="R16:U16" si="19">LEFT("ciao",C16)</f>
+        <f t="shared" ref="R16:U16" si="29">LEFT("ciao",C16)</f>
         <v>c</v>
       </c>
       <c r="S16" s="4" t="str">
@@ -22943,11 +25335,11 @@
         <v>2.</v>
       </c>
       <c r="T16" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="29"/>
         <v>ciao</v>
       </c>
       <c r="U16" s="4" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="29"/>
         <v>#VALUE!</v>
       </c>
       <c r="V16" s="4" t="str">
@@ -22963,31 +25355,31 @@
         <v>c</v>
       </c>
       <c r="Y16" s="4" t="e">
-        <f t="shared" ref="Y16:AE16" si="20">LEFT("ciao",J16)</f>
+        <f t="shared" ref="Y16:AE16" si="30">LEFT("ciao",J16)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z16" s="4" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>#N/A</v>
       </c>
       <c r="AA16" s="4" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB16" s="4" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>#NAME?</v>
       </c>
       <c r="AC16" s="4" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>#NULL!</v>
       </c>
       <c r="AD16" s="4" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>#NUM!</v>
       </c>
       <c r="AE16" s="4" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>#REF!</v>
       </c>
       <c r="AF16" s="4" t="str">
@@ -23103,59 +25495,59 @@
         <v>1</v>
       </c>
       <c r="R18" s="4">
-        <f t="shared" ref="R18:AE18" si="21">LEN(C18)</f>
+        <f t="shared" ref="R18:AE18" si="31">LEN(C18)</f>
         <v>3</v>
       </c>
       <c r="S18" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>3</v>
       </c>
       <c r="T18" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>2</v>
       </c>
       <c r="U18" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>2</v>
       </c>
       <c r="V18" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="W18" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="X18" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="Y18" s="4" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z18" s="4" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>#N/A</v>
       </c>
       <c r="AA18" s="4" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB18" s="4" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>#NAME?</v>
       </c>
       <c r="AC18" s="4" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>#NULL!</v>
       </c>
       <c r="AD18" s="4" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>#NUM!</v>
       </c>
       <c r="AE18" s="4" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>#REF!</v>
       </c>
       <c r="AF18" s="4" t="e">
@@ -23270,59 +25662,59 @@
         <v>0</v>
       </c>
       <c r="R20" s="4" t="str">
-        <f t="shared" ref="R20:AE20" si="22">LOWER(C20)</f>
+        <f t="shared" ref="R20:AE20" si="32">LOWER(C20)</f>
         <v>1.9</v>
       </c>
       <c r="S20" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>2.3</v>
       </c>
       <c r="T20" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>10</v>
       </c>
       <c r="U20" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>-1</v>
       </c>
       <c r="V20" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="W20" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>ciao</v>
       </c>
       <c r="X20" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>true</v>
       </c>
       <c r="Y20" s="4" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z20" s="4" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>#N/A</v>
       </c>
       <c r="AA20" s="4" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB20" s="4" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>#NAME?</v>
       </c>
       <c r="AC20" s="4" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>#NULL!</v>
       </c>
       <c r="AD20" s="4" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>#NUM!</v>
       </c>
       <c r="AE20" s="4" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>#REF!</v>
       </c>
       <c r="AF20" s="4" t="e">
@@ -23464,27 +25856,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z21" s="4" t="e">
-        <f t="shared" ref="Z21:AE21" si="23">MID("ciao",K21,2)</f>
+        <f t="shared" ref="Z21:AE21" si="33">MID("ciao",K21,2)</f>
         <v>#N/A</v>
       </c>
       <c r="AA21" s="4" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB21" s="4" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>#NAME?</v>
       </c>
       <c r="AC21" s="4" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>#NULL!</v>
       </c>
       <c r="AD21" s="4" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>#NUM!</v>
       </c>
       <c r="AE21" s="4" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>#REF!</v>
       </c>
       <c r="AF21" s="4" t="str">
@@ -23647,27 +26039,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z26" s="4" t="e">
-        <f t="shared" ref="Z26:AE26" si="24">REPLACE("ciao",K26,2,"vv")</f>
+        <f t="shared" ref="Z26:AE26" si="34">REPLACE("ciao",K26,2,"vv")</f>
         <v>#N/A</v>
       </c>
       <c r="AA26" s="4" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB26" s="4" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>#NAME?</v>
       </c>
       <c r="AC26" s="4" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>#NULL!</v>
       </c>
       <c r="AD26" s="4" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>#NUM!</v>
       </c>
       <c r="AE26" s="4" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>#REF!</v>
       </c>
       <c r="AF26" s="4" t="str">
@@ -23796,51 +26188,51 @@
         <v>3</v>
       </c>
       <c r="T29" s="4" t="str">
-        <f t="shared" ref="T29:AE29" si="25">RIGHT("ciao",E29)</f>
+        <f t="shared" ref="T29:AE29" si="35">RIGHT("ciao",E29)</f>
         <v>ciao</v>
       </c>
       <c r="U29" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>#VALUE!</v>
       </c>
       <c r="V29" s="4" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="W29" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>#VALUE!</v>
       </c>
       <c r="X29" s="4" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>o</v>
       </c>
       <c r="Y29" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z29" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>#N/A</v>
       </c>
       <c r="AA29" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB29" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>#NAME?</v>
       </c>
       <c r="AC29" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>#NULL!</v>
       </c>
       <c r="AD29" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>#NUM!</v>
       </c>
       <c r="AE29" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>#REF!</v>
       </c>
       <c r="AF29" s="4" t="str">
@@ -23956,11 +26348,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="R31" s="4">
-        <f t="shared" ref="R31:Z31" si="26">SEARCH("BASE","database",C31)</f>
+        <f t="shared" ref="R31:Z31" si="36">SEARCH("BASE","database",C31)</f>
         <v>5</v>
       </c>
       <c r="S31" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>5</v>
       </c>
       <c r="T31" s="4" t="e">
@@ -23980,31 +26372,31 @@
         <v>#VALUE!</v>
       </c>
       <c r="X31" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>5</v>
       </c>
       <c r="Y31" s="4" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z31" s="4" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>#N/A</v>
       </c>
       <c r="AA31" s="4" t="e">
-        <f t="shared" ref="AA31" si="27">SEARCH("BASE","database",L31)</f>
+        <f t="shared" ref="AA31" si="37">SEARCH("BASE","database",L31)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB31" s="4" t="e">
-        <f t="shared" ref="AB31" si="28">SEARCH("BASE","database",M31)</f>
+        <f t="shared" ref="AB31" si="38">SEARCH("BASE","database",M31)</f>
         <v>#NAME?</v>
       </c>
       <c r="AC31" s="4" t="e">
-        <f t="shared" ref="AC31" si="29">SEARCH("BASE","database",N31)</f>
+        <f t="shared" ref="AC31" si="39">SEARCH("BASE","database",N31)</f>
         <v>#NULL!</v>
       </c>
       <c r="AD31" s="4" t="e">
-        <f t="shared" ref="AD31" si="30">SEARCH("BASE","database",O31)</f>
+        <f t="shared" ref="AD31" si="40">SEARCH("BASE","database",O31)</f>
         <v>#NUM!</v>
       </c>
       <c r="AE31" s="4" t="e">
@@ -24135,19 +26527,19 @@
         <v>.00</v>
       </c>
       <c r="R35" s="4" t="str">
-        <f t="shared" ref="R35:U35" si="31">TEXT(C35,"#.00")</f>
+        <f t="shared" ref="R35:U35" si="41">TEXT(C35,"#.00")</f>
         <v>1.90</v>
       </c>
       <c r="S35" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>2.30</v>
       </c>
       <c r="T35" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>10.00</v>
       </c>
       <c r="U35" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>-1.00</v>
       </c>
       <c r="V35" s="4" t="str">
@@ -24155,39 +26547,39 @@
         <v>.00</v>
       </c>
       <c r="W35" s="4" t="str">
-        <f t="shared" ref="W35:AE35" si="32">TEXT(H35,"#.00")</f>
+        <f t="shared" ref="W35:AE35" si="42">TEXT(H35,"#.00")</f>
         <v>32015.00</v>
       </c>
       <c r="X35" s="4" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>TRUE</v>
       </c>
       <c r="Y35" s="4" t="e">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z35" s="4" t="e">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>#N/A</v>
       </c>
       <c r="AA35" s="4" t="e">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB35" s="4" t="e">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>#NAME?</v>
       </c>
       <c r="AC35" s="4" t="e">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>#NULL!</v>
       </c>
       <c r="AD35" s="4" t="e">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>#NUM!</v>
       </c>
       <c r="AE35" s="4" t="e">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>#REF!</v>
       </c>
       <c r="AF35" s="4" t="e">
@@ -24302,59 +26694,59 @@
         <v>0</v>
       </c>
       <c r="R37" s="4" t="str">
-        <f t="shared" ref="R37:AE37" si="33">TRIM(C37)</f>
+        <f t="shared" ref="R37:AE37" si="43">TRIM(C37)</f>
         <v>1.9</v>
       </c>
       <c r="S37" s="4" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>2.3</v>
       </c>
       <c r="T37" s="4" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>10</v>
       </c>
       <c r="U37" s="4" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>-1</v>
       </c>
       <c r="V37" s="4" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="W37" s="4" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>ciao</v>
       </c>
       <c r="X37" s="4" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>TRUE</v>
       </c>
       <c r="Y37" s="4" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z37" s="4" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>#N/A</v>
       </c>
       <c r="AA37" s="4" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB37" s="4" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>#NAME?</v>
       </c>
       <c r="AC37" s="4" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>#NULL!</v>
       </c>
       <c r="AD37" s="4" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>#NUM!</v>
       </c>
       <c r="AE37" s="4" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>#REF!</v>
       </c>
       <c r="AF37" s="4" t="e">
@@ -24474,59 +26866,59 @@
         <v>0</v>
       </c>
       <c r="R40" s="4" t="str">
-        <f t="shared" ref="R40:AE40" si="34">UPPER(C40)</f>
+        <f t="shared" ref="R40:AE40" si="44">UPPER(C40)</f>
         <v>1.9</v>
       </c>
       <c r="S40" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>2.3</v>
       </c>
       <c r="T40" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>10</v>
       </c>
       <c r="U40" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>-1</v>
       </c>
       <c r="V40" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="W40" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>CIAO</v>
       </c>
       <c r="X40" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>TRUE</v>
       </c>
       <c r="Y40" s="4" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z40" s="4" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>#N/A</v>
       </c>
       <c r="AA40" s="4" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB40" s="4" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>#NAME?</v>
       </c>
       <c r="AC40" s="4" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>#NULL!</v>
       </c>
       <c r="AD40" s="4" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>#NUM!</v>
       </c>
       <c r="AE40" s="4" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>#REF!</v>
       </c>
       <c r="AF40" s="4" t="e">
@@ -24632,63 +27024,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q41" s="4">
-        <f t="shared" ref="Q41:AE41" si="35">VALUE(B41)</f>
+        <f t="shared" ref="Q41:AE41" si="45">VALUE(B41)</f>
         <v>0</v>
       </c>
       <c r="R41" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>1.9</v>
       </c>
       <c r="S41" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="T41" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>10</v>
       </c>
       <c r="U41" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>-1</v>
       </c>
       <c r="V41" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="W41" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>32015</v>
       </c>
       <c r="X41" s="4" t="e">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y41" s="4" t="e">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z41" s="4" t="e">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>#N/A</v>
       </c>
       <c r="AA41" s="4" t="e">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB41" s="4" t="e">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>#NAME?</v>
       </c>
       <c r="AC41" s="4" t="e">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>#NULL!</v>
       </c>
       <c r="AD41" s="4" t="e">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>#NUM!</v>
       </c>
       <c r="AE41" s="4" t="e">
-        <f t="shared" si="35"/>
+        <f t="shared" si="45"/>
         <v>#REF!</v>
       </c>
       <c r="AF41" s="4" t="e">
@@ -27692,8 +30084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AV113"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A22" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -37296,7 +39688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BJ74"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -44315,12 +46707,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -44332,6 +46718,12 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -44346,7 +46738,7 @@
   <dimension ref="A1:BJ22"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="AJ11" sqref="AJ11"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -44541,7 +46933,7 @@
       <c r="F3" s="4">
         <v>-1</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
         <v>428</v>
       </c>
@@ -44588,7 +46980,7 @@
         <v>0</v>
       </c>
       <c r="U3" s="4" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(F3,TRUE)</f>
         <v>1</v>
       </c>
       <c r="V3" s="4" t="b">
@@ -44604,7 +46996,7 @@
         <v>0</v>
       </c>
       <c r="Y3" s="4" t="e">
-        <f t="shared" si="0"/>
+        <f>AND(J3,TRUE)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z3" s="4" t="e">

</xml_diff>

<commit_message>
feat(tokens), #139: Allow last parameters to be empty in a function call.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BE37C7-CC90-E74E-A0A4-1CEC46659974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7149CA-5432-5844-A5EC-14287F69D629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15760" tabRatio="770" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15760" tabRatio="770" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -12707,8 +12707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T286"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13341,6 +13341,10 @@
         <f t="array" ref="D29:D30">_xlfn.IFS(C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,C27:C28,E27:E28,TRUE,D27:D28)</f>
         <v>5</v>
       </c>
+      <c r="F29">
+        <f>IF(,,4)</f>
+        <v>4</v>
+      </c>
       <c r="H29">
         <v>3</v>
       </c>
@@ -13362,6 +13366,10 @@
       </c>
       <c r="D30">
         <v>6</v>
+      </c>
+      <c r="F30">
+        <f>IF(,4,)</f>
+        <v>0</v>
       </c>
       <c r="H30">
         <f>AVERAGE(H26:H29)</f>
@@ -25404,8 +25412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BJ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="AF9" sqref="AF9"/>
+    <sheetView topLeftCell="K1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -47895,6 +47903,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -47906,12 +47920,6 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat(functions), #109, #111, #124, #125: Update test cases.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7149CA-5432-5844-A5EC-14287F69D629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB80B16A-A7D7-F241-B525-D45E6780C511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15760" tabRatio="770" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="10400" tabRatio="770" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -33,6 +33,8 @@
     <externalReference r:id="rId16"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_1234\5678\90">CORE!$G$21</definedName>
+    <definedName name="_1234\5678\91">CORE!$F$21</definedName>
     <definedName name="a">CORE!$B$2:$C$3</definedName>
     <definedName name="b">CORE!$D$2:$E$3</definedName>
     <definedName name="d">CORE!$B$4:$C$5</definedName>
@@ -89,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="511">
   <si>
     <t>ca</t>
   </si>
@@ -2151,8 +2153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV81"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A60" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -12027,50 +12029,165 @@
       </c>
     </row>
     <row r="75" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G75" s="6"/>
-      <c r="H75" s="6"/>
-      <c r="I75" s="6"/>
-      <c r="J75" s="6"/>
-      <c r="K75" s="6"/>
-      <c r="L75" s="6"/>
-      <c r="M75" s="6"/>
-      <c r="N75" s="6"/>
-      <c r="O75" s="6"/>
-      <c r="P75" s="6"/>
-      <c r="Q75" s="6"/>
-      <c r="R75" s="6"/>
-      <c r="S75" s="6"/>
-      <c r="T75" s="6"/>
-      <c r="U75" s="6"/>
-      <c r="V75" s="6"/>
-      <c r="W75" s="6"/>
-      <c r="X75" s="6"/>
-      <c r="Y75" s="6"/>
-      <c r="Z75" s="6"/>
-      <c r="AA75" s="6"/>
-      <c r="AB75" s="6"/>
-      <c r="AC75" s="6"/>
-      <c r="AD75" s="6"/>
-      <c r="AE75" s="6"/>
-      <c r="AF75" s="9"/>
-      <c r="AG75" s="6"/>
-      <c r="AH75" s="6"/>
-      <c r="AI75" s="6"/>
-      <c r="AJ75" s="6"/>
-      <c r="AK75" s="6"/>
-      <c r="AL75" s="6"/>
-      <c r="AM75" s="6"/>
-      <c r="AN75" s="6"/>
-      <c r="AO75" s="6"/>
-      <c r="AP75" s="6"/>
-      <c r="AQ75" s="6"/>
-      <c r="AR75" s="6"/>
-      <c r="AS75" s="6"/>
-      <c r="AT75" s="6"/>
-      <c r="AU75" s="6"/>
+      <c r="B75" s="12">
+        <v>0</v>
+      </c>
+      <c r="C75" s="12">
+        <v>2</v>
+      </c>
+      <c r="D75" s="12">
+        <v>1.2</v>
+      </c>
+      <c r="E75" s="12">
+        <v>-4</v>
+      </c>
+      <c r="F75" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="G75" s="33"/>
+      <c r="H75" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="I75" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J75" s="33" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K75" s="33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L75" s="33" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M75" s="33" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N75" s="33" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O75" s="33" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P75" s="33" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q75" s="33">
+        <f>SUMSQ(B75:C75,C75:D75,D75:E75)</f>
+        <v>26.88</v>
+      </c>
+      <c r="R75" s="33">
+        <f>SUMSQ(C75:D75,D75:E75,E75:F75)</f>
+        <v>40.569999999999993</v>
+      </c>
+      <c r="S75" s="33">
+        <f>SUMSQ(E75:F75,E75:F75,C75:D75)</f>
+        <v>40.819999999999993</v>
+      </c>
+      <c r="T75" s="33">
+        <f>SUMSQ(E75:F75,B75:C75,C75:D75)</f>
+        <v>27.130000000000003</v>
+      </c>
+      <c r="U75" s="33">
+        <f>SUMSQ(D75:F75,B75:D75,C75:E75)</f>
+        <v>46.010000000000005</v>
+      </c>
+      <c r="V75" s="33">
+        <f>SUMSQ(E75:F75,F75:G75,D75:E75)</f>
+        <v>36.820000000000007</v>
+      </c>
+      <c r="W75" s="33">
+        <f>SUMSQ(G75:H75,D75:E75,E75:F75)</f>
+        <v>35.129999999999995</v>
+      </c>
+      <c r="X75" s="33">
+        <f>SUMSQ(H75:I75,E75:F75,F75:G75)</f>
+        <v>19.380000000000003</v>
+      </c>
+      <c r="Y75" s="33" t="e">
+        <f>SUMSQ(J75:K75,B75:C75,C75:D75)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z75" s="33" t="e">
+        <f>SUMSQ(K75:L75,C75:D75,D75:E75)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA75" s="33" t="e">
+        <f>SUMSQ(L75:M75,D75:E75,E75:F75)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB75" s="33" t="e">
+        <f>SUMSQ(M75:N75,E75:F75,F75:G75)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC75" s="33" t="e">
+        <f>SUMSQ(N75:O75,F75:G75,G75:H75)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD75" s="33" t="e">
+        <f>SUMSQ(O75:P75,G75:H75,H75:J75)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE75" s="33" t="e">
+        <f>SUMSQ(P75:Q75,H75:J75,J75:K75)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF75" s="33">
+        <f>SUMSQ(C75:G75,B75:F75)</f>
+        <v>46.26</v>
+      </c>
+      <c r="AG75" s="33">
+        <f t="array" ref="AG75:AV75">SUMSQ(C75:G75,B75:F75)</f>
+        <v>46.26</v>
+      </c>
+      <c r="AH75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AI75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AJ75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AK75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AL75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AM75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AN75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AO75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AP75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AQ75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AR75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AS75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AT75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AU75" s="33">
+        <v>46.26</v>
+      </c>
+      <c r="AV75" s="12">
+        <v>46.26</v>
+      </c>
     </row>
     <row r="76" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A76" s="4" t="s">
@@ -12707,8 +12824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13256,6 +13373,10 @@
       <c r="E25" t="e">
         <f>REF!#REF!</f>
         <v>#REF!</v>
+      </c>
+      <c r="F25">
+        <f>_1234\5678\90+_1234\5678\91</f>
+        <v>1</v>
       </c>
       <c r="M25" s="39" t="str">
         <f>"Exchange(1 "&amp;NAMEDCELL123&amp;"=)"</f>
@@ -16736,8 +16857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10335504-69CA-E540-89E9-50659E4CE027}">
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A22" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:AV30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -16757,23 +16878,27 @@
     <col min="14" max="14" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="25" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="4" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="38" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="48" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="3.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="48" width="6" style="4" bestFit="1" customWidth="1"/>
     <col min="49" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
@@ -17472,89 +17597,1025 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A17" s="12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A19" s="12" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A20" s="12" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A21" s="12" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="A26" s="7" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A27" s="4" t="s">
+      <c r="B26" s="4">
+        <v>0</v>
+      </c>
+      <c r="C26" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E26" s="4">
+        <v>3</v>
+      </c>
+      <c r="F26" s="4">
+        <v>4</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="20" t="s">
+        <v>460</v>
+      </c>
+      <c r="I26" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K26" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L26" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M26" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N26" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O26" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P26" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q26" s="6" t="e">
+        <f>NORMDIST(B26,,,)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="R26" s="6">
+        <f>NORMDIST(C26,1,2,FALSE)</f>
+        <v>0.17147192750969195</v>
+      </c>
+      <c r="S26" s="6">
+        <f>NORMDIST(D26,"1","3",5)</f>
+        <v>0.46017216272297101</v>
+      </c>
+      <c r="T26" s="6">
+        <f>NORMDIST(E26,-1,2,"TRUE")</f>
+        <v>0.97724986805182079</v>
+      </c>
+      <c r="U26" s="6" t="e">
+        <f>NORMDIST(F26, 0,0,1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="V26" s="6">
+        <f>NORMDIST(G26,G26,F26,1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="W26" s="6">
+        <f>NORMDIST(H26,,H26,1)</f>
+        <v>0.84134474606854304</v>
+      </c>
+      <c r="X26" s="6">
+        <f>NORMDIST(I26,H26,D26,1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y26" s="6" t="e">
+        <f>NORMDIST(J26,H26,F26,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z26" s="6" t="e">
+        <f t="shared" ref="Z26:AE26" si="2">NORMDIST(K26,I26,G26,1)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA26" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB26" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC26" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD26" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE26" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF26" s="6" t="e">
+        <f>NORMDIST(B26:P26,3,3,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG26" s="6">
+        <f t="array" ref="AG26:AV26">NORMDIST(B26:P26,B26:P26,4,1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="AH26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AI26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AJ26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AK26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AL26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AM26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AN26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AO26" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP26" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ26" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR26" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS26" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT26" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU26" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV26" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="A27" s="7" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A28" s="4" t="s">
+      <c r="B27" s="4">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E27" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="F27" s="4">
+        <v>4</v>
+      </c>
+      <c r="G27" s="6"/>
+      <c r="H27" s="20" t="s">
+        <v>460</v>
+      </c>
+      <c r="I27" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K27" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L27" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M27" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N27" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O27" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P27" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q27" s="6" t="e">
+        <f>NORMINV(B27,4,4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="R27" s="6" t="e">
+        <f>NORMINV(C27,2,2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="S27" s="6">
+        <f>NORMINV(0.4,2,D27)</f>
+        <v>1.8226570278049401</v>
+      </c>
+      <c r="T27" s="6">
+        <f>NORMINV(E27,4,3)</f>
+        <v>-4.6344852172864481</v>
+      </c>
+      <c r="U27" s="6" t="e">
+        <f>NORMINV(F27,C27,D27)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="V27" s="6" t="e">
+        <f>NORMINV(G27,3,2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="W27" s="6">
+        <f>NORMINV(0.3,H27,2)</f>
+        <v>58.951198974583917</v>
+      </c>
+      <c r="X27" s="6">
+        <f>NORMINV(0.3,I27,2)</f>
+        <v>-4.8801025416081778E-2</v>
+      </c>
+      <c r="Y27" s="6" t="e">
+        <f>NORMINV(J27,B27,D27)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z27" s="6" t="e">
+        <f t="shared" ref="Z27:AE27" si="3">NORMINV(K27,C27,E27)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA27" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB27" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC27" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD27" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE27" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF27" s="6" t="e">
+        <f>NORMINV(B27:P27,3,3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG27" s="6" t="e">
+        <f t="array" ref="AG27:AV27">NORMINV(B27:P27, 3,2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AH27" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AI27" s="6">
+        <v>4.0488010254160818</v>
+      </c>
+      <c r="AJ27" s="6">
+        <v>-2.7563234781909651</v>
+      </c>
+      <c r="AK27" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AL27" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AM27" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AN27" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AO27" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP27" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ27" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR27" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS27" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT27" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU27" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV27" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="A28" s="7" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A29" s="4" t="s">
+      <c r="B28" s="4">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E28" s="4">
+        <v>3</v>
+      </c>
+      <c r="F28" s="4">
+        <v>4</v>
+      </c>
+      <c r="G28" s="6"/>
+      <c r="H28" s="20" t="s">
+        <v>460</v>
+      </c>
+      <c r="I28" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K28" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L28" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M28" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N28" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O28" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P28" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q28" s="6">
+        <f>NORMSDIST(B28)</f>
+        <v>0.5</v>
+      </c>
+      <c r="R28" s="6">
+        <f>NORMSDIST(C28)</f>
+        <v>0.46017216272297101</v>
+      </c>
+      <c r="S28" s="6">
+        <f>NORMSDIST(D28)</f>
+        <v>0.75803634777692697</v>
+      </c>
+      <c r="T28" s="6">
+        <f>NORMSDIST(E28)</f>
+        <v>0.9986501019683699</v>
+      </c>
+      <c r="U28" s="6">
+        <f>NORMSDIST(F28)</f>
+        <v>0.99996832875816688</v>
+      </c>
+      <c r="V28" s="6">
+        <f>NORMSDIST(G28)</f>
+        <v>0.5</v>
+      </c>
+      <c r="W28" s="6">
+        <f>NORMSDIST(H28)</f>
+        <v>1</v>
+      </c>
+      <c r="X28" s="6">
+        <f>NORMSDIST(I28)</f>
+        <v>0.84134474606854304</v>
+      </c>
+      <c r="Y28" s="6" t="e">
+        <f>NORMSDIST(J28)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z28" s="6" t="e">
+        <f t="shared" ref="Z28:AE28" si="4">NORMSDIST(K28)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA28" s="6" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB28" s="6" t="e">
+        <f t="shared" si="4"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC28" s="6" t="e">
+        <f t="shared" si="4"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD28" s="6" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE28" s="6" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF28" s="6" t="e">
+        <f>NORMSDIST(B28:P28)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG28" s="6">
+        <f t="array" ref="AG28:AV28">NORMSDIST(B28:P28)</f>
+        <v>0.5</v>
+      </c>
+      <c r="AH28" s="6">
+        <v>0.46017216272297101</v>
+      </c>
+      <c r="AI28" s="6">
+        <v>0.75803634777692697</v>
+      </c>
+      <c r="AJ28" s="6">
+        <v>0.9986501019683699</v>
+      </c>
+      <c r="AK28" s="6">
+        <v>0.99996832875816688</v>
+      </c>
+      <c r="AL28" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AM28" s="6">
+        <v>1</v>
+      </c>
+      <c r="AN28" s="6">
+        <v>0.84134474606854304</v>
+      </c>
+      <c r="AO28" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP28" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ28" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR28" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS28" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT28" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU28" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV28" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="A29" s="7" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A30" s="4" t="s">
+      <c r="B29" s="4">
+        <v>0</v>
+      </c>
+      <c r="C29" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E29" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="F29" s="4">
+        <v>4</v>
+      </c>
+      <c r="G29" s="6"/>
+      <c r="H29" s="20" t="s">
+        <v>460</v>
+      </c>
+      <c r="I29" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K29" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L29" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M29" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N29" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O29" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P29" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q29" s="6" t="e">
+        <f>NORMSINV(B29)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="R29" s="6" t="e">
+        <f>NORMSINV(C29)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="S29" s="6">
+        <f>NORMSINV(D29)</f>
+        <v>0.52440051270804078</v>
+      </c>
+      <c r="T29" s="6">
+        <f>NORMSINV(E29)</f>
+        <v>-2.8781617390954826</v>
+      </c>
+      <c r="U29" s="6" t="e">
+        <f>NORMSINV(F29)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="V29" s="6" t="e">
+        <f>NORMSINV(G29)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="W29" s="6" t="e">
+        <f>NORMSINV(H29)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="X29" s="6" t="e">
+        <f>NORMSINV(I29)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="Y29" s="6" t="e">
+        <f>NORMSINV(J29)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z29" s="6" t="e">
+        <f t="shared" ref="Z29:AE29" si="5">NORMSINV(K29)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA29" s="6" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB29" s="6" t="e">
+        <f t="shared" si="5"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC29" s="6" t="e">
+        <f t="shared" si="5"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD29" s="6" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE29" s="6" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF29" s="6" t="e">
+        <f>NORMSINV(B29:P29)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG29" s="6" t="e">
+        <f t="array" ref="AG29:AV29">NORMSINV(B29:P29)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AH29" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AI29" s="6">
+        <v>0.52440051270804078</v>
+      </c>
+      <c r="AJ29" s="6">
+        <v>-2.8781617390954826</v>
+      </c>
+      <c r="AK29" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AL29" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AM29" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AN29" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AO29" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP29" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ29" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR29" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS29" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT29" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU29" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV29" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:48" x14ac:dyDescent="0.15">
+      <c r="A30" s="7" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B30" s="4">
+        <v>0</v>
+      </c>
+      <c r="C30" s="4">
+        <v>-10</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="F30" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="20" t="s">
+        <v>464</v>
+      </c>
+      <c r="I30" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K30" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L30" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M30" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N30" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O30" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P30" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q30" s="6">
+        <f>PERCENTILE(B30:C30,".2")</f>
+        <v>-8</v>
+      </c>
+      <c r="R30" s="6">
+        <f>PERCENTILE(B30:G30,D30)</f>
+        <v>0.57999999999999974</v>
+      </c>
+      <c r="S30" s="6">
+        <f>PERCENTILE(D30:E30,E30)</f>
+        <v>0.18000000000000008</v>
+      </c>
+      <c r="T30" s="6" t="e">
+        <f>PERCENTILE(E30:F30,F30)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="U30" s="6">
+        <f>PERCENTILE(F30:G30,G30)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="V30" s="6">
+        <f>PERCENTILE(C30:D30,H30)</f>
+        <v>0.9</v>
+      </c>
+      <c r="W30" s="6">
+        <f>PERCENTILE(D30:H30,I30)</f>
+        <v>0.9</v>
+      </c>
+      <c r="X30" s="6" t="e">
+        <f>PERCENTILE(H30:I30,J30)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y30" s="6" t="e">
+        <f>PERCENTILE(J30:K30,K30)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z30" s="6" t="e">
+        <f t="shared" ref="Z30:AE30" si="6">PERCENTILE(K30:L30,L30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA30" s="6" t="e">
+        <f t="shared" si="6"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AB30" s="6" t="e">
+        <f t="shared" si="6"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AC30" s="6" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AD30" s="6" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AE30" s="6" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF30" s="6" t="e">
+        <f>PERCENTILE(_xlfn.SINGLE(B30:F30),0.03)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG30" s="6">
+        <f t="array" ref="AG30:AV30">PERCENTILE(B30:I30,B30:P30)</f>
+        <v>-10</v>
+      </c>
+      <c r="AH30" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AI30" s="6">
+        <v>0.57999999999999974</v>
+      </c>
+      <c r="AJ30" s="6">
+        <v>-6.0400000000000009</v>
+      </c>
+      <c r="AK30" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AL30" s="6">
+        <v>-10</v>
+      </c>
+      <c r="AM30" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="AN30" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="AO30" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP30" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ30" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR30" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS30" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT30" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU30" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV30" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="33" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="7" t="s">
         <v>492</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0</v>
+      </c>
+      <c r="C33" s="4">
+        <v>-10</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E33" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F33" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="20" t="s">
+        <v>464</v>
+      </c>
+      <c r="I33" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K33" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L33" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M33" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N33" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O33" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P33" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q33" s="6">
+        <f>QUARTILE(B33:C33,"2")</f>
+        <v>-5</v>
+      </c>
+      <c r="R33" s="6">
+        <f>QUARTILE(B33:G33,D33)</f>
+        <v>-10</v>
+      </c>
+      <c r="S33" s="6">
+        <f>QUARTILE(D33:E33,E33)</f>
+        <v>1.5500000000000003</v>
+      </c>
+      <c r="T33" s="6" t="e">
+        <f t="shared" ref="S33:U33" si="7">QUARTILE(E33:F33,F33)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="U33" s="6">
+        <f>QUARTILE(F33:G33,G33)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="V33" s="6">
+        <f>QUARTILE(C33:D33,H33)</f>
+        <v>-7.2750000000000004</v>
+      </c>
+      <c r="W33" s="6">
+        <f>QUARTILE(D33:H33,I33)</f>
+        <v>0.4</v>
+      </c>
+      <c r="X33" s="6" t="e">
+        <f>QUARTILE(H33:I33,J33)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y33" s="6" t="e">
+        <f t="shared" ref="Y33" si="8">QUARTILE(J33:K33,K33)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z33" s="6" t="e">
+        <f>QUARTILE(K33:L33,H33)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA33" s="6" t="e">
+        <f>QUARTILE(L33:M33,M33)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AB33" s="6" t="e">
+        <f t="shared" ref="AB33" si="9">QUARTILE(M33:N33,N33)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AC33" s="6" t="e">
+        <f t="shared" ref="AC33:AD33" si="10">QUARTILE(N33:O33,O33)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AD33" s="6" t="e">
+        <f t="shared" si="10"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AE33" s="6" t="e">
+        <f>QUARTILE(P33:Q33,Q33)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF33" s="6">
+        <f>QUARTILE(B33:F33,H33)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="AG33" s="6">
+        <f t="array" ref="AG33:AV33">QUARTILE(B33:I33,B33:P33)</f>
+        <v>-10</v>
+      </c>
+      <c r="AH33" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AI33" s="6">
+        <v>-10</v>
+      </c>
+      <c r="AJ33" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK33" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AL33" s="6">
+        <v>-10</v>
+      </c>
+      <c r="AM33" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="AN33" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="AO33" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP33" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ33" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR33" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS33" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT33" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU33" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV33" s="4" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="34" spans="1:48" x14ac:dyDescent="0.15">
@@ -17650,23 +18711,23 @@
         <v>#N/A</v>
       </c>
       <c r="AA35" s="6" t="e">
-        <f t="shared" ref="AA35:AE35" si="2">STDEV(L35:M35)</f>
+        <f t="shared" ref="AA35:AE35" si="11">STDEV(L35:M35)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB35" s="6" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>#NAME?</v>
       </c>
       <c r="AC35" s="6" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>#NULL!</v>
       </c>
       <c r="AD35" s="6" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
       <c r="AE35" s="6" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>#REF!</v>
       </c>
       <c r="AF35" s="6">
@@ -17985,27 +19046,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z40" s="6" t="e">
-        <f t="shared" ref="Z40:AE40" si="3">VAR(K40:L40)</f>
+        <f t="shared" ref="Z40:AE40" si="12">VAR(K40:L40)</f>
         <v>#N/A</v>
       </c>
       <c r="AA40" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB40" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>#NAME?</v>
       </c>
       <c r="AC40" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>#NULL!</v>
       </c>
       <c r="AD40" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>#NUM!</v>
       </c>
       <c r="AE40" s="6" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>#REF!</v>
       </c>
       <c r="AF40" s="6">
@@ -18147,27 +19208,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z41" s="6" t="e">
-        <f t="shared" ref="Z41:AE41" si="4">VARP(K41:L41)</f>
+        <f t="shared" ref="Z41:AE41" si="13">VARP(K41:L41)</f>
         <v>#N/A</v>
       </c>
       <c r="AA41" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB41" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>#NAME?</v>
       </c>
       <c r="AC41" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>#NULL!</v>
       </c>
       <c r="AD41" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
       <c r="AE41" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>#REF!</v>
       </c>
       <c r="AF41" s="6">
@@ -31280,8 +32341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AV113"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A70" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -31298,17 +32359,12 @@
     <col min="13" max="14" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="21" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="27" max="29" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="4" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="33" max="38" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="39" max="48" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
@@ -34395,23 +35451,647 @@
       </c>
     </row>
     <row r="71" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A71" s="12" t="s">
+      <c r="A71" s="13" t="s">
         <v>165</v>
       </c>
+      <c r="B71" s="4">
+        <v>0</v>
+      </c>
+      <c r="C71" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="D71" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E71" s="4">
+        <v>3</v>
+      </c>
+      <c r="F71" s="4">
+        <v>4</v>
+      </c>
+      <c r="G71" s="6"/>
+      <c r="H71" s="20" t="s">
+        <v>460</v>
+      </c>
+      <c r="I71" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J71" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K71" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L71" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M71" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N71" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O71" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P71" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q71" s="6" t="e">
+        <f>_xlfn.NORM.DIST(B71,,,)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="R71" s="6">
+        <f>_xlfn.NORM.DIST(C71,1,2,FALSE)</f>
+        <v>0.17147192750969195</v>
+      </c>
+      <c r="S71" s="6">
+        <f>_xlfn.NORM.DIST(D71,"1","3",5)</f>
+        <v>0.46017216272297101</v>
+      </c>
+      <c r="T71" s="6">
+        <f>_xlfn.NORM.DIST(E71,-1,2,"TRUE")</f>
+        <v>0.97724986805182079</v>
+      </c>
+      <c r="U71" s="6" t="e">
+        <f>_xlfn.NORM.DIST(F71, 0,0,1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="V71" s="6">
+        <f>_xlfn.NORM.DIST(G71,G71,F71,1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="W71" s="6">
+        <f>_xlfn.NORM.DIST(H71,,H71,1)</f>
+        <v>0.84134474606854304</v>
+      </c>
+      <c r="X71" s="6">
+        <f>_xlfn.NORM.DIST(I71,H71,D71,1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y71" s="6" t="e">
+        <f>_xlfn.NORM.DIST(J71,H71,F71,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z71" s="6" t="e">
+        <f>_xlfn.NORM.DIST(K71,I71,G71,1)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA71" s="6" t="e">
+        <f t="shared" ref="Z71:AE71" si="18">_xlfn.NORM.DIST(L71,J71,H71,1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB71" s="6" t="e">
+        <f t="shared" si="18"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC71" s="6" t="e">
+        <f t="shared" si="18"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD71" s="6" t="e">
+        <f t="shared" si="18"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE71" s="6" t="e">
+        <f t="shared" si="18"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF71" s="6" t="e">
+        <f>_xlfn.NORM.DIST(B71:P71,3,3,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG71" s="6">
+        <f t="array" ref="AG71:AV71">_xlfn.NORM.DIST(B71:P71,3,4,1)</f>
+        <v>0.22662735237686821</v>
+      </c>
+      <c r="AH71" s="6">
+        <v>0.21916982979337737</v>
+      </c>
+      <c r="AI71" s="6">
+        <v>0.28264564849720064</v>
+      </c>
+      <c r="AJ71" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AK71" s="6">
+        <v>0.5987063256829237</v>
+      </c>
+      <c r="AL71" s="6">
+        <v>0.22662735237686821</v>
+      </c>
+      <c r="AM71" s="6">
+        <v>1</v>
+      </c>
+      <c r="AN71" s="6">
+        <v>0.30853753872598688</v>
+      </c>
+      <c r="AO71" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP71" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ71" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR71" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS71" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT71" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU71" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV71" s="4" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="72" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A72" s="12" t="s">
+      <c r="A72" s="13" t="s">
         <v>166</v>
       </c>
+      <c r="B72" s="4">
+        <v>0</v>
+      </c>
+      <c r="C72" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="D72" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E72" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="F72" s="4">
+        <v>4</v>
+      </c>
+      <c r="G72" s="6"/>
+      <c r="H72" s="20" t="s">
+        <v>460</v>
+      </c>
+      <c r="I72" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J72" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K72" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L72" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M72" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N72" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O72" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P72" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q72" s="6" t="e">
+        <f>_xlfn.NORM.INV(B72,4,4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="R72" s="6" t="e">
+        <f>_xlfn.NORM.INV(C72,2,2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="S72" s="6">
+        <f>_xlfn.NORM.INV(0.4,2,D72)</f>
+        <v>1.8226570278049401</v>
+      </c>
+      <c r="T72" s="6">
+        <f>_xlfn.NORM.INV(E72,4,3)</f>
+        <v>-4.6344852172864481</v>
+      </c>
+      <c r="U72" s="6" t="e">
+        <f>_xlfn.NORM.INV(F72,C72,D72)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="V72" s="6" t="e">
+        <f>_xlfn.NORM.INV(G72,3,2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="W72" s="6">
+        <f>_xlfn.NORM.INV(0.3,H72,2)</f>
+        <v>58.951198974583917</v>
+      </c>
+      <c r="X72" s="6">
+        <f>_xlfn.NORM.INV(0.3,I72,2)</f>
+        <v>-4.8801025416081778E-2</v>
+      </c>
+      <c r="Y72" s="6" t="e">
+        <f>_xlfn.NORM.INV(J72,B72,D72)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z72" s="6" t="e">
+        <f t="shared" ref="Z72:AE72" si="19">_xlfn.NORM.INV(K72,C72,E72)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA72" s="6" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB72" s="6" t="e">
+        <f t="shared" si="19"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC72" s="6" t="e">
+        <f t="shared" si="19"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD72" s="6" t="e">
+        <f t="shared" si="19"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE72" s="6" t="e">
+        <f t="shared" si="19"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF72" s="6" t="e">
+        <f>_xlfn.NORM.INV(B72:P72,3,3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG72" s="6" t="e">
+        <f t="array" ref="AG72:AV72">_xlfn.NORM.INV(B72:P72, 3,2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AH72" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AI72" s="6">
+        <v>4.0488010254160818</v>
+      </c>
+      <c r="AJ72" s="6">
+        <v>-2.7563234781909651</v>
+      </c>
+      <c r="AK72" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AL72" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AM72" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AN72" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AO72" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP72" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ72" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR72" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS72" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT72" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU72" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV72" s="4" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="73" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A73" s="12" t="s">
+      <c r="A73" s="13" t="s">
         <v>167</v>
       </c>
+      <c r="B73" s="4">
+        <v>0</v>
+      </c>
+      <c r="C73" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="D73" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E73" s="4">
+        <v>3</v>
+      </c>
+      <c r="F73" s="4">
+        <v>4</v>
+      </c>
+      <c r="G73" s="6"/>
+      <c r="H73" s="20" t="s">
+        <v>460</v>
+      </c>
+      <c r="I73" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J73" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K73" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L73" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M73" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N73" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O73" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P73" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q73" s="6">
+        <f>_xlfn.NORM.S.DIST(B73,)</f>
+        <v>0.3989422804014327</v>
+      </c>
+      <c r="R73" s="6">
+        <f>_xlfn.NORM.S.DIST(C73,FALSE)</f>
+        <v>0.39695254747701181</v>
+      </c>
+      <c r="S73" s="6" t="e">
+        <f>_xlfn.NORM.S.DIST(D73,"1")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T73" s="6">
+        <f>_xlfn.NORM.S.DIST(E73,"TRUE")</f>
+        <v>0.9986501019683699</v>
+      </c>
+      <c r="U73" s="6">
+        <f>_xlfn.NORM.S.DIST(F73,1)</f>
+        <v>0.99996832875816688</v>
+      </c>
+      <c r="V73" s="6">
+        <f t="shared" ref="V73:AF73" si="20">_xlfn.NORM.S.DIST(G73,1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="W73" s="6">
+        <f>_xlfn.NORM.S.DIST(H73,1)</f>
+        <v>1</v>
+      </c>
+      <c r="X73" s="6">
+        <f>_xlfn.NORM.S.DIST(I73,1)</f>
+        <v>0.84134474606854304</v>
+      </c>
+      <c r="Y73" s="6" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z73" s="6" t="e">
+        <f t="shared" si="20"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA73" s="6" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB73" s="6" t="e">
+        <f t="shared" si="20"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC73" s="6" t="e">
+        <f t="shared" si="20"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD73" s="6" t="e">
+        <f t="shared" si="20"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE73" s="6" t="e">
+        <f t="shared" si="20"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AF73" s="6" t="e">
+        <f>_xlfn.NORM.S.DIST(B73:P73,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG73" s="6">
+        <f t="array" ref="AG73:AV73">_xlfn.NORM.S.DIST(B73:P73,1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="AH73" s="6">
+        <v>0.46017216272297101</v>
+      </c>
+      <c r="AI73" s="6">
+        <v>0.75803634777692697</v>
+      </c>
+      <c r="AJ73" s="6">
+        <v>0.9986501019683699</v>
+      </c>
+      <c r="AK73" s="6">
+        <v>0.99996832875816688</v>
+      </c>
+      <c r="AL73" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AM73" s="6">
+        <v>1</v>
+      </c>
+      <c r="AN73" s="6">
+        <v>0.84134474606854304</v>
+      </c>
+      <c r="AO73" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP73" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ73" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR73" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS73" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT73" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU73" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV73" s="4" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="74" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A74" s="12" t="s">
+      <c r="A74" s="13" t="s">
         <v>168</v>
+      </c>
+      <c r="B74" s="4">
+        <v>0</v>
+      </c>
+      <c r="C74" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="D74" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E74" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="F74" s="4">
+        <v>4</v>
+      </c>
+      <c r="G74" s="6"/>
+      <c r="H74" s="20" t="s">
+        <v>460</v>
+      </c>
+      <c r="I74" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J74" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K74" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L74" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M74" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N74" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O74" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P74" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q74" s="6" t="e">
+        <f>_xlfn.NORM.S.INV(B74)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="R74" s="6" t="e">
+        <f>_xlfn.NORM.S.INV(C74)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="S74" s="6">
+        <f>_xlfn.NORM.S.INV(D74)</f>
+        <v>0.52440051270804078</v>
+      </c>
+      <c r="T74" s="6">
+        <f t="shared" ref="S74:AE74" si="21">_xlfn.NORM.S.INV(E74)</f>
+        <v>-2.8781617390954826</v>
+      </c>
+      <c r="U74" s="6" t="e">
+        <f t="shared" si="21"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="V74" s="6" t="e">
+        <f t="shared" si="21"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="W74" s="6" t="e">
+        <f t="shared" si="21"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="X74" s="6" t="e">
+        <f>_xlfn.NORM.S.INV(I74)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="Y74" s="6" t="e">
+        <f>_xlfn.NORM.S.INV(J74)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z74" s="6" t="e">
+        <f t="shared" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA74" s="6" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB74" s="6" t="e">
+        <f t="shared" si="21"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC74" s="6" t="e">
+        <f t="shared" si="21"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD74" s="6" t="e">
+        <f t="shared" si="21"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE74" s="6" t="e">
+        <f>_xlfn.NORM.S.INV(P74)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF74" s="6" t="e">
+        <f>_xlfn.NORM.S.INV(B74:P74)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG74" s="6" t="e">
+        <f t="array" ref="AG74:AV74">_xlfn.NORM.S.INV(B74:P74)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AH74" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AI74" s="6">
+        <v>0.52440051270804078</v>
+      </c>
+      <c r="AJ74" s="6">
+        <v>-2.8781617390954826</v>
+      </c>
+      <c r="AK74" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AL74" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AM74" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AN74" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AO74" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP74" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ74" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR74" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS74" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT74" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU74" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV74" s="4" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="75" spans="1:48" x14ac:dyDescent="0.15">
@@ -34420,24 +36100,424 @@
       </c>
     </row>
     <row r="76" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="13" t="s">
         <v>170</v>
       </c>
+      <c r="B76" s="4">
+        <v>0</v>
+      </c>
+      <c r="C76" s="4">
+        <v>-10</v>
+      </c>
+      <c r="D76" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E76" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="F76" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="G76" s="6"/>
+      <c r="H76" s="20" t="s">
+        <v>464</v>
+      </c>
+      <c r="I76" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J76" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K76" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L76" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M76" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N76" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O76" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P76" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q76" s="6">
+        <f>_xlfn.PERCENTILE.EXC(B76:E76,".2")</f>
+        <v>-10</v>
+      </c>
+      <c r="R76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(B76:G76,D76)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="S76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(C76:E76,E76)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="T76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(E76:F76,F76)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="U76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(F76:G76,G76)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="V76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(C76:D76,H76)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="W76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(D76:H76,I76)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="X76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(H76:I76,J76)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(J76:K76,K76)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(K76:L76,L76)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(L76:M76,M76)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AB76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(M76:N76,N76)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AC76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(N76:O76,O76)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AD76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(O76:P76,P76)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AE76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(P76:Q76,Q76)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF76" s="6" t="e">
+        <f>_xlfn.PERCENTILE.EXC(_xlfn.SINGLE(B76:F76),0.03)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG76" s="6" t="e">
+        <f t="array" ref="AG76:AV76">_xlfn.PERCENTILE.EXC(B76:I76,B76:P76)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AH76" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AI76" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AJ76" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AK76" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AL76" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AM76" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AN76" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AO76" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP76" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ76" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR76" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS76" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT76" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU76" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV76" s="4" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="77" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A77" s="12" t="s">
+      <c r="A77" s="13" t="s">
         <v>171</v>
+      </c>
+      <c r="B77" s="4">
+        <v>0</v>
+      </c>
+      <c r="C77" s="4">
+        <v>-10</v>
+      </c>
+      <c r="D77" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E77" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="F77" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="G77" s="6"/>
+      <c r="H77" s="20" t="s">
+        <v>464</v>
+      </c>
+      <c r="I77" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J77" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K77" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L77" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M77" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N77" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O77" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P77" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q77" s="6">
+        <f>_xlfn.PERCENTILE.INC(B77:C77,".2")</f>
+        <v>-8</v>
+      </c>
+      <c r="R77" s="6">
+        <f>_xlfn.PERCENTILE.INC(B77:I77,D77)</f>
+        <v>0.57999999999999974</v>
+      </c>
+      <c r="S77" s="6">
+        <f>_xlfn.PERCENTILE.INC(D77:E77,E77)</f>
+        <v>0.18000000000000008</v>
+      </c>
+      <c r="T77" s="6" t="e">
+        <f>_xlfn.PERCENTILE.INC(E77:F77,F77)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="U77" s="6">
+        <f>_xlfn.PERCENTILE.INC(F77:G77,G77)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="V77" s="6">
+        <f>_xlfn.PERCENTILE.INC(C77:D77,H77)</f>
+        <v>0.9</v>
+      </c>
+      <c r="W77" s="6">
+        <f>_xlfn.PERCENTILE.INC(D77:H77,I77)</f>
+        <v>0.9</v>
+      </c>
+      <c r="X77" s="6" t="e">
+        <f>_xlfn.PERCENTILE.INC(H77:I77,J77)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y77" s="6" t="e">
+        <f>_xlfn.PERCENTILE.INC(J77:K77,K77)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z77" s="6" t="e">
+        <f>_xlfn.PERCENTILE.INC(K77:L77,L77)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA77" s="6" t="e">
+        <f>_xlfn.PERCENTILE.INC(L77:M77,M77)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AB77" s="6" t="e">
+        <f>_xlfn.PERCENTILE.INC(M77:N77,N77)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AC77" s="6" t="e">
+        <f>_xlfn.PERCENTILE.INC(N77:O77,O77)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AD77" s="6" t="e">
+        <f>_xlfn.PERCENTILE.INC(O77:P77,P77)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AE77" s="6" t="e">
+        <f>_xlfn.PERCENTILE.INC(P77:Q77,Q77)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF77" s="6" t="e">
+        <f>_xlfn.PERCENTILE.INC(_xlfn.SINGLE(B77:F77),0.03)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG77" s="6">
+        <f t="array" ref="AG77:AV77">_xlfn.PERCENTILE.INC(B77:I77,B77:P77)</f>
+        <v>-10</v>
+      </c>
+      <c r="AH77" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AI77" s="6">
+        <v>0.57999999999999974</v>
+      </c>
+      <c r="AJ77" s="6">
+        <v>-6.0400000000000009</v>
+      </c>
+      <c r="AK77" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AL77" s="6">
+        <v>-10</v>
+      </c>
+      <c r="AM77" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="AN77" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="AO77" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP77" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ77" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR77" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS77" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT77" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU77" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV77" s="4" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="78" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A78" s="12" t="s">
         <v>172</v>
       </c>
+      <c r="G78" s="6"/>
+      <c r="H78" s="20"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="8"/>
+      <c r="M78" s="8"/>
+      <c r="N78" s="8"/>
+      <c r="O78" s="8"/>
+      <c r="P78" s="8"/>
+      <c r="Q78" s="6"/>
+      <c r="R78" s="6"/>
+      <c r="S78" s="6"/>
+      <c r="T78" s="6"/>
+      <c r="U78" s="6"/>
+      <c r="V78" s="6"/>
+      <c r="W78" s="6"/>
+      <c r="X78" s="6"/>
+      <c r="Y78" s="6"/>
+      <c r="Z78" s="6"/>
+      <c r="AA78" s="6"/>
+      <c r="AB78" s="6"/>
+      <c r="AC78" s="6"/>
+      <c r="AD78" s="6"/>
+      <c r="AE78" s="6"/>
+      <c r="AF78" s="6"/>
+      <c r="AG78" s="6"/>
+      <c r="AH78" s="6"/>
+      <c r="AI78" s="6"/>
+      <c r="AJ78" s="6"/>
+      <c r="AK78" s="6"/>
+      <c r="AL78" s="6"/>
+      <c r="AM78" s="6"/>
+      <c r="AN78" s="6"/>
+      <c r="AO78" s="6"/>
+      <c r="AP78" s="6"/>
+      <c r="AQ78" s="6"/>
+      <c r="AR78" s="6"/>
+      <c r="AS78" s="6"/>
+      <c r="AT78" s="6"/>
+      <c r="AU78" s="6"/>
     </row>
     <row r="79" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A79" s="12" t="s">
         <v>173</v>
       </c>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="33"/>
+      <c r="H79" s="34"/>
+      <c r="I79" s="33"/>
+      <c r="J79" s="33"/>
+      <c r="K79" s="33"/>
+      <c r="L79" s="33"/>
+      <c r="M79" s="33"/>
+      <c r="N79" s="33"/>
+      <c r="O79" s="33"/>
+      <c r="P79" s="33"/>
+      <c r="Q79" s="33"/>
+      <c r="R79" s="33"/>
+      <c r="S79" s="33"/>
+      <c r="T79" s="33"/>
+      <c r="U79" s="33"/>
+      <c r="V79" s="33"/>
+      <c r="W79" s="33"/>
+      <c r="X79" s="33"/>
+      <c r="Y79" s="33"/>
+      <c r="Z79" s="33"/>
+      <c r="AA79" s="33"/>
+      <c r="AB79" s="33"/>
+      <c r="AC79" s="33"/>
+      <c r="AD79" s="33"/>
+      <c r="AE79" s="33"/>
+      <c r="AF79" s="33"/>
+      <c r="AG79" s="33"/>
+      <c r="AH79" s="33"/>
+      <c r="AI79" s="33"/>
+      <c r="AJ79" s="33"/>
+      <c r="AK79" s="33"/>
+      <c r="AL79" s="33"/>
+      <c r="AM79" s="33"/>
+      <c r="AN79" s="33"/>
+      <c r="AO79" s="33"/>
+      <c r="AP79" s="33"/>
+      <c r="AQ79" s="33"/>
+      <c r="AR79" s="33"/>
+      <c r="AS79" s="33"/>
+      <c r="AT79" s="33"/>
+      <c r="AU79" s="33"/>
+      <c r="AV79" s="12"/>
     </row>
     <row r="80" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A80" s="12" t="s">
@@ -34465,13 +36545,325 @@
       </c>
     </row>
     <row r="85" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="13" t="s">
         <v>179</v>
       </c>
+      <c r="B85" s="4">
+        <v>0</v>
+      </c>
+      <c r="C85" s="4">
+        <v>-10</v>
+      </c>
+      <c r="D85" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E85" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F85" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="G85" s="6"/>
+      <c r="H85" s="20" t="s">
+        <v>464</v>
+      </c>
+      <c r="I85" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J85" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K85" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L85" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M85" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N85" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O85" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P85" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q85" s="6">
+        <f>_xlfn.QUARTILE.EXC(B85:C85,"2")</f>
+        <v>-5</v>
+      </c>
+      <c r="R85" s="6">
+        <f>_xlfn.QUARTILE.EXC(B85:F85,2)</f>
+        <v>0</v>
+      </c>
+      <c r="S85" s="6">
+        <f>_xlfn.QUARTILE.EXC(D85:E85,E85)</f>
+        <v>1.5500000000000003</v>
+      </c>
+      <c r="T85" s="6" t="e">
+        <f>_xlfn.QUARTILE.EXC(D85:E85,1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="U85" s="6" t="e">
+        <f>_xlfn.QUARTILE.EXC(C85:G85,G85)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="V85" s="6" t="e">
+        <f>_xlfn.QUARTILE.EXC(C85:D85,H85)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="W85" s="6">
+        <f>_xlfn.QUARTILE.EXC(D85:H85,I85)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="X85" s="6" t="e">
+        <f>_xlfn.QUARTILE.EXC(H85:I85,J85)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y85" s="6" t="e">
+        <f>_xlfn.QUARTILE.EXC(J85:K85,K85)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z85" s="6" t="e">
+        <f>_xlfn.QUARTILE.EXC(K85:L85,L85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA85" s="6" t="e">
+        <f>_xlfn.QUARTILE.EXC(L85:M85,M85)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AB85" s="6" t="e">
+        <f>_xlfn.QUARTILE.EXC(M85:N85,N85)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AC85" s="6" t="e">
+        <f>_xlfn.QUARTILE.EXC(N85:O85,O85)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AD85" s="6" t="e">
+        <f>_xlfn.QUARTILE.EXC(O85:P85,P85)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AE85" s="6" t="e">
+        <f>_xlfn.QUARTILE.EXC(P85:Q85,Q85)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF85" s="6" t="e">
+        <f>_xlfn.QUARTILE.EXC(_xlfn.SINGLE(B85:F85),3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG85" s="6" t="e">
+        <f t="array" ref="AG85:AV85">_xlfn.QUARTILE.EXC(B85:I85,B85:P85)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AH85" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AI85" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AJ85" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK85" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AL85" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AM85" s="6">
+        <v>-5.05</v>
+      </c>
+      <c r="AN85" s="6">
+        <v>-5.05</v>
+      </c>
+      <c r="AO85" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP85" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ85" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR85" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS85" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT85" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU85" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV85" s="4" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="86" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A86" s="12" t="s">
+      <c r="A86" s="13" t="s">
         <v>180</v>
+      </c>
+      <c r="B86" s="12">
+        <v>0</v>
+      </c>
+      <c r="C86" s="12">
+        <v>-10</v>
+      </c>
+      <c r="D86" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="E86" s="12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F86" s="12">
+        <v>-0.1</v>
+      </c>
+      <c r="G86" s="33"/>
+      <c r="H86" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="I86" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J86" s="33" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K86" s="33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L86" s="33" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M86" s="33" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N86" s="33" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O86" s="33" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P86" s="33" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q86" s="33">
+        <f>_xlfn.QUARTILE.INC(B86:C86,"2")</f>
+        <v>-5</v>
+      </c>
+      <c r="R86" s="33">
+        <f>_xlfn.QUARTILE.INC(B86:F86,2)</f>
+        <v>0</v>
+      </c>
+      <c r="S86" s="33">
+        <f>_xlfn.QUARTILE.INC(D86:E86,E86)</f>
+        <v>1.5500000000000003</v>
+      </c>
+      <c r="T86" s="33">
+        <f>_xlfn.QUARTILE.INC(D86:E86,1)</f>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="U86" s="33">
+        <f>_xlfn.QUARTILE.INC(C86:G86,G86)</f>
+        <v>-10</v>
+      </c>
+      <c r="V86" s="33">
+        <f>_xlfn.QUARTILE.INC(C86:D86,H86)</f>
+        <v>-7.2750000000000004</v>
+      </c>
+      <c r="W86" s="33">
+        <f>_xlfn.QUARTILE.INC(D86:H86,I86)</f>
+        <v>0.4</v>
+      </c>
+      <c r="X86" s="33" t="e">
+        <f>_xlfn.QUARTILE.INC(H86:I86,J86)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y86" s="33" t="e">
+        <f>_xlfn.QUARTILE.INC(J86:K86,K86)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z86" s="33" t="e">
+        <f>_xlfn.QUARTILE.INC(K86:L86,L86)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA86" s="33" t="e">
+        <f>_xlfn.QUARTILE.INC(L86:M86,M86)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AB86" s="33" t="e">
+        <f>_xlfn.QUARTILE.INC(M86:N86,N86)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AC86" s="33" t="e">
+        <f>_xlfn.QUARTILE.INC(N86:O86,O86)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AD86" s="33" t="e">
+        <f>_xlfn.QUARTILE.INC(O86:P86,P86)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AE86" s="33" t="e">
+        <f>_xlfn.QUARTILE.INC(P86:Q86,Q86)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF86" s="33" t="e">
+        <f>_xlfn.QUARTILE.INC(_xlfn.SINGLE(B86:F86),3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG86" s="33">
+        <f t="array" ref="AG86:AV86">_xlfn.QUARTILE.INC(B86:I86,B86:P86)</f>
+        <v>-10</v>
+      </c>
+      <c r="AH86" s="33" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AI86" s="33">
+        <v>-10</v>
+      </c>
+      <c r="AJ86" s="33">
+        <v>0</v>
+      </c>
+      <c r="AK86" s="33" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AL86" s="33">
+        <v>-10</v>
+      </c>
+      <c r="AM86" s="33">
+        <v>-0.1</v>
+      </c>
+      <c r="AN86" s="33">
+        <v>-0.1</v>
+      </c>
+      <c r="AO86" s="33" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP86" s="33" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ86" s="33" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR86" s="33" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS86" s="33" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT86" s="33" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU86" s="33" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV86" s="12" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="87" spans="1:48" x14ac:dyDescent="0.15">
@@ -34588,31 +36980,31 @@
         <v>-10</v>
       </c>
       <c r="Y93" s="6" t="e">
-        <f t="shared" ref="Y93:AE93" si="18">SMALL($B93:$J93,J93)</f>
+        <f t="shared" ref="Y93:AE93" si="22">SMALL($B93:$J93,J93)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z93" s="6" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>#N/A</v>
       </c>
       <c r="AA93" s="6" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB93" s="6" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>#NAME?</v>
       </c>
       <c r="AC93" s="6" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>#NULL!</v>
       </c>
       <c r="AD93" s="6" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>#NUM!</v>
       </c>
       <c r="AE93" s="6" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>#REF!</v>
       </c>
       <c r="AF93" s="6" t="e">
@@ -34762,19 +37154,19 @@
         <v>#N/A</v>
       </c>
       <c r="AA95" s="6" t="e">
-        <f t="shared" ref="AA95:AD95" si="19">_xlfn.STDEV.P(L95:M95)</f>
+        <f t="shared" ref="AA95:AD95" si="23">_xlfn.STDEV.P(L95:M95)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB95" s="6" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>#NAME?</v>
       </c>
       <c r="AC95" s="6" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>#NULL!</v>
       </c>
       <c r="AD95" s="6" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>#NUM!</v>
       </c>
       <c r="AE95" s="6" t="e">
@@ -34924,23 +37316,23 @@
         <v>#N/A</v>
       </c>
       <c r="AA96" s="6" t="e">
-        <f t="shared" ref="AA96:AE96" si="20">_xlfn.STDEV.S(L96:M96)</f>
+        <f t="shared" ref="AA96:AE96" si="24">_xlfn.STDEV.S(L96:M96)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB96" s="6" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#NAME?</v>
       </c>
       <c r="AC96" s="6" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#NULL!</v>
       </c>
       <c r="AD96" s="6" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#NUM!</v>
       </c>
       <c r="AE96" s="6" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>#REF!</v>
       </c>
       <c r="AF96" s="6">
@@ -35086,23 +37478,23 @@
         <v>#N/A</v>
       </c>
       <c r="AA97" s="6" t="e">
-        <f t="shared" ref="AA97:AE97" si="21">STDEVA(L97:M97)</f>
+        <f t="shared" ref="AA97:AE97" si="25">STDEVA(L97:M97)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB97" s="6" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#NAME?</v>
       </c>
       <c r="AC97" s="6" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#NULL!</v>
       </c>
       <c r="AD97" s="6" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#NUM!</v>
       </c>
       <c r="AE97" s="6" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#REF!</v>
       </c>
       <c r="AF97" s="6">
@@ -35248,23 +37640,23 @@
         <v>#N/A</v>
       </c>
       <c r="AA98" s="6" t="e">
-        <f t="shared" ref="AA98:AE98" si="22">STDEVPA(L98:M98)</f>
+        <f t="shared" ref="AA98:AE98" si="26">STDEVPA(L98:M98)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB98" s="6" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>#NAME?</v>
       </c>
       <c r="AC98" s="6" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>#NULL!</v>
       </c>
       <c r="AD98" s="6" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
       <c r="AE98" s="6" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>#REF!</v>
       </c>
       <c r="AF98" s="6">
@@ -35452,27 +37844,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z108" s="6" t="e">
-        <f t="shared" ref="Z108:AE108" si="23">_xlfn.VAR.P(K108:L108)</f>
+        <f t="shared" ref="Z108:AE108" si="27">_xlfn.VAR.P(K108:L108)</f>
         <v>#N/A</v>
       </c>
       <c r="AA108" s="6" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB108" s="6" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#NAME?</v>
       </c>
       <c r="AC108" s="6" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#NULL!</v>
       </c>
       <c r="AD108" s="6" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#NUM!</v>
       </c>
       <c r="AE108" s="6" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#REF!</v>
       </c>
       <c r="AF108" s="6">
@@ -35614,27 +38006,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z109" s="6" t="e">
-        <f t="shared" ref="Z109:AE109" si="24">_xlfn.VAR.S(K109:L109)</f>
+        <f t="shared" ref="Z109:AE109" si="28">_xlfn.VAR.S(K109:L109)</f>
         <v>#N/A</v>
       </c>
       <c r="AA109" s="6" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB109" s="6" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>#NAME?</v>
       </c>
       <c r="AC109" s="6" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>#NULL!</v>
       </c>
       <c r="AD109" s="6" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>#NUM!</v>
       </c>
       <c r="AE109" s="6" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>#REF!</v>
       </c>
       <c r="AF109" s="6">
@@ -35776,27 +38168,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z110" s="6" t="e">
-        <f t="shared" ref="Z110:AE110" si="25">VARA(K110:L110)</f>
+        <f t="shared" ref="Z110:AE110" si="29">VARA(K110:L110)</f>
         <v>#N/A</v>
       </c>
       <c r="AA110" s="6" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB110" s="6" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#NAME?</v>
       </c>
       <c r="AC110" s="6" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#NULL!</v>
       </c>
       <c r="AD110" s="6" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#NUM!</v>
       </c>
       <c r="AE110" s="6" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#REF!</v>
       </c>
       <c r="AF110" s="6">
@@ -35938,27 +38330,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z111" s="6" t="e">
-        <f t="shared" ref="Z111:AE111" si="26">VARPA(K111:L111)</f>
+        <f t="shared" ref="Z111:AE111" si="30">VARPA(K111:L111)</f>
         <v>#N/A</v>
       </c>
       <c r="AA111" s="6" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB111" s="6" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>#NAME?</v>
       </c>
       <c r="AC111" s="6" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>#NULL!</v>
       </c>
       <c r="AD111" s="6" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>#NUM!</v>
       </c>
       <c r="AE111" s="6" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>#REF!</v>
       </c>
       <c r="AF111" s="6">
@@ -47903,12 +50295,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -47920,6 +50306,12 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
test(core): Update test cases.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10710"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB80B16A-A7D7-F241-B525-D45E6780C511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5552203-F0E6-5444-ADA0-3B3341C80EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="10400" tabRatio="770" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="27040" windowHeight="17680" tabRatio="770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="511">
   <si>
     <t>ca</t>
   </si>
@@ -1635,7 +1635,7 @@
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1699,6 +1699,13 @@
       <color rgb="FFE6DB74"/>
       <name val="Menlo"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11.3"/>
+      <color rgb="FFE6DB74"/>
+      <name val="Menlo"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1769,7 +1776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1831,6 +1838,7 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2153,8 +2161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV81"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -2166,7 +2174,7 @@
     <col min="5" max="5" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -8169,34 +8177,112 @@
       </c>
     </row>
     <row r="43" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="7" t="s">
         <v>65</v>
       </c>
+      <c r="B43" s="4">
+        <v>1</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1</v>
+      </c>
+      <c r="D43" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E43" s="4">
+        <v>10</v>
+      </c>
+      <c r="F43" s="4">
+        <v>-1</v>
+      </c>
       <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="6"/>
-      <c r="S43" s="6"/>
-      <c r="T43" s="6"/>
-      <c r="U43" s="6"/>
-      <c r="V43" s="6"/>
-      <c r="W43" s="6"/>
-      <c r="X43" s="6"/>
-      <c r="Y43" s="6"/>
-      <c r="Z43" s="6"/>
-      <c r="AA43" s="6"/>
-      <c r="AB43" s="6"/>
-      <c r="AC43" s="6"/>
-      <c r="AD43" s="6"/>
-      <c r="AE43" s="6"/>
+      <c r="H43" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I43" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J43" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K43" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L43" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M43" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N43" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O43" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P43" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q43" s="6">
+        <f>MDETERM(B43:C44)</f>
+        <v>0</v>
+      </c>
+      <c r="R43" s="6">
+        <f>MDETERM(C43:D44)</f>
+        <v>0</v>
+      </c>
+      <c r="S43" s="6">
+        <f t="shared" ref="R43:AE43" si="48">MDETERM(D43:E44)</f>
+        <v>0</v>
+      </c>
+      <c r="T43" s="6">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="U43" s="6" t="e">
+        <f t="shared" si="48"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V43" s="6" t="e">
+        <f t="shared" si="48"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W43" s="6" t="e">
+        <f t="shared" si="48"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X43" s="6" t="e">
+        <f t="shared" si="48"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y43" s="6" t="e">
+        <f t="shared" si="48"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z43" s="6" t="e">
+        <f t="shared" si="48"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA43" s="6" t="e">
+        <f t="shared" si="48"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB43" s="6" t="e">
+        <f t="shared" si="48"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC43" s="6" t="e">
+        <f t="shared" si="48"/>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD43" s="6" t="e">
+        <f t="shared" si="48"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE43" s="6" t="e">
+        <f t="shared" si="48"/>
+        <v>#REF!</v>
+      </c>
       <c r="AF43" s="9"/>
       <c r="AG43" s="6"/>
       <c r="AH43" s="6"/>
@@ -8215,34 +8301,109 @@
       <c r="AU43" s="6"/>
     </row>
     <row r="44" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="7" t="s">
         <v>66</v>
       </c>
+      <c r="B44" s="4">
+        <v>1</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+      <c r="D44" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E44" s="4">
+        <v>10</v>
+      </c>
+      <c r="F44" s="4">
+        <v>-1</v>
+      </c>
       <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="6"/>
+      <c r="H44" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I44" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K44" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L44" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M44" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N44" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O44" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P44" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q44" s="6">
+        <f t="array" ref="Q44">MINVERSE(B44:C45)</f>
+        <v>1</v>
+      </c>
       <c r="R44" s="6"/>
-      <c r="S44" s="6"/>
-      <c r="T44" s="6"/>
-      <c r="U44" s="6"/>
-      <c r="V44" s="6"/>
-      <c r="W44" s="6"/>
-      <c r="X44" s="6"/>
-      <c r="Y44" s="6"/>
-      <c r="Z44" s="6"/>
-      <c r="AA44" s="6"/>
-      <c r="AB44" s="6"/>
-      <c r="AC44" s="6"/>
-      <c r="AD44" s="6"/>
-      <c r="AE44" s="6"/>
+      <c r="S44" s="6" t="e" cm="1">
+        <f t="array" ref="S44">MINVERSE(D44:E45)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="T44" s="6" t="e" cm="1">
+        <f t="array" ref="T44">MINVERSE(E44:F45)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="U44" s="6" t="e">
+        <f>SUM(MINVERSE({1,1;1,1}))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="V44" s="6" t="e" cm="1">
+        <f t="array" ref="V44">MINVERSE({1,3,8,5;1,3,6,1})</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W44" s="6" t="e" cm="1">
+        <f t="array" ref="W44">MINVERSE(E44:F45)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="X44" s="6" t="e" cm="1">
+        <f t="array" ref="X44">MINVERSE(F44:G45)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y44" s="6" t="e" cm="1">
+        <f t="array" ref="Y44">MINVERSE(G44:H45)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z44" s="6" t="e" cm="1">
+        <f t="array" ref="Z44">MINVERSE(H44:I45)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA44" s="6" t="e" cm="1">
+        <f t="array" ref="AA44">MINVERSE(I44:J45)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB44" s="6" t="e" cm="1">
+        <f t="array" ref="AB44">MINVERSE(J44:K45)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AC44" s="6" t="e" cm="1">
+        <f t="array" ref="AC44">MINVERSE(K44:L45)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AD44" s="6" t="e" cm="1">
+        <f t="array" ref="AD44">MINVERSE(L44:M45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE44" s="6" t="e" cm="1">
+        <f t="array" ref="AE44">MINVERSE(M44:N45)</f>
+        <v>#NAME?</v>
+      </c>
       <c r="AF44" s="9"/>
       <c r="AG44" s="6"/>
       <c r="AH44" s="6"/>
@@ -8261,35 +8422,116 @@
       <c r="AU44" s="6"/>
     </row>
     <row r="45" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="7" t="s">
         <v>67</v>
       </c>
+      <c r="B45" s="4">
+        <v>0</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
+      <c r="D45" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E45" s="4">
+        <v>10</v>
+      </c>
+      <c r="F45" s="4">
+        <v>-1</v>
+      </c>
       <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="6"/>
-      <c r="R45" s="6"/>
-      <c r="S45" s="6"/>
-      <c r="T45" s="6"/>
-      <c r="U45" s="6"/>
-      <c r="V45" s="6"/>
-      <c r="W45" s="6"/>
-      <c r="X45" s="6"/>
-      <c r="Y45" s="6"/>
-      <c r="Z45" s="6"/>
-      <c r="AA45" s="6"/>
-      <c r="AB45" s="6"/>
-      <c r="AC45" s="6"/>
-      <c r="AD45" s="6"/>
-      <c r="AE45" s="6"/>
-      <c r="AF45" s="9"/>
+      <c r="H45" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I45" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J45" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K45" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L45" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M45" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N45" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O45" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P45" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q45" s="6" t="e" cm="1">
+        <f t="array" ref="Q45">MMULT(B45:C46,D45:E45)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R45" s="6">
+        <f t="array" ref="R45">MMULT(C45:D46,E45:E46)</f>
+        <v>33</v>
+      </c>
+      <c r="S45" s="6" cm="1">
+        <f t="array" ref="S45">MMULT(D45:E45,F45:F46)</f>
+        <v>-32.299999999999997</v>
+      </c>
+      <c r="T45" s="6" t="e" cm="1">
+        <f t="array" ref="T45">MMULT(E45:F45,G45:G46)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U45" s="6" t="e" cm="1">
+        <f t="array" ref="U45">MMULT(F45:G45,H45:H46)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V45" s="6" t="e" cm="1">
+        <f t="array" ref="V45">MMULT(G45:H45,I45:I46)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W45" s="6" t="e" cm="1">
+        <f t="array" ref="W45">MMULT(H45:I45,J45:J46)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X45" s="6" t="e" cm="1">
+        <f t="array" ref="X45">MMULT(I45:J45,K45:K46)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y45" s="6" t="e" cm="1">
+        <f t="array" ref="Y45">MMULT(J45:K45,L45:L46)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z45" s="6" t="e" cm="1">
+        <f t="array" ref="Z45">MMULT(K45:L45,M45:M46)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA45" s="6" t="e" cm="1">
+        <f t="array" ref="AA45">MMULT(L45:M45,N45:N46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB45" s="6" t="e" cm="1">
+        <f t="array" ref="AB45">MMULT(M45:N45,O45:O46)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC45" s="6" t="e" cm="1">
+        <f t="array" ref="AC45">MMULT(N45:O45,P45:P46)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD45" s="6" t="e" cm="1">
+        <f t="array" ref="AD45">MMULT(O45:P45,Q45:Q46)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE45" s="6" t="e" cm="1">
+        <f t="array" ref="AE45">MMULT(P45:Q45,R45:R46)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF45" s="6" cm="1">
+        <f t="array" ref="AF45">MMULT(D45:F45,F45:F47)</f>
+        <v>-32.533999999999999</v>
+      </c>
       <c r="AG45" s="6"/>
       <c r="AH45" s="6"/>
       <c r="AI45" s="6"/>
@@ -8386,27 +8628,27 @@
         <v>0.79999999999999982</v>
       </c>
       <c r="Y46" s="6" t="e">
-        <f t="shared" ref="Y46:AD46" si="48">MOD(J46,K46)</f>
+        <f t="shared" ref="Y46:AD46" si="49">MOD(J46,K46)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z46" s="6" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>#N/A</v>
       </c>
       <c r="AA46" s="6" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB46" s="6" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>#NAME?</v>
       </c>
       <c r="AC46" s="6" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>#NULL!</v>
       </c>
       <c r="AD46" s="6" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>#NUM!</v>
       </c>
       <c r="AE46" s="6" t="e">
@@ -8548,27 +8790,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z47" s="6" t="e">
-        <f t="shared" ref="Z47:AE47" si="49">MROUND(K47,J47)</f>
+        <f t="shared" ref="Z47:AE47" si="50">MROUND(K47,J47)</f>
         <v>#N/A</v>
       </c>
       <c r="AA47" s="6" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB47" s="6" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>#NAME?</v>
       </c>
       <c r="AC47" s="6" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>#NULL!</v>
       </c>
       <c r="AD47" s="6" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>#NUM!</v>
       </c>
       <c r="AE47" s="6" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>#REF!</v>
       </c>
       <c r="AF47" s="9"/>
@@ -8670,50 +8912,165 @@
       <c r="AU48" s="6"/>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.15">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="7" t="s">
         <v>70</v>
       </c>
+      <c r="B49" s="4">
+        <v>0</v>
+      </c>
+      <c r="C49" s="4">
+        <v>2</v>
+      </c>
+      <c r="D49" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E49" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="F49" s="4">
+        <v>-2</v>
+      </c>
       <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="6"/>
-      <c r="R49" s="6"/>
-      <c r="S49" s="6"/>
-      <c r="T49" s="6"/>
-      <c r="U49" s="6"/>
-      <c r="V49" s="6"/>
-      <c r="W49" s="6"/>
-      <c r="X49" s="6"/>
-      <c r="Y49" s="6"/>
-      <c r="Z49" s="6"/>
-      <c r="AA49" s="6"/>
-      <c r="AB49" s="6"/>
-      <c r="AC49" s="6"/>
-      <c r="AD49" s="6"/>
-      <c r="AE49" s="6"/>
-      <c r="AF49" s="9"/>
-      <c r="AG49" s="6"/>
-      <c r="AH49" s="6"/>
-      <c r="AI49" s="6"/>
-      <c r="AJ49" s="6"/>
-      <c r="AK49" s="6"/>
-      <c r="AL49" s="6"/>
-      <c r="AM49" s="6"/>
-      <c r="AN49" s="6"/>
-      <c r="AO49" s="6"/>
-      <c r="AP49" s="6"/>
-      <c r="AQ49" s="6"/>
-      <c r="AR49" s="6"/>
-      <c r="AS49" s="6"/>
-      <c r="AT49" s="6"/>
-      <c r="AU49" s="6"/>
+      <c r="H49" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I49" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J49" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K49" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L49" s="8" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M49" s="8" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="N49" s="8" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="O49" s="8" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P49" s="8" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Q49" s="6" t="e" cm="1">
+        <f t="array" ref="Q49">_xlfn.MUNIT(B49)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R49" s="6">
+        <f t="array" ref="R49">_xlfn.MUNIT(C49)</f>
+        <v>1</v>
+      </c>
+      <c r="S49" s="6">
+        <f t="array" ref="S49">_xlfn.MUNIT(D49)</f>
+        <v>1</v>
+      </c>
+      <c r="T49" s="6" t="e" cm="1">
+        <f t="array" ref="T49">_xlfn.MUNIT(E49)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U49" s="6" t="e" cm="1">
+        <f t="array" ref="U49">_xlfn.MUNIT(F49)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V49" s="6" t="e" cm="1">
+        <f t="array" ref="V49">_xlfn.MUNIT(G49)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W49" s="6" t="e" cm="1">
+        <f t="array" ref="W49">_xlfn.MUNIT(H49)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X49" s="6" cm="1">
+        <f t="array" ref="X49">_xlfn.MUNIT(I49)</f>
+        <v>1</v>
+      </c>
+      <c r="Y49" s="6" t="e" cm="1">
+        <f t="array" ref="Y49">_xlfn.MUNIT(J49)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z49" s="6" t="e" cm="1">
+        <f t="array" ref="Z49">_xlfn.MUNIT(K49)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA49" s="6" t="e" cm="1">
+        <f t="array" ref="AA49">_xlfn.MUNIT(L49)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB49" s="6" t="e" cm="1">
+        <f t="array" ref="AB49">_xlfn.MUNIT(M49)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AC49" s="6" t="e" cm="1">
+        <f t="array" ref="AC49">_xlfn.MUNIT(N49)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AD49" s="6" t="e" cm="1">
+        <f t="array" ref="AD49">_xlfn.MUNIT(O49)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE49" s="6" t="e" cm="1">
+        <f t="array" ref="AE49">_xlfn.MUNIT(P49)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AF49" s="9" t="e">
+        <f t="array" ref="AF49">_xlfn.MUNIT(B49:P49)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG49" s="6" t="e">
+        <f t="array" ref="AG49:AV49">_xlfn.MUNIT(B49:P49)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AH49" s="6">
+        <v>1</v>
+      </c>
+      <c r="AI49" s="6">
+        <v>1</v>
+      </c>
+      <c r="AJ49" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AK49" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL49" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM49" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN49" s="6">
+        <v>1</v>
+      </c>
+      <c r="AO49" s="6" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP49" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ49" s="6" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR49" s="6" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="AS49" s="6" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="AT49" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AU49" s="6" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="AV49" s="4" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
@@ -8767,59 +9124,59 @@
         <v>1</v>
       </c>
       <c r="R50" s="6">
-        <f t="shared" ref="R50:AE50" si="50">ODD(C50)</f>
+        <f t="shared" ref="R50:AE50" si="51">ODD(C50)</f>
         <v>3</v>
       </c>
       <c r="S50" s="6">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>3</v>
       </c>
       <c r="T50" s="6">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-1</v>
       </c>
       <c r="U50" s="6">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-3</v>
       </c>
       <c r="V50" s="6">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1</v>
       </c>
       <c r="W50" s="6" t="e">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>#VALUE!</v>
       </c>
       <c r="X50" s="6">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1</v>
       </c>
       <c r="Y50" s="6" t="e">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z50" s="6" t="e">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>#N/A</v>
       </c>
       <c r="AA50" s="6" t="e">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB50" s="6" t="e">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>#NAME?</v>
       </c>
       <c r="AC50" s="6" t="e">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>#NULL!</v>
       </c>
       <c r="AD50" s="6" t="e">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>#NUM!</v>
       </c>
       <c r="AE50" s="6" t="e">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>#REF!</v>
       </c>
       <c r="AF50" s="9"/>
@@ -9041,27 +9398,27 @@
         <v>1</v>
       </c>
       <c r="Y52" s="6" t="e">
-        <f t="shared" ref="Y52:AD52" si="51">POWER(J52,K52)</f>
+        <f t="shared" ref="Y52:AD52" si="52">POWER(J52,K52)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z52" s="6" t="e">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>#N/A</v>
       </c>
       <c r="AA52" s="6" t="e">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB52" s="6" t="e">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>#NAME?</v>
       </c>
       <c r="AC52" s="6" t="e">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>#NULL!</v>
       </c>
       <c r="AD52" s="6" t="e">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>#NUM!</v>
       </c>
       <c r="AE52" s="6" t="e">
@@ -9376,63 +9733,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q55" s="6">
-        <f t="shared" ref="Q55:AE55" si="52">RADIANS(B55)</f>
+        <f t="shared" ref="Q55:AE55" si="53">RADIANS(B55)</f>
         <v>0</v>
       </c>
       <c r="R55" s="6">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>1.7453292519943295E-2</v>
       </c>
       <c r="S55" s="6">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>4.014257279586958E-2</v>
       </c>
       <c r="T55" s="6">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>0.17453292519943295</v>
       </c>
       <c r="U55" s="6">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-1.7453292519943295E-2</v>
       </c>
       <c r="V55" s="6">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="W55" s="6" t="e">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>#VALUE!</v>
       </c>
       <c r="X55" s="6">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>1.7453292519943295E-2</v>
       </c>
       <c r="Y55" s="6" t="e">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z55" s="6" t="e">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>#N/A</v>
       </c>
       <c r="AA55" s="6" t="e">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB55" s="6" t="e">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>#NAME?</v>
       </c>
       <c r="AC55" s="6" t="e">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>#NULL!</v>
       </c>
       <c r="AD55" s="6" t="e">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>#NUM!</v>
       </c>
       <c r="AE55" s="6" t="e">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>#REF!</v>
       </c>
       <c r="AF55" s="9"/>
@@ -9621,7 +9978,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="Y57" s="6" t="e">
-        <f t="shared" ref="Y57:AC57" ca="1" si="53">RANDBETWEEN(J57,K57)</f>
+        <f t="shared" ref="Y57:AC57" ca="1" si="54">RANDBETWEEN(J57,K57)</f>
         <v>#N/A</v>
       </c>
       <c r="Z57" s="6" t="e">
@@ -9633,11 +9990,11 @@
         <v>#NAME?</v>
       </c>
       <c r="AB57" s="6" t="e">
-        <f t="shared" ca="1" si="53"/>
+        <f t="shared" ca="1" si="54"/>
         <v>#NULL!</v>
       </c>
       <c r="AC57" s="6" t="e">
-        <f t="shared" ca="1" si="53"/>
+        <f t="shared" ca="1" si="54"/>
         <v>#NUM!</v>
       </c>
       <c r="AD57" s="6" t="e">
@@ -9722,15 +10079,15 @@
         <v>LMVLIV</v>
       </c>
       <c r="S58" s="6" t="str">
-        <f t="shared" ref="S58:AE58" si="54">ROMAN(999.9,D58)</f>
+        <f t="shared" ref="S58:AE58" si="55">ROMAN(999.9,D58)</f>
         <v>XMIX</v>
       </c>
       <c r="T58" s="6" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>VMIV</v>
       </c>
       <c r="U58" s="6" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>IM</v>
       </c>
       <c r="V58" s="6" t="str">
@@ -9738,7 +10095,7 @@
         <v>CMXCIX</v>
       </c>
       <c r="W58" s="6" t="e">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>#VALUE!</v>
       </c>
       <c r="X58" s="6" t="str">
@@ -9746,31 +10103,31 @@
         <v>CMXCIX</v>
       </c>
       <c r="Y58" s="6" t="e">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z58" s="6" t="e">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>#N/A</v>
       </c>
       <c r="AA58" s="6" t="e">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB58" s="6" t="e">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>#NAME?</v>
       </c>
       <c r="AC58" s="6" t="e">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>#NULL!</v>
       </c>
       <c r="AD58" s="6" t="e">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>#NUM!</v>
       </c>
       <c r="AE58" s="6" t="e">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>#REF!</v>
       </c>
       <c r="AF58" s="9"/>
@@ -9908,23 +10265,23 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z59" s="6" t="e">
-        <f t="shared" ref="Z59:AD59" si="55">ROUND(K59,J59)</f>
+        <f t="shared" ref="Z59:AD59" si="56">ROUND(K59,J59)</f>
         <v>#N/A</v>
       </c>
       <c r="AA59" s="6" t="e">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB59" s="6" t="e">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>#NAME?</v>
       </c>
       <c r="AC59" s="6" t="e">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>#NULL!</v>
       </c>
       <c r="AD59" s="6" t="e">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>#NUM!</v>
       </c>
       <c r="AE59" s="6" t="e">
@@ -10062,31 +10419,31 @@
         <v>1</v>
       </c>
       <c r="Y60" s="6" t="e">
-        <f t="shared" ref="Y60:AE60" si="56">ROUNDDOWN(J60,I60)</f>
+        <f t="shared" ref="Y60:AE60" si="57">ROUNDDOWN(J60,I60)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z60" s="6" t="e">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>#N/A</v>
       </c>
       <c r="AA60" s="6" t="e">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB60" s="6" t="e">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>#NAME?</v>
       </c>
       <c r="AC60" s="6" t="e">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>#NULL!</v>
       </c>
       <c r="AD60" s="6" t="e">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>#NUM!</v>
       </c>
       <c r="AE60" s="6" t="e">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>#REF!</v>
       </c>
       <c r="AF60" s="9"/>
@@ -10220,31 +10577,31 @@
         <v>1</v>
       </c>
       <c r="Y61" s="6" t="e">
-        <f t="shared" ref="Y61:AE61" si="57">ROUNDUP(J61,I61)</f>
+        <f t="shared" ref="Y61:AE61" si="58">ROUNDUP(J61,I61)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z61" s="6" t="e">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>#N/A</v>
       </c>
       <c r="AA61" s="6" t="e">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB61" s="6" t="e">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>#NAME?</v>
       </c>
       <c r="AC61" s="6" t="e">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>#NULL!</v>
       </c>
       <c r="AD61" s="6" t="e">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>#NUM!</v>
       </c>
       <c r="AE61" s="6" t="e">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>#REF!</v>
       </c>
       <c r="AF61" s="9"/>
@@ -10350,59 +10707,59 @@
         <v>1</v>
       </c>
       <c r="R62" s="6">
-        <f t="shared" ref="R62:AE62" si="58">_xlfn.SEC(C62)</f>
+        <f t="shared" ref="R62:AE62" si="59">_xlfn.SEC(C62)</f>
         <v>1.8508157176809255</v>
       </c>
       <c r="S62" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>-1.500879467460255</v>
       </c>
       <c r="T62" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>-1.1917935066878957</v>
       </c>
       <c r="U62" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>1.8508157176809255</v>
       </c>
       <c r="V62" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>1</v>
       </c>
       <c r="W62" s="6" t="e">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>#VALUE!</v>
       </c>
       <c r="X62" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>1.8508157176809255</v>
       </c>
       <c r="Y62" s="6" t="e">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z62" s="6" t="e">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>#N/A</v>
       </c>
       <c r="AA62" s="6" t="e">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB62" s="6" t="e">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>#NAME?</v>
       </c>
       <c r="AC62" s="6" t="e">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>#NULL!</v>
       </c>
       <c r="AD62" s="6" t="e">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>#NUM!</v>
       </c>
       <c r="AE62" s="6" t="e">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>#REF!</v>
       </c>
       <c r="AF62" s="9"/>
@@ -10508,59 +10865,59 @@
         <v>1</v>
       </c>
       <c r="R63" s="6">
-        <f t="shared" ref="R63:AE63" si="59">_xlfn.SECH(C63)</f>
+        <f t="shared" ref="R63:AE63" si="60">_xlfn.SECH(C63)</f>
         <v>0.64805427366388546</v>
       </c>
       <c r="S63" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>0.19852217514933898</v>
       </c>
       <c r="T63" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>9.0799859337817237E-5</v>
       </c>
       <c r="U63" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>0.64805427366388546</v>
       </c>
       <c r="V63" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="W63" s="6" t="e">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>#VALUE!</v>
       </c>
       <c r="X63" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>0.64805427366388546</v>
       </c>
       <c r="Y63" s="6" t="e">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z63" s="6" t="e">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>#N/A</v>
       </c>
       <c r="AA63" s="6" t="e">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB63" s="6" t="e">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>#NAME?</v>
       </c>
       <c r="AC63" s="6" t="e">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>#NULL!</v>
       </c>
       <c r="AD63" s="6" t="e">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>#NUM!</v>
       </c>
       <c r="AE63" s="6" t="e">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>#REF!</v>
       </c>
       <c r="AF63" s="9"/>
@@ -10713,23 +11070,23 @@
         <v>0</v>
       </c>
       <c r="R65" s="6">
-        <f t="shared" ref="R65:AE65" si="60">SIGN(C65)</f>
+        <f t="shared" ref="R65:AE65" si="61">SIGN(C65)</f>
         <v>1</v>
       </c>
       <c r="S65" s="6">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="T65" s="6">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="U65" s="6">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-1</v>
       </c>
       <c r="V65" s="6">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="W65" s="6" t="e">
@@ -10737,35 +11094,35 @@
         <v>#VALUE!</v>
       </c>
       <c r="X65" s="6">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="Y65" s="6" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z65" s="6" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>#N/A</v>
       </c>
       <c r="AA65" s="6" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB65" s="6" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>#NAME?</v>
       </c>
       <c r="AC65" s="6" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>#NULL!</v>
       </c>
       <c r="AD65" s="6" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>#NUM!</v>
       </c>
       <c r="AE65" s="6" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>#REF!</v>
       </c>
       <c r="AF65" s="9"/>
@@ -10867,63 +11224,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q66" s="6">
-        <f t="shared" ref="Q66:AE66" si="61">SIN(B66)</f>
+        <f t="shared" ref="Q66:AE66" si="62">SIN(B66)</f>
         <v>0</v>
       </c>
       <c r="R66" s="6">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>0.8414709848078965</v>
       </c>
       <c r="S66" s="6">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>0.74570521217672037</v>
       </c>
       <c r="T66" s="6">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>-0.54402111088936977</v>
       </c>
       <c r="U66" s="6">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>-0.8414709848078965</v>
       </c>
       <c r="V66" s="6">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="W66" s="6" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>#VALUE!</v>
       </c>
       <c r="X66" s="6">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>0.8414709848078965</v>
       </c>
       <c r="Y66" s="6" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z66" s="6" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>#N/A</v>
       </c>
       <c r="AA66" s="6" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB66" s="6" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>#NAME?</v>
       </c>
       <c r="AC66" s="6" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>#NULL!</v>
       </c>
       <c r="AD66" s="6" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>#NUM!</v>
       </c>
       <c r="AE66" s="6" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>#REF!</v>
       </c>
       <c r="AF66" s="9"/>
@@ -11025,63 +11382,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q67" s="6">
-        <f t="shared" ref="Q67:AE67" si="62">SINH(B67)</f>
+        <f t="shared" ref="Q67:AE67" si="63">SINH(B67)</f>
         <v>0</v>
       </c>
       <c r="R67" s="6">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>1.1752011936438014</v>
       </c>
       <c r="S67" s="6">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>4.9369618055459572</v>
       </c>
       <c r="T67" s="6">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>11013.232874703393</v>
       </c>
       <c r="U67" s="6">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-1.1752011936438014</v>
       </c>
       <c r="V67" s="6">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="W67" s="6" t="e">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>#VALUE!</v>
       </c>
       <c r="X67" s="6">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>1.1752011936438014</v>
       </c>
       <c r="Y67" s="6" t="e">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z67" s="6" t="e">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>#N/A</v>
       </c>
       <c r="AA67" s="6" t="e">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB67" s="6" t="e">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>#NAME?</v>
       </c>
       <c r="AC67" s="6" t="e">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>#NULL!</v>
       </c>
       <c r="AD67" s="6" t="e">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>#NUM!</v>
       </c>
       <c r="AE67" s="6" t="e">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>#REF!</v>
       </c>
       <c r="AF67" s="9"/>
@@ -11183,63 +11540,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q68" s="6">
-        <f t="shared" ref="Q68:AE68" si="63">SQRT(B68)</f>
+        <f t="shared" ref="Q68:AE68" si="64">SQRT(B68)</f>
         <v>0</v>
       </c>
       <c r="R68" s="6">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="S68" s="6">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>1.51657508881031</v>
       </c>
       <c r="T68" s="6">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>3.1622776601683795</v>
       </c>
       <c r="U68" s="6" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>#NUM!</v>
       </c>
       <c r="V68" s="6">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="W68" s="6" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>#VALUE!</v>
       </c>
       <c r="X68" s="6">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="Y68" s="6" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z68" s="6" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>#N/A</v>
       </c>
       <c r="AA68" s="6" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB68" s="6" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>#NAME?</v>
       </c>
       <c r="AC68" s="6" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>#NULL!</v>
       </c>
       <c r="AD68" s="6" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>#NUM!</v>
       </c>
       <c r="AE68" s="6" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>#REF!</v>
       </c>
       <c r="AF68" s="9"/>
@@ -11345,19 +11702,19 @@
         <v>0</v>
       </c>
       <c r="R69" s="6">
-        <f t="shared" ref="R69:AE69" si="64">SQRTPI(C69)</f>
+        <f t="shared" ref="R69:AE69" si="65">SQRTPI(C69)</f>
         <v>1.7724538509055159</v>
       </c>
       <c r="S69" s="6">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>2.6880593563492088</v>
       </c>
       <c r="T69" s="6">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>5.604991216397929</v>
       </c>
       <c r="U69" s="6" t="e">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>#NUM!</v>
       </c>
       <c r="V69" s="6">
@@ -11373,31 +11730,31 @@
         <v>#VALUE!</v>
       </c>
       <c r="Y69" s="6" t="e">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z69" s="6" t="e">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>#N/A</v>
       </c>
       <c r="AA69" s="6" t="e">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB69" s="6" t="e">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>#NAME?</v>
       </c>
       <c r="AC69" s="6" t="e">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>#NULL!</v>
       </c>
       <c r="AD69" s="6" t="e">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>#NUM!</v>
       </c>
       <c r="AE69" s="6" t="e">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>#REF!</v>
       </c>
       <c r="AF69" s="9"/>
@@ -11744,27 +12101,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z72" s="6" t="e">
-        <f t="shared" ref="Z72:AE72" si="65">SUMIF(I72:J72,I72,K72:L72)</f>
+        <f t="shared" ref="Z72:AE72" si="66">SUMIF(I72:J72,I72,K72:L72)</f>
         <v>#N/A</v>
       </c>
       <c r="AA72" s="6" t="e">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB72" s="6" t="e">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>#NAME?</v>
       </c>
       <c r="AC72" s="6" t="e">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>#NULL!</v>
       </c>
       <c r="AD72" s="6" t="e">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>#NUM!</v>
       </c>
       <c r="AE72" s="6" t="e">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>#REF!</v>
       </c>
       <c r="AF72" s="6">
@@ -12375,63 +12732,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q79" s="6">
-        <f t="shared" ref="Q79:AE79" si="66">TAN(B79)</f>
+        <f t="shared" ref="Q79:AE79" si="67">TAN(B79)</f>
         <v>0</v>
       </c>
       <c r="R79" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>1.5574077246549021</v>
       </c>
       <c r="S79" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>-1.1192136417341327</v>
       </c>
       <c r="T79" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>0.64836082745908674</v>
       </c>
       <c r="U79" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>-1.5574077246549021</v>
       </c>
       <c r="V79" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="W79" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#VALUE!</v>
       </c>
       <c r="X79" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>1.5574077246549021</v>
       </c>
       <c r="Y79" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z79" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#N/A</v>
       </c>
       <c r="AA79" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB79" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#NAME?</v>
       </c>
       <c r="AC79" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#NULL!</v>
       </c>
       <c r="AD79" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#NUM!</v>
       </c>
       <c r="AE79" s="6" t="e">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>#REF!</v>
       </c>
       <c r="AF79" s="9"/>
@@ -12533,63 +12890,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q80" s="6">
-        <f t="shared" ref="Q80:AE80" si="67">TANH(B80)</f>
+        <f t="shared" ref="Q80:AE80" si="68">TANH(B80)</f>
         <v>0</v>
       </c>
       <c r="R80" s="6">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>0.76159415595576485</v>
       </c>
       <c r="S80" s="6">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>0.98009639626619138</v>
       </c>
       <c r="T80" s="6">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>0.99999999587769262</v>
       </c>
       <c r="U80" s="6">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>-0.76159415595576485</v>
       </c>
       <c r="V80" s="6">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="W80" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#VALUE!</v>
       </c>
       <c r="X80" s="6">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>0.76159415595576485</v>
       </c>
       <c r="Y80" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z80" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#N/A</v>
       </c>
       <c r="AA80" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB80" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#NAME?</v>
       </c>
       <c r="AC80" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#NULL!</v>
       </c>
       <c r="AD80" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#NUM!</v>
       </c>
       <c r="AE80" s="6" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>#REF!</v>
       </c>
       <c r="AF80" s="9"/>
@@ -12723,31 +13080,31 @@
         <v>1</v>
       </c>
       <c r="Y81" s="6" t="e">
-        <f t="shared" ref="Y81:AE81" si="68">TRUNC(J81,I81)</f>
+        <f t="shared" ref="Y81:AE81" si="69">TRUNC(J81,I81)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z81" s="6" t="e">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>#N/A</v>
       </c>
       <c r="AA81" s="6" t="e">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB81" s="6" t="e">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>#NAME?</v>
       </c>
       <c r="AC81" s="6" t="e">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>#NULL!</v>
       </c>
       <c r="AD81" s="6" t="e">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>#NUM!</v>
       </c>
       <c r="AE81" s="6" t="e">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>#REF!</v>
       </c>
       <c r="AF81" s="9"/>
@@ -12824,13 +13181,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -13242,7 +13606,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B17">
         <f>[1]Sheet1!$A$1+1</f>
         <v>3</v>
@@ -13262,7 +13626,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B18">
         <f>[1]Sheet1!$A$1+[1]Sheet1!$A$2</f>
         <v>4</v>
@@ -13285,13 +13649,13 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E19">
         <f>D16*3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H20">
         <f t="array" ref="H20:H24">IF(G9:G12&lt;&gt;H10:H13,1,0)</f>
         <v>0</v>
@@ -13300,7 +13664,7 @@
       <c r="N20" s="37"/>
       <c r="O20" s="37"/>
     </row>
-    <row r="21" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="F21">
         <f>C19+1</f>
         <v>1</v>
@@ -13318,7 +13682,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C22" s="24">
         <v>60</v>
       </c>
@@ -13333,7 +13697,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H23">
         <v>1</v>
       </c>
@@ -13357,7 +13721,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H24" t="e">
         <v>#N/A</v>
       </c>
@@ -13366,7 +13730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D25" s="1" t="s">
         <v>503</v>
       </c>
@@ -13385,7 +13749,7 @@
       <c r="N25" s="39"/>
       <c r="O25" s="39"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H26">
         <f>VAL1</f>
         <v>0</v>
@@ -13399,7 +13763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>510</v>
       </c>
@@ -13423,8 +13787,21 @@
       <c r="J27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P27">
+        <f t="array" ref="P27:S30">MINVERSE({1,2,3;2,5,6;7,8,9})</f>
+        <v>0.25</v>
+      </c>
+      <c r="Q27">
+        <v>-0.49999999999999989</v>
+      </c>
+      <c r="R27">
+        <v>0.25</v>
+      </c>
+      <c r="S27" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>507</v>
       </c>
@@ -13449,8 +13826,20 @@
       <c r="J28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P28">
+        <v>-1.9999999999999993</v>
+      </c>
+      <c r="Q28">
+        <v>0.99999999999999967</v>
+      </c>
+      <c r="R28">
+        <v>-2.0451476769410777E-17</v>
+      </c>
+      <c r="S28" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>508</v>
       </c>
@@ -13476,8 +13865,20 @@
       <c r="J29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P29">
+        <v>1.5833333333333328</v>
+      </c>
+      <c r="Q29">
+        <v>-0.49999999999999983</v>
+      </c>
+      <c r="R29">
+        <v>-8.3333333333333301E-2</v>
+      </c>
+      <c r="S29" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>509</v>
       </c>
@@ -13500,8 +13901,30 @@
         <f>AVERAGE(I26:I29, VAL1)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M30" s="40">
+        <f>SUM(MINVERSE({1,2,-1;3,4,-1;0,2,0}))</f>
+        <v>-0.49999999999999978</v>
+      </c>
+      <c r="P30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S30" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P31" cm="1">
+        <f t="array" ref="P31">SUM(_xlfn.MUNIT({1,2;3,4;7,8}))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -13516,6 +13939,17 @@
       <c r="D32">
         <f>CODE("AB")</f>
         <v>65</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="P32" cm="1">
+        <f t="array" ref="P32">_xlfn.MUNIT(O32)</f>
+        <v>1</v>
+      </c>
+      <c r="Q32" t="e" cm="1">
+        <f t="array" ref="Q32">SUM(_xlfn.MUNIT({1,#NUM!;3,4;7,8}))</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -16857,8 +17291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10335504-69CA-E540-89E9-50659E4CE027}">
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:AV30"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -18012,63 +18446,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q28" s="6">
-        <f>NORMSDIST(B28)</f>
+        <f t="shared" ref="Q28:Y28" si="4">NORMSDIST(B28)</f>
         <v>0.5</v>
       </c>
       <c r="R28" s="6">
-        <f>NORMSDIST(C28)</f>
+        <f t="shared" si="4"/>
         <v>0.46017216272297101</v>
       </c>
       <c r="S28" s="6">
-        <f>NORMSDIST(D28)</f>
+        <f t="shared" si="4"/>
         <v>0.75803634777692697</v>
       </c>
       <c r="T28" s="6">
-        <f>NORMSDIST(E28)</f>
+        <f t="shared" si="4"/>
         <v>0.9986501019683699</v>
       </c>
       <c r="U28" s="6">
-        <f>NORMSDIST(F28)</f>
+        <f t="shared" si="4"/>
         <v>0.99996832875816688</v>
       </c>
       <c r="V28" s="6">
-        <f>NORMSDIST(G28)</f>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="W28" s="6">
-        <f>NORMSDIST(H28)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="X28" s="6">
-        <f>NORMSDIST(I28)</f>
+        <f t="shared" si="4"/>
         <v>0.84134474606854304</v>
       </c>
       <c r="Y28" s="6" t="e">
-        <f>NORMSDIST(J28)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z28" s="6" t="e">
-        <f t="shared" ref="Z28:AE28" si="4">NORMSDIST(K28)</f>
+        <f t="shared" ref="Z28:AE28" si="5">NORMSDIST(K28)</f>
         <v>#N/A</v>
       </c>
       <c r="AA28" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB28" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#NAME?</v>
       </c>
       <c r="AC28" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#NULL!</v>
       </c>
       <c r="AD28" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AE28" s="6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
       <c r="AF28" s="6" t="e">
@@ -18173,63 +18607,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q29" s="6" t="e">
-        <f>NORMSINV(B29)</f>
+        <f t="shared" ref="Q29:Y29" si="6">NORMSINV(B29)</f>
         <v>#NUM!</v>
       </c>
       <c r="R29" s="6" t="e">
-        <f>NORMSINV(C29)</f>
+        <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
       <c r="S29" s="6">
-        <f>NORMSINV(D29)</f>
+        <f t="shared" si="6"/>
         <v>0.52440051270804078</v>
       </c>
       <c r="T29" s="6">
-        <f>NORMSINV(E29)</f>
+        <f t="shared" si="6"/>
         <v>-2.8781617390954826</v>
       </c>
       <c r="U29" s="6" t="e">
-        <f>NORMSINV(F29)</f>
+        <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
       <c r="V29" s="6" t="e">
-        <f>NORMSINV(G29)</f>
+        <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
       <c r="W29" s="6" t="e">
-        <f>NORMSINV(H29)</f>
+        <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
       <c r="X29" s="6" t="e">
-        <f>NORMSINV(I29)</f>
+        <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
       <c r="Y29" s="6" t="e">
-        <f>NORMSINV(J29)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z29" s="6" t="e">
-        <f t="shared" ref="Z29:AE29" si="5">NORMSINV(K29)</f>
+        <f t="shared" ref="Z29:AE29" si="7">NORMSINV(K29)</f>
         <v>#N/A</v>
       </c>
       <c r="AA29" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB29" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#NAME?</v>
       </c>
       <c r="AC29" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#NULL!</v>
       </c>
       <c r="AD29" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#NUM!</v>
       </c>
       <c r="AE29" s="6" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
       <c r="AF29" s="6" t="e">
@@ -18370,27 +18804,27 @@
         <v>#N/A</v>
       </c>
       <c r="Z30" s="6" t="e">
-        <f t="shared" ref="Z30:AE30" si="6">PERCENTILE(K30:L30,L30)</f>
+        <f t="shared" ref="Z30:AE30" si="8">PERCENTILE(K30:L30,L30)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AA30" s="6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#NAME?</v>
       </c>
       <c r="AB30" s="6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#NULL!</v>
       </c>
       <c r="AC30" s="6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AD30" s="6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
       <c r="AE30" s="6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
       <c r="AF30" s="6" t="e">
@@ -18517,7 +18951,7 @@
         <v>1.5500000000000003</v>
       </c>
       <c r="T33" s="6" t="e">
-        <f t="shared" ref="S33:U33" si="7">QUARTILE(E33:F33,F33)</f>
+        <f t="shared" ref="T33" si="9">QUARTILE(E33:F33,F33)</f>
         <v>#NUM!</v>
       </c>
       <c r="U33" s="6">
@@ -18537,7 +18971,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="Y33" s="6" t="e">
-        <f t="shared" ref="Y33" si="8">QUARTILE(J33:K33,K33)</f>
+        <f t="shared" ref="Y33" si="10">QUARTILE(J33:K33,K33)</f>
         <v>#N/A</v>
       </c>
       <c r="Z33" s="6" t="e">
@@ -18549,15 +18983,15 @@
         <v>#NAME?</v>
       </c>
       <c r="AB33" s="6" t="e">
-        <f t="shared" ref="AB33" si="9">QUARTILE(M33:N33,N33)</f>
+        <f t="shared" ref="AB33" si="11">QUARTILE(M33:N33,N33)</f>
         <v>#NULL!</v>
       </c>
       <c r="AC33" s="6" t="e">
-        <f t="shared" ref="AC33:AD33" si="10">QUARTILE(N33:O33,O33)</f>
+        <f t="shared" ref="AC33:AD33" si="12">QUARTILE(N33:O33,O33)</f>
         <v>#NUM!</v>
       </c>
       <c r="AD33" s="6" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>#REF!</v>
       </c>
       <c r="AE33" s="6" t="e">
@@ -18711,23 +19145,23 @@
         <v>#N/A</v>
       </c>
       <c r="AA35" s="6" t="e">
-        <f t="shared" ref="AA35:AE35" si="11">STDEV(L35:M35)</f>
+        <f t="shared" ref="AA35:AE35" si="13">STDEV(L35:M35)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB35" s="6" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>#NAME?</v>
       </c>
       <c r="AC35" s="6" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>#NULL!</v>
       </c>
       <c r="AD35" s="6" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
       <c r="AE35" s="6" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>#REF!</v>
       </c>
       <c r="AF35" s="6">
@@ -19046,27 +19480,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z40" s="6" t="e">
-        <f t="shared" ref="Z40:AE40" si="12">VAR(K40:L40)</f>
+        <f t="shared" ref="Z40:AE40" si="14">VAR(K40:L40)</f>
         <v>#N/A</v>
       </c>
       <c r="AA40" s="6" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB40" s="6" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#NAME?</v>
       </c>
       <c r="AC40" s="6" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#NULL!</v>
       </c>
       <c r="AD40" s="6" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AE40" s="6" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#REF!</v>
       </c>
       <c r="AF40" s="6">
@@ -19208,27 +19642,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z41" s="6" t="e">
-        <f t="shared" ref="Z41:AE41" si="13">VARP(K41:L41)</f>
+        <f t="shared" ref="Z41:AE41" si="15">VARP(K41:L41)</f>
         <v>#N/A</v>
       </c>
       <c r="AA41" s="6" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB41" s="6" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#NAME?</v>
       </c>
       <c r="AC41" s="6" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#NULL!</v>
       </c>
       <c r="AD41" s="6" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#NUM!</v>
       </c>
       <c r="AE41" s="6" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#REF!</v>
       </c>
       <c r="AF41" s="6">
@@ -21924,8 +22358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:BJ56"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A14"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -23791,7 +24225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AV59"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -26473,8 +26907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BJ41"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -29414,9 +29848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6C48B-2D77-2542-8BB6-71EF8476BBAF}">
   <dimension ref="A1:E160"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -32341,7 +32773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AV113"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
@@ -35538,7 +35970,7 @@
         <v>#N/A</v>
       </c>
       <c r="AA71" s="6" t="e">
-        <f t="shared" ref="Z71:AE71" si="18">_xlfn.NORM.DIST(L71,J71,H71,1)</f>
+        <f t="shared" ref="AA71:AE71" si="18">_xlfn.NORM.DIST(L71,J71,H71,1)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB71" s="6" t="e">
@@ -35840,7 +36272,7 @@
         <v>0.99996832875816688</v>
       </c>
       <c r="V73" s="6">
-        <f t="shared" ref="V73:AF73" si="20">_xlfn.NORM.S.DIST(G73,1)</f>
+        <f t="shared" ref="V73:AE73" si="20">_xlfn.NORM.S.DIST(G73,1)</f>
         <v>0.5</v>
       </c>
       <c r="W73" s="6">
@@ -35993,7 +36425,7 @@
         <v>0.52440051270804078</v>
       </c>
       <c r="T74" s="6">
-        <f t="shared" ref="S74:AE74" si="21">_xlfn.NORM.S.INV(E74)</f>
+        <f t="shared" ref="T74:AD74" si="21">_xlfn.NORM.S.INV(E74)</f>
         <v>-2.8781617390954826</v>
       </c>
       <c r="U74" s="6" t="e">
@@ -36179,31 +36611,31 @@
         <v>#VALUE!</v>
       </c>
       <c r="Y76" s="6" t="e">
-        <f>_xlfn.PERCENTILE.EXC(J76:K76,K76)</f>
+        <f t="shared" ref="Y76:AE76" si="22">_xlfn.PERCENTILE.EXC(J76:K76,K76)</f>
         <v>#N/A</v>
       </c>
       <c r="Z76" s="6" t="e">
-        <f>_xlfn.PERCENTILE.EXC(K76:L76,L76)</f>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA76" s="6" t="e">
-        <f>_xlfn.PERCENTILE.EXC(L76:M76,M76)</f>
+        <f t="shared" si="22"/>
         <v>#NAME?</v>
       </c>
       <c r="AB76" s="6" t="e">
-        <f>_xlfn.PERCENTILE.EXC(M76:N76,N76)</f>
+        <f t="shared" si="22"/>
         <v>#NULL!</v>
       </c>
       <c r="AC76" s="6" t="e">
-        <f>_xlfn.PERCENTILE.EXC(N76:O76,O76)</f>
+        <f t="shared" si="22"/>
         <v>#NUM!</v>
       </c>
       <c r="AD76" s="6" t="e">
-        <f>_xlfn.PERCENTILE.EXC(O76:P76,P76)</f>
+        <f t="shared" si="22"/>
         <v>#REF!</v>
       </c>
       <c r="AE76" s="6" t="e">
-        <f>_xlfn.PERCENTILE.EXC(P76:Q76,Q76)</f>
+        <f t="shared" si="22"/>
         <v>#REF!</v>
       </c>
       <c r="AF76" s="6" t="e">
@@ -36340,31 +36772,31 @@
         <v>#VALUE!</v>
       </c>
       <c r="Y77" s="6" t="e">
-        <f>_xlfn.PERCENTILE.INC(J77:K77,K77)</f>
+        <f t="shared" ref="Y77:AE77" si="23">_xlfn.PERCENTILE.INC(J77:K77,K77)</f>
         <v>#N/A</v>
       </c>
       <c r="Z77" s="6" t="e">
-        <f>_xlfn.PERCENTILE.INC(K77:L77,L77)</f>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA77" s="6" t="e">
-        <f>_xlfn.PERCENTILE.INC(L77:M77,M77)</f>
+        <f t="shared" si="23"/>
         <v>#NAME?</v>
       </c>
       <c r="AB77" s="6" t="e">
-        <f>_xlfn.PERCENTILE.INC(M77:N77,N77)</f>
+        <f t="shared" si="23"/>
         <v>#NULL!</v>
       </c>
       <c r="AC77" s="6" t="e">
-        <f>_xlfn.PERCENTILE.INC(N77:O77,O77)</f>
+        <f t="shared" si="23"/>
         <v>#NUM!</v>
       </c>
       <c r="AD77" s="6" t="e">
-        <f>_xlfn.PERCENTILE.INC(O77:P77,P77)</f>
+        <f t="shared" si="23"/>
         <v>#REF!</v>
       </c>
       <c r="AE77" s="6" t="e">
-        <f>_xlfn.PERCENTILE.INC(P77:Q77,Q77)</f>
+        <f t="shared" si="23"/>
         <v>#REF!</v>
       </c>
       <c r="AF77" s="6" t="e">
@@ -36624,31 +37056,31 @@
         <v>#VALUE!</v>
       </c>
       <c r="Y85" s="6" t="e">
-        <f>_xlfn.QUARTILE.EXC(J85:K85,K85)</f>
+        <f t="shared" ref="Y85:AE85" si="24">_xlfn.QUARTILE.EXC(J85:K85,K85)</f>
         <v>#N/A</v>
       </c>
       <c r="Z85" s="6" t="e">
-        <f>_xlfn.QUARTILE.EXC(K85:L85,L85)</f>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA85" s="6" t="e">
-        <f>_xlfn.QUARTILE.EXC(L85:M85,M85)</f>
+        <f t="shared" si="24"/>
         <v>#NAME?</v>
       </c>
       <c r="AB85" s="6" t="e">
-        <f>_xlfn.QUARTILE.EXC(M85:N85,N85)</f>
+        <f t="shared" si="24"/>
         <v>#NULL!</v>
       </c>
       <c r="AC85" s="6" t="e">
-        <f>_xlfn.QUARTILE.EXC(N85:O85,O85)</f>
+        <f t="shared" si="24"/>
         <v>#NUM!</v>
       </c>
       <c r="AD85" s="6" t="e">
-        <f>_xlfn.QUARTILE.EXC(O85:P85,P85)</f>
+        <f t="shared" si="24"/>
         <v>#REF!</v>
       </c>
       <c r="AE85" s="6" t="e">
-        <f>_xlfn.QUARTILE.EXC(P85:Q85,Q85)</f>
+        <f t="shared" si="24"/>
         <v>#REF!</v>
       </c>
       <c r="AF85" s="6" t="e">
@@ -36785,31 +37217,31 @@
         <v>#VALUE!</v>
       </c>
       <c r="Y86" s="33" t="e">
-        <f>_xlfn.QUARTILE.INC(J86:K86,K86)</f>
+        <f t="shared" ref="Y86:AE86" si="25">_xlfn.QUARTILE.INC(J86:K86,K86)</f>
         <v>#N/A</v>
       </c>
       <c r="Z86" s="33" t="e">
-        <f>_xlfn.QUARTILE.INC(K86:L86,L86)</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA86" s="33" t="e">
-        <f>_xlfn.QUARTILE.INC(L86:M86,M86)</f>
+        <f t="shared" si="25"/>
         <v>#NAME?</v>
       </c>
       <c r="AB86" s="33" t="e">
-        <f>_xlfn.QUARTILE.INC(M86:N86,N86)</f>
+        <f t="shared" si="25"/>
         <v>#NULL!</v>
       </c>
       <c r="AC86" s="33" t="e">
-        <f>_xlfn.QUARTILE.INC(N86:O86,O86)</f>
+        <f t="shared" si="25"/>
         <v>#NUM!</v>
       </c>
       <c r="AD86" s="33" t="e">
-        <f>_xlfn.QUARTILE.INC(O86:P86,P86)</f>
+        <f t="shared" si="25"/>
         <v>#REF!</v>
       </c>
       <c r="AE86" s="33" t="e">
-        <f>_xlfn.QUARTILE.INC(P86:Q86,Q86)</f>
+        <f t="shared" si="25"/>
         <v>#REF!</v>
       </c>
       <c r="AF86" s="33" t="e">
@@ -36980,31 +37412,31 @@
         <v>-10</v>
       </c>
       <c r="Y93" s="6" t="e">
-        <f t="shared" ref="Y93:AE93" si="22">SMALL($B93:$J93,J93)</f>
+        <f t="shared" ref="Y93:AE93" si="26">SMALL($B93:$J93,J93)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Z93" s="6" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>#N/A</v>
       </c>
       <c r="AA93" s="6" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB93" s="6" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>#NAME?</v>
       </c>
       <c r="AC93" s="6" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>#NULL!</v>
       </c>
       <c r="AD93" s="6" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
       <c r="AE93" s="6" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>#REF!</v>
       </c>
       <c r="AF93" s="6" t="e">
@@ -37154,19 +37586,19 @@
         <v>#N/A</v>
       </c>
       <c r="AA95" s="6" t="e">
-        <f t="shared" ref="AA95:AD95" si="23">_xlfn.STDEV.P(L95:M95)</f>
+        <f t="shared" ref="AA95:AD95" si="27">_xlfn.STDEV.P(L95:M95)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB95" s="6" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#NAME?</v>
       </c>
       <c r="AC95" s="6" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#NULL!</v>
       </c>
       <c r="AD95" s="6" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#NUM!</v>
       </c>
       <c r="AE95" s="6" t="e">
@@ -37316,23 +37748,23 @@
         <v>#N/A</v>
       </c>
       <c r="AA96" s="6" t="e">
-        <f t="shared" ref="AA96:AE96" si="24">_xlfn.STDEV.S(L96:M96)</f>
+        <f t="shared" ref="AA96:AE96" si="28">_xlfn.STDEV.S(L96:M96)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB96" s="6" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>#NAME?</v>
       </c>
       <c r="AC96" s="6" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>#NULL!</v>
       </c>
       <c r="AD96" s="6" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>#NUM!</v>
       </c>
       <c r="AE96" s="6" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>#REF!</v>
       </c>
       <c r="AF96" s="6">
@@ -37478,23 +37910,23 @@
         <v>#N/A</v>
       </c>
       <c r="AA97" s="6" t="e">
-        <f t="shared" ref="AA97:AE97" si="25">STDEVA(L97:M97)</f>
+        <f t="shared" ref="AA97:AE97" si="29">STDEVA(L97:M97)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB97" s="6" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#NAME?</v>
       </c>
       <c r="AC97" s="6" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#NULL!</v>
       </c>
       <c r="AD97" s="6" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#NUM!</v>
       </c>
       <c r="AE97" s="6" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#REF!</v>
       </c>
       <c r="AF97" s="6">
@@ -37640,23 +38072,23 @@
         <v>#N/A</v>
       </c>
       <c r="AA98" s="6" t="e">
-        <f t="shared" ref="AA98:AE98" si="26">STDEVPA(L98:M98)</f>
+        <f t="shared" ref="AA98:AE98" si="30">STDEVPA(L98:M98)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB98" s="6" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>#NAME?</v>
       </c>
       <c r="AC98" s="6" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>#NULL!</v>
       </c>
       <c r="AD98" s="6" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>#NUM!</v>
       </c>
       <c r="AE98" s="6" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>#REF!</v>
       </c>
       <c r="AF98" s="6">
@@ -37844,27 +38276,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z108" s="6" t="e">
-        <f t="shared" ref="Z108:AE108" si="27">_xlfn.VAR.P(K108:L108)</f>
+        <f t="shared" ref="Z108:AE108" si="31">_xlfn.VAR.P(K108:L108)</f>
         <v>#N/A</v>
       </c>
       <c r="AA108" s="6" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB108" s="6" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#NAME?</v>
       </c>
       <c r="AC108" s="6" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#NULL!</v>
       </c>
       <c r="AD108" s="6" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#NUM!</v>
       </c>
       <c r="AE108" s="6" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#REF!</v>
       </c>
       <c r="AF108" s="6">
@@ -38006,27 +38438,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z109" s="6" t="e">
-        <f t="shared" ref="Z109:AE109" si="28">_xlfn.VAR.S(K109:L109)</f>
+        <f t="shared" ref="Z109:AE109" si="32">_xlfn.VAR.S(K109:L109)</f>
         <v>#N/A</v>
       </c>
       <c r="AA109" s="6" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB109" s="6" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#NAME?</v>
       </c>
       <c r="AC109" s="6" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#NULL!</v>
       </c>
       <c r="AD109" s="6" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#NUM!</v>
       </c>
       <c r="AE109" s="6" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#REF!</v>
       </c>
       <c r="AF109" s="6">
@@ -38168,27 +38600,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z110" s="6" t="e">
-        <f t="shared" ref="Z110:AE110" si="29">VARA(K110:L110)</f>
+        <f t="shared" ref="Z110:AE110" si="33">VARA(K110:L110)</f>
         <v>#N/A</v>
       </c>
       <c r="AA110" s="6" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB110" s="6" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#NAME?</v>
       </c>
       <c r="AC110" s="6" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#NULL!</v>
       </c>
       <c r="AD110" s="6" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#NUM!</v>
       </c>
       <c r="AE110" s="6" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#REF!</v>
       </c>
       <c r="AF110" s="6">
@@ -38330,27 +38762,27 @@
         <v>#VALUE!</v>
       </c>
       <c r="Z111" s="6" t="e">
-        <f t="shared" ref="Z111:AE111" si="30">VARPA(K111:L111)</f>
+        <f t="shared" ref="Z111:AE111" si="34">VARPA(K111:L111)</f>
         <v>#N/A</v>
       </c>
       <c r="AA111" s="6" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB111" s="6" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#NAME?</v>
       </c>
       <c r="AC111" s="6" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#NULL!</v>
       </c>
       <c r="AD111" s="6" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#NUM!</v>
       </c>
       <c r="AE111" s="6" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#REF!</v>
       </c>
       <c r="AF111" s="6">
@@ -43276,7 +43708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BJ74"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -50295,6 +50727,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q1:AV1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="AG2:AV2"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A57:A59"/>
@@ -50306,12 +50744,6 @@
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="Q1:AV1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="AG2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>